<commit_message>
:up: adicionadas as questoes do pdf 1 de portugues
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q40"/>
+  <dimension ref="A1:Q58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3624,6 +3624,1536 @@
         <v>0</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>UNIRIO</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Considere a frase: “a avenida Rio Branco, &lt;u&gt;via &lt;/u&gt;do Centro da cidade ocupada por estabelecimentos financeiros e comerciais.”.
+A palavra que tem mesmo sentido e classe gramatical de via no trecho original está destacada em:</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Substantivo</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Esta estrada é a melhor &lt;u&gt;via &lt;/u&gt;para chegar a São Paulo</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Eu te aviso &lt;u&gt;via &lt;/u&gt;e-mail</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>Antigamente você &lt;u&gt;via&lt;/u&gt; muita TV em minha casa</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>A segunda &lt;u&gt;via &lt;/u&gt;do documento é sua</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>O jogo será transmitido &lt;u&gt;via &lt;/u&gt;satélite</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>UNIRIO</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Considere-se a seguinte passagem de Texto: “Dir-se-ia que os blocos &lt;u&gt;impostos &lt;/u&gt;são opressivos e obrigatórios”
+A classe da palavra &lt;u&gt;impostos &lt;/u&gt;no trecho acima é a mesma da palavra destacada em:</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Substantivo</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Fácil</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>O Congresso debateu muito, mas autorizou o aumento do &lt;u&gt;imposto &lt;/u&gt;de renda</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>Muitaspessoas se impressionam com qualquer estilo &lt;u&gt;imposto &lt;/u&gt;pela mídia</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>A enfermeira chegoulogo a seguir de um grito esganiçado que foi &lt;u&gt;imposto &lt;/u&gt;pelo futuro pai</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>A mudança damoda é o &lt;u&gt;imposto &lt;/u&gt;que a indústria do pobre lança sobre a vaidade do rico</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>O padre tinha &lt;u&gt;imposto &lt;/u&gt;uma pesada penitência àquele infeliz pecador</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Ocorre a formação do plural de maneira idêntica à que acontece com a palavra irmão
+em</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Substantivo</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Fácil</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>aproximação</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>alemão</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>cirurgião</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>órgão</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>guardião</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P43" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>No trecho do Texto “capazes de sentar, interagir e &lt;u&gt;celebrar &lt;/u&gt;com nossos semelhantes.”, o verbo destacado dá origem ao substantivo derivado celebração, grafado com ç. Os dois verbos que formam substantivos derivados grafados com ç são</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Substantivo</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>combinar, nomear</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>elaborar, agredir</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>permitir, denominar</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>progredir, coroar</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>trair, compreender</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P44" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>O fragmento do texto em que o vocábulo em destaque foi substantivado é:</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Substantivo</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Difícil</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>“sua imagem foi literalmente apagada de fotografias dos líderes da revolução”</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>“A técnica usada para eliminar o Trotsky”</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>“Existe até uma técnica para retocar a imagem em movimento”</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>“Se a prova fotográfica não vale mais nada nestes novos tempos inconfiáveis, a assinaturamuito menos”</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>“E se eu estiver fazendo a barba e escovando os dentes de um impostor, de um eu apócrifo?”</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P45" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Observe a expressão “velhas casas brasileiras”.
+Caso o redator tivesse escrito “casas velhas brasileiras”, o trecho</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Adjetivo</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Fácil</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>permaneceria com o mesmo sentido</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>indicaria que as casas estavam abandonadas</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>mostraria as casas como construções populares</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>inverteria o sentido de &lt;u&gt;casas &lt;/u&gt;e de &lt;u&gt;velhas&lt;/u&gt;</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">passaria a indicar as casas como gastas pelo tempo.ComentáriosNo trecho original, a estrutura </t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>CEFET-RJ</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Em qual dos períodos abaixo, a troca de posição entre a palavra sublinhada e o substantivo a que se refere mantém o sentido?</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Adjetivo</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Fácil</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>&lt;u&gt;Algum &lt;/u&gt;autor desejava a minha opinião sobre o seu trabalho</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>O &lt;u&gt;mesmo &lt;/u&gt;porteiro me entregou o pacote na recepção do hotel</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>Meu pai procurou uma &lt;u&gt;certa &lt;/u&gt;pessoa para me entregar o embrulho</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>Contar histórias é uma &lt;u&gt;prazerosa &lt;/u&gt;forma de aproximar os indivíduos</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>&lt;u&gt;Grandes &lt;/u&gt;poemas épicos servem para perpetuar a cultura de um povo</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P47" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>CEFET-RJ</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>No Texto I, em “Ele me observa, incrédulo” (L. 21), a palavra que substitui o termo destacado, sem haver alteração de sentido, é</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Adjetivo</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>feliz</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>inconsciente</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>indignado</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>cético</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>furioso</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P48" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>BANRISUL</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Implantação do código de ética nas empresas
+Desde a infância, estamos sujeitos à influência de nosso meio social, por intermédio da família, da escola, dos amigos, dos meios de comunicação de massa. Ao nascer, o homem já se defronta com um conjunto de regras, normas e valores aceitos em seu grupo social. As palavras “ética” e “moral” indicam costumes acumulados — conjunto de normas e valores dos grupos sociais em
+um contexto.
+A ética é um conjunto de princípios e disposições cujo objetivo é balizar as ações humanas. A ética existe como uma referência para os seres humanos em sociedade, de modo tal que a sociedade possa se tornar cada vez mais humana. Ela pode e deve ser incorporada pelos indivíduos, sob a forma de uma atitude diante da vida cotidiana. Mas ela não é um conjunto de verdades fixas, imutáveis. A ética se move historicamente, se amplia e se adensa. Para entendermos como isso acontece na história da humanidade, basta lembrarmos que, um dia, a
+escravidão foi considerada "natural".
+Ética é o que diz respeito à ação quando ela é refletida, pensada. A ética preocupa-se com o certo e com o errado, mas não é um conjunto simples de normas de conduta como a moral. Ela promove um estilo de ação que procura refletir sobre o melhor modo de agir que não abale a vida em sociedade e não desrespeite a individualidade dos outros.
+As empresas precisam desenvolver-se de tal forma que a conduta ética de seus integrantes, bem como os valores e convicções primários da organização, se tornem parte de sua cultura. Assim, a ética vem sendo vista como uma espécie de requisito para a sobrevivência das empresas no mundo moderno e pode ser definida como a transparência nas relações e a preocupação com o impacto das suas atividades na sociedade.
+Muitos exemplos poderiam ser citados de empresas que estão começando a valorizar e a alertar seus funcionários sobre a ética. Algumas empresas já implantaram, inclusive, um comitê de ética, o qual se destina à proteção da imagem da companhia. É preciso, portanto, que haja uma conscientização da importância de uma conduta ética ou mesmo a implantação de um código de ética nas organizações, pois a cada dia que passa a ética tem mostrado ser um dos caminhos para o sucesso e para o bem comum, agregando valor moral ao patrimônio da organização.
+O Código de Ética é um instrumento de realização dos princípios, da visão e da missão da empresa. Serve para orientar as ações de seus colaboradores e explicitar a postura social da empresa em face dos diferentes públicos com os quais interage. É da máxima importância que seu conteúdo seja refletido nas atitudes das pessoas a que se dirige e encontre respaldo na alta administração da empresa, que, tanto quanto o último empregado contratado, tem a responsabilidade de vivenciá-lo.
+As relações com os funcionários, desde o processo de contratação, desenvolvimento profissional, lealdade mútua, respeito entre chefes e subordinados, saúde e segurança, propriedade da informação, assédio profissional e sexual, alcoolismo, uso de drogas, entre outros, são aspectos que costumam ser abordados em um Código de Ética. Cumprir horários, entregar o trabalho no prazo, dar o seu melhor ao executar uma tarefa e manter a palavra dada são exemplos de atitudes que mostram aos superiores e aos colegas que o funcionário valoriza
+os princípios éticos da empresa ou da instituição.
+O Código também pode envolver situações de relacionamento com clientes, fornecedores, acionistas, investidores, comunidade vizinha, concorrentes e mídia.
+O Código de Ética pode estabelecer ações de responsabilidade social dirigidas ao desenvolvimento social de comunidades vizinhas, bem como apoio a projetos de educação voltados ao crescimento pessoal e profissional de jovens carentes. Também pode fazer referência à participação da empresa na comunidade, dando diretrizes sobre as relações com os sindicatos, outros órgãos da esfera pública, relações com o governo, entre outras.
+Portanto, conclui-se que o Código de Ética se fundamenta em deveres para com os colegas, clientes, profissão, sociedade e para consigo próprio.
+(MARTINS,Rosemir.UFPR,2003.Disponívelem:https://acervodigital.ufpr.br.Acessoem:16nov.2022.Adaptado)
+No texto, a circunstância apresentada pela palavra ou expressão em destaque está corretamente explicitada, entre colchetes, em:</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Advérbio</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Em breve os estudantes de tecnologia terão a oportunidade de adquirir informações sobremoral e ética em suas aulas. [TEMPO]</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>Jamais saberemos o resultado do concurso se não forem divulgados os gabaritos.[TEMPO/NEGAÇÃO]</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>O bom relacionamento entre os participantes da instituição era esperado pelo gerente por sertão satisfatório o ambiente de trabalho. [INTENSIDADE]</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>O comportamento dos funcionários da empresa encarregados de orientar os candidatos àvaga de escriturário provavelmente é muito eficaz. [MODO]</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>O modo de agir dos empresários é responsável pela importância de sua instituição, uma vezque eles é que gerenciam efetivamente/DE FATO/COM EFEITO os meios econômicos.[afirmação]</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P49" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>As moedas, bem mais portáteis (do que barras de sal), acabariam se tornando o grande meio universal de troca – seja em Roma, seja em qualquer outro lugar. Mas a palavra “salário” segue viva, como um fóssil etimológico.
+A palavra destacada em “bem &lt;mark&gt;&lt;u&gt;mais &lt;/u&gt;&lt;/mark&gt;portáteis” (parágrafo 4) traz para o trecho uma ideia de</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Advérbio</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>adição</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>adversidade</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>comparação</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>extensão</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>soma</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P50" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>O trecho em que a palavra destacada expressa uma opinião do autor é</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Advérbio</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Fácil</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>“&lt;i&gt;Atualmente&lt;/i&gt;, somos mais de 126,4 milhões de brasileiros” (parágrafo 1)</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>“&lt;i&gt;Infelizmente&lt;/i&gt;, basta ter um endereço de e-mail para ser rastreado” (parágrafo 3)</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>“modo como cada sociedade vem &lt;u&gt;paulatinamente &lt;/u&gt;estruturando a sua política” (parágrafo 4)</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>“&lt;u&gt;Independentemente &lt;/u&gt;da demanda de armazenamento de dados de clientes” (parágrafo 5)</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>“época em que todo mundo pode falar &lt;u&gt;permanentemente &lt;/u&gt;o que quer.”(parágrafo 9)</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P51" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>A palavra destacada está corretamente grafada de acordo com a norma-padrão da língua portuguesa em:</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Advérbio</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Fácil</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>A existência de indivíduos com suas diferentes culturas faz com que o mundo se torne muito complexo, &lt;u&gt;mais &lt;/u&gt;essa convivência só se tornará possível se as diferenças forem respeitadas</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>A superlotação das cidades prejudica a qualidade de vida, &lt;u&gt;mais &lt;/u&gt;a busca por melhores oportunidades mantém o processo de migração rural para os centros urbanos</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>A tecnologia nos torna muito dependentes porque precisamos dela em todos os momentos,&lt;u&gt;mais &lt;/u&gt;ela tem proporcionado grandes conquistas para a humanidade</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>As novas tecnologias de comunicação têm contribuído para a vida das pessoas de formadecisiva, &lt;u&gt;mais &lt;/u&gt;precisamente nas relações interpessoais de caráter virtual</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>As recentes discussões a respeito das desigualdades sociais revelam que ainda falta muitopara serem eliminadas, &lt;u&gt;mais &lt;/u&gt;é preciso enfrentar questões fundamentais.ComentáriosBasicamente, a questão pede que identifiquemos a diferença entre o advérbio de intensidade</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P52" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>UNIRIO</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>No trecho “No dia seguinte, &lt;u&gt;os &lt;/u&gt;jornais diriam que fora o mais quente deste verão”, a palavra destacada contribui para</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Artigo</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>especificar o tipo de jornal referido</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>marcar o momento da publicação dos jornais</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>relativizar a função dos jornais</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>impessoalizar os jornais, pois qualquer um daria a notícia</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>tornar ambíguo o sentido do vocábulo “jornais”</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P53" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q53" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>No período “Ah, que minha história fosse como um raio de sol, irresistivelmente louro, quente, vivo, em sua vida de moça reclusa, enlutada, doente.” (L. 9-12), a interjeição em destaque apresenta o efeito expressivo de</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Interjeição</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>retificação</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>espanto</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>realce</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>adversidade</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>descontinuidade</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P54" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>BANRISUL</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Implantação do código de ética nas empresas
+Desde a infância, estamos sujeitos à influência de nosso meio social, por intermédio da família,
+da escola, dos amigos, dos meios de comunicação de massa. Ao nascer, o homem já se defronta
+com um conjunto de regras, normas e valores aceitos em seu grupo social. As palavras “ética” e
+“moral” indicam costumes acumulados — conjunto de normas e valores dos grupos sociais em
+um contexto.
+A ética é um conjunto de princípios e disposições cujo objetivo é balizar as ações humanas. A
+ética existe como uma referência para os seres humanos em sociedade, de modo tal que a
+sociedade possa se tornar cada vez mais humana. Ela pode e deve ser incorporada pelos
+indivíduos, sob a forma de uma atitude diante da vida cotidiana. Mas ela não é um conjunto de
+verdades fixas, imutáveis. A ética se move historicamente, se amplia e se adensa. Para
+entendermos como isso acontece na história da humanidade, basta lembrarmos que, um dia, a
+escravidão foi considerada "natural".
+Ética é o que diz respeito à ação quando ela é refletida, pensada. A ética preocupa-se com o
+certo e com o errado, mas não é um conjunto simples de normas de conduta como a moral. Ela
+promove um estilo de ação que procura refletir sobre o melhor modo de agir que não abale a
+vida em sociedade e não desrespeite a individualidade dos outros.
+As empresas precisam desenvolver-se de tal forma que a conduta ética de seus integrantes, bem
+como os valores e convicções primários da organização, se tornem parte de sua cultura. Assim, a
+ética vem sendo vista como uma espécie de requisito para a sobrevivência das empresas no
+mundo moderno e pode ser definida como a transparência nas relações e a preocupação com o
+impacto das suas atividades na sociedade.
+Muitos exemplos poderiam ser citados de empresas que estão começando a valorizar e a alertar
+seus funcionários sobre a ética. Algumas empresas já implantaram, inclusive, um comitê de ética,
+o qual se destina à proteção da imagem da companhia. É preciso, portanto, que haja uma
+conscientização da importância de uma conduta ética ou mesmo a implantação de um código de
+ética nas organizações, pois a cada dia que passa a ética tem mostrado ser um dos caminhos
+para o sucesso e para o bem comum, agregando valor moral ao patrimônio da organização.
+O Código de Ética é um instrumento de realização dos princípios, da visão e da missão da
+empresa. Serve para orientar as ações de seus colaboradores e explicitar a postura social da
+empresa em face dos diferentes públicos com os quais interage. É da máxima importância que
+seu conteúdo seja refletido nas atitudes das pessoas a que se dirige e encontre respaldo na alta
+administração da empresa, que, tanto quanto o último empregado contratado, tem a
+responsabilidade de vivenciá-lo.
+As relações com os funcionários, desde o processo de contratação, desenvolvimento
+profissional, lealdade mútua, respeito entre chefes e subordinados, saúde e segurança,
+propriedade da informação, assédio profissional e sexual, alcoolismo, uso de drogas, entre
+outros, são aspectos que costumam ser abordados em um Código de Ética. Cumprir horários,
+entregar o trabalho no prazo, dar o seu melhor ao executar uma tarefa e manter a palavra dada
+são exemplos de atitudes que mostram aos superiores e aos colegas que o funcionário valoriza
+os princípios éticos da empresa ou da instituição.
+O Código também pode envolver situações de relacionamento com clientes, fornecedores,
+acionistas, investidores, comunidade vizinha, concorrentes e mídia. O Código de Ética pode
+estabelecer ações de responsabilidade social dirigidas ao desenvolvimento social de
+comunidades vizinhas, bem como apoio a projetos de educação voltados ao crescimento pessoal
+e profissional de jovens carentes. Também pode fazer referência à participação da empresa na
+comunidade, dando diretrizes sobre as relações com os sindicatos, outros órgãos da esfera
+pública, relações com o governo, entre outras.
+Portanto, conclui-se que o Código de Ética se fundamenta em deveres para com os colegas, clientes, profissão, sociedade e para consigo próprio.
+(MARTINS,Rosemir.UFPR,2003.Disponívelem:https://acervodigital.ufpr.br.Acessoem:16nov.2022.Adaptado)
+No texto, a circunstância apresentada pela palavra ou expressão em destaque está corretamente
+explicitada, entre colchetes, em:</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Advérbio</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>Em breve os estudantes de tecnologia terão a oportunidade de adquirir informações sobremoral e ética em suas aulas. [dúvida]</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>Jamais saberemos o resultado do concurso se não forem divulgados os gabaritos.[intensidade]</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>O bom relacionamento entre os participantes da instituição era esperado pelo gerente por sertão satisfatório o ambiente de trabalho. [causa]</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>O comportamento dos funcionários da empresa encarregados de orientar os candidatos àvaga de escriturário provavelmente é muito eficaz. [negação]</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>O modo de agir dos empresários é responsável pela importância de sua instituição, uma vezque eles é que gerenciam efetivamente os meios econômicos. [afirmação]</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q55" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>As moedas, bem mais portáteis (do que barras de sal), acabariam se tornando o grande meio universal de troca – seja em Roma, seja em qualquer outro lugar. Mas a palavra “salário” segue viva, como um fóssil etimológico.
+A palavra destacada em “bem &lt;u&gt;&lt;mark&gt;mais &lt;/mark&gt;&lt;/u&gt;portáteis” (parágrafo 4) traz para o trecho uma ideia de</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Advérbio</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Fácil</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>adição</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>adversidade</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>comparação</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>extensão</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>soma</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P56" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>O trecho em que a palavra destacada expressa uma opinião do autor é</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Advérbio</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Fácil</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>“&lt;u&gt;Atualmente&lt;/u&gt;, somos mais de 126,4 milhões de brasileiros” (parágrafo 1)</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>“&lt;u&gt;Infelizmente&lt;/u&gt;, basta ter um endereço de e-mail para ser rastreado” (parágrafo 3)</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>“modo como cada sociedade vem &lt;u&gt;paulatinamente &lt;/u&gt;estruturando a sua política” (parágrafo 4)</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>“&lt;u&gt;Independentemente &lt;/u&gt;da demanda de armazenamento de dados de clientes” (parágrafo 5)</t>
+        </is>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>“época em que todo mundo pode falar &lt;u&gt;permanentemente&lt;/u&gt; o que quer.”(parágrafo 9)</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P57" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q57" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>A palavra destacada está corretamente grafada de acordo com a norma-padrão da língua portuguesa em:</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Advérbio</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Fácil</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>A existência de indivíduos com suas diferentes culturas faz com que o mundo se torne muitocomplexo, &lt;u&gt;mais &lt;/u&gt;essa convivência só se tornará possível se as diferenças forem respeitadas</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>A superlotação das cidades prejudica a qualidade de vida, &lt;u&gt;mais &lt;/u&gt;a busca por melhoresoportunidades mantém o processo de migração rural para os centros urbanos</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>A tecnologia nos torna muito dependentes porque precisamos dela em todos os momentos, &lt;u&gt;mais &lt;/u&gt;ela tem proporcionado grandes conquistas para a humanidade</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>As novas tecnologias de comunicação têm contribuído para a vida das pessoas de formadecisiva, &lt;u&gt;mais &lt;/u&gt;precisamente nas relações interpessoais de caráter virtual</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>As recentes discussões a respeito das desigualdades sociais revelam que ainda falta muitopara serem eliminadas, &lt;u&gt;mais &lt;/u&gt;é preciso enfrentar questões fundamentais</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P58" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q58" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
:up: adicionadas as questoes do pdf 2 de protugues
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q58"/>
+  <dimension ref="A1:Q81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5154,6 +5154,2235 @@
         <v>0</v>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>À moda brasileira
+1 Estou me vendo debaixo de uma árvore, lendo a pequena história da literatura
+brasileira.
+2 Olavo Bilac! – eu disse em voz alta e de repente parei quase num susto depois que li
+os primeiros versos do soneto à língua portuguesa: Última flor do Lácio, inculta e bela / És, a um
+tempo, esplendor e sepultura.
+3 Fiquei pensando, mas o poeta disse sepultura?! O tal de Lácio eu não sabia onde
+ficava, mas de sepultura eu entendia bem, disso eu entendia, repensei baixando o olhar para a
+terra. Se escrevia (e já escrevia) pequenos contos nessa língua, quer dizer que era a sepultura que
+esperava por esses meus escritos?
+4 Fui falar com meu pai. Comecei por aquelas minhas sondagens antes de chegar até
+onde queria, os tais rodeios que ele ia ouvindo com paciência enquanto enrolava o cigarro de
+palha, fumava nessa época esses cigarros. Comecei por perguntar se minha mãe e ele não tinham
+viajado para o exterior.
+5 Meu pai fixou em mim o olhar verde. Viagens, só pelo Brasil, meus avós é que tinham
+feito aquelas longas viagens de navio, Portugal, França, Itália... Não esquecer que a minha avó,
+Pedrina Perucchi, era italiana, ele acrescentou. Mas por que essa curiosidade?
+6 Sentei-me ao lado dele, respirei fundo e comecei a gaguejar, é que seria tão bom se
+ambos tivessem nascido lá longe e assim eu estaria hoje escrevendo em italiano, italiano! – fiquei
+repetindo e abri o livro que trazia na mão: Olha aí, pai, o poeta escreveu com todas as letras,
+nossa língua é sepultura mesmo, tudo o que a gente fizer vai para debaixo da terra, desaparece!
+7 Calmamente ele pousou o cigarro no cinzeiro ao lado. Pegou os óculos. O soneto é
+muito bonito, disse me encarando com severidade. Feio é isso, filha, isso de querer renegar a
+própria língua. Se você chegar a escrever bem, não precisa ser em italiano ou espanhol ou alemão,
+você ficará na nossa língua mesmo, está me compreendendo? E as traduções? Renegar a língua é
+renegar o país, guarde isso nessa cabecinha. E depois (ele voltou a abrir o livro), olha que beleza o
+que o poeta escreveu em seguida, Amo-te assim, desconhecida e obscura, veja que confissão de
+amor ele fez à nossa língua! Tem mais, ele precisava da rima para sepultura e calhou tão bem essa
+obscura, entendeu agora? – acrescentou e levantou-se. Deu alguns passos e ficou olhando a
+borboleta que entrou na varanda: Já fez a sua lição de casa?
+8 Fechei o livro e recuei. Sempre que meu pai queria mudar de assunto ele mudava de
+lugar: saía da poltrona e ia para a cadeira de vime. Saía da cadeira de vime e ia para a rede ou
+simplesmente começava a andar. Era o sinal, Não quero falar nisso, chega. Então a gente falava
+noutra coisa ou ficava quieta.
+9 Tantos anos depois, quando me avisaram lá do pequeno hotel em Jacareí que ele
+tinha morrido, fiquei pensando nisso, ah! se quando a morte entrou, se nesse instante ele tivesse
+mudado de lugar. Mudar depressa de lugar e de assunto. Depressa, pai, saia da cama e fique na
+cadeira ou vá pra rua e feche a porta!
+(TELLES,LygiaFagundes.Duranteaqueleestranhochá:perdidoseachados.RiodeJaneiro:Rocco,2002,p.109-111.
+Fragmentoadaptado).
+No parágrafo 6, “nossa língua é sepultura mesmo, tudo o que a gente fizer vai para debaixo da
+terra, desaparece!”, o segmento em destaque pode articular-se com o segmento anterior, sem
+alteração do sentido original, empregando-se o conector</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>quando</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>portanto</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>enquanto</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>embora</t>
+        </is>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>ou</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P59" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q59" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>BANRISUL</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Implantação do código de ética nas empresas
+Desde a infância, estamos sujeitos à influência de nosso meio social, por intermédio da família,
+da escola, dos amigos, dos meios de comunicação de massa. Ao nascer, o homem já se defronta
+com um conjunto de regras, normas e valores aceitos em seu grupo social. As palavras “ética” e
+“moral” indicam costumes acumulados — conjunto de normas e valores dos grupos sociais em
+um contexto.
+A ética é um conjunto de princípios e disposições cujo objetivo é balizar as ações humanas. A
+ética existe como uma referência para os seres humanos em sociedade, de modo tal que a
+sociedade possa se tornar cada vez mais humana. Ela pode e deve ser incorporada pelos
+indivíduos, sob a forma de uma atitude diante da vida cotidiana. Mas ela não é um conjunto de
+verdades fixas, imutáveis. A ética se move historicamente, se amplia e se adensa. Para
+entendermos como isso acontece na história da humanidade, basta lembrarmos que, um dia, a
+escravidão foi considerada "natural".
+Ética é o que diz respeito à ação quando ela é refletida, pensada. A ética preocupa-se com o
+certo e com o errado, mas não é um conjunto simples de normas de conduta como a moral. Ela
+promove um estilo de ação que procura refletir sobre o melhor modo de agir que não abale a
+vida em sociedade e não desrespeite a individualidade dos outros.
+As empresas precisam desenvolver-se de tal forma que a conduta ética de seus integrantes, bem
+como os valores e convicções primários da organização, se tornem parte de sua cultura. Assim, a
+ética vem sendo vista como uma espécie de requisito para a sobrevivência das empresas no
+mundo moderno e pode ser definida como a transparência nas relações e a preocupação com o
+impacto das suas atividades na sociedade.
+Muitos exemplos poderiam ser citados de empresas que estão começando a valorizar e a alertar
+seus funcionários sobre a ética. Algumas empresas já implantaram, inclusive, um comitê de ética,
+o qual se destina à proteção da imagem da companhia. É preciso, portanto, que haja uma
+conscientização da importância de uma conduta ética ou mesmo a implantação de um código de
+ética nas organizações, pois a cada dia que passa a ética tem mostrado ser um dos caminhos
+para o sucesso e para o bem comum, agregando valor moral ao patrimônio da organização.
+O Código de Ética é um instrumento de realização dos princípios, da visão e da missão da
+empresa. Serve para orientar as ações de seus colaboradores e explicitar a postura social da
+empresa em face dos diferentes públicos com os quais interage. É da máxima importância que
+seu conteúdo seja refletido nas atitudes das pessoas a que se dirige e encontre respaldo na alta
+administração da empresa, que, tanto quanto o último empregado contratado, tem a
+responsabilidade de vivenciá-lo.
+As relações com os funcionários, desde o processo de contratação, desenvolvimento
+profissional, lealdade mútua, respeito entre chefes e subordinados, saúde e segurança,
+propriedade da informação, assédio profissional e sexual, alcoolismo, uso de drogas, entre
+outros, são aspectos que costumam ser abordados em um Código de Ética. Cumprir horários,
+entregar o trabalho no prazo, dar o seu melhor ao executar uma tarefa e manter a palavra dada
+são exemplos de atitudes que mostram aos superiores e aos colegas que o funcionário valoriza
+os princípios éticos da empresa ou da instituição.
+O Código também pode envolver situações de relacionamento com clientes, fornecedores,
+acionistas, investidores, comunidade vizinha, concorrentes e mídia. O Código de Ética pode
+estabelecer ações de responsabilidade social dirigidas ao desenvolvimento social de
+comunidades vizinhas, bem como apoio a projetos de educação voltados ao crescimento pessoal
+e profissional de jovens carentes. Também pode fazer referência à participação da empresa na
+comunidade, dando diretrizes sobre as relações com os sindicatos, outros órgãos da esfera
+pública, relações com o governo, entre outras.
+Portanto, conclui-se que o Código de Ética se fundamenta em deveres para com os colegas,
+clientes, profissão, sociedade e para consigo próprio.
+(MARTINS,Rosemir.UFPR,2003.Disponívelem:https://acervodigital.ufpr.br.Acessoem:16nov.2022.
+Adaptado)
+O trecho “A ética se move historicamente, se amplia e se adensa” exerce, em relação ao período
+anterior, a função discursiva de</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>contradição</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>explicação</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>gradação</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>negação</t>
+        </is>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>recapitulação</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P60" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>BANRISUL</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Implantação do código de ética nas empresas
+Desde a infância, estamos sujeitos à influência de nosso meio social, por intermédio da família,
+da escola, dos amigos, dos meios de comunicação de massa. Ao nascer, o homem já se defronta
+com um conjunto de regras, normas e valores aceitos em seu grupo social. As palavras “ética” e
+“moral” indicam costumes acumulados — conjunto de normas e valores dos grupos sociais em
+um contexto.
+A ética é um conjunto de princípios e disposições cujo objetivo é balizar as ações humanas. A
+ética existe como uma referência para os seres humanos em sociedade, de modo tal que a
+sociedade possa se tornar cada vez mais humana. Ela pode e deve ser incorporada pelos
+indivíduos, sob a forma de uma atitude diante da vida cotidiana. Mas ela não é um conjunto de
+verdades fixas, imutáveis. A ética se move historicamente, se amplia e se adensa. Para
+entendermos como isso acontece na história da humanidade, basta lembrarmos que, um dia, a
+escravidão foi considerada "natural".
+Ética é o que diz respeito à ação quando ela é refletida, pensada. A ética preocupa-se com o
+certo e com o errado, mas não é um conjunto simples de normas de conduta como a moral. Ela
+promove um estilo de ação que procura refletir sobre o melhor modo de agir que não abale a
+vida em sociedade e não desrespeite a individualidade dos outros.
+As empresas precisam desenvolver-se de tal forma que a conduta ética de seus integrantes, bem
+como os valores e convicções primários da organização, se tornem parte de sua cultura. Assim, a
+ética vem sendo vista como uma espécie de requisito para a sobrevivência das empresas no
+mundo moderno e pode ser definida como a transparência nas relações e a preocupação com o
+impacto das suas atividades na sociedade.
+Muitos exemplos poderiam ser citados de empresas que estão começando a valorizar e a alertar
+seus funcionários sobre a ética. Algumas empresas já implantaram, inclusive, um comitê de ética,
+o qual se destina à proteção da imagem da companhia. É preciso, portanto, que haja uma
+conscientização da importância de uma conduta ética ou mesmo a implantação de um código de
+ética nas organizações, pois a cada dia que passa a ética tem mostrado ser um dos caminhos
+para o sucesso e para o bem comum, agregando valor moral ao patrimônio da organização.
+O Código de Ética é um instrumento de realização dos princípios, da visão e da missão da
+empresa. Serve para orientar as ações de seus colaboradores e explicitar a postura social da
+empresa em face dos diferentes públicos com os quais interage. É da máxima importância que
+seu conteúdo seja refletido nas atitudes das pessoas a que se dirige e encontre respaldo na alta
+administração da empresa, que, tanto quanto o último empregado contratado, tem a
+responsabilidade de vivenciá-lo.
+As relações com os funcionários, desde o processo de contratação, desenvolvimento
+profissional, lealdade mútua, respeito entre chefes e subordinados, saúde e segurança,
+propriedade da informação, assédio profissional e sexual, alcoolismo, uso de drogas, entre
+outros, são aspectos que costumam ser abordados em um Código de Ética. Cumprir horários,
+entregar o trabalho no prazo, dar o seu melhor ao executar uma tarefa e manter a palavra dada
+são exemplos de atitudes que mostram aos superiores e aos colegas que o funcionário valoriza
+os princípios éticos da empresa ou da instituição.
+O Código também pode envolver situações de relacionamento com clientes, fornecedores,
+acionistas, investidores, comunidade vizinha, concorrentes e mídia. O Código de Ética pode
+estabelecer ações de responsabilidade social dirigidas ao desenvolvimento social de
+comunidades vizinhas, bem como apoio a projetos de educação voltados ao crescimento pessoal
+e profissional de jovens carentes. Também pode fazer referência à participação da empresa na
+comunidade, dando diretrizes sobre as relações com os sindicatos, outros órgãos da esfera
+pública, relações com o governo, entre outras.
+Portanto, conclui-se que o Código de Ética se fundamenta em deveres para com os colegas,
+clientes, profissão, sociedade e para consigo próprio.
+(MARTINS,Rosemir.UFPR,2003.Disponívelem:https://acervodigital.ufpr.br.Acessoem:16nov.2022.
+Adaptado)
+No trecho “a conduta ética de seus integrantes, bem como os valores e convicções primários da
+organização”, a expressão destacada veicula a relação lógica de</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>adição</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>concessão</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>conclusão</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>explicação</t>
+        </is>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>temporalidade</t>
+        </is>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P61" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q61" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>BANRISUL</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Implantação do código de ética nas empresas
+Desde a infância, estamos sujeitos à influência de nosso meio social, por intermédio da família,
+da escola, dos amigos, dos meios de comunicação de massa. Ao nascer, o homem já se defronta
+com um conjunto de regras, normas e valores aceitos em seu grupo social. As palavras “ética” e
+“moral” indicam costumes acumulados — conjunto de normas e valores dos grupos sociais em
+um contexto.
+A ética é um conjunto de princípios e disposições cujo objetivo é balizar as ações humanas. A
+ética existe como uma referência para os seres humanos em sociedade, de modo tal que a
+sociedade possa se tornar cada vez mais humana. Ela pode e deve ser incorporada pelos
+indivíduos, sob a forma de uma atitude diante da vida cotidiana. Mas ela não é um conjunto de
+verdades fixas, imutáveis. A ética se move historicamente, se amplia e se adensa. Para
+entendermos como isso acontece na história da humanidade, basta lembrarmos que, um dia, a
+escravidão foi considerada "natural".
+Ética é o que diz respeito à ação quando ela é refletida, pensada. A ética preocupa-se com o
+certo e com o errado, mas não é um conjunto simples de normas de conduta como a moral. Ela
+promove um estilo de ação que procura refletir sobre o melhor modo de agir que não abale a
+vida em sociedade e não desrespeite a individualidade dos outros.
+As empresas precisam desenvolver-se de tal forma que a conduta ética de seus integrantes, bem
+como os valores e convicções primários da organização, se tornem parte de sua cultura. Assim, a
+ética vem sendo vista como uma espécie de requisito para a sobrevivência das empresas no
+mundo moderno e pode ser definida como a transparência nas relações e a preocupação com o
+impacto das suas atividades na sociedade.
+Muitos exemplos poderiam ser citados de empresas que estão começando a valorizar e a alertar
+seus funcionários sobre a ética. Algumas empresas já implantaram, inclusive, um comitê de ética,
+o qual se destina à proteção da imagem da companhia. É preciso, portanto, que haja uma
+conscientização da importância de uma conduta ética ou mesmo a implantação de um código de
+ética nas organizações, pois a cada dia que passa a ética tem mostrado ser um dos caminhos
+para o sucesso e para o bem comum, agregando valor moral ao patrimônio da organização.
+O Código de Ética é um instrumento de realização dos princípios, da visão e da missão da
+empresa. Serve para orientar as ações de seus colaboradores e explicitar a postura social da
+empresa em face dos diferentes públicos com os quais interage. É da máxima importância que
+seu conteúdo seja refletido nas atitudes das pessoas a que se dirige e encontre respaldo na alta
+administração da empresa, que, tanto quanto o último empregado contratado, tem a
+responsabilidade de vivenciá-lo.
+As relações com os funcionários, desde o processo de contratação, desenvolvimento
+profissional, lealdade mútua, respeito entre chefes e subordinados, saúde e segurança,
+propriedade da informação, assédio profissional e sexual, alcoolismo, uso de drogas, entre
+outros, são aspectos que costumam ser abordados em um Código de Ética. Cumprir horários,
+entregar o trabalho no prazo, dar o seu melhor ao executar uma tarefa e manter a palavra dada
+são exemplos de atitudes que mostram aos superiores e aos colegas que o funcionário valoriza
+os princípios éticos da empresa ou da instituição.
+O Código também pode envolver situações de relacionamento com clientes, fornecedores,
+acionistas, investidores, comunidade vizinha, concorrentes e mídia. O Código de Ética pode
+estabelecer ações de responsabilidade social dirigidas ao desenvolvimento social de
+comunidades vizinhas, bem como apoio a projetos de educação voltados ao crescimento pessoal
+e profissional de jovens carentes. Também pode fazer referência à participação da empresa na
+comunidade, dando diretrizes sobre as relações com os sindicatos, outros órgãos da esfera
+pública, relações com o governo, entre outras.
+Portanto, conclui-se que o Código de Ética se fundamenta em deveres para com os colegas,
+clientes, profissão, sociedade e para consigo próprio.
+(MARTINS,Rosemir.UFPR,2003.Disponívelem:https://acervodigital.ufpr.br.Acessoem:16nov.2022.
+Adaptado)
+No trecho “É preciso, portanto, que haja uma conscientização da importância de uma conduta
+ética”, a palavra destacada expressa a ideia de</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>alternância</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>causa</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>condição</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>conclusão</t>
+        </is>
+      </c>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>contradição</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P62" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q62" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>AgeRIO</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Eu sei, mas não devia&lt;/b&gt;
+Eu sei que a gente se acostuma. Mas não devia. A gente se acostuma a morar em apartamentos
+de fundos e a não ter outra vista que não as janelas ao redor. E, porque não tem vista, logo se
+acostuma a não olhar para fora. E, porque não olha para fora, logo se acostuma a não abrir de
+todo as cortinas. E, porque não abre as cortinas, logo se acostuma a acender mais cedo a luz. E,
+à medida que se acostuma, esquece o sol, esquece o ar, esquece a amplidão.
+A gente se acostuma a acordar de manhã sobressaltado porque está na hora. A tomar o café
+correndo porque está atrasado. A ler o jornal no ônibus porque não pode perder o tempo da
+viagem. A comer sanduíche porque não dá para almoçar. A sair do trabalho porque já é noite. A
+cochilar no ônibus porque está cansado. A deitar cedo e dormir pesado sem ter vivido o dia.
+A gente se acostuma a abrir o jornal e a ler sobre a guerra. E, aceitando a guerra, aceita os
+mortos e que haja números para os mortos. E, aceitando os números, aceita não acreditar nas
+negociações de paz. E, não acreditando nas negociações de paz, aceita ler todo dia da guerra,
+dos números, da longa duração.
+A gente se acostuma a esperar o dia inteiro e ouvir no telefone: hoje não posso ir. A sorrir para
+as pessoas sem receber um sorriso de volta. A ser ignorado quando precisava tanto ser visto.
+A gente se acostuma a pagar por tudo o que deseja e o de que necessita. E a lutar para ganhar
+o dinheiro com que pagar. E a ganhar menos do que precisa. E a fazer fila para pagar. E a pagar
+mais do que as coisas valem. E a saber que cada vez paga mais. E a procurar mais trabalho, para
+ganhar mais dinheiro, para ter com que pagar nas filas em que se cobra.
+A gente se acostuma a andar na rua e ver cartazes. A abrir as revistas e ver anúncios. A ligar a
+televisão e assistir a comerciais. A ir ao cinema e engolir publicidade. A ser instigado, conduzido,
+desnorteado, lançado na infindável catarata dos produtos.
+A gente se acostuma à poluição. Às salas fechadas de ar-condicionado e cheiro de cigarro. À luz
+artificial de ligeiro tremor. Ao choque que os olhos levam na luz natural. Às bactérias da água
+potável. À contaminação da água do mar. À lenta morte dos rios. Se acostuma a não ouvir
+passarinho, a não ter galo de madrugada, a temer a hidrofobia dos cães, a não colher fruta no
+pé, a não ter sequer uma planta.
+A gente se acostuma a coisas de mais, para não sofrer. Em doses pequenas, tentando não
+perceber, vai afastando uma dor aqui, um ressentimento ali, uma revolta acolá. Se o cinema está
+cheio, a gente senta na primeira fila e torce um pouco o pescoço. Se a praia está contaminada, a
+gente molha só os pés e sua no resto do corpo. Se o trabalho está duro, a gente se consola
+pensando no fim de semana. E se, no fim de semana, não há muito o que fazer, a gente vai
+dormir cedo e ainda fica satisfeito porque tem sempre sono atrasado.
+A gente se acostuma para não se ralar na aspereza, para preservar a pele. Se acostuma para
+evitar feridas, sangramentos, para esquivar-se de faca e baioneta, para poupar o peito. A gente
+se acostuma para poupar a vida. Que aos poucos se gasta, e que, gasta de tanto acostumar, se
+perde de si mesma.
+(COLASANTI,M.Eusei,masnãodevia.RiodeJaneiro:RoccoEditora,1996.p.9.Adaptado)
+“A gente se acostuma a abrir o jornal e a ler sobre a guerra. E, &lt;u&gt;aceitando a guerra&lt;/u&gt;, aceita os
+mortos” (parágrafo
+Nesse trecho, a oração destacada apresenta, em relação à seguinte, o valor semântico de</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>causa</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>concessão</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>comparação</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>conformidade</t>
+        </is>
+      </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>consequência</t>
+        </is>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P63" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q63" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Agente Comercial</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Entenda o que édeepfakee saiba como se proteger&lt;/b&gt;
+Vídeos que viralizam nas redes sociais mostrando figuras públicas em situações quase
+inacreditáveis são verdadeiros? Afinal de contas tudo parece tão real... A resposta é não, pois se
+trata de uma “deepfake”,“falsificação profunda” em português, que, como a tradução indica, é
+tão bem feita que pode enganar até os mais atentos. Segundo estudo de uma empresa de
+segurança, 65% dos brasileiros ignoram a sua existência e 71% não reconhecem quando um
+vídeo foi editado digitalmente usando essa técnica.
+O que muita gente não sabe, porém, é que esse tipo de golpe, além de manipular vídeos com
+celebridades e políticos famosos, também prejudica empresas e cidadãos comuns, que podem
+ser envolvidos em fraudes de identidade e extorsões.
+“Deepfakepode ser definida como a criação de vídeos e áudios falsos por meio de inteligência
+artificial”, explica um especialista de segurança cibernética e fraude. A prática costuma utilizar um
+vídeo de referência e a face (ou corpo) de outra pessoa, que não fazia parte do vídeo original.
+Criam-se áudios falsos, fazendo a inteligência artificial aprender como uma pessoa fala e, a partir
+daí, obter uma montagem com outras falas, inclusive alterando os lábios para acompanhar as
+palavras que são ditas.
+Esse processo vem evoluindo rapidamente, tornando cada vez mais difícil a sua identificação. Isso
+ocorre porque as novas redes neurais (sistemas de computação que funcionam como neurônios
+do cérebro humano), a evolução da capacidade de processamento e a redução de custos da
+computação em nuvem têm facilitado o acesso a essa tecnologia, contribuindo para aumentar a
+qualidade dos vídeos.
+No entanto, os criminosos não precisam de tanto conhecimento e tecnologia para aplicar seus
+golpes.
+Isso porque deepfakescriadas para serem distribuídas porappsde mensagens não exigem tanta
+qualidade. O perigo é que, para o cidadão comum, a deepfakepode ser o ponto de partida
+para uma fraude financeira, entre outros problemas.
+A recomendação para pessoas físicas se protegerem é diminuir a exposição de fotos com rostos
+e vídeos pessoais na internet. “As redes sociais devem se manter configuradas como privadas, já
+que fotos, áudios ou vídeos disponíveis publicamente podem ser utilizados para alimentar a
+inteligência artificial e engendrardeepfakes.”
+Além disso, ao receber um vídeo suspeito, observe se o rosto e os lábios da pessoa se movem
+em conjunto com o que ela diz. Preste atenção se a fala parece contínua ou se em algum
+momento apresenta cortes entre uma palavra e outra. E considere o contexto — ainda que
+tecnicamente o vídeo esteja muito bem manipulado, avalie se faz sentido que aquela pessoa
+diga o que parece dizer naquele momento.
+Disponívelem:https://estudio.folha.uol.com.br/unico.Acessoem:20out.2022.Adaptado.
+No trecho “que, como a tradução indica, é &lt;u&gt;tão &lt;/u&gt;bem feita &lt;u&gt;que &lt;/u&gt;pode enganar até os mais atentos”,
+as palavras destacadas contribuem para expressar, entre as duas ideias, a relação lógica de</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>adição</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>condição</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>contradição</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>consequência</t>
+        </is>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>temporalidade</t>
+        </is>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P64" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q64" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Agente Comercial</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Pix: é o fim do dinheiro em espécie?&lt;/b&gt;
+O Pix muda a forma como realizamos transações financeiras. Representará realmente o fim do
+DOC e da TED? O boleto bancário está ainda mais ameaçado de extinção? E o velho cheque vai
+resistir a esses novos tempos?
+Abrangente como é, o Pix pode reduzir ou acabar com a circulação das notas de real? Essa é
+uma pergunta sem resposta fácil. O fato é que o avanço das transações financeiras eletrônicas,
+em detrimento do uso do dinheiro em papel, pode ser benéfico para o Brasil, em vários sentidos.
+O Pix tem tudo para ser o empurrãozinho que nos falta para chegarmos a esse cenário.
+E por que o dinheiro em espécie resiste? Talvez você esteja entre aqueles que compram no
+supermercado com cartão de crédito ou usam QR Code para pagar a farmácia. Mas a feira da
+semana e os churros na esquina você paga com “dinheiro vivo”, certo? Um dos fatores que
+escoram a circulação de papel-moeda no Brasil é a informalidade.
+Atrelada a isso está a situação dos desbancarizados. A dificuldade que muita gente teve para
+receber o auxílio emergencial, durante a pandemia, jogou luz sobre um problema notado há
+tempos: a enorme quantidade de brasileiros que não têm acesso a serviços bancários. O pouco
+de dinheiro que entra no orçamento dessas pessoas precisa ser gasto rapidamente para
+subsistência.
+Não há base financeira suficiente para justificar movimentações bancárias. Também pesa para o
+time dos “sem-banco” o baixo nível de educação ou a falta de familiaridade com a tecnologia.
+O fator cultural também favorece a circulação do dinheiro em espécie. É provável que você
+conheça alguém que, mesmo tendo boa renda, prefere pagar boletos ou receber pagamentos
+com cédulas simplesmente por estar acostumado a elas. Para muita gente que faz parte dessa
+turma, dinheiro vivo é dinheiro recebido ou pago na hora. Não é preciso esperar a TED cair ou o
+dia virar para o boleto ser compensado. Isso pesa mais do que a conveniência de se livrar da fila
+da lotérica.
+Embora o Brasil tenha um sistema bancário que suporta vários tipos de transações, o país estava
+ficando para trás no que diz respeito a pagamentos instantâneos. O Pix veio para preencher essa
+lacuna.
+A modalidade permite transações em qualquer horário e dia, incluindo finais de semana e
+feriados.
+Essa característica, por si só, já é capaz de mudar a forma como lidamos com o dinheiro, pois
+implica envio ou recebimento imediato: as transações via Pix são concluídas rapidamente.
+É o fim do papel-moeda? Não é tão simples assim. O Pix não foi idealizado com o propósito
+exclusivo de acabar com os meios de pagamento e transferência atuais, muito menos com o
+papelmoeda, mas para fazer o sistema financeiro do Brasil evoluir e ficar mais competitivo.
+Apesar disso, não é exagero esperar que, à medida que a população incorpore o sistema à sua
+rotina, o uso de DOC, TED, boletos e cartões caia. Eventualmente, algum desses meios poderá
+ser descontinuado, mas isso não acontecerá tão cedo — vide o exemplo do cheque, que não
+“morreu” com a chegada do cartão.
+No caso das cédulas, especialistas do mercado financeiro apontam para uma diminuição de
+circulação, mas não para um futuro próximo em que o papel-moeda deixará de existir. Para que
+esse cenário se torne realidade, é necessário, sobretudo, atacar a desbancarização. O medo ou a
+pouca familiaridade com a tecnologia podem ser obstáculos, mas o Pix é tão interessante para o
+país que o próprio comércio incentiva o público mais resistente a aderir a ele.
+ALECRIM,E.Disponívelem:https://tecnoblog.net/especiais/pix-fim-dinheiro-especie-
+brasil/.Publicadoemnovembrode2020.Acessoem:2dez.2022.Adaptado.
+No trecho “O fato é que o avanço das transações financeiras eletrônicas, em detrimento do uso do dinheiro em papel, pode ser benéfico para o Brasil, em vários sentidos. O Pix tem tudo para ser o empurrãozinho que nos falta para chegarmos a esse cenário.”, a segunda frase expressa, em relação à primeira, a ideia de</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>condição</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>tempo</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>contradição</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>finalidade</t>
+        </is>
+      </c>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>conclusão</t>
+        </is>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P65" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q65" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>UNIRIO</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>No período “Essa estratégia da indústria pode ser vista como inimiga do consumidor, uma vez que o incentiva a adquirir mais produtos sem realmente necessitar deles.”, o conector &lt;u&gt;uma vez que&lt;/u&gt; poderia ser substituído, sem alteração do sentido, por</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>conforme</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>quando</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>como</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>pois</t>
+        </is>
+      </c>
+      <c r="N66" t="inlineStr">
+        <is>
+          <t>se</t>
+        </is>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P66" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q66" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Transpetro</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Em “Como adorasse a mulher, não se vexava de dizer muitas vezes” (Machado de Assis), o conector &lt;u&gt;como &lt;/u&gt;estabelece, com a oração seguinte, uma relação semântica de</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>causa</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>condição</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>contraste</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>comparação</t>
+        </is>
+      </c>
+      <c r="N67" t="inlineStr">
+        <is>
+          <t>consequência</t>
+        </is>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P67" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q67" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS DISTRIBUIDORA S. A</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>No trecho do Texto “Eu nunca mais vou respirar / &lt;u&gt;Se &lt;/u&gt;você não me notar” (l. 13-14), a palavra em destaque introduz a ideia de</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>Fácil</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>adversidade</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>conclusão</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>lugar</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>condição</t>
+        </is>
+      </c>
+      <c r="N68" t="inlineStr">
+        <is>
+          <t>tempo</t>
+        </is>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P68" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q68" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>PETRÓLEO BRASILEIRO S. A</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>No trecho “Conectar pontos distantes do globo só vale a pena se o roteiro for cumprido com o máximo de aproveitamento. A tendência, &lt;u&gt;então&lt;/u&gt;, é que os voos maiores sejam remanejados para momentos menos quentes do dia”, o conector destacado estabelece, com o período anterior,
+uma relação semântica de</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>causa</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>tempo</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>oposição</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>conclusão</t>
+        </is>
+      </c>
+      <c r="N69" t="inlineStr">
+        <is>
+          <t>explicação</t>
+        </is>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P69" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q69" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>IBGE</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>No trecho do Texto “&lt;u&gt;Para que&lt;/u&gt; pudesse enxergar seu caminho à noite, o homem buscou o desenvolvimento de fontes de iluminação artificial.” (L. 9-11), a expressão em destaque pode ser substituída, mantendo-se a mesma relação lógica, por</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>À medida que</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>Já que</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>A fim de que</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>Logo que</t>
+        </is>
+      </c>
+      <c r="N70" t="inlineStr">
+        <is>
+          <t>Desde que</t>
+        </is>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P70" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q70" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>IBGE</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Em “Passamos ao largo. Tomamos distância. Fugimos. Deles, sim. &lt;u&gt;Mas&lt;/u&gt;, no mais fundo das nossas consciências adormecidas, fugimos de nós.”, o conector destacado introduz uma</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>quebra de expectativa</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>causa da sequência anterior</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>dúvida sobre o enunciado</t>
+        </is>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>proporcionalidade de ideias</t>
+        </is>
+      </c>
+      <c r="N71" t="inlineStr">
+        <is>
+          <t>consequência do pensamento antecedente</t>
+        </is>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P71" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q71" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>CEFET-RJ</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>No trecho do Texto “Vou levar [o paletó], &lt;u&gt;apesar &lt;/u&gt;da barriga encolhida”, observa-se, entre as duas orações que o compõem, uma relação de concessão entre as informações, marcada pela palavra destacada.
+Em qual dos períodos a reescritura desse trecho mantém o mesmo sentido?</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>Mesmo que a barriga fique encolhida, vou levar [o paletó]</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>Vou levar [o paletó] porque a barriga está encolhida</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>Como a barriga está encolhida, vou levar [o paletó]</t>
+        </is>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>Por estar com a barriga encolhida, vou levar [o paletó]</t>
+        </is>
+      </c>
+      <c r="N72" t="inlineStr">
+        <is>
+          <t>Vou levar [o paletó], visto que a barriga está encolhida</t>
+        </is>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P72" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q72" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>FINEP</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>No Texto, no trecho “&lt;u&gt;É &lt;/u&gt;a hora de abrir-se profundamente para uma pessoa que não está ali para condenar ou absolver, &lt;u&gt;e &lt;/u&gt;sim para estimular que você escute atentamente a si mesmo &lt;u&gt;e &lt;/u&gt;assim consiga exorcizar seus fantasmas e viver de forma mais desestressada.”, as conjunções destacadas introduzem, respectivamente, orações com o valor semântico de</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>conclusão e alternância</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>concessão e condição</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>oposição e adição</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>explicação e conclusão</t>
+        </is>
+      </c>
+      <c r="N73" t="inlineStr">
+        <is>
+          <t>causa e restrição</t>
+        </is>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P73" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q73" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>CHESF</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>No fragmento: “&lt;u&gt;Contudo&lt;/u&gt;, a fila não é só uma maneira de organizar uma determinada demanda”, a conjunção destacada pode ser substituída, mantendo o mesmo significado, por</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Fácil</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>como</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>pois</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>porém</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>portanto</t>
+        </is>
+      </c>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>por isso</t>
+        </is>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P74" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q74" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>CHESF</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>No período composto: “&lt;u&gt;Enquanto &lt;/u&gt;isso não acontece, as filas continuam se formando", a conjunção destacada estabelece entre as duas orações uma relação de</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>consequência</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>concessão</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>finalidade</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>causa</t>
+        </is>
+      </c>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>tempo</t>
+        </is>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P75" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q75" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>BNDES</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Na passagem “Você tem sido um vizinho muito compreensivo, e eu ando muito relapsa na criação dos meus cachorros. Isso vai mudar!” a conjunção que permite a junção da última oração acima com sua antecedente, sem alterar o sentido, é</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>logo</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>porque</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>mas</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>pois</t>
+        </is>
+      </c>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>embora</t>
+        </is>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P76" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q76" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>FINEP</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Considere a sentença abaixo.
+Mariza saiu de casa atrasada e perdeu o ônibus. As duas orações do período estão unidas pela palavra “e", que, além de indicar adição, introduz a ideia de</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>oposição</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>condição</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>consequência</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>comparação</t>
+        </is>
+      </c>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>união</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P77" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q77" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>BNDES</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>“O diabo é que, de tanto ver, a gente banaliza o olhar.”
+Na linha argumentativa do texto, a oração “que a gente banaliza o olhar” em relação à oração “de tanto ver” encerra uma</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>causa</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>consequência</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>conformidade</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>condição</t>
+        </is>
+      </c>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>concessão</t>
+        </is>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P78" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q78" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>BNDES</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>A conjunção/locução conjuntiva entre parênteses que NÃO expressa a mesma relação de sentido da conjunção/locução conjuntiva destacada é:</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Difícil</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>“&lt;u&gt;assim &lt;/u&gt;como não estamos aqui,”– (bem como)</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>“...&lt;u&gt;quando &lt;/u&gt;procuramos estar com alguém,” – (sempre que)</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>“...&lt;u&gt;porque &lt;/u&gt;gostamos,” – (ao passo que)</t>
+        </is>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>“...&lt;u&gt;para que&lt;/u&gt; elas venham até você.” – (a fim de que)</t>
+        </is>
+      </c>
+      <c r="N79" t="inlineStr">
+        <is>
+          <t>“&lt;u&gt;mas &lt;/u&gt;quem estava procurando por você!” – (porém)</t>
+        </is>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P79" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q79" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Banco do Brasil</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Entenda o que édeepfakee saiba como se proteger&lt;/b&gt;
+Vídeos que viralizam nas redes sociais mostrando figuras públicas em situações quase
+inacreditáveis são verdadeiros? Afinal de contas tudo parece tão real... A resposta é não, pois se
+trata de uma “deepfake”,“falsificação profunda” em português, que, como a tradução indica, é
+tão bem feita que pode enganar até os mais atentos. Segundo estudo de uma empresa de
+segurança, 65% dos brasileiros ignoram a sua existência e 71% não reconhecem quando um
+vídeo foi editado digitalmente usando essa técnica.
+O que muita gente não sabe, porém, é que esse tipo de golpe, além de manipular vídeos com
+celebridades e políticos famosos, também prejudica empresas e cidadãos comuns, que podem
+ser envolvidos em fraudes de identidade e extorsões.
+“Deepfakepode ser definida como a criação de vídeos e áudios falsos por meio de inteligência
+artificial”, explica um especialista de segurança cibernética e fraude. A prática costuma utilizar um
+vídeo de referência e a face (ou corpo) de outra pessoa, que não fazia parte do vídeo original.
+Criam-se áudios falsos, fazendo a inteligência artificial aprender como uma pessoa fala e, a partir
+daí, obter uma montagem com outras falas, inclusive alterando os lábios para acompanhar as
+palavras que são ditas.
+Esse processo vem evoluindo rapidamente, tornando cada vez mais difícil a sua identificação. Isso
+ocorre porque as novas redes neurais (sistemas de computação que funcionam como neurônios
+do cérebro humano), a evolução da capacidade de processamento e a redução de custos da
+computação em nuvem têm facilitado o acesso a essa tecnologia, contribuindo para aumentar a
+==2e5d94==
+qualidade dos vídeos.
+No entanto, os criminosos não precisam de tanto conhecimento e tecnologia para aplicar seus
+golpes.
+Isso porque deepfakescriadas para serem distribuídas porappsde mensagens não exigem tanta
+qualidade. O perigo é que, para o cidadão comum, a deepfakepode ser o ponto de partida
+para uma fraude financeira, entre outros problemas.
+A recomendação para pessoas físicas se protegerem é diminuir a exposição de fotos com rostos
+e vídeos pessoais na internet. “As redes sociais devem se manter configuradas como privadas, já
+que fotos, áudios ou vídeos disponíveis publicamente podem ser utilizados para alimentar a
+inteligência artificial e engendrardeepfakes.”
+Além disso, ao receber um vídeo suspeito, observe se o rosto e os lábios da pessoa se movem
+em conjunto com o que ela diz. Preste atenção se a fala parece contínua ou se em algum
+momento apresenta cortes entre uma palavra e outra. E considere o contexto — ainda que
+tecnicamente o vídeo esteja muito bem manipulado, avalie se faz sentido que aquela pessoa
+diga o que parece dizer naquele momento.
+Disponívelem:https://estudio.folha.uol.com.br/unico.Acessoem:20out.2022.Adaptado.
+No trecho “que, como a tradução indica, é &lt;u&gt;tão &lt;/u&gt;bem feita &lt;u&gt;que &lt;/u&gt;pode enganar até os mais atentos”, as palavras destacadas contribuem para expressar, entre as duas ideias, a relação lógica de</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>adição</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>condição</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>contradição</t>
+        </is>
+      </c>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>consequência</t>
+        </is>
+      </c>
+      <c r="N80" t="inlineStr">
+        <is>
+          <t>temporalidade</t>
+        </is>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P80" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q80" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>UNIRIO</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>No Texto, em “Já um celular tem maior taxa de obsolescência e pode ter de ser substituído em um ano ou dois” (l. 53-55), a palavra &lt;u&gt;Já &lt;/u&gt;apresenta o sentido de</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>tempo</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>exclusão</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>oposição</t>
+        </is>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>intensidade</t>
+        </is>
+      </c>
+      <c r="N81" t="inlineStr">
+        <is>
+          <t>conformidade</t>
+        </is>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P81" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q81" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
:lady_beetle: consertado a captação de assunto do pdf 3 de portugues:
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q81"/>
+  <dimension ref="A1:Q80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -583,7 +583,7 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
         <v>0</v>
@@ -5803,7 +5803,7 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -5821,124 +5821,6 @@
         </is>
       </c>
       <c r="E64" t="inlineStr">
-        <is>
-          <t>&lt;b&gt;Entenda o que édeepfakee saiba como se proteger&lt;/b&gt;
-Vídeos que viralizam nas redes sociais mostrando figuras públicas em situações quase
-inacreditáveis são verdadeiros? Afinal de contas tudo parece tão real... A resposta é não, pois se
-trata de uma “deepfake”,“falsificação profunda” em português, que, como a tradução indica, é
-tão bem feita que pode enganar até os mais atentos. Segundo estudo de uma empresa de
-segurança, 65% dos brasileiros ignoram a sua existência e 71% não reconhecem quando um
-vídeo foi editado digitalmente usando essa técnica.
-O que muita gente não sabe, porém, é que esse tipo de golpe, além de manipular vídeos com
-celebridades e políticos famosos, também prejudica empresas e cidadãos comuns, que podem
-ser envolvidos em fraudes de identidade e extorsões.
-“Deepfakepode ser definida como a criação de vídeos e áudios falsos por meio de inteligência
-artificial”, explica um especialista de segurança cibernética e fraude. A prática costuma utilizar um
-vídeo de referência e a face (ou corpo) de outra pessoa, que não fazia parte do vídeo original.
-Criam-se áudios falsos, fazendo a inteligência artificial aprender como uma pessoa fala e, a partir
-daí, obter uma montagem com outras falas, inclusive alterando os lábios para acompanhar as
-palavras que são ditas.
-Esse processo vem evoluindo rapidamente, tornando cada vez mais difícil a sua identificação. Isso
-ocorre porque as novas redes neurais (sistemas de computação que funcionam como neurônios
-do cérebro humano), a evolução da capacidade de processamento e a redução de custos da
-computação em nuvem têm facilitado o acesso a essa tecnologia, contribuindo para aumentar a
-qualidade dos vídeos.
-No entanto, os criminosos não precisam de tanto conhecimento e tecnologia para aplicar seus
-golpes.
-Isso porque deepfakescriadas para serem distribuídas porappsde mensagens não exigem tanta
-qualidade. O perigo é que, para o cidadão comum, a deepfakepode ser o ponto de partida
-para uma fraude financeira, entre outros problemas.
-A recomendação para pessoas físicas se protegerem é diminuir a exposição de fotos com rostos
-e vídeos pessoais na internet. “As redes sociais devem se manter configuradas como privadas, já
-que fotos, áudios ou vídeos disponíveis publicamente podem ser utilizados para alimentar a
-inteligência artificial e engendrardeepfakes.”
-Além disso, ao receber um vídeo suspeito, observe se o rosto e os lábios da pessoa se movem
-em conjunto com o que ela diz. Preste atenção se a fala parece contínua ou se em algum
-momento apresenta cortes entre uma palavra e outra. E considere o contexto — ainda que
-tecnicamente o vídeo esteja muito bem manipulado, avalie se faz sentido que aquela pessoa
-diga o que parece dizer naquele momento.
-Disponívelem:https://estudio.folha.uol.com.br/unico.Acessoem:20out.2022.Adaptado.
-No trecho “que, como a tradução indica, é &lt;u&gt;tão &lt;/u&gt;bem feita &lt;u&gt;que &lt;/u&gt;pode enganar até os mais atentos”,
-as palavras destacadas contribuem para expressar, entre as duas ideias, a relação lógica de</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>Português</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>Conjunção</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>Médio</t>
-        </is>
-      </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>ME</t>
-        </is>
-      </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>adição</t>
-        </is>
-      </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>condição</t>
-        </is>
-      </c>
-      <c r="L64" t="inlineStr">
-        <is>
-          <t>contradição</t>
-        </is>
-      </c>
-      <c r="M64" t="inlineStr">
-        <is>
-          <t>consequência</t>
-        </is>
-      </c>
-      <c r="N64" t="inlineStr">
-        <is>
-          <t>temporalidade</t>
-        </is>
-      </c>
-      <c r="O64" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="P64" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q64" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>64</v>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>CESGRANRIO</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Agente Comercial</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
         <is>
           <t>&lt;b&gt;Pix: é o fim do dinheiro em espécie?&lt;/b&gt;
 O Pix muda a forma como realizamos transações financeiras. Representará realmente o fim do
@@ -5989,6 +5871,87 @@
 No trecho “O fato é que o avanço das transações financeiras eletrônicas, em detrimento do uso do dinheiro em papel, pode ser benéfico para o Brasil, em vários sentidos. O Pix tem tudo para ser o empurrãozinho que nos falta para chegarmos a esse cenário.”, a segunda frase expressa, em relação à primeira, a ideia de</t>
         </is>
       </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>condição</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>tempo</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>contradição</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>finalidade</t>
+        </is>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>conclusão</t>
+        </is>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P64" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q64" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>65</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>UNIRIO</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>No período “Essa estratégia da indústria pode ser vista como inimiga do consumidor, uma vez que o incentiva a adquirir mais produtos sem realmente necessitar deles.”, o conector &lt;u&gt;uma vez que&lt;/u&gt; poderia ser substituído, sem alteração do sentido, por</t>
+        </is>
+      </c>
       <c r="F65" t="inlineStr">
         <is>
           <t>Português</t>
@@ -6011,32 +5974,32 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>condição</t>
+          <t>conforme</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>tempo</t>
+          <t>quando</t>
         </is>
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>contradição</t>
+          <t>como</t>
         </is>
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>finalidade</t>
+          <t>pois</t>
         </is>
       </c>
       <c r="N65" t="inlineStr">
         <is>
-          <t>conclusão</t>
+          <t>se</t>
         </is>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="P65" t="n">
@@ -6048,7 +6011,7 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -6057,17 +6020,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>UNIRIO</t>
+          <t>Transpetro</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>No período “Essa estratégia da indústria pode ser vista como inimiga do consumidor, uma vez que o incentiva a adquirir mais produtos sem realmente necessitar deles.”, o conector &lt;u&gt;uma vez que&lt;/u&gt; poderia ser substituído, sem alteração do sentido, por</t>
+          <t>Em “Como adorasse a mulher, não se vexava de dizer muitas vezes” (Machado de Assis), o conector &lt;u&gt;como &lt;/u&gt;estabelece, com a oração seguinte, uma relação semântica de</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -6092,32 +6055,32 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>conforme</t>
+          <t>causa</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>quando</t>
+          <t>condição</t>
         </is>
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>como</t>
+          <t>contraste</t>
         </is>
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>pois</t>
+          <t>comparação</t>
         </is>
       </c>
       <c r="N66" t="inlineStr">
         <is>
-          <t>se</t>
+          <t>consequência</t>
         </is>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P66" t="n">
@@ -6129,7 +6092,7 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -6138,7 +6101,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Transpetro</t>
+          <t>LIQUIGÁS DISTRIBUIDORA S. A</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -6148,7 +6111,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Em “Como adorasse a mulher, não se vexava de dizer muitas vezes” (Machado de Assis), o conector &lt;u&gt;como &lt;/u&gt;estabelece, com a oração seguinte, uma relação semântica de</t>
+          <t>No trecho do Texto “Eu nunca mais vou respirar / &lt;u&gt;Se &lt;/u&gt;você não me notar” (l. 13-14), a palavra em destaque introduz a ideia de</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -6163,7 +6126,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Fácil</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
@@ -6173,32 +6136,32 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>causa</t>
+          <t>adversidade</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
         <is>
+          <t>conclusão</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>lugar</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
           <t>condição</t>
         </is>
       </c>
-      <c r="L67" t="inlineStr">
-        <is>
-          <t>contraste</t>
-        </is>
-      </c>
-      <c r="M67" t="inlineStr">
-        <is>
-          <t>comparação</t>
-        </is>
-      </c>
       <c r="N67" t="inlineStr">
         <is>
-          <t>consequência</t>
+          <t>tempo</t>
         </is>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="P67" t="n">
@@ -6210,7 +6173,7 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -6219,17 +6182,18 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>LIQUIGÁS DISTRIBUIDORA S. A</t>
+          <t>PETRÓLEO BRASILEIRO S. A</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>No trecho do Texto “Eu nunca mais vou respirar / &lt;u&gt;Se &lt;/u&gt;você não me notar” (l. 13-14), a palavra em destaque introduz a ideia de</t>
+          <t>No trecho “Conectar pontos distantes do globo só vale a pena se o roteiro for cumprido com o máximo de aproveitamento. A tendência, &lt;u&gt;então&lt;/u&gt;, é que os voos maiores sejam remanejados para momentos menos quentes do dia”, o conector destacado estabelece, com o período anterior,
+uma relação semântica de</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -6244,7 +6208,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Fácil</t>
+          <t>Médio</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
@@ -6254,27 +6218,27 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>adversidade</t>
+          <t>causa</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
         <is>
+          <t>tempo</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>oposição</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
           <t>conclusão</t>
         </is>
       </c>
-      <c r="L68" t="inlineStr">
-        <is>
-          <t>lugar</t>
-        </is>
-      </c>
-      <c r="M68" t="inlineStr">
-        <is>
-          <t>condição</t>
-        </is>
-      </c>
       <c r="N68" t="inlineStr">
         <is>
-          <t>tempo</t>
+          <t>explicação</t>
         </is>
       </c>
       <c r="O68" t="inlineStr">
@@ -6291,7 +6255,7 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
@@ -6300,18 +6264,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>PETRÓLEO BRASILEIRO S. A</t>
+          <t>IBGE</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>No trecho “Conectar pontos distantes do globo só vale a pena se o roteiro for cumprido com o máximo de aproveitamento. A tendência, &lt;u&gt;então&lt;/u&gt;, é que os voos maiores sejam remanejados para momentos menos quentes do dia”, o conector destacado estabelece, com o período anterior,
-uma relação semântica de</t>
+          <t>No trecho do Texto “&lt;u&gt;Para que&lt;/u&gt; pudesse enxergar seu caminho à noite, o homem buscou o desenvolvimento de fontes de iluminação artificial.” (L. 9-11), a expressão em destaque pode ser substituída, mantendo-se a mesma relação lógica, por</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -6336,32 +6299,32 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>causa</t>
+          <t>À medida que</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>tempo</t>
+          <t>Já que</t>
         </is>
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>oposição</t>
+          <t>A fim de que</t>
         </is>
       </c>
       <c r="M69" t="inlineStr">
         <is>
-          <t>conclusão</t>
+          <t>Logo que</t>
         </is>
       </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>explicação</t>
+          <t>Desde que</t>
         </is>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="P69" t="n">
@@ -6373,7 +6336,7 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
@@ -6392,7 +6355,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>No trecho do Texto “&lt;u&gt;Para que&lt;/u&gt; pudesse enxergar seu caminho à noite, o homem buscou o desenvolvimento de fontes de iluminação artificial.” (L. 9-11), a expressão em destaque pode ser substituída, mantendo-se a mesma relação lógica, por</t>
+          <t>Em “Passamos ao largo. Tomamos distância. Fugimos. Deles, sim. &lt;u&gt;Mas&lt;/u&gt;, no mais fundo das nossas consciências adormecidas, fugimos de nós.”, o conector destacado introduz uma</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -6417,32 +6380,32 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>À medida que</t>
+          <t>quebra de expectativa</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>Já que</t>
+          <t>causa da sequência anterior</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>A fim de que</t>
+          <t>dúvida sobre o enunciado</t>
         </is>
       </c>
       <c r="M70" t="inlineStr">
         <is>
-          <t>Logo que</t>
+          <t>proporcionalidade de ideias</t>
         </is>
       </c>
       <c r="N70" t="inlineStr">
         <is>
-          <t>Desde que</t>
+          <t>consequência do pensamento antecedente</t>
         </is>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P70" t="n">
@@ -6454,7 +6417,7 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
@@ -6463,17 +6426,18 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>IBGE</t>
+          <t>CEFET-RJ</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Em “Passamos ao largo. Tomamos distância. Fugimos. Deles, sim. &lt;u&gt;Mas&lt;/u&gt;, no mais fundo das nossas consciências adormecidas, fugimos de nós.”, o conector destacado introduz uma</t>
+          <t>No trecho do Texto “Vou levar [o paletó], &lt;u&gt;apesar &lt;/u&gt;da barriga encolhida”, observa-se, entre as duas orações que o compõem, uma relação de concessão entre as informações, marcada pela palavra destacada.
+Em qual dos períodos a reescritura desse trecho mantém o mesmo sentido?</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -6498,27 +6462,27 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>quebra de expectativa</t>
+          <t>Mesmo que a barriga fique encolhida, vou levar [o paletó]</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>causa da sequência anterior</t>
+          <t>Vou levar [o paletó] porque a barriga está encolhida</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>dúvida sobre o enunciado</t>
+          <t>Como a barriga está encolhida, vou levar [o paletó]</t>
         </is>
       </c>
       <c r="M71" t="inlineStr">
         <is>
-          <t>proporcionalidade de ideias</t>
+          <t>Por estar com a barriga encolhida, vou levar [o paletó]</t>
         </is>
       </c>
       <c r="N71" t="inlineStr">
         <is>
-          <t>consequência do pensamento antecedente</t>
+          <t>Vou levar [o paletó], visto que a barriga está encolhida</t>
         </is>
       </c>
       <c r="O71" t="inlineStr">
@@ -6535,7 +6499,7 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -6544,7 +6508,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>CEFET-RJ</t>
+          <t>FINEP</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -6554,8 +6518,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>No trecho do Texto “Vou levar [o paletó], &lt;u&gt;apesar &lt;/u&gt;da barriga encolhida”, observa-se, entre as duas orações que o compõem, uma relação de concessão entre as informações, marcada pela palavra destacada.
-Em qual dos períodos a reescritura desse trecho mantém o mesmo sentido?</t>
+          <t>No Texto, no trecho “&lt;u&gt;É &lt;/u&gt;a hora de abrir-se profundamente para uma pessoa que não está ali para condenar ou absolver, &lt;u&gt;e &lt;/u&gt;sim para estimular que você escute atentamente a si mesmo &lt;u&gt;e &lt;/u&gt;assim consiga exorcizar seus fantasmas e viver de forma mais desestressada.”, as conjunções destacadas introduzem, respectivamente, orações com o valor semântico de</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -6580,32 +6543,32 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>Mesmo que a barriga fique encolhida, vou levar [o paletó]</t>
+          <t>conclusão e alternância</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>Vou levar [o paletó] porque a barriga está encolhida</t>
+          <t>concessão e condição</t>
         </is>
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Como a barriga está encolhida, vou levar [o paletó]</t>
+          <t>oposição e adição</t>
         </is>
       </c>
       <c r="M72" t="inlineStr">
         <is>
-          <t>Por estar com a barriga encolhida, vou levar [o paletó]</t>
+          <t>explicação e conclusão</t>
         </is>
       </c>
       <c r="N72" t="inlineStr">
         <is>
-          <t>Vou levar [o paletó], visto que a barriga está encolhida</t>
+          <t>causa e restrição</t>
         </is>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="P72" t="n">
@@ -6617,7 +6580,7 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -6626,17 +6589,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>FINEP</t>
+          <t>CHESF</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>2012</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>No Texto, no trecho “&lt;u&gt;É &lt;/u&gt;a hora de abrir-se profundamente para uma pessoa que não está ali para condenar ou absolver, &lt;u&gt;e &lt;/u&gt;sim para estimular que você escute atentamente a si mesmo &lt;u&gt;e &lt;/u&gt;assim consiga exorcizar seus fantasmas e viver de forma mais desestressada.”, as conjunções destacadas introduzem, respectivamente, orações com o valor semântico de</t>
+          <t>No fragmento: “&lt;u&gt;Contudo&lt;/u&gt;, a fila não é só uma maneira de organizar uma determinada demanda”, a conjunção destacada pode ser substituída, mantendo o mesmo significado, por</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -6651,7 +6614,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Fácil</t>
         </is>
       </c>
       <c r="I73" t="inlineStr">
@@ -6661,27 +6624,27 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>conclusão e alternância</t>
+          <t>como</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>concessão e condição</t>
+          <t>pois</t>
         </is>
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>oposição e adição</t>
+          <t>porém</t>
         </is>
       </c>
       <c r="M73" t="inlineStr">
         <is>
-          <t>explicação e conclusão</t>
+          <t>portanto</t>
         </is>
       </c>
       <c r="N73" t="inlineStr">
         <is>
-          <t>causa e restrição</t>
+          <t>por isso</t>
         </is>
       </c>
       <c r="O73" t="inlineStr">
@@ -6698,7 +6661,7 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -6717,7 +6680,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>No fragmento: “&lt;u&gt;Contudo&lt;/u&gt;, a fila não é só uma maneira de organizar uma determinada demanda”, a conjunção destacada pode ser substituída, mantendo o mesmo significado, por</t>
+          <t>No período composto: “&lt;u&gt;Enquanto &lt;/u&gt;isso não acontece, as filas continuam se formando", a conjunção destacada estabelece entre as duas orações uma relação de</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6732,7 +6695,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Fácil</t>
+          <t>Médio</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
@@ -6742,32 +6705,32 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>como</t>
+          <t>consequência</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>pois</t>
+          <t>concessão</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>porém</t>
+          <t>finalidade</t>
         </is>
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>portanto</t>
+          <t>causa</t>
         </is>
       </c>
       <c r="N74" t="inlineStr">
         <is>
-          <t>por isso</t>
+          <t>tempo</t>
         </is>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>E</t>
         </is>
       </c>
       <c r="P74" t="n">
@@ -6779,7 +6742,7 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -6788,17 +6751,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>CHESF</t>
+          <t>BNDES</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2012</t>
+          <t>2011</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>No período composto: “&lt;u&gt;Enquanto &lt;/u&gt;isso não acontece, as filas continuam se formando", a conjunção destacada estabelece entre as duas orações uma relação de</t>
+          <t>Na passagem “Você tem sido um vizinho muito compreensivo, e eu ando muito relapsa na criação dos meus cachorros. Isso vai mudar!” a conjunção que permite a junção da última oração acima com sua antecedente, sem alterar o sentido, é</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6823,32 +6786,32 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>consequência</t>
+          <t>logo</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>concessão</t>
+          <t>porque</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>finalidade</t>
+          <t>mas</t>
         </is>
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>causa</t>
+          <t>pois</t>
         </is>
       </c>
       <c r="N75" t="inlineStr">
         <is>
-          <t>tempo</t>
+          <t>embora</t>
         </is>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>C</t>
         </is>
       </c>
       <c r="P75" t="n">
@@ -6860,7 +6823,7 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -6869,7 +6832,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>BNDES</t>
+          <t>FINEP</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -6879,7 +6842,8 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Na passagem “Você tem sido um vizinho muito compreensivo, e eu ando muito relapsa na criação dos meus cachorros. Isso vai mudar!” a conjunção que permite a junção da última oração acima com sua antecedente, sem alterar o sentido, é</t>
+          <t>Considere a sentença abaixo.
+Mariza saiu de casa atrasada e perdeu o ônibus. As duas orações do período estão unidas pela palavra “e", que, além de indicar adição, introduz a ideia de</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6904,27 +6868,27 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>logo</t>
+          <t>oposição</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>porque</t>
+          <t>condição</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>mas</t>
+          <t>consequência</t>
         </is>
       </c>
       <c r="M76" t="inlineStr">
         <is>
-          <t>pois</t>
+          <t>comparação</t>
         </is>
       </c>
       <c r="N76" t="inlineStr">
         <is>
-          <t>embora</t>
+          <t>união</t>
         </is>
       </c>
       <c r="O76" t="inlineStr">
@@ -6941,7 +6905,7 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -6950,7 +6914,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>FINEP</t>
+          <t>BNDES</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -6960,8 +6924,8 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Considere a sentença abaixo.
-Mariza saiu de casa atrasada e perdeu o ônibus. As duas orações do período estão unidas pela palavra “e", que, além de indicar adição, introduz a ideia de</t>
+          <t>“O diabo é que, de tanto ver, a gente banaliza o olhar.”
+Na linha argumentativa do texto, a oração “que a gente banaliza o olhar” em relação à oração “de tanto ver” encerra uma</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6986,32 +6950,32 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>oposição</t>
+          <t>causa</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
         <is>
+          <t>consequência</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>conformidade</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
           <t>condição</t>
         </is>
       </c>
-      <c r="L77" t="inlineStr">
-        <is>
-          <t>consequência</t>
-        </is>
-      </c>
-      <c r="M77" t="inlineStr">
-        <is>
-          <t>comparação</t>
-        </is>
-      </c>
       <c r="N77" t="inlineStr">
         <is>
-          <t>união</t>
+          <t>concessão</t>
         </is>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="P77" t="n">
@@ -7023,7 +6987,7 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -7042,8 +7006,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>“O diabo é que, de tanto ver, a gente banaliza o olhar.”
-Na linha argumentativa do texto, a oração “que a gente banaliza o olhar” em relação à oração “de tanto ver” encerra uma</t>
+          <t>A conjunção/locução conjuntiva entre parênteses que NÃO expressa a mesma relação de sentido da conjunção/locução conjuntiva destacada é:</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -7058,7 +7021,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Difícil</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
@@ -7068,32 +7031,32 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>causa</t>
+          <t>“&lt;u&gt;assim &lt;/u&gt;como não estamos aqui,”– (bem como)</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>consequência</t>
+          <t>“...&lt;u&gt;quando &lt;/u&gt;procuramos estar com alguém,” – (sempre que)</t>
         </is>
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>conformidade</t>
+          <t>“...&lt;u&gt;porque &lt;/u&gt;gostamos,” – (ao passo que)</t>
         </is>
       </c>
       <c r="M78" t="inlineStr">
         <is>
-          <t>condição</t>
+          <t>“...&lt;u&gt;para que&lt;/u&gt; elas venham até você.” – (a fim de que)</t>
         </is>
       </c>
       <c r="N78" t="inlineStr">
         <is>
-          <t>concessão</t>
+          <t>“&lt;u&gt;mas &lt;/u&gt;quem estava procurando por você!” – (porém)</t>
         </is>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="P78" t="n">
@@ -7105,105 +7068,24 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>CESGRANRIO</t>
+          <t>Cesgranrio</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>BNDES</t>
+          <t>Banco do Brasil</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2011</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
-        <is>
-          <t>A conjunção/locução conjuntiva entre parênteses que NÃO expressa a mesma relação de sentido da conjunção/locução conjuntiva destacada é:</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>Português</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>Conjunção</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>Difícil</t>
-        </is>
-      </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>ME</t>
-        </is>
-      </c>
-      <c r="J79" t="inlineStr">
-        <is>
-          <t>“&lt;u&gt;assim &lt;/u&gt;como não estamos aqui,”– (bem como)</t>
-        </is>
-      </c>
-      <c r="K79" t="inlineStr">
-        <is>
-          <t>“...&lt;u&gt;quando &lt;/u&gt;procuramos estar com alguém,” – (sempre que)</t>
-        </is>
-      </c>
-      <c r="L79" t="inlineStr">
-        <is>
-          <t>“...&lt;u&gt;porque &lt;/u&gt;gostamos,” – (ao passo que)</t>
-        </is>
-      </c>
-      <c r="M79" t="inlineStr">
-        <is>
-          <t>“...&lt;u&gt;para que&lt;/u&gt; elas venham até você.” – (a fim de que)</t>
-        </is>
-      </c>
-      <c r="N79" t="inlineStr">
-        <is>
-          <t>“&lt;u&gt;mas &lt;/u&gt;quem estava procurando por você!” – (porém)</t>
-        </is>
-      </c>
-      <c r="O79" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="P79" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q79" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>79</v>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>Cesgranrio</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>Banco do Brasil</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
         <is>
           <t>&lt;b&gt;Entenda o que é deepfakee saiba como se proteger&lt;/b&gt;
 Vídeos que viralizam nas redes sociais mostrando figuras públicas em situações quase
@@ -7245,6 +7127,87 @@
 No trecho “que, como a tradução indica, é &lt;u&gt;tão &lt;/u&gt;bem feita &lt;u&gt;que &lt;/u&gt;pode enganar até os mais atentos”, as palavras destacadas contribuem para expressar, entre as duas ideias, a relação lógica de</t>
         </is>
       </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>adição</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>condição</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>contradição</t>
+        </is>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>consequência</t>
+        </is>
+      </c>
+      <c r="N79" t="inlineStr">
+        <is>
+          <t>temporalidade</t>
+        </is>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P79" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q79" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>80</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>UNIRIO</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>No Texto, em “Já um celular tem maior taxa de obsolescência e pode ter de ser substituído em um ano ou dois” (l. 53-55), a palavra &lt;u&gt;Já &lt;/u&gt;apresenta o sentido de</t>
+        </is>
+      </c>
       <c r="F80" t="inlineStr">
         <is>
           <t>Português</t>
@@ -7267,119 +7230,38 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>adição</t>
+          <t>tempo</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>condição</t>
+          <t>exclusão</t>
         </is>
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>contradição</t>
+          <t>oposição</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>consequência</t>
+          <t>intensidade</t>
         </is>
       </c>
       <c r="N80" t="inlineStr">
         <is>
-          <t>temporalidade</t>
+          <t>conformidade</t>
         </is>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="P80" t="n">
         <v>0</v>
       </c>
       <c r="Q80" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>80</v>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>CESGRANRIO</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>UNIRIO</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>2019</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>No Texto, em “Já um celular tem maior taxa de obsolescência e pode ter de ser substituído em um ano ou dois” (l. 53-55), a palavra &lt;u&gt;Já &lt;/u&gt;apresenta o sentido de</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>Português</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>Conjunção</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>Médio</t>
-        </is>
-      </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>ME</t>
-        </is>
-      </c>
-      <c r="J81" t="inlineStr">
-        <is>
-          <t>tempo</t>
-        </is>
-      </c>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>exclusão</t>
-        </is>
-      </c>
-      <c r="L81" t="inlineStr">
-        <is>
-          <t>oposição</t>
-        </is>
-      </c>
-      <c r="M81" t="inlineStr">
-        <is>
-          <t>intensidade</t>
-        </is>
-      </c>
-      <c r="N81" t="inlineStr">
-        <is>
-          <t>conformidade</t>
-        </is>
-      </c>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="P81" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q81" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
:up: chave de seguranca para nao ler pdf e excluir questoes
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q80"/>
+  <dimension ref="A1:Q105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7265,6 +7265,2070 @@
         <v>0</v>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>81</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;A história do método braile&lt;/b&gt;
+Ler no escuro. Quem já tentou sabe que é impossível. Mas foi exatamente a isso que um francês chamado Louis Braille dedicou a vida. Nascido em Coupvray, uma pequena aldeia nos arredores de Paris, em 1809, desde cedo ele mostrou muito interesse pelo trabalho do pai. Seus olhos azuis brilhavam da admiração de vê-lo cortar, com extrema perícia, selas e arreios. Pouco depois de completar 3 anos, o menino começou a brincar na selaria do pai, cortando pequenas tiras de couro. Uma tarde, uma sovela, instrumento usado para perfurar o couro, escapou-lhe da mão e atingiu o seu olho esquerdo. O resultado foi uma infecção que, seis meses depois, afetaria também o olho direito. Aos 5 anos, o garoto estava completamente cego.
+A tragédia não o impediu, porém, de frequentar a escola por dois anos e de se tornar ainda um aluno brilhante. Por essa razão, ele ganhou uma bolsa de estudos no Instituto Nacional para Jovens Cegos, em Paris, um colégio interno fundado por Valentin Haüy (1745-182. Além do currículo normal, Haüy introduzira um sistema especial de alfabetização, no qual letras de forma impressas em relevo, em papelão, eram reconhecidas pelos contornos. Desde o início do curso, Braille destacou-se como o melhor aluno da turma e logo começou a ajudar os colegas. Em 1821, aos 12 anos, conheceu um método inventado pouco antes por Charles Barbier de La Serre, oficial do Exército francês.
+O método Barbier, também chamado escrita noturna, era um código de pontos e traços em relevo impressos também em papelão. Destinava-se a enviar ordens cifradas a sentinelas em postos avançados. Estes decodificariam a mensagem até no escuro. Mas, como a ideia não pegou na tropa, Barbier adaptou o método para a leitura de cegos, com o nome de grafia sonora. O sistema permitia a comunicação entre os cegos, pois com ele era possível escrever, algo que o método de Haüy não possibilitava. O de Barbier era fonético: registrava sons e não letras. Dessa forma, as palavras não podiam ser soletradas. Além disso, o fato de um grande número de sinais ser usado para uma única palavra tornava o sistema muito complicado. Apesar dos inconvenientes, foi adotado como método auxiliar por Haüy.
+Pesquisando a fundo a grafia sonora, Braille percebeu suas limitações e pôs-se a aperfeiçoá-la.
+Em 1824, seu método estava pronto. Primeiro, eliminou os traços, para evitar erros de leitura: em seguida, criou uma célula de seis pontos, divididos em duas colunas de três pontos cada, que podem ser combinados de 63 maneiras diferentes. A posição dos pontos na célula está ao lado.
+Em 1826, aos 17 anos, ainda estudante, Braille começou a dar aulas. Embora seu método fizesse sucesso entre os alunos, não podia ensiná-lo na sala de aula, pois ainda não era reconhecido oficialmente. Por isso, Braille dava aulas do revolucionário sistema escondido no quarto, que logo se transformou numa segunda sala de aula.
+O braile é lido passando-se a ponta dos dedos sobre os sinais de relevo. Normalmente se usa a mão direita com um ou mais dedos, conforme a habilidade do leitor, enquanto a mão esquerda procura o início da outra linha. Aplica-se a qualquer língua, sem exceção, e também à estenografia, à música – Braille, por sinal, era ainda exímio pianista – e às notações científicas em geral. A escrita é feita mediante o uso da reglete, também idealizada por Braille: trata-se de uma régua especial, de duas linhas, com uma série de janelas de seis furos cada, correspondentes às células braile.
+Louis Braille morreu de tuberculose em 1852, com apenas 43 anos. Temia que seu método desaparecesse com ele, mas, finalmente, em 1854 foi oficializado pelo governo francês. No ano seguinte, foi apresentado ao mundo, na Exposição Internacional de Paris, por ordem do imperador Napoleão III (1808-187, que programou ainda uma série de concertos de piano com ex-alunos de Braille. O sucesso foi imediato, e o sistema se espalhou pelo mundo. Em 1952, o governo francês transferiu os restos mortais de Braille para o Panthéon, em Paris, onde estão sepultados os heróis nacionais.
+(ATANES,Silvio.SuperInteressante.Disponívelem:https://super .abril.]com.br/historia/.Acessoem:23out.2022.Adaptado).
+O pronome oblíquo átono está colocado de acordo com a norma-padrão da língua portuguesa em:</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>Me surpreende a história de vida de Braille</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>Seu método não trouxe-lhe reconhecimento em vida</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>O menino cego aos cinco anos tornar-se-ia um herói nacional na França</t>
+        </is>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>Quantos impressionaram-nos como Braille?</t>
+        </is>
+      </c>
+      <c r="N81" t="inlineStr">
+        <is>
+          <t>Braille recebia os alunos e sempre auxiliava-os com o método criado</t>
+        </is>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P81" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q81" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>82</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Entenda o que é &lt;i&gt;deep fake&lt;/i&gt; e saiba como se proteger&lt;/b&gt;
+Vídeos que viralizam nas redes sociais mostrando figuras públicas em situações quase inacreditáveis são verdadeiros? Afinal de contas tudo parece tão real... A resposta é não, pois se trata de uma “deepfake”,“falsificação profunda” em português, que, como a tradução indica, é tão bem feita que pode enganar até os mais atentos. Segundo estudo de uma empresa de segurança, 65% dos brasileiros ignoram a sua existência e 71% não reconhecem quando um vídeo foi editado digitalmente usando essa técnica.
+O que muita gente não sabe, porém, é que esse tipo de golpe, além de manipular vídeos com celebridades e políticos famosos, também prejudica empresas e cidadãos comuns, que podem ser envolvidos em fraudes de identidade e extorsões. “Deepfakepode ser definida como a criação de vídeos e áudios falsos por meio de inteligência artificial”, explica um especialista de segurança cibernética e fraude. A prática costuma utilizar um vídeo de referência e a face (ou corpo) de outra pessoa, que não fazia parte do vídeo original.
+Criam-se áudios falsos, fazendo a inteligência artificial aprender como uma pessoa fala e, a partir daí, obter uma montagem com outras falas, inclusive alterando os lábios para acompanhar as palavras que são ditas.
+Esse processo vem evoluindo rapidamente, tornando cada vez mais difícil a sua identificação. Isso ocorre porque as novas redes neurais (sistemas de computação que funcionam como neurônios do cérebro humano), a evolução da capacidade de processamento e a redução de custos da computação em nuvem têm facilitado o acesso a essa tecnologia, contribuindo para aumentar a qualidade dos vídeos.
+No entanto, os criminosos não precisam de tanto conhecimento e tecnologia para aplicar seus golpes.
+Isso porque deepfakescriadas para serem distribuídas porappsde mensagens não exigem tanta qualidade. O perigo é que, para o cidadão comum, a deepfakepode ser o ponto de partida para uma fraude financeira, entre outros problemas.
+A recomendação para pessoas físicas se protegerem é diminuir a exposição de fotos com rostos e vídeos pessoais na internet. “As redes sociais devem se manter configuradas como privadas, já que fotos, áudios ou vídeos disponíveis publicamente podem ser utilizados para alimentar a inteligência artificial e engendrardeepfakes.” Além disso, ao receber um vídeo suspeito, observe se o rosto e os lábios da pessoa se movem em conjunto com o que ela diz. Preste atenção se a fala parece contínua ou se em algum momento apresenta cortes entre uma palavra e outra. E considere o contexto — ainda que tecnicamente o vídeo esteja muito bem manipulado, avalie se faz sentido que aquela pessoa diga o que parece dizer naquele momento.
+(Disponívelem:https://estudio.folha.uol.com.br/unico.Acessoem:20out.2022.Adaptado).
+O pronome oblíquo átono em destaque está empregado de acordo com a norma-padrão em:</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>Convidaremo-&lt;u&gt;lo &lt;/u&gt;para experimentar algumas novidades tecnológicas em oferta no interior da loja</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>Aquele funcionário, que foi aprovado no exame seletivo de uma instituição, para o cargo de tecnólogo, estava em dúvida em aceitá-&lt;u&gt;lo&lt;/u&gt;</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>Os profissionais da informática, ao serem entrevistados sobre sua carreira, nunca cansavam-&lt;u&gt;se &lt;/u&gt;de citar as fontes em que poderiam encontrar novos conteúdos de interesse para a sua área</t>
+        </is>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>Quando os produtos tecnológicos mantêm-&lt;u&gt;se &lt;/u&gt;nas prateleiras das lojas por muito tempo, é sinal de que despertaram pouca atenção das pessoas ou que o preço cobrado estava além das possibilidades de compra dos interessados</t>
+        </is>
+      </c>
+      <c r="N82" t="inlineStr">
+        <is>
+          <t>Se os pesquisadores especializados em conserto de computadores ou outros dispositivos eletrônicos conservarem-&lt;u&gt;se &lt;/u&gt;atualizados, a ciência que se dedica ao tratamento da informação apresentará maior progresso</t>
+        </is>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P82" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q82" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>83</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Pix: é o fim do dinheiro em espécie?&lt;/b&gt;
+O Pix muda a forma como realizamos transações financeiras. Representará realmente o fim do DOC e da TED? O boleto bancário está ainda mais ameaçado de extinção? E o velho cheque vai resistir a esses novos tempos?
+Abrangente como é, o Pix pode reduzir ou acabar com a circulação das notas de real? Essa é uma pergunta sem resposta fácil. O fato é que o avanço das transações financeiras eletrônicas, em detrimento do uso do dinheiro em papel, pode ser benéfico para o Brasil, em vários sentidos. O Pix tem tudo para ser o empurrãozinho que nos falta para chegarmos a esse cenário.
+E por que o dinheiro em espécie resiste? Talvez você esteja entre aqueles que compram no supermercado com cartão de crédito ou usam QR Code para pagar a farmácia. Mas a feira da semana e os churros na esquina você paga com “dinheiro vivo”, certo? Um dos fatores que escoram a circulação de papel-moeda no Brasil é a informalidade.
+Atrelada a isso está a situação dos desbancarizados. A dificuldade que muita gente teve para receber o auxílio emergencial, durante a pandemia, jogou luz sobre um problema notado há tempos: a enorme quantidade de brasileiros que não têm acesso a serviços bancários. O pouco de dinheiro que entra no orçamento dessas pessoas precisa ser gasto rapidamente para subsistência.
+Não há base financeira suficiente para justificar movimentações bancárias. Também pesa para o time dos “sem-banco” o baixo nível de educação ou a falta de familiaridade com a tecnologia.
+O fator cultural também favorece a circulação do dinheiro em espécie. É provável que você conheça alguém que, mesmo tendo boa renda, prefere pagar boletos ou receber pagamentos com cédulas simplesmente por estar acostumado a elas. Para muita gente que faz parte dessa turma, dinheiro vivo é dinheiro recebido ou pago na hora. Não é preciso esperar a TED cair ou o dia virar para o boleto ser compensado. Isso pesa mais do que a conveniência de se livrar da fila da lotérica.
+Embora o Brasil tenha um sistema bancário que suporta vários tipos de transações, o país estava ficando para trás no que diz respeito a pagamentos instantâneos. O Pix veio para preencher essa lacuna.
+A modalidade permite transações em qualquer horário e dia, incluindo finais de semana e feriados.
+Essa característica, por si só, já é capaz de mudar a forma como lidamos com o dinheiro, pois implica envio ou recebimento imediato: as transações via Pix são concluídas rapidamente. É o fim do papel-moeda? Não é tão simples assim. O Pix não foi idealizado com o propósito exclusivo de acabar com os meios de pagamento e transferência atuais, muito menos com o papelmoeda, mas para fazer o sistema financeiro do Brasil evoluir e ficar mais competitivo.
+Apesar disso, não é exagero esperar que, à medida que a população incorpore o sistema à sua rotina, o uso de DOC, TED, boletos e cartões caia. Eventualmente, algum desses meios poderá ser descontinuado, mas isso não acontecerá tão cedo — vide o exemplo do cheque, que não “morreu” com a chegada do cartão.
+No caso das cédulas, especialistas do mercado financeiro apontam para uma diminuição de circulação, mas não para um futuro próximo em que o papel-moeda deixará de existir. Para que esse cenário se torne realidade, é necessário, sobretudo, atacar a desbancarização. O medo ou a pouca familiaridade com a tecnologia podem ser obstáculos, mas o Pix é tão interessante para o país que o próprio comércio incentiva o público mais resistente a aderir a ele.
+(ALECRIM,E.Disponívelem:https://tecnoblog.net/especiais/pix-fim-dinheiro-especiebrasil/.Publicadoemnovembrode2020.Acessoem:2dez.2022.Adaptado).
+O pronome em destaque está colocado de acordo com a norma-padrão da língua portuguesa em:</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>As transações bancárias, atualmente, podem ser feitas pelo celular, a qualquer hora, para que obtenha-&lt;u&gt;se &lt;/u&gt;o ideal de maior eficiência e rapidez</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>O cadastramento do Pix pode ser realizado em mais de uma instituição bancária, o que considera-&lt;u&gt;se &lt;/u&gt;benéfico para as pessoas que precisam diversificar suas operações financeiras</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>Os cidadãos que se recusam a utilizar os serviços bancários para efetuar movimentações financeiras, por preferirem o uso de cédulas, encontram muita dificuldade para realizá-&lt;u&gt;las&lt;/u&gt;</t>
+        </is>
+      </c>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>Desde que implantou-&lt;u&gt;se &lt;/u&gt;o Pix, as pessoas podem realizar até a compra de produtos extremamente baratos por transferência bancária instantânea, porque esse sistema atingiu um significativo grau de confiabilidade</t>
+        </is>
+      </c>
+      <c r="N83" t="inlineStr">
+        <is>
+          <t>Embora tenham sido ampliadas as medidas de segurança tecnológica para a movimentação bancária, não sentimo-&lt;u&gt;nos &lt;/u&gt;confiantes para operar com grandes somas de dinheiro</t>
+        </is>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P83" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q83" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>84</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>&lt;u&gt;Empreendedorismo social: um caminho para quem quer mudar o mundo&lt;/u&gt;
+Ainda que não exista uma concepção única sobre o empreendedorismo social, de forma geral, o conceito está relacionado ao ato de empreender ou inovar com o objetivo de alavancar causas sociais e ambientais. A meta é transformar uma realidade, promover o bem-estar da sociedade e agregar valor com cunho social.
+Um empreendedor social produz bens e serviços que irão impactar positivamente a comunidade em que ele está inserido e solucionar algum problema ou necessidade daquele grupo. Apesar de poder ter retorno financeiro, os empreendimentos sociais analisam seu desempenho a partir do impacto social gerado por sua atuação.
+Vale ressaltar que, apesar de apresentarem muitas similaridades, empreendedorismo social e negócio social não são sinônimos. O empreendedorismo social cria valor por meio da inovação, que gera uma transformação social. O foco não é o retorno financeiro, mas a resolução de problemas sociais e o impacto positivo. Enquanto isso, os negócios sociais seguem a lógica tradicional do mercado, porém com a ambição de gerar valor social.
+Cinco características também são essenciais para a iniciativa: ser inovadora; realizável; autossustentável; contar com a participação de diversos segmentos da sociedade, incluindo as pessoas impactadas; e promover impacto social com resultados mensuráveis.
+Quem tem interesse de atuar nessa área precisa trabalhar em grupo e formar parcerias, saber lidar bem com as pessoas e buscar formas de trazer resultados de impacto social.
+Além disso, o profissional precisa ter flexibilidade e vontade de explorar, pois é possível que ele acabe exercendo um papel que não seja necessariamente na sua área de formação, ou que sua atuação se transforme rapidamente, por conta do dinamismo e das necessidades do negócio.
+(MENDES,T.Empreendedorismosocial:umcaminhoparaquemquermudaromundo.Naprática,7jul.2022.
+Disponívelem:https://www.napratica.org.br/empreendedorismo-social/.Acessoem:2set.2022.Adaptado).
+O pronome oblíquo destacado foi colocado na posição correta, segundo as exigências da norma-padrão da língua portuguesa, em:</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>A área da saúde não encontra-&lt;u&gt;se &lt;/u&gt;atendida em regiões afastadas dos grandes centros urbanos nem em comunidades que vivem nas periferias das cidades</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>A preocupação com o meio ambiente tem sido um dos segmentos mais relevantes do empreendedorismo social, porque destina-&lt;u&gt;se &lt;/u&gt;a transformar positivamente a sociedade</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Governantes que têm como missão viabilizar o acesso universal à educação pública de qualidade sempre preocupam-&lt;u&gt;se &lt;/u&gt;com ações de inovação e empreendedorismo</t>
+        </is>
+      </c>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>Para uma iniciativa de empreendedorismo destinada à formação de educadores tornar-&lt;u&gt;se &lt;/u&gt;produtiva, é preciso identificar as necessidades do público-alvo de cada comunidade</t>
+        </is>
+      </c>
+      <c r="N84" t="inlineStr">
+        <is>
+          <t>Quando os profissionais que atuam na área de empreendedorismo social sentem-&lt;u&gt;se &lt;/u&gt;desanimados, é preciso que eles avaliem todo o progresso que ajudaram a desenvolver</t>
+        </is>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P84" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q84" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>85</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>AgeRIO</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>A frase em que a colocação do pronome destacado NÃO obedece aos ditames da norma-padrão é:</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>Feliz é quem &lt;u&gt;se &lt;/u&gt;dá o direito de estar bem</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>As pessoas nunca acostumam-&lt;u&gt;se &lt;/u&gt;com a felicidade</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>Agradar-&lt;u&gt;nos&lt;/u&gt;-ia a ideia de que todos têm direito à paz</t>
+        </is>
+      </c>
+      <c r="M85" t="inlineStr">
+        <is>
+          <t>Viver a vida intensamente é o que &lt;u&gt;lhe &lt;/u&gt;confere sentido</t>
+        </is>
+      </c>
+      <c r="N85" t="inlineStr">
+        <is>
+          <t>Afastando-&lt;u&gt;nos &lt;/u&gt;de quem nos quer bem, saudamos a solidão</t>
+        </is>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P85" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q85" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>86</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>/BASA/Tecnologia da Informação/2022) O emprego do pronome oblíquo em destaque respeita a norma-padrão da língua em:</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>Quando perguntaram sobre as grades, fiquei sem saber o que &lt;u&gt;lhes &lt;/u&gt;dizer</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>O sol oblíquo nasce atrás dos prédios, mas ainda não conseguiu vencer-&lt;u&gt;lhes&lt;/u&gt;</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>A velha senhora está sempre lá. Já espero &lt;u&gt;lhe &lt;/u&gt;ver quando saio todas as manhãs</t>
+        </is>
+      </c>
+      <c r="M86" t="inlineStr">
+        <is>
+          <t>Ainda demora para o sol nascer, mas, mesmo assim, a velha senhora já está lá a &lt;u&gt;lhe &lt;/u&gt;esperar</t>
+        </is>
+      </c>
+      <c r="N86" t="inlineStr">
+        <is>
+          <t>Quando as pessoas passam na calçada, aquela senhora tem o sorriso pronto para &lt;u&gt;lhes &lt;/u&gt;cumprimentar</t>
+        </is>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P86" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q86" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>87</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>CAIXA ECONÔMICA</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>A colocação do pronome oblíquo átono está em acordo com a norma-padrão da língua portuguesa em:</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>Poder-se-á levar a educação financeira para as salas de aula, o que será muito proveitoso</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>Nos perguntam sempre sobre como gerir melhor a vida financeira</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>As famílias nunca preocuparam-se com a educação financeira como parte da formação de seus filhos</t>
+        </is>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>Aqueles que relacionam-se bem com o dinheiro têm uma vida mais organizada</t>
+        </is>
+      </c>
+      <c r="N87" t="inlineStr">
+        <is>
+          <t>Compreenderia-se melhor o desempenho da empresa, se o mercado fosse estudado</t>
+        </is>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P87" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q87" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>88</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>A colocação do pronome oblíquo átono destacado está de acordo com o que prevê a norma-padrão da língua portuguesa no seguinte período:</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>Consideraria-&lt;b&gt;se &lt;/b&gt;o QA mais importante que o QI há duas décadas?</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Se &lt;/b&gt;busca investir naquilo que pode fazer a diferença entre a máquina e o homem</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>As mudanças no mercado de trabalho jamais dar-&lt;b&gt;se&lt;/b&gt;-ão sem investimento no capital humano</t>
+        </is>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>Os candidatos que saem-&lt;b&gt;se &lt;/b&gt;melhor nas entrevistas são contratados mais rapidamente</t>
+        </is>
+      </c>
+      <c r="N88" t="inlineStr">
+        <is>
+          <t>Alguns &lt;b&gt;se &lt;/b&gt;consideram mais preparados para enfrentar adversidades no trabalho do que em família</t>
+        </is>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P88" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q88" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>89</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>A colocação do pronome oblíquo destacado está de acordo com a norma-padrão em:</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>O dinheiro não foi-&lt;b&gt;me &lt;/b&gt;bastante</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>O depósito só estará concretizado, se houver quem validá-&lt;b&gt;lo&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>Se você pudesse emprestar esse dinheiro, depositaria-&lt;b&gt;o &lt;/b&gt;ainda esta semana?</t>
+        </is>
+      </c>
+      <c r="M89" t="inlineStr">
+        <is>
+          <t>Explique-&lt;b&gt;me &lt;/b&gt;como funciona esse financiamento</t>
+        </is>
+      </c>
+      <c r="N89" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Me &lt;/b&gt;empreste seu cartão, que eu faço a transação hoje</t>
+        </is>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P89" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>90</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>O pronome destacado foi utilizado na posição correta, segundo as exigências da norma-padrão da língua portuguesa, em:</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>A associação brasileira de mercados financeiros publicou uma diretriz de segurança, na qual mostra-&lt;u&gt;se &lt;/u&gt;a necessidade de adequação de proteção de dados</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>A segurança da informação já transformou-&lt;u&gt;se &lt;/u&gt;em uma área estratégica para qualquer tipo de empresa</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>Naquele evento, ninguém tinha-&lt;u&gt;se &lt;/u&gt;incomodado com o palestrante no início do debate a respeito de privacidade digital</t>
+        </is>
+      </c>
+      <c r="M90" t="inlineStr">
+        <is>
+          <t>Apesar das dificuldades encontradas, sempre referimo-&lt;u&gt;nos &lt;/u&gt;com cuidado aos nossos dados pessoais, como CPF, RG, e-mail, para proteção da vida privada</t>
+        </is>
+      </c>
+      <c r="N90" t="inlineStr">
+        <is>
+          <t>Quando a privacidade dos dados bancários é mantida, como &lt;u&gt;nos &lt;/u&gt;garantem as instituições, ficamos tranquilos</t>
+        </is>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P90" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>91</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>O pronome oblíquo átono em destaque está colocado de acordo com a norma-padrão em:</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>No processo ensino-aprendizagem, o objetivo deve ser desenvolver aptidões para que os alunos sempre mantenham-&lt;u&gt;se &lt;/u&gt;em dia com os avanços da ciência</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>&lt;u&gt;Se &lt;/u&gt;reclama muito das dificuldades do ensino remoto devido a problemas de conexão</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>Os profissionais da educação nunca cansam-&lt;u&gt;se &lt;/u&gt;de estudar os conteúdos que possam interessar os alunos nas aulas</t>
+        </is>
+      </c>
+      <c r="M91" t="inlineStr">
+        <is>
+          <t>Para garantir o progresso dos estudantes, os professores sempre dedicam-&lt;u&gt;se &lt;/u&gt;a pesquisar novos métodos de ensino</t>
+        </is>
+      </c>
+      <c r="N91" t="inlineStr">
+        <is>
+          <t>Quando as escolas &lt;u&gt;se &lt;/u&gt;preocuparem em empregar novas metodologias no ensino-aprendizagem, alcançarão melhores resultados</t>
+        </is>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P91" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q91" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>92</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>UNIRIO</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>A substituição da expressão destacada pelo que se encontra entre colchetes está de acordo com a norma-padrão em:</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>Jorge Amado &lt;u&gt;tomava a bebida&lt;/u&gt; sem açúcar. [tomava-lhe]</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>Diolino gostava de &lt;u&gt;mostrar a receita&lt;/u&gt;. [mostrá-la]</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>Pelé &lt;u&gt;bebia no carro&lt;/u&gt; porque era discreto. [bebia-lhe]</t>
+        </is>
+      </c>
+      <c r="M92" t="inlineStr">
+        <is>
+          <t>Wando e Rô também &lt;u&gt;frequentavam o bar&lt;/u&gt;. [frequentavam-nos]</t>
+        </is>
+      </c>
+      <c r="N92" t="inlineStr">
+        <is>
+          <t>O MiniBar &lt;u&gt;produzia 6.000 litros&lt;/u&gt; por mês. [produzia-se]</t>
+        </is>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P92" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q92" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>93</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>UNIRIO</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>A frase em que a colocação do pronome oblíquo obedece aos ditames da norma-padrão é:</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>Abri o estojo, cheirando-o por um longo tempo</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>Seria-lhe útil ter um notebook de última geração</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>Me fascinou reviver o tempo de minha primeira infância</t>
+        </is>
+      </c>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>O que lembrou-lhe o estojo escolar foi o novo notebook</t>
+        </is>
+      </c>
+      <c r="N93" t="inlineStr">
+        <is>
+          <t>Conforme abria-o, sentia seu cheiro agradável cada vez mais forte</t>
+        </is>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P93" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>94</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>O uso do pronome relativo destacado está de acordo com a norma-padrão em:</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>Eram artistas de &lt;u&gt;cujos &lt;/u&gt;trabalho todos gostavam</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>A arquitetura, &lt;u&gt;onde &lt;/u&gt;é uma arte, faz grandes mestres</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>Visitamos obras &lt;u&gt;que &lt;/u&gt;os livros faziam menção a elas</t>
+        </is>
+      </c>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>Os artistas &lt;u&gt;que &lt;/u&gt;todos elogiavam eram sempre os mesmos</t>
+        </is>
+      </c>
+      <c r="N94" t="inlineStr">
+        <is>
+          <t>Os mestres dentre &lt;u&gt;as quais&lt;/u&gt; faziam um bom trabalho eram elogiados</t>
+        </is>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P94" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q94" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>95</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>O pronome em destaque está colocado de acordo com a norma-padrão em:</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>Os jovens não dedicam-&lt;u&gt;se &lt;/u&gt;suficientemente à leitura</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>Quando alguém apresentar-&lt;u&gt;se &lt;/u&gt;como salvador, é bom pesquisar sobre sua história</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>Oferecemos-&lt;u&gt;lhes &lt;/u&gt;as melhores condições de pesquisa em nossa biblioteca</t>
+        </is>
+      </c>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>É preciso estarmos atentos às notícias, pois elas têm deturpado-&lt;u&gt;se&lt;/u&gt;</t>
+        </is>
+      </c>
+      <c r="N95" t="inlineStr">
+        <is>
+          <t>Encontraremo-&lt;u&gt;nos &lt;/u&gt;em condições de discutir a realidade, caso sejamos bons leitores</t>
+        </is>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P95" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>96</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>O pronome destacado foi utilizado na posição correta, segundo as exigências da norma-padrão da língua portuguesa, em:</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>Quando as carreiras tradicionais saturam-&lt;u&gt;se&lt;/u&gt;, os futuros profissionais têm de recorrer a outras alternativas</t>
+        </is>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>Caso os responsáveis pela limpeza urbana descuidem-&lt;u&gt;se &lt;/u&gt;de sua tarefa, muitas doenças transmissíveis podem proliferar</t>
+        </is>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>As empresas têm mantido-&lt;u&gt;se &lt;/u&gt;atentas às leis de proteção ambiental vigentes no país poderão ser penalizadas</t>
+        </is>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>Os dirigentes devem esforçar-&lt;u&gt;se &lt;/u&gt;para que os funcionários tenham consciência de ações de proteção ao meio ambiente</t>
+        </is>
+      </c>
+      <c r="N96" t="inlineStr">
+        <is>
+          <t>Os trabalhadores das áreas rurais nunca enganaram-&lt;u&gt;se &lt;/u&gt;a respeito da importância da agricultura para a subsistência da humanidade</t>
+        </is>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P96" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q96" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>97</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>BANCO DA AMAZÔNIA</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>A norma-padrão em sua variedade formal prevê uma organização da frase em que a observância da colocação pronominal é fundamental.
+A frase em que o pronome oblíquo átono está empregado corretamente, segundo as regras da colocação pronominal, é:</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>Ninguém ensinou-me a manter a cabeça à tona d’água</t>
+        </is>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>O subconsciente boicota-nos a todo momento de nossa vida</t>
+        </is>
+      </c>
+      <c r="L97" t="inlineStr">
+        <is>
+          <t>O ser humano que molda-se à diferentes realidades vive melhor</t>
+        </is>
+      </c>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>Boicotaremo-nos todas as vezes que houver a chance de felicidade</t>
+        </is>
+      </c>
+      <c r="N97" t="inlineStr">
+        <is>
+          <t>Se considerar mau menino é justificar o não merecimento da felicidade</t>
+        </is>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P97" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q97" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>98</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>De acordo com as normas da linguagem padrão, a colocação pronominal está INCORRETA em:</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>Virgínia encontrava-se acamada há semanas</t>
+        </is>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>A ferida não se curava com os remédios</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>A benzedeira usava uma peruca que não favorecia-a</t>
+        </is>
+      </c>
+      <c r="M98" t="inlineStr">
+        <is>
+          <t>Imediatamente lhe deram uma caneta-tinteiro vermelha</t>
+        </is>
+      </c>
+      <c r="N98" t="inlineStr">
+        <is>
+          <t>Enquanto se rezavam Ave-Marias, a ferida era circundada</t>
+        </is>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P98" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q98" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>99</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>O termo destacado foi utilizado na posição correta, segundo as exigências da norma-padrão da língua portuguesa, em:</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>Embora lembrem-&lt;u&gt;se &lt;/u&gt;da importância de uma nova utilização, como é o caso das garrafas plásticas, há pessoas que desconhecem o valor da reciclagem</t>
+        </is>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>O desafio da limpeza urbana não limita-&lt;u&gt;se &lt;/u&gt;apenas a manter limpas as ruas, mas, também, a coletar e dar destino adequado ao lixo urbano</t>
+        </is>
+      </c>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>Quando o lixo aloja-&lt;u&gt;se &lt;/u&gt;no meio ambiente, causa danos irreparáveis a todos os seres vivos, assim como a toda a natureza.</t>
+        </is>
+      </c>
+      <c r="M99" t="inlineStr">
+        <is>
+          <t>Sempre fazem-&lt;u&gt;se &lt;/u&gt;necessárias políticas eficazes para ressaltar a importância do saneamento, mantendo-se as cidades mais limpas</t>
+        </is>
+      </c>
+      <c r="N99" t="inlineStr">
+        <is>
+          <t>Todos os moradores do bairro mobilizaram-&lt;u&gt;se &lt;/u&gt;ao perceber que os esforços dispensados para manter o funcionamento dos edifícios deram bons resultados</t>
+        </is>
+      </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P99" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q99" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>100</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Segundo as exigências da norma-padrão da língua portuguesa, o pronome destacado foi utilizado na posição correta em:</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>Os jornais noticiaram que alguns países mobilizam-se para combater a disseminação de notícias falsas nas redes sociais</t>
+        </is>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>Para criar leis eficientes no combate aos boatos, sempre deve-se ter em mente que o problema de divulgação de notícias falsas é grave e muito atual</t>
+        </is>
+      </c>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>Entre os numerosos usuários da internet, constata-se um sentimento generalizado de reprovação à prática de divulgação de inverdades</t>
+        </is>
+      </c>
+      <c r="M100" t="inlineStr">
+        <is>
+          <t>Uma nova lei contra as fake news promulgada na Alemanha não aplica-se aos sites e redes sociais com menos de 2 milhões de membros</t>
+        </is>
+      </c>
+      <c r="N100" t="inlineStr">
+        <is>
+          <t>Uma vultosa multa é, muitas vezes, o estímulo mais eficaz para que adote-se a conduta correta em relação à reputação das celebridades</t>
+        </is>
+      </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P100" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q100" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>101</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>No trecho “perde-&lt;u&gt;se &lt;/u&gt;o dinheiro e o amigo”, a colocação do pronome átono em destaque está de acordo com a norma-padrão da língua portuguesa.
+O mesmo ocorre em:</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>Não se perde nem o dinheiro nem o amigo</t>
+        </is>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>Perderia-se o dinheiro e o amigo</t>
+        </is>
+      </c>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t>O dinheiro e o amigo tinham perdido-se</t>
+        </is>
+      </c>
+      <c r="M101" t="inlineStr">
+        <is>
+          <t>Se perdeu o dinheiro, mas não o amigo</t>
+        </is>
+      </c>
+      <c r="N101" t="inlineStr">
+        <is>
+          <t>Se o amigo que perdeu-se voltasse, ficaria feliz</t>
+        </is>
+      </c>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P101" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q101" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>102</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>O termo destacado foi utilizado na posição correta, segundo as exigências da norma-padrão da língua portuguesa, em:</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>A poluição do ar será irreversível, caso as medidas preventivas esgotem-&lt;u&gt;se&lt;/u&gt;</t>
+        </is>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>Os cientistas nunca equivocaram-&lt;u&gt;se &lt;/u&gt;a respeito dos perigos do uso de combustível fóssil</t>
+        </is>
+      </c>
+      <c r="L102" t="inlineStr">
+        <is>
+          <t>Quando as substâncias tóxicas alojam-&lt;u&gt;se &lt;/u&gt;no meio ambiente, causam danos aos seres vivos</t>
+        </is>
+      </c>
+      <c r="M102" t="inlineStr">
+        <is>
+          <t>Se as fontes de energia alternativa &lt;u&gt;se &lt;/u&gt;esgotarem, poderemos sofrer sérias consequências</t>
+        </is>
+      </c>
+      <c r="N102" t="inlineStr">
+        <is>
+          <t>Uma das exigências do mundo atual é que o ser humano sempre mantenha-&lt;u&gt;se &lt;/u&gt;em dia com as atividades físicas</t>
+        </is>
+      </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P102" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q102" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>103</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>IBGE</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>A posição do pronome &lt;u&gt;se &lt;/u&gt;destacado atende às exigências da norma-padrão da língua portuguesa em:</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>É preciso que os estados em que há maior degradação ambiental não neguem-&lt;u&gt;se &lt;/u&gt;a tomar as providências necessárias para enfrentar o problema</t>
+        </is>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>Há uma grande pressão social para que as pessoas mantenham-&lt;u&gt;se &lt;/u&gt;felizes e sintam-se realizadas permanentemente</t>
+        </is>
+      </c>
+      <c r="L103" t="inlineStr">
+        <is>
+          <t>Se os órgãos responsáveis pela proteção ambiental dedicarem-&lt;u&gt;se &lt;/u&gt;mais a sua missão, as matas brasileiras poderão sobreviver à degradação</t>
+        </is>
+      </c>
+      <c r="M103" t="inlineStr">
+        <is>
+          <t>Quando os institutos de pesquisa &lt;u&gt;se &lt;/u&gt;preocuparem em analisar o grau de felicidade da população, descobrirão que os índices são muito baixos</t>
+        </is>
+      </c>
+      <c r="N103" t="inlineStr">
+        <is>
+          <t>Livros de autoajuda fazem muito sucesso atualmente porque ensinam as pessoas a nunca sentirem-&lt;u&gt;se &lt;/u&gt;infelizes ao enfrentarem dificuldades</t>
+        </is>
+      </c>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P103" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q103" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>104</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>UNIRIO</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>O pronome átono destacado está colocado de acordo com a norma-padrão em:</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>Meu caro, &lt;u&gt;me &lt;/u&gt;não engano dizendo que antigamente o tempo do carnaval era obrigatório</t>
+        </is>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>As pessoas não davam-&lt;u&gt;se &lt;/u&gt;conta de que o tempo do carnaval era obrigatório</t>
+        </is>
+      </c>
+      <c r="L104" t="inlineStr">
+        <is>
+          <t>Quando o tempo do carnaval era obrigatório, meu pai &lt;u&gt;me &lt;/u&gt;levava a bailes à fantasia</t>
+        </is>
+      </c>
+      <c r="M104" t="inlineStr">
+        <is>
+          <t>O tempo do carnaval era obrigatório, mas não havia deixado-&lt;u&gt;me &lt;/u&gt;muitas lembranças</t>
+        </is>
+      </c>
+      <c r="N104" t="inlineStr">
+        <is>
+          <t>Os foliões divertiriam-&lt;u&gt;se&lt;/u&gt; mais se soubessem que o tempo do carnaval era obrigatório</t>
+        </is>
+      </c>
+      <c r="O104" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P104" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q104" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>105</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>BASA</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>O emprego do pronome oblíquo em destaque respeita a norma-padrão da língua em:</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>Colocação Pronominal</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>Quando perguntaram sobre as grades, fiquei sem saber o que &lt;u&gt;lhes &lt;/u&gt;dizer</t>
+        </is>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>O sol oblíquo nasce atrás dos prédios, mas ainda não conseguiu vencer-&lt;u&gt;lhes&lt;/u&gt;</t>
+        </is>
+      </c>
+      <c r="L105" t="inlineStr">
+        <is>
+          <t>A velha senhora está sempre lá. Já espero &lt;u&gt;lhe &lt;/u&gt;ver quando saio todas as manhãs</t>
+        </is>
+      </c>
+      <c r="M105" t="inlineStr">
+        <is>
+          <t>Ainda demora para o sol nascer, mas, mesmo assim, a velha senhora já está lá a &lt;u&gt;lhe &lt;/u&gt;esperar</t>
+        </is>
+      </c>
+      <c r="N105" t="inlineStr">
+        <is>
+          <t>Quando as pessoas passam na calçada, aquela senhora tem o sorriso pronto para &lt;u&gt;lhes &lt;/u&gt;cumprimentar</t>
+        </is>
+      </c>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P105" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q105" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
:up: botao de adicao individual e alerta de questao ja cadastrada finalizado
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q105"/>
+  <dimension ref="A1:Q111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7720,7 +7720,6 @@
           <t>CESGRANRIO</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr"/>
       <c r="D86" t="inlineStr">
         <is>
           <t>2025</t>
@@ -9326,6 +9325,518 @@
         <v>0</v>
       </c>
       <c r="Q105" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>106</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;A história do método braile&lt;/b&gt;
+Ler no escuro. Quem já tentou sabe que é impossível. Mas foi exatamente a isso que um francês chamado Louis Braille dedicou a vida. Nascido em Coupvray, uma pequena aldeia nos arredores de Paris, em 1809, desde cedo ele mostrou muito interesse pelo trabalho do pai. Seus olhos azuis brilhavam da admiração de vê-lo cortar, com extrema perícia, selas e arreios. Pouco depois de completar 3 anos, o menino começou a brincar na selaria do pai, cortando pequenas tiras de couro. Uma tarde, uma sovela, instrumento usado para perfurar o couro, escapou-lhe da mão e atingiu o seu olho esquerdo. O resultado foi uma infecção que, seis meses depois, afetaria também o olho direito. Aos 5 anos, o garoto estava completamente cego.
+A tragédia não o impediu, porém, de frequentar a escola por dois anos e de se tornar ainda um aluno brilhante. Por essa razão, ele ganhou uma bolsa de estudos no Instituto Nacional para Jovens Cegos, em Paris, um colégio interno fundado por Valentin Haüy (1745-182. Além do currículo normal, Haüy introduzira um sistema especial de alfabetização, no qual letras de forma impressas em relevo, em papelão, eram reconhecidas pelos contornos. Desde o início do curso, Braille destacou-se como o melhor aluno da turma e logo começou a ajudar os colegas. Em 1821, aos 12 anos, conheceu um método inventado pouco antes por Charles Barbier de La Serre, oficial do Exército francês.
+O método Barbier, também chamado escrita noturna, era um código de pontos e traços em relevo impressos também em papelão. Destinava-se a enviar ordens cifradas a sentinelas em postos avançados. Estes decodificariam a mensagem até no escuro. Mas, como a ideia não pegou na tropa, Barbier adaptou o método para a leitura de cegos, com o nome de grafia sonora. O sistema permitia a comunicação entre os cegos, pois com ele era possível escrever, algo que o método de Haüy não possibilitava. O de Barbier era fonético: registrava sons e não letras. Dessa forma, as palavras não podiam ser soletradas. Além disso, o fato de um grande número de sinais ser usado para uma única palavra tornava o sistema muito complicado. Apesar dos inconvenientes, foi adotado como método auxiliar por Haüy.
+Pesquisando a fundo a grafia sonora, Braille percebeu suas limitações e pôs-se a aperfeiçoá-la.
+Em 1824, seu método estava pronto. Primeiro, eliminou os traços, para evitar erros de leitura: em seguida, criou uma célula de seis pontos, divididos em duas colunas de três pontos cada, que podem ser combinados de 63 maneiras diferentes. A posição dos pontos na célula está ao lado.
+Em 1826, aos 17 anos, ainda estudante, Braille começou a dar aulas. Embora seu método fizesse sucesso entre os alunos, não podia ensiná-lo na sala de aula, pois ainda não era reconhecido oficialmente. Por isso, Braille dava aulas do revolucionário sistema escondido no quarto, que logo se transformou numa segunda sala de aula.
+O braile é lido passando-se a ponta dos dedos sobre os sinais de relevo. Normalmente se usa a mão direita com um ou mais dedos, conforme a habilidade do leitor, enquanto a mão esquerda procura o início da outra linha. Aplica-se a qualquer língua, sem exceção, e também à estenografia, à música – Braille, por sinal, era ainda exímio pianista – e às notações científicas em geral. A escrita é feita mediante o uso da reglete, também idealizada por Braille: trata-se de uma régua especial, de duas linhas, com uma série de janelas de seis furos cada, correspondentes às células braile.
+Louis Braille morreu de tuberculose em 1852, com apenas 43 anos. Temia que seu método desaparecesse com ele, mas, finalmente, em 1854 foi oficializado pelo governo francês. No ano seguinte, foi apresentado ao mundo, na Exposição Internacional de Paris, por ordem do imperador Napoleão III (1808-187, que programou ainda uma série de concertos de piano com ex-alunos de Braille. O sucesso foi imediato, e o sistema se espalhou pelo mundo. Em 1952, o governo francês transferiu os restos mortais de Braille para o Panthéon, em Paris, onde estão sepultados os heróis nacionais.
+(ATANES,Silvio.SuperInteressante.Disponívelem:https://super.abril.]com.br/historia/.Acessoem:23out.2022.
+Adaptado).
+O trecho do parágrafo “Pesquisando a fundo a grafia sonora, Braille percebeu suas limitações e pôs-se a aperfeiçoá- la” pode ser reescrito, sem alterar o sentido que apresenta no texto, como:</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>Emprego de Tempos e Modos</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>Para pesquisar a fundo a grafia sonora, Braille percebeu suas limitações e pôs-se a aperfeiçoá-la</t>
+        </is>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>Embora pesquisasse a fundo a grafia sonora, Braille percebeu suas limitações e pôs-se a aperfeiçoá-la</t>
+        </is>
+      </c>
+      <c r="L106" t="inlineStr">
+        <is>
+          <t>Quando pesquisava a fundo a grafia sonora, Braille percebeu suas limitações e pôs-se a aperfeiçoá-la</t>
+        </is>
+      </c>
+      <c r="M106" t="inlineStr">
+        <is>
+          <t>Apesar de pesquisar a fundo a grafia sonora, Braille percebia suas limitações e punha-se a aperfeiçoá-la</t>
+        </is>
+      </c>
+      <c r="N106" t="inlineStr">
+        <is>
+          <t>Se pesquisasse a fundo a grafia sonora, Braille perceberia suas limitações e pôr-se-ia a aperfeiçoá-la</t>
+        </is>
+      </c>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P106" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q106" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>107</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>ELETRONUCLEAR</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Maria José&lt;/b&gt;
+&lt;i&gt;Paulo Mendes Campos&lt;/i&gt;
+Faz um ano que Maria José morreu. Era meiga quase sempre, violenta quando necessário. Eu era menino e apanhava de um companheiro maior, quando ela me gritou da sacada se eu não via a pedra que marcava o gol. Dei uma pedrada no outro e acabei com a briga por milagre.
+Visitava os miseráveis, internava indigentes enfermos, devotava-se ao alívio de misérias físicas e morais do próximo, estudava o mistério teológico, exigia sempre o mais difícil de si mesma, comungava todos os dias, ingressou na Ordem Terceira de São Francisco. Mas nunca deixou de ter na gaveta o revólver que havia recebido, m enina-e-moça, das mãos do pai, e que empunhou no quintal noturno, perseguindo um ladrão, para espanto de meus cinco anos.
+Já perto dos setenta anos, ela explicava para um amigo meu que tinha chegado à humildade da velhice; já não se importava com quem tentasse ofendê-la, mas conservava o revólver para a defesa dos filhos e dos netos.
+Tratou-me com a dureza e o carinho que mereciam a rebeldia e o verdor da minha meninice.
+Ensinou- me a ler as primeiras sentenças; me falava do Cura d’Ars e nos dois Franciscos, o de Sales e o de Assis; apresentou-me aos contos de Edgar Poe e aos poemas de Baudelaire; dizia-me sorrindo versos de Antônio Nobre que havia decorado quando menina; discutia comigo as ideias finais de Tolstoi; escutava maternalmente meus contos toscos. Quando me desgarrei nos primeiros envolvimentos adolescentes, Maria José, com irônico afeto, me repetia a advertência de Drummond: “Paulo, sossegue, o amor é isso que você está vendo: hoje beija, amanhã não beija, depois de amanhã é domingo e segunda-feira ninguém sabe o que será”.
+Logo que me fiz homenzinho, deixou a dureza e se fez minha amiga: nada me perguntava, adivinhava tudo.
+Terna e firme, nunca lhe vi a fraqueza da pieguice. Com o gosto espontâneo da qualidade das coisas, renunciou às vaidades mais singelas. Sensível, alegre, aprendeu a encarar o sofrimento de olhos lúcidos. Fiel à disciplina religiosa, compreendia celestialmente as almas que perdiam o rumo. Fé, Esperança e Caridade eram para ela a flecha e o alvo das criaturas.
+Tornara-se tão íntima da substância terrestre – a dor – que se fazia difícil para o médico saber o que sentia; acabava dizendo que doía um pouco, por delicadeza.
+Capaz de longos jejuns e abstinências, já no final da vida, podia acompanhar um casal amigo a Copacabana, passar do bar da moda ao restaurante diferente, beber dois cafés ou três uísques em santa serenidade e aceitar com alegria o prato exótico.
+Gostava das pessoas erradas, consumidas de paixão, admirava São Paulo e Santo Agostinho, acreditava que era preciso se fazer violência para entrar no reino celeste.
+Poucas horas antes de morrer, pediu um conhaque e sorriu, destemida e doce, como quem vai partir para o céu. Santificara-se. Deus era o dia e a noite de seu coração, o Pai, a piedade, o fogo do espírito. Perdi quem me amava e perdoava, quem me encomendava à compaixão do Criador e me defendia contra o mundo de revólver na mão.
+Disponívelem:https://cronicabrasileira.org.br/cronicas/7173/maria-jose.Acessoem:05fev.2022.
+No trecho: “Mas nunca deixou de ter na gaveta o revólver que recebera, menina-e-moça, das mãos do pai, e que empunhou no quintal noturno, perseguindo um ladrão”, (parágrafo 2), a oração destacada pode ser substituída, sem prejuízo de seu significado, por</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>Emprego de Tempos e Modos</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>por isso perseguia um ladrão</t>
+        </is>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>enquanto perseguia um ladrão</t>
+        </is>
+      </c>
+      <c r="L107" t="inlineStr">
+        <is>
+          <t>embora perseguisse um ladrão</t>
+        </is>
+      </c>
+      <c r="M107" t="inlineStr">
+        <is>
+          <t>desde que perseguisse um ladrão</t>
+        </is>
+      </c>
+      <c r="N107" t="inlineStr">
+        <is>
+          <t>por mais que perseguisse um ladrão</t>
+        </is>
+      </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P107" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q107" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>108</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>No trecho “Esse limite &lt;b&gt;poderia &lt;/b&gt;ser dado pelo próprio consumidor, se ele assim quiser?” (parágrafo 6), a forma verbal destacada expressa a noção de</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>Emprego de Tempos e Modos</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>dever</t>
+        </is>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>certeza</t>
+        </is>
+      </c>
+      <c r="L108" t="inlineStr">
+        <is>
+          <t>hipótese</t>
+        </is>
+      </c>
+      <c r="M108" t="inlineStr">
+        <is>
+          <t>obrigação</t>
+        </is>
+      </c>
+      <c r="N108" t="inlineStr">
+        <is>
+          <t>necessidade</t>
+        </is>
+      </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P108" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q108" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>109</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>BANCO DA AMAZÔNIA</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Em que frase o verbo destacado está flexionado, quanto a número e pessoa, de acordo com a norma-padrão da língua portuguesa?</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>Emprego de Tempos e Modos</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>No texto, &lt;u&gt;relacionam&lt;/u&gt;-se aos chicles a ideia de eternidade</t>
+        </is>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>&lt;u&gt;Referiu&lt;/u&gt;-se à eternidade, sem se dar conta, as duas meninas</t>
+        </is>
+      </c>
+      <c r="L109" t="inlineStr">
+        <is>
+          <t>&lt;u&gt;Enganam&lt;/u&gt;-se a respeito da eternidade aqueles que creem nela</t>
+        </is>
+      </c>
+      <c r="M109" t="inlineStr">
+        <is>
+          <t>Todos os anos, &lt;u&gt;consome&lt;/u&gt;-se muitas balas e chicletes em todo o país</t>
+        </is>
+      </c>
+      <c r="N109" t="inlineStr">
+        <is>
+          <t>Em muitas culturas, &lt;u&gt;defendem&lt;/u&gt;-se calorosamente a existência da eternidade</t>
+        </is>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P109" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q109" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>110</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Considere o trecho “Depois vieram as mães e avós doentes.” (l. 8-9).
+A frase em que se emprega uma flexão do verbo destacado, de acordo com a norma-padrão da língua portuguesa, é:</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>Emprego de Tempos e Modos</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>Não sei o que fazer depois que vinherem as mães e avós doentes</t>
+        </is>
+      </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>Depois que as mães e avós doentes virem, faremos alguma coisa</t>
+        </is>
+      </c>
+      <c r="L110" t="inlineStr">
+        <is>
+          <t>Depois que eu vim, as mães e avós doentes ficaram curadas</t>
+        </is>
+      </c>
+      <c r="M110" t="inlineStr">
+        <is>
+          <t>Depois, as mães e avós doentes tiveram vindo até aqui</t>
+        </is>
+      </c>
+      <c r="N110" t="inlineStr">
+        <is>
+          <t>Talvez seja melhor ir depois de vierem as mães e avós doentes</t>
+        </is>
+      </c>
+      <c r="O110" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P110" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q110" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>111</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>TRANSPETRO / SEGUN. OFICIAL</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>O distanciamento do autor em relação à história narrada para destacar um ponto de vista seu sobre a temática em foco é marcado pelo uso do verbo &lt;u&gt;ser&lt;/u&gt;, no período “&lt;u&gt;É &lt;/u&gt;um exercício estranho esse de começar a remoçar um corpo na imaginação, injetar movimento e desejo nos seus músculos, acelerando nele, de novo, a avareza de viver cada instante.” Caso o enunciador queira conferir ao trecho um caráter de possibilidade, a reescritura adequada à norma-padrão e ao contexto empregará o verbo &lt;u&gt;ser &lt;/u&gt;da seguinte forma:</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>Emprego de Tempos e Modos</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>Fosse</t>
+        </is>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>Seria</t>
+        </is>
+      </c>
+      <c r="L111" t="inlineStr">
+        <is>
+          <t>Foi</t>
+        </is>
+      </c>
+      <c r="M111" t="inlineStr">
+        <is>
+          <t>Era</t>
+        </is>
+      </c>
+      <c r="N111" t="inlineStr">
+        <is>
+          <t>Fora</t>
+        </is>
+      </c>
+      <c r="O111" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P111" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q111" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
:up: :lady_beetle: agora permitese imagem nas questoes e foi consertado o cargo aparecendo junto com a instit
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q111"/>
+  <dimension ref="A1:R112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,6 +507,11 @@
           <t>acertos</t>
         </is>
       </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>imagem</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -588,6 +593,7 @@
       <c r="Q2" t="n">
         <v>0</v>
       </c>
+      <c r="R2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -668,6 +674,7 @@
       <c r="Q3" t="n">
         <v>0</v>
       </c>
+      <c r="R3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -747,6 +754,7 @@
       <c r="Q4" t="n">
         <v>0</v>
       </c>
+      <c r="R4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -826,6 +834,7 @@
       <c r="Q5" t="n">
         <v>0</v>
       </c>
+      <c r="R5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -905,6 +914,7 @@
       <c r="Q6" t="n">
         <v>0</v>
       </c>
+      <c r="R6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -984,6 +994,7 @@
       <c r="Q7" t="n">
         <v>0</v>
       </c>
+      <c r="R7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1063,6 +1074,7 @@
       <c r="Q8" t="n">
         <v>0</v>
       </c>
+      <c r="R8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1142,6 +1154,7 @@
       <c r="Q9" t="n">
         <v>0</v>
       </c>
+      <c r="R9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1221,6 +1234,7 @@
       <c r="Q10" t="n">
         <v>0</v>
       </c>
+      <c r="R10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1300,6 +1314,7 @@
       <c r="Q11" t="n">
         <v>0</v>
       </c>
+      <c r="R11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1379,6 +1394,7 @@
       <c r="Q12" t="n">
         <v>0</v>
       </c>
+      <c r="R12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1458,6 +1474,7 @@
       <c r="Q13" t="n">
         <v>0</v>
       </c>
+      <c r="R13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1537,6 +1554,7 @@
       <c r="Q14" t="n">
         <v>0</v>
       </c>
+      <c r="R14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1616,6 +1634,7 @@
       <c r="Q15" t="n">
         <v>0</v>
       </c>
+      <c r="R15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1695,6 +1714,7 @@
       <c r="Q16" t="n">
         <v>0</v>
       </c>
+      <c r="R16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1774,6 +1794,7 @@
       <c r="Q17" t="n">
         <v>0</v>
       </c>
+      <c r="R17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1853,6 +1874,7 @@
       <c r="Q18" t="n">
         <v>0</v>
       </c>
+      <c r="R18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1932,6 +1954,7 @@
       <c r="Q19" t="n">
         <v>0</v>
       </c>
+      <c r="R19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -2011,6 +2034,7 @@
       <c r="Q20" t="n">
         <v>0</v>
       </c>
+      <c r="R20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -2091,6 +2115,7 @@
       <c r="Q21" t="n">
         <v>0</v>
       </c>
+      <c r="R21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -2170,6 +2195,7 @@
       <c r="Q22" t="n">
         <v>0</v>
       </c>
+      <c r="R22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -2249,6 +2275,7 @@
       <c r="Q23" t="n">
         <v>0</v>
       </c>
+      <c r="R23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -2328,6 +2355,7 @@
       <c r="Q24" t="n">
         <v>0</v>
       </c>
+      <c r="R24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -2407,6 +2435,7 @@
       <c r="Q25" t="n">
         <v>0</v>
       </c>
+      <c r="R25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2486,6 +2515,7 @@
       <c r="Q26" t="n">
         <v>0</v>
       </c>
+      <c r="R26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2567,6 +2597,7 @@
       <c r="Q27" t="n">
         <v>0</v>
       </c>
+      <c r="R27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2648,6 +2679,7 @@
       <c r="Q28" t="n">
         <v>0</v>
       </c>
+      <c r="R28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2729,6 +2761,7 @@
       <c r="Q29" t="n">
         <v>0</v>
       </c>
+      <c r="R29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -2811,6 +2844,7 @@
       <c r="Q30" t="n">
         <v>0</v>
       </c>
+      <c r="R30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -2892,6 +2926,7 @@
       <c r="Q31" t="n">
         <v>0</v>
       </c>
+      <c r="R31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -2974,6 +3009,7 @@
       <c r="Q32" t="n">
         <v>0</v>
       </c>
+      <c r="R32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -3055,6 +3091,7 @@
       <c r="Q33" t="n">
         <v>0</v>
       </c>
+      <c r="R33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3136,6 +3173,7 @@
       <c r="Q34" t="n">
         <v>0</v>
       </c>
+      <c r="R34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -3217,6 +3255,7 @@
       <c r="Q35" t="n">
         <v>0</v>
       </c>
+      <c r="R35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -3298,6 +3337,7 @@
       <c r="Q36" t="n">
         <v>0</v>
       </c>
+      <c r="R36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -3379,6 +3419,7 @@
       <c r="Q37" t="n">
         <v>0</v>
       </c>
+      <c r="R37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -3461,6 +3502,7 @@
       <c r="Q38" t="n">
         <v>0</v>
       </c>
+      <c r="R38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -3542,6 +3584,7 @@
       <c r="Q39" t="n">
         <v>0</v>
       </c>
+      <c r="R39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -3623,6 +3666,7 @@
       <c r="Q40" t="n">
         <v>0</v>
       </c>
+      <c r="R40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -3705,6 +3749,7 @@
       <c r="Q41" t="n">
         <v>0</v>
       </c>
+      <c r="R41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -3787,6 +3832,7 @@
       <c r="Q42" t="n">
         <v>0</v>
       </c>
+      <c r="R42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -3869,6 +3915,7 @@
       <c r="Q43" t="n">
         <v>0</v>
       </c>
+      <c r="R43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -3950,6 +3997,7 @@
       <c r="Q44" t="n">
         <v>0</v>
       </c>
+      <c r="R44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -4031,6 +4079,7 @@
       <c r="Q45" t="n">
         <v>0</v>
       </c>
+      <c r="R45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -4113,6 +4162,7 @@
       <c r="Q46" t="n">
         <v>0</v>
       </c>
+      <c r="R46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -4194,6 +4244,7 @@
       <c r="Q47" t="n">
         <v>0</v>
       </c>
+      <c r="R47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -4275,6 +4326,7 @@
       <c r="Q48" t="n">
         <v>0</v>
       </c>
+      <c r="R48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -4371,6 +4423,7 @@
       <c r="Q49" t="n">
         <v>0</v>
       </c>
+      <c r="R49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -4453,6 +4506,7 @@
       <c r="Q50" t="n">
         <v>0</v>
       </c>
+      <c r="R50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -4534,6 +4588,7 @@
       <c r="Q51" t="n">
         <v>0</v>
       </c>
+      <c r="R51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -4615,6 +4670,7 @@
       <c r="Q52" t="n">
         <v>0</v>
       </c>
+      <c r="R52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -4696,6 +4752,7 @@
       <c r="Q53" t="n">
         <v>0</v>
       </c>
+      <c r="R53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -4777,6 +4834,7 @@
       <c r="Q54" t="n">
         <v>0</v>
       </c>
+      <c r="R54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -4909,6 +4967,7 @@
       <c r="Q55" t="n">
         <v>0</v>
       </c>
+      <c r="R55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -4991,6 +5050,7 @@
       <c r="Q56" t="n">
         <v>0</v>
       </c>
+      <c r="R56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -5072,6 +5132,7 @@
       <c r="Q57" t="n">
         <v>0</v>
       </c>
+      <c r="R57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -5153,6 +5214,7 @@
       <c r="Q58" t="n">
         <v>0</v>
       </c>
+      <c r="R58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -5276,6 +5338,7 @@
       <c r="Q59" t="n">
         <v>0</v>
       </c>
+      <c r="R59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -5410,6 +5473,7 @@
       <c r="Q60" t="n">
         <v>0</v>
       </c>
+      <c r="R60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -5544,6 +5608,7 @@
       <c r="Q61" t="n">
         <v>0</v>
       </c>
+      <c r="R61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -5678,6 +5743,7 @@
       <c r="Q62" t="n">
         <v>0</v>
       </c>
+      <c r="R62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -5800,6 +5866,7 @@
       <c r="Q63" t="n">
         <v>0</v>
       </c>
+      <c r="R63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -5927,6 +5994,7 @@
       <c r="Q64" t="n">
         <v>0</v>
       </c>
+      <c r="R64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -6008,6 +6076,7 @@
       <c r="Q65" t="n">
         <v>0</v>
       </c>
+      <c r="R65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -6089,6 +6158,7 @@
       <c r="Q66" t="n">
         <v>0</v>
       </c>
+      <c r="R66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -6170,6 +6240,7 @@
       <c r="Q67" t="n">
         <v>0</v>
       </c>
+      <c r="R67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -6252,6 +6323,7 @@
       <c r="Q68" t="n">
         <v>0</v>
       </c>
+      <c r="R68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -6333,6 +6405,7 @@
       <c r="Q69" t="n">
         <v>0</v>
       </c>
+      <c r="R69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -6414,6 +6487,7 @@
       <c r="Q70" t="n">
         <v>0</v>
       </c>
+      <c r="R70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -6496,6 +6570,7 @@
       <c r="Q71" t="n">
         <v>0</v>
       </c>
+      <c r="R71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -6577,6 +6652,7 @@
       <c r="Q72" t="n">
         <v>0</v>
       </c>
+      <c r="R72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -6658,6 +6734,7 @@
       <c r="Q73" t="n">
         <v>0</v>
       </c>
+      <c r="R73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -6739,6 +6816,7 @@
       <c r="Q74" t="n">
         <v>0</v>
       </c>
+      <c r="R74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -6820,6 +6898,7 @@
       <c r="Q75" t="n">
         <v>0</v>
       </c>
+      <c r="R75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -6902,6 +6981,7 @@
       <c r="Q76" t="n">
         <v>0</v>
       </c>
+      <c r="R76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -6984,6 +7064,7 @@
       <c r="Q77" t="n">
         <v>0</v>
       </c>
+      <c r="R77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -7065,6 +7146,7 @@
       <c r="Q78" t="n">
         <v>0</v>
       </c>
+      <c r="R78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -7183,6 +7265,7 @@
       <c r="Q79" t="n">
         <v>0</v>
       </c>
+      <c r="R79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -7264,6 +7347,7 @@
       <c r="Q80" t="n">
         <v>0</v>
       </c>
+      <c r="R80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -7355,6 +7439,7 @@
       <c r="Q81" t="n">
         <v>0</v>
       </c>
+      <c r="R81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -7445,6 +7530,7 @@
       <c r="Q82" t="n">
         <v>0</v>
       </c>
+      <c r="R82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -7539,6 +7625,7 @@
       <c r="Q83" t="n">
         <v>0</v>
       </c>
+      <c r="R83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -7629,6 +7716,7 @@
       <c r="Q84" t="n">
         <v>0</v>
       </c>
+      <c r="R84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -7710,6 +7798,7 @@
       <c r="Q85" t="n">
         <v>0</v>
       </c>
+      <c r="R85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -7786,6 +7875,7 @@
       <c r="Q86" t="n">
         <v>0</v>
       </c>
+      <c r="R86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -7867,6 +7957,7 @@
       <c r="Q87" t="n">
         <v>0</v>
       </c>
+      <c r="R87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -7948,6 +8039,7 @@
       <c r="Q88" t="n">
         <v>0</v>
       </c>
+      <c r="R88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -8029,6 +8121,7 @@
       <c r="Q89" t="n">
         <v>0</v>
       </c>
+      <c r="R89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -8110,6 +8203,7 @@
       <c r="Q90" t="n">
         <v>0</v>
       </c>
+      <c r="R90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -8191,6 +8285,7 @@
       <c r="Q91" t="n">
         <v>0</v>
       </c>
+      <c r="R91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -8272,6 +8367,7 @@
       <c r="Q92" t="n">
         <v>0</v>
       </c>
+      <c r="R92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -8353,6 +8449,7 @@
       <c r="Q93" t="n">
         <v>0</v>
       </c>
+      <c r="R93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -8434,6 +8531,7 @@
       <c r="Q94" t="n">
         <v>0</v>
       </c>
+      <c r="R94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -8515,6 +8613,7 @@
       <c r="Q95" t="n">
         <v>0</v>
       </c>
+      <c r="R95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -8596,6 +8695,7 @@
       <c r="Q96" t="n">
         <v>0</v>
       </c>
+      <c r="R96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -8678,6 +8778,7 @@
       <c r="Q97" t="n">
         <v>0</v>
       </c>
+      <c r="R97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -8759,6 +8860,7 @@
       <c r="Q98" t="n">
         <v>0</v>
       </c>
+      <c r="R98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -8840,6 +8942,7 @@
       <c r="Q99" t="n">
         <v>0</v>
       </c>
+      <c r="R99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -8921,6 +9024,7 @@
       <c r="Q100" t="n">
         <v>0</v>
       </c>
+      <c r="R100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -9003,6 +9107,7 @@
       <c r="Q101" t="n">
         <v>0</v>
       </c>
+      <c r="R101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -9084,6 +9189,7 @@
       <c r="Q102" t="n">
         <v>0</v>
       </c>
+      <c r="R102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -9165,6 +9271,7 @@
       <c r="Q103" t="n">
         <v>0</v>
       </c>
+      <c r="R103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -9246,6 +9353,7 @@
       <c r="Q104" t="n">
         <v>0</v>
       </c>
+      <c r="R104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -9327,6 +9435,7 @@
       <c r="Q105" t="n">
         <v>0</v>
       </c>
+      <c r="R105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -9419,6 +9528,7 @@
       <c r="Q106" t="n">
         <v>0</v>
       </c>
+      <c r="R106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -9514,6 +9624,7 @@
       <c r="Q107" t="n">
         <v>0</v>
       </c>
+      <c r="R107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -9595,6 +9706,7 @@
       <c r="Q108" t="n">
         <v>0</v>
       </c>
+      <c r="R108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -9676,6 +9788,7 @@
       <c r="Q109" t="n">
         <v>0</v>
       </c>
+      <c r="R109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -9758,6 +9871,7 @@
       <c r="Q110" t="n">
         <v>0</v>
       </c>
+      <c r="R110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -9838,6 +9952,93 @@
       </c>
       <c r="Q111" t="n">
         <v>0</v>
+      </c>
+      <c r="R111" t="inlineStr"/>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>112</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>UNIRIO</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>No final do primeiro parágrafo do Texto III, o autor compara o tempo a um imperador sem rivais, pois é o tempo “que diz que passa quando, de fato, quem passa somos nós”. O presente do indicativo, empregado três vezes nessa passagem, produz o seguinte efeito de sentido:</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>Emprego de Tempos e Modos</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>atribui validade permanente a uma afirmação</t>
+        </is>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>confere atualidade a uma ação ocorrida no passado</t>
+        </is>
+      </c>
+      <c r="L112" t="inlineStr">
+        <is>
+          <t>retrata algo ocorrido no momento da fala do imperador</t>
+        </is>
+      </c>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>indica um fato próximo, cuja realização é dada como certa</t>
+        </is>
+      </c>
+      <c r="N112" t="inlineStr">
+        <is>
+          <t>infere à cena apresentada uma descrição do momento vivido</t>
+        </is>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P112" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q112" t="n">
+        <v>0</v>
+      </c>
+      <c r="R112" t="inlineStr">
+        <is>
+          <t>c9d85a2c-787d-4cdf-9180-4064fa5dcf83.png</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:up: verificação cruzada em todas as alternativas
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R112"/>
+  <dimension ref="A1:R123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -593,7 +593,6 @@
       <c r="Q2" t="n">
         <v>0</v>
       </c>
-      <c r="R2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -674,7 +673,6 @@
       <c r="Q3" t="n">
         <v>0</v>
       </c>
-      <c r="R3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -754,7 +752,6 @@
       <c r="Q4" t="n">
         <v>0</v>
       </c>
-      <c r="R4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -834,7 +831,6 @@
       <c r="Q5" t="n">
         <v>0</v>
       </c>
-      <c r="R5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -914,7 +910,6 @@
       <c r="Q6" t="n">
         <v>0</v>
       </c>
-      <c r="R6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -994,7 +989,6 @@
       <c r="Q7" t="n">
         <v>0</v>
       </c>
-      <c r="R7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1074,7 +1068,6 @@
       <c r="Q8" t="n">
         <v>0</v>
       </c>
-      <c r="R8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1154,7 +1147,6 @@
       <c r="Q9" t="n">
         <v>0</v>
       </c>
-      <c r="R9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1234,7 +1226,6 @@
       <c r="Q10" t="n">
         <v>0</v>
       </c>
-      <c r="R10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1314,7 +1305,6 @@
       <c r="Q11" t="n">
         <v>0</v>
       </c>
-      <c r="R11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1394,7 +1384,6 @@
       <c r="Q12" t="n">
         <v>0</v>
       </c>
-      <c r="R12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1474,7 +1463,6 @@
       <c r="Q13" t="n">
         <v>0</v>
       </c>
-      <c r="R13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1554,7 +1542,6 @@
       <c r="Q14" t="n">
         <v>0</v>
       </c>
-      <c r="R14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1634,7 +1621,6 @@
       <c r="Q15" t="n">
         <v>0</v>
       </c>
-      <c r="R15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1714,7 +1700,6 @@
       <c r="Q16" t="n">
         <v>0</v>
       </c>
-      <c r="R16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1794,7 +1779,6 @@
       <c r="Q17" t="n">
         <v>0</v>
       </c>
-      <c r="R17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1874,7 +1858,6 @@
       <c r="Q18" t="n">
         <v>0</v>
       </c>
-      <c r="R18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1954,7 +1937,6 @@
       <c r="Q19" t="n">
         <v>0</v>
       </c>
-      <c r="R19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -2034,7 +2016,6 @@
       <c r="Q20" t="n">
         <v>0</v>
       </c>
-      <c r="R20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -2115,7 +2096,6 @@
       <c r="Q21" t="n">
         <v>0</v>
       </c>
-      <c r="R21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -2195,7 +2175,6 @@
       <c r="Q22" t="n">
         <v>0</v>
       </c>
-      <c r="R22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -2275,7 +2254,6 @@
       <c r="Q23" t="n">
         <v>0</v>
       </c>
-      <c r="R23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -2355,7 +2333,6 @@
       <c r="Q24" t="n">
         <v>0</v>
       </c>
-      <c r="R24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -2435,7 +2412,6 @@
       <c r="Q25" t="n">
         <v>0</v>
       </c>
-      <c r="R25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2515,7 +2491,6 @@
       <c r="Q26" t="n">
         <v>0</v>
       </c>
-      <c r="R26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2597,7 +2572,6 @@
       <c r="Q27" t="n">
         <v>0</v>
       </c>
-      <c r="R27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2679,7 +2653,6 @@
       <c r="Q28" t="n">
         <v>0</v>
       </c>
-      <c r="R28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2761,7 +2734,6 @@
       <c r="Q29" t="n">
         <v>0</v>
       </c>
-      <c r="R29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -2844,7 +2816,6 @@
       <c r="Q30" t="n">
         <v>0</v>
       </c>
-      <c r="R30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -2926,7 +2897,6 @@
       <c r="Q31" t="n">
         <v>0</v>
       </c>
-      <c r="R31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -3009,7 +2979,6 @@
       <c r="Q32" t="n">
         <v>0</v>
       </c>
-      <c r="R32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -3091,7 +3060,6 @@
       <c r="Q33" t="n">
         <v>0</v>
       </c>
-      <c r="R33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3173,7 +3141,6 @@
       <c r="Q34" t="n">
         <v>0</v>
       </c>
-      <c r="R34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -3255,7 +3222,6 @@
       <c r="Q35" t="n">
         <v>0</v>
       </c>
-      <c r="R35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -3337,7 +3303,6 @@
       <c r="Q36" t="n">
         <v>0</v>
       </c>
-      <c r="R36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -3419,7 +3384,6 @@
       <c r="Q37" t="n">
         <v>0</v>
       </c>
-      <c r="R37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -3502,7 +3466,6 @@
       <c r="Q38" t="n">
         <v>0</v>
       </c>
-      <c r="R38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -3584,7 +3547,6 @@
       <c r="Q39" t="n">
         <v>0</v>
       </c>
-      <c r="R39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -3666,7 +3628,6 @@
       <c r="Q40" t="n">
         <v>0</v>
       </c>
-      <c r="R40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -3749,7 +3710,6 @@
       <c r="Q41" t="n">
         <v>0</v>
       </c>
-      <c r="R41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -3832,7 +3792,6 @@
       <c r="Q42" t="n">
         <v>0</v>
       </c>
-      <c r="R42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -3915,7 +3874,6 @@
       <c r="Q43" t="n">
         <v>0</v>
       </c>
-      <c r="R43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -3997,7 +3955,6 @@
       <c r="Q44" t="n">
         <v>0</v>
       </c>
-      <c r="R44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -4079,7 +4036,6 @@
       <c r="Q45" t="n">
         <v>0</v>
       </c>
-      <c r="R45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -4162,7 +4118,6 @@
       <c r="Q46" t="n">
         <v>0</v>
       </c>
-      <c r="R46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -4244,7 +4199,6 @@
       <c r="Q47" t="n">
         <v>0</v>
       </c>
-      <c r="R47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -4326,7 +4280,6 @@
       <c r="Q48" t="n">
         <v>0</v>
       </c>
-      <c r="R48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -4423,7 +4376,6 @@
       <c r="Q49" t="n">
         <v>0</v>
       </c>
-      <c r="R49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -4506,7 +4458,6 @@
       <c r="Q50" t="n">
         <v>0</v>
       </c>
-      <c r="R50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -4588,7 +4539,6 @@
       <c r="Q51" t="n">
         <v>0</v>
       </c>
-      <c r="R51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -4670,7 +4620,6 @@
       <c r="Q52" t="n">
         <v>0</v>
       </c>
-      <c r="R52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -4752,7 +4701,6 @@
       <c r="Q53" t="n">
         <v>0</v>
       </c>
-      <c r="R53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -4834,7 +4782,6 @@
       <c r="Q54" t="n">
         <v>0</v>
       </c>
-      <c r="R54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -4967,7 +4914,6 @@
       <c r="Q55" t="n">
         <v>0</v>
       </c>
-      <c r="R55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -5050,7 +4996,6 @@
       <c r="Q56" t="n">
         <v>0</v>
       </c>
-      <c r="R56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -5132,7 +5077,6 @@
       <c r="Q57" t="n">
         <v>0</v>
       </c>
-      <c r="R57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -5214,7 +5158,6 @@
       <c r="Q58" t="n">
         <v>0</v>
       </c>
-      <c r="R58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -5338,7 +5281,6 @@
       <c r="Q59" t="n">
         <v>0</v>
       </c>
-      <c r="R59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -5473,7 +5415,6 @@
       <c r="Q60" t="n">
         <v>0</v>
       </c>
-      <c r="R60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -5608,7 +5549,6 @@
       <c r="Q61" t="n">
         <v>0</v>
       </c>
-      <c r="R61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -5743,7 +5683,6 @@
       <c r="Q62" t="n">
         <v>0</v>
       </c>
-      <c r="R62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -5866,7 +5805,6 @@
       <c r="Q63" t="n">
         <v>0</v>
       </c>
-      <c r="R63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -5994,7 +5932,6 @@
       <c r="Q64" t="n">
         <v>0</v>
       </c>
-      <c r="R64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -6076,7 +6013,6 @@
       <c r="Q65" t="n">
         <v>0</v>
       </c>
-      <c r="R65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -6158,7 +6094,6 @@
       <c r="Q66" t="n">
         <v>0</v>
       </c>
-      <c r="R66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -6240,7 +6175,6 @@
       <c r="Q67" t="n">
         <v>0</v>
       </c>
-      <c r="R67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -6323,7 +6257,6 @@
       <c r="Q68" t="n">
         <v>0</v>
       </c>
-      <c r="R68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -6405,7 +6338,6 @@
       <c r="Q69" t="n">
         <v>0</v>
       </c>
-      <c r="R69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -6487,7 +6419,6 @@
       <c r="Q70" t="n">
         <v>0</v>
       </c>
-      <c r="R70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -6570,7 +6501,6 @@
       <c r="Q71" t="n">
         <v>0</v>
       </c>
-      <c r="R71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -6652,7 +6582,6 @@
       <c r="Q72" t="n">
         <v>0</v>
       </c>
-      <c r="R72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -6734,7 +6663,6 @@
       <c r="Q73" t="n">
         <v>0</v>
       </c>
-      <c r="R73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -6816,7 +6744,6 @@
       <c r="Q74" t="n">
         <v>0</v>
       </c>
-      <c r="R74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -6898,7 +6825,6 @@
       <c r="Q75" t="n">
         <v>0</v>
       </c>
-      <c r="R75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -6981,7 +6907,6 @@
       <c r="Q76" t="n">
         <v>0</v>
       </c>
-      <c r="R76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -7064,7 +6989,6 @@
       <c r="Q77" t="n">
         <v>0</v>
       </c>
-      <c r="R77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -7146,7 +7070,6 @@
       <c r="Q78" t="n">
         <v>0</v>
       </c>
-      <c r="R78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -7265,7 +7188,6 @@
       <c r="Q79" t="n">
         <v>0</v>
       </c>
-      <c r="R79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -7347,7 +7269,6 @@
       <c r="Q80" t="n">
         <v>0</v>
       </c>
-      <c r="R80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -7439,7 +7360,6 @@
       <c r="Q81" t="n">
         <v>0</v>
       </c>
-      <c r="R81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -7530,7 +7450,6 @@
       <c r="Q82" t="n">
         <v>0</v>
       </c>
-      <c r="R82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -7625,7 +7544,6 @@
       <c r="Q83" t="n">
         <v>0</v>
       </c>
-      <c r="R83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -7716,7 +7634,6 @@
       <c r="Q84" t="n">
         <v>0</v>
       </c>
-      <c r="R84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -7798,7 +7715,6 @@
       <c r="Q85" t="n">
         <v>0</v>
       </c>
-      <c r="R85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -7875,7 +7791,6 @@
       <c r="Q86" t="n">
         <v>0</v>
       </c>
-      <c r="R86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -7957,7 +7872,6 @@
       <c r="Q87" t="n">
         <v>0</v>
       </c>
-      <c r="R87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -8039,7 +7953,6 @@
       <c r="Q88" t="n">
         <v>0</v>
       </c>
-      <c r="R88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -8121,7 +8034,6 @@
       <c r="Q89" t="n">
         <v>0</v>
       </c>
-      <c r="R89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -8203,7 +8115,6 @@
       <c r="Q90" t="n">
         <v>0</v>
       </c>
-      <c r="R90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -8285,7 +8196,6 @@
       <c r="Q91" t="n">
         <v>0</v>
       </c>
-      <c r="R91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -8367,7 +8277,6 @@
       <c r="Q92" t="n">
         <v>0</v>
       </c>
-      <c r="R92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -8449,7 +8358,6 @@
       <c r="Q93" t="n">
         <v>0</v>
       </c>
-      <c r="R93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -8531,7 +8439,6 @@
       <c r="Q94" t="n">
         <v>0</v>
       </c>
-      <c r="R94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -8613,7 +8520,6 @@
       <c r="Q95" t="n">
         <v>0</v>
       </c>
-      <c r="R95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -8695,7 +8601,6 @@
       <c r="Q96" t="n">
         <v>0</v>
       </c>
-      <c r="R96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -8778,7 +8683,6 @@
       <c r="Q97" t="n">
         <v>0</v>
       </c>
-      <c r="R97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -8860,7 +8764,6 @@
       <c r="Q98" t="n">
         <v>0</v>
       </c>
-      <c r="R98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -8942,7 +8845,6 @@
       <c r="Q99" t="n">
         <v>0</v>
       </c>
-      <c r="R99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -9024,7 +8926,6 @@
       <c r="Q100" t="n">
         <v>0</v>
       </c>
-      <c r="R100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -9107,7 +9008,6 @@
       <c r="Q101" t="n">
         <v>0</v>
       </c>
-      <c r="R101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -9189,7 +9089,6 @@
       <c r="Q102" t="n">
         <v>0</v>
       </c>
-      <c r="R102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -9271,7 +9170,6 @@
       <c r="Q103" t="n">
         <v>0</v>
       </c>
-      <c r="R103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -9353,7 +9251,6 @@
       <c r="Q104" t="n">
         <v>0</v>
       </c>
-      <c r="R104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -9435,7 +9332,6 @@
       <c r="Q105" t="n">
         <v>0</v>
       </c>
-      <c r="R105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -9528,7 +9424,6 @@
       <c r="Q106" t="n">
         <v>0</v>
       </c>
-      <c r="R106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -9624,7 +9519,6 @@
       <c r="Q107" t="n">
         <v>0</v>
       </c>
-      <c r="R107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -9706,7 +9600,6 @@
       <c r="Q108" t="n">
         <v>0</v>
       </c>
-      <c r="R108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -9788,7 +9681,6 @@
       <c r="Q109" t="n">
         <v>0</v>
       </c>
-      <c r="R109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -9871,7 +9763,6 @@
       <c r="Q110" t="n">
         <v>0</v>
       </c>
-      <c r="R110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -9953,7 +9844,6 @@
       <c r="Q111" t="n">
         <v>0</v>
       </c>
-      <c r="R111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -10040,6 +9930,905 @@
           <t>c9d85a2c-787d-4cdf-9180-4064fa5dcf83.png</t>
         </is>
       </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>113</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>UNIRIO</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Em “Fazia calor no Rio, 40 graus e qualquer coisa, quase 41.” (l. 1-2), o uso do pretérito imperfeito do indicativo busca.</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>Emprego de Tempos e Modos</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>estabelecer uma relação de causa e efeito</t>
+        </is>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>contextualizar o tempo da narrativa</t>
+        </is>
+      </c>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>introduzir uma ambiência de suspense</t>
+        </is>
+      </c>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>banalizar o calor que fazia no Rio</t>
+        </is>
+      </c>
+      <c r="N113" t="inlineStr">
+        <is>
+          <t>projetar uma possibilidade</t>
+        </is>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P113" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q113" t="n">
+        <v>0</v>
+      </c>
+      <c r="R113" t="inlineStr">
+        <is>
+          <t>7b209d1e-87f0-48a2-b97f-00b3f541acb2.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>114</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>BANCO DA AMAZÔNIA</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>O verbo em destaque está conjugado de acordo com a norma-padrão em:</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>Emprego de Tempos e Modos</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>&lt;u&gt;Pegue &lt;/u&gt;o outro elevador, por favor</t>
+        </is>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>É preciso que você &lt;u&gt;esteje &lt;/u&gt;atento a situações de perigo</t>
+        </is>
+      </c>
+      <c r="L114" t="inlineStr">
+        <is>
+          <t>Será muito bom se você &lt;u&gt;propor &lt;/u&gt;um outro acesso aos passageiros</t>
+        </is>
+      </c>
+      <c r="M114" t="inlineStr">
+        <is>
+          <t>&lt;u&gt;Seje&lt;/u&gt; sempre bem-humorado com os passageiros</t>
+        </is>
+      </c>
+      <c r="N114" t="inlineStr">
+        <is>
+          <t>Gostaríamos de que você &lt;u&gt;vesse &lt;/u&gt;esse filme</t>
+        </is>
+      </c>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P114" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q114" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>115</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>A forma verbal destacada está empregada de acordo com a norma-padrão em:</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>Emprego de Tempos e Modos</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>Quando as pessoas &lt;u&gt;fazerem &lt;/u&gt;compras nas lojas locais, poderão usar o cartão de crédito comunitário</t>
+        </is>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>Os consumidores preocupados com os gastos tinham &lt;u&gt;trago &lt;/u&gt;pouco dinheiro para as suas compras</t>
+        </is>
+      </c>
+      <c r="L115" t="inlineStr">
+        <is>
+          <t>Os financiamentos serão ampliados quando os bancos &lt;u&gt;estarem &lt;/u&gt;com os juros baixos</t>
+        </is>
+      </c>
+      <c r="M115" t="inlineStr">
+        <is>
+          <t>O ideal seria que os clientes dos bancos comunitários &lt;u&gt;pudessem &lt;/u&gt;aumentar sua renda mensal</t>
+        </is>
+      </c>
+      <c r="N115" t="inlineStr">
+        <is>
+          <t>Se os bancos &lt;u&gt;darem &lt;/u&gt;mais crédito aos moradores, aumentará a construção de casas na comunidade</t>
+        </is>
+      </c>
+      <c r="O115" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P115" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q115" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>116</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Em “os movimentos caóticos atuais já &lt;u&gt;eram &lt;/u&gt;os primeiros passos afinando-se e orquestrando-se para uma situação econômica mais digna", observa-se a adequada flexão do verbo destacado, o que também se verifica em</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>Emprego de Tempos e Modos</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t>O povo brasileiro sois articulado politicamente</t>
+        </is>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>Se fôssemos menos explorados, o país prosperaria mais</t>
+        </is>
+      </c>
+      <c r="L116" t="inlineStr">
+        <is>
+          <t>Quando fores corretos os políticos brasileiros, a fome terá fim</t>
+        </is>
+      </c>
+      <c r="M116" t="inlineStr">
+        <is>
+          <t>É fundamental que sejemos um povo mais politizado</t>
+        </is>
+      </c>
+      <c r="N116" t="inlineStr">
+        <is>
+          <t>A população deseja que o sistema de saúde sejais melhor</t>
+        </is>
+      </c>
+      <c r="O116" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P116" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q116" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>117</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>O emprego do verbo destacado no trecho “queremos contribuir para o crescimento sustentável das empresas” contribui para indicar uma pretensão do presidente do Sindicato dos Lojistas, que começa no presente e se estende no futuro.
+Se, respeitando-se o contexto original, a frase indicasse uma pretensão que começasse no passado e se estendesse no tempo, o verbo adequado seria o que se destaca em:</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>Emprego de Tempos e Modos</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t>&lt;u&gt;quisemos &lt;/u&gt;contribuir para o crescimento sustentável das empresas</t>
+        </is>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>&lt;u&gt;quisermos &lt;/u&gt;contribuir para o crescimento sustentável das empresas</t>
+        </is>
+      </c>
+      <c r="L117" t="inlineStr">
+        <is>
+          <t>&lt;u&gt;quiséssemos &lt;/u&gt;contribuir para o crescimento sustentável das empresas</t>
+        </is>
+      </c>
+      <c r="M117" t="inlineStr">
+        <is>
+          <t>&lt;u&gt;quereremos &lt;/u&gt;contribuir para o crescimento sustentável das empresas</t>
+        </is>
+      </c>
+      <c r="N117" t="inlineStr">
+        <is>
+          <t>&lt;u&gt;quisera &lt;/u&gt;poder contribuir para o crescimento sustentável das empresas</t>
+        </is>
+      </c>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P117" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q117" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>118</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Flexionado na 1ª pessoa do singular do presente do indicativo, o verbo fazer assume forma irregular: faço.
+O mesmo acontece com o seguinte verbo:</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>Emprego de Tempos e Modos</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J118" t="inlineStr">
+        <is>
+          <t>depender</t>
+        </is>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>dominar</t>
+        </is>
+      </c>
+      <c r="L118" t="inlineStr">
+        <is>
+          <t>medir</t>
+        </is>
+      </c>
+      <c r="M118" t="inlineStr">
+        <is>
+          <t>pensar</t>
+        </is>
+      </c>
+      <c r="N118" t="inlineStr">
+        <is>
+          <t>dever</t>
+        </is>
+      </c>
+      <c r="O118" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P118" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q118" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>119</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>A frase em que a flexão do verbo auxiliar destacado obedece aos princípios da norma padrão é</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>Emprego de Tempos e Modos</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J119" t="inlineStr">
+        <is>
+          <t>Alguns estudiosos consideram que &lt;u&gt;podem &lt;/u&gt;haver robôs tão inteligentes quanto o homem</t>
+        </is>
+      </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>&lt;u&gt;Devem &lt;/u&gt;existir formas de garantir a exploração de outras tarefas destinadas aos robôs</t>
+        </is>
+      </c>
+      <c r="L119" t="inlineStr">
+        <is>
+          <t>No futuro, &lt;u&gt;devem &lt;/u&gt;haver outras formas de investimentos para garantir a evolução da robótica</t>
+        </is>
+      </c>
+      <c r="M119" t="inlineStr">
+        <is>
+          <t>&lt;u&gt;Pode &lt;/u&gt;existir obstáculos que os robôs sejam capazes de superar, como a locomoção e o diálogo</t>
+        </is>
+      </c>
+      <c r="N119" t="inlineStr">
+        <is>
+          <t>&lt;u&gt;Pode &lt;/u&gt;surgir novas tecnologias para aperfeiçoar a conquista espacial</t>
+        </is>
+      </c>
+      <c r="O119" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P119" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q119" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>120</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>No trecho “Para o futuro, prenunciam-se perguntas mais difíceis, mais desafiadoras — e até ameaçadoras — do que aquelas relativas ao uso de drones.”, o verbo prenunciar foi utilizado no plural por se tratar de uma construção de passiva pronominal com sujeito também no plural. O mesmo procedimento é adotado no verbo destacado em:</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>Emprego de Tempos e Modos</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J120" t="inlineStr">
+        <is>
+          <t>Para conquistar posição de vanguarda na corrida espacial, &lt;u&gt;obedecem&lt;/u&gt;-se a princípios básicos de inovação tecnológica</t>
+        </is>
+      </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>Na missão espacial ao solo marciano, ambiente inóspito aos humanos, &lt;u&gt;assistiram&lt;/u&gt;-se a episódios inesquecíveis</t>
+        </is>
+      </c>
+      <c r="L120" t="inlineStr">
+        <is>
+          <t>Nos livros e filmes de ficção científica do século passado, &lt;u&gt;falavam&lt;/u&gt;-se de robôs como uma possibilidade muito próxima e viável</t>
+        </is>
+      </c>
+      <c r="M120" t="inlineStr">
+        <is>
+          <t>Com o avanço das pesquisas em robótica nas últimas décadas, &lt;u&gt;delegam&lt;/u&gt;-se atividades eminentemente humanas às máquinas</t>
+        </is>
+      </c>
+      <c r="N120" t="inlineStr">
+        <is>
+          <t>Para evitar que o crescimento da robótica provoque distorções incontroláveis, &lt;u&gt;necessitam&lt;/u&gt;-se de leis protecionistas</t>
+        </is>
+      </c>
+      <c r="O120" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P120" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q120" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>121</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>ELETRONUCLEAR</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Em que frase o verbo irregular destacado está empregado de acordo com a norma-padrão da Língua Portuguesa?</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>Verbos Traiçoeiros</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J121" t="inlineStr">
+        <is>
+          <t>Os médicos &lt;u&gt;preveram &lt;/u&gt;que ela teria complicações da doença. (verbo PREVER)</t>
+        </is>
+      </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>Se eu me &lt;u&gt;oposse &lt;/u&gt;a suas orientações, ela me advertia. (verbo OPOR)</t>
+        </is>
+      </c>
+      <c r="L121" t="inlineStr">
+        <is>
+          <t>Minha mãe sempre me &lt;u&gt;acodia &lt;/u&gt;nos momentos difíceis. (verbo ACUDIR)</t>
+        </is>
+      </c>
+      <c r="M121" t="inlineStr">
+        <is>
+          <t>Maria José sempre &lt;u&gt;soube &lt;/u&gt;defender filhos e netos. (verbo SABER)</t>
+        </is>
+      </c>
+      <c r="N121" t="inlineStr">
+        <is>
+          <t>Quando entrava numa briga, ela sempre &lt;u&gt;intervia &lt;/u&gt;em meu favor. (verbo INTERVIR)</t>
+        </is>
+      </c>
+      <c r="O121" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P121" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q121" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>122</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>A forma verbal destacada está empregada de acordo com a norma-padrão da Língua Portuguesa em:</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>Verbos Traiçoeiros</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J122" t="inlineStr">
+        <is>
+          <t>Se os governantes &lt;u&gt;verem &lt;/u&gt;o prejuízo causado pelas variações do clima, talvez tomem medidas cautelares</t>
+        </is>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>A construção de novas hidrelétricas dependia de que as verbas se &lt;u&gt;mantessem &lt;/u&gt;inalteradas</t>
+        </is>
+      </c>
+      <c r="L122" t="inlineStr">
+        <is>
+          <t>As variações do clima não afetariam o meio ambiente se a população &lt;u&gt;interviesse &lt;/u&gt;nas políticas públicas</t>
+        </is>
+      </c>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>Todos &lt;u&gt;ansiam &lt;/u&gt;que os eventos climáticos extremos não cheguem a causar problemas ambientais</t>
+        </is>
+      </c>
+      <c r="N122" t="inlineStr">
+        <is>
+          <t>Um grupo de pesquisadores &lt;u&gt;entreveu &lt;/u&gt;a possibilidade de prejuízos na produção de energia por causa das alterações das chuvas na Amazônia</t>
+        </is>
+      </c>
+      <c r="O122" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P122" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q122" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>123</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>A forma verbal destacada está empregada de acordo com a norma-padrão da Língua Portuguesa em:</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>Verbos Traiçoeiros</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J123" t="inlineStr">
+        <is>
+          <t>Se os governantes &lt;u&gt;verem &lt;/u&gt;o prejuízo causado pelas variações do clima, talvez tomem medidas cautelares</t>
+        </is>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>A construção de novas hidrelétricas dependia de que as verbas se &lt;u&gt;mantessem &lt;/u&gt;inalteradas</t>
+        </is>
+      </c>
+      <c r="L123" t="inlineStr">
+        <is>
+          <t>As variações do clima não afetariam o meio ambiente se a população &lt;u&gt;interviesse &lt;/u&gt;nas políticas públicas</t>
+        </is>
+      </c>
+      <c r="M123" t="inlineStr">
+        <is>
+          <t>Todos &lt;u&gt;ansiam &lt;/u&gt;que os eventos climáticos extremos não cheguem a causar problemas ambientais</t>
+        </is>
+      </c>
+      <c r="N123" t="inlineStr">
+        <is>
+          <t>Um grupo de pesquisadores &lt;u&gt;entreveu &lt;/u&gt;a possibilidade de prejuízos na produção de energia por causa das alterações das chuvas na Amazônia.G ABARITO 1. LETRA D 2. LETRA C</t>
+        </is>
+      </c>
+      <c r="O123" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P123" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q123" t="n">
+        <v>0</v>
+      </c>
+      <c r="R123" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
:ladtbeetle: consertado o problema com listas suspensas e chamadas de questoes sem parentes
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R123"/>
+  <dimension ref="A1:R163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10828,7 +10828,3438 @@
       <c r="Q123" t="n">
         <v>0</v>
       </c>
-      <c r="R123" t="inlineStr"/>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>124</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;À moda brasileira&lt;/b&gt;
+1 Estou me vendo debaixo de uma árvore, lendo a pequena história da literatura brasileira.
+2 Olavo Bilac! – eu disse em voz alta e de repente parei quase num susto depois que li os primeiros versos do soneto à língua portuguesa: Última flor do Lácio, inculta e bela / És, a um tempo, esplendor e sepultura.
+3 Fiquei pensando, mas o poeta disse sepultura?! O tal de Lácio eu não sabia onde ficava, mas de sepultura eu entendia bem, disso eu entendia, repensei baixando o olhar para a terra. Se escrevia (e já escrevia) pequenos contos nessa língua, quer dizer que era a sepultura que esperava por esses meus escritos?
+4 Fui falar com meu pai. Comecei por aquelas minhas sondagens antes de chegar até onde queria, os tais rodeios que ele ia ouvindo com paciência enquanto enrolava o cigarro de palha, fumava nessa época esses cigarros. Comecei por perguntar se minha mãe e ele não tinham viajado para o exterior.
+5 Meu pai fixou em mim o olhar verde. Viagens, só pelo Brasil, meus avós é que tinham feito aquelas longas viagens de navio, Portugal, França, Itália... Não esquecer que a minha avó, Pedrina Perucchi, era italiana, ele acrescentou. Mas por que essa curiosidade?
+6 Sentei-me ao lado dele, respirei fundo e comecei a gaguejar, é que seria tão bom se ambos tivessem nascido lá longe e assim eu estaria hoje escrevendo em italiano, italiano! – fiquei repetindo e abri o livro que trazia na mão: Olha aí, pai, o poeta escreveu com todas as letras, nossa língua é sepultura mesmo, tudo o que a gente fizer vai para debaixo da terra, desaparece!
+7 Calmamente ele pousou o cigarro no cinzeiro ao lado. Pegou os óculos. O soneto é muito bonito, disse me encarando com severidade. Feio é isso, filha, isso de querer renegar a própria língua. Se você chegar a escrever bem, não precisa ser em italiano ou espanhol ou alemão, você ficará na nossa língua mesmo, está me compreendendo? E as traduções? Renegar a língua é renegar o país, guarde isso nessa cabecinha. E depois (ele voltou a abrir o livro), olha que beleza o que o poeta escreveu em seguida, Amo-te assim, desconhecida e obscura, veja que confissão de amor ele fez à nossa língua! Tem mais, ele precisava da rima para sepultura e calhou tão bem essa obscura, entendeu agora? – acrescentou e levantou-se. Deu alguns passos e ficou olhando a borboleta que entrou na varanda: Já fez a sua lição de casa?
+8 Fechei o livro e recuei. Sempre que meu pai queria mudar de assunto ele mudava de lugar: saía da poltrona e ia para a cadeira de vime. Saía da cadeira de vime e ia para a rede ou simplesmente começava a andar. Era o sinal, Não quero falar nisso, chega. Então a gente falava noutra coisa ou ficava quieta.
+9 Tantos anos depois, quando me avisaram lá do pequeno hotel em Jacareí que ele tinha morrido, fiquei pensando nisso, ah! se quando a morte entrou, se nesse instante ele tivesse mudado de lugar. Mudar depressa de lugar e de assunto. Depressa, pai, saia da cama e fique na cadeira ou vá pra rua e feche a porta!
+(TELLES,LygiaFagundes.Duranteaqueleestranhochá:perdidoseachados.RiodeJaneiro:Rocco,2002,p.109-111.
+Fragmentoadaptado).
+Considerando-se a correlação adequada entre tempos e modos verbais, a alternativa que, respeitando a norma-padrão, completa o período iniciado pelo trecho “A autora também teria sido lida se...” é</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>Correlação Verbal</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J124" t="inlineStr">
+        <is>
+          <t>escrever seus contos em outra língua.</t>
+        </is>
+      </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>escrevera seus contos em outra língua.</t>
+        </is>
+      </c>
+      <c r="L124" t="inlineStr">
+        <is>
+          <t>tiver escrito seus contos em outra língua.</t>
+        </is>
+      </c>
+      <c r="M124" t="inlineStr">
+        <is>
+          <t>teria escrito seus contos em outra língua.</t>
+        </is>
+      </c>
+      <c r="N124" t="inlineStr">
+        <is>
+          <t>tivesse escrito seus contos em outra língua.</t>
+        </is>
+      </c>
+      <c r="O124" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P124" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q124" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>125</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>AgeRIO</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Eu sei, mas não devia&lt;/b&gt;
+Eu sei que a gente se acostuma. Mas não devia. A gente se acostuma a morar em apartamentos de fundos e a não ter outra vista que não as janelas ao redor. E, porque não tem vista, logo se acostuma a não olhar para fora. E, porque não olha para fora, logo se acostuma a não abrir de todo as cortinas. E, porque não abre as cortinas, logo se acostuma a acender mais cedo a luz. E, à medida que se acostuma, esquece o sol, esquece o ar, esquece a amplidão.
+A gente se acostuma a acordar de manhã sobressaltado porque está na hora. A tomar o café correndo porque está atrasado. A ler o jornal no ônibus porque não pode perder o tempo da viagem. A comer sanduíche porque não dá para almoçar. A sair do trabalho porque já é noite. A cochilar no ônibus porque está cansado. A deitar cedo e dormir pesado sem ter vivido o dia.
+A gente se acostuma a abrir o jornal e a ler sobre a guerra. E, aceitando a guerra, aceita os mortos e que haja números para os mortos. E, aceitando os números, aceita não acreditar nas negociações de paz. E, não acreditando nas negociações de paz, aceita ler todo dia da guerra, dos números, da longa duração.
+A gente se acostuma a esperar o dia inteiro e ouvir no telefone: hoje não posso ir. A sorrir para as pessoas sem receber um sorriso de volta. A ser ignorado quando precisava tanto ser visto.
+A gente se acostuma a pagar por tudo o que deseja e o de que necessita. E a lutar para ganhar o dinheiro com que pagar. E a ganhar menos do que precisa. E a fazer fila para pagar. E a pagar mais do que as coisas valem. E a saber que cada vez paga mais. E a procurar mais trabalho, para ganhar mais dinheiro, para ter com que pagar nas filas em que se cobra.
+A gente se acostuma a andar na rua e ver cartazes. A abrir as revistas e ver anúncios. A ligar a televisão e assistir a comerciais. A ir ao cinema e engolir publicidade. A ser instigado, conduzido, desnorteado, lançado na infindável catarata dos produtos.
+A gente se acostuma à poluição. Às salas fechadas de ar-condicionado e cheiro de cigarro. À luz artificial de ligeiro tremor. Ao choque que os olhos levam na luz natural. Às bactérias da água potável. À contaminação da água do mar. À lenta morte dos rios. Se acostuma a não ouvir passarinho, a não ter galo de madrugada, a temer a hidrofobia dos cães, a não colher fruta no pé, a não ter sequer uma planta.
+A gente se acostuma a coisas de mais, para não sofrer. Em doses pequenas, tentando não perceber, vai afastando uma dor aqui, um ressentimento ali, uma revolta acolá. Se o cinema está cheio, a gente senta na primeira fila e torce um pouco o pescoço. Se a praia está contaminada, a gente molha só os pés e sua no resto do corpo. Se o trabalho está duro, a gente se consola pensando no fim de semana. E se, no fim de semana, não há muito o que fazer, a gente vai dormir cedo e ainda fica satisfeito porque tem sempre sono atrasado.
+A gente se acostuma para não se ralar na aspereza, para preservar a pele. Se acostuma para evitar feridas, sangramentos, para esquivar-se de faca e baioneta, para poupar o peito. A gente se acostuma para poupar a vida. Que aos poucos se gasta, e que, gasta de tanto acostumar, se perde de si mesma.
+(COLASANTI,M.Eusei,masnãodevia.RiodeJaneiro:RoccoEditora,1996.p.9.Adaptado).
+Considerando-se a combinação entre tempos e modos, a frase que atende à norma-padrão é:</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>Correlação Verbal</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J125" t="inlineStr">
+        <is>
+          <t>Como chovesse muito pela manhã, resolvi sair à tarde.</t>
+        </is>
+      </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>Se nós nos acostumássemos, seremos felizes.</t>
+        </is>
+      </c>
+      <c r="L125" t="inlineStr">
+        <is>
+          <t>Ela ligaria para mim quando chegar.</t>
+        </is>
+      </c>
+      <c r="M125" t="inlineStr">
+        <is>
+          <t>Embora eu precisava ser visto, sou ignorado.</t>
+        </is>
+      </c>
+      <c r="N125" t="inlineStr">
+        <is>
+          <t>Se você dormir cedo, ficaria satisfeito.</t>
+        </is>
+      </c>
+      <c r="O125" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P125" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q125" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>126</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>A frase em que o verbo apresenta a mesma predicação que o verbo ocorrer em “Isso ocorre porque um algoritmo pode executar essas tarefas” (parágrafo 5) é:</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>Funções Sintáticas</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J126" t="inlineStr">
+        <is>
+          <t>“Entra em cena então um novo quociente”. (parágrafo 3)</t>
+        </is>
+      </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>“Esse quociente envolve também características como flexibilidade, curiosidade, coragem e resiliência.” (parágrafo 4)</t>
+        </is>
+      </c>
+      <c r="L126" t="inlineStr">
+        <is>
+          <t>“A tecnologia mudou bastante a forma como alguns trabalhos são feitos”. (parágrafo 5)</t>
+        </is>
+      </c>
+      <c r="M126" t="inlineStr">
+        <is>
+          <t>“você é um contador.” (parágrafo 7)</t>
+        </is>
+      </c>
+      <c r="N126" t="inlineStr">
+        <is>
+          <t>“Seu QI o ajuda nas provas”. (parágrafo 7)</t>
+        </is>
+      </c>
+      <c r="O126" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P126" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q126" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>127</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>UFRJ</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Em “Como adorasse a mulher, não se vexava de mo dizer muitas vezes” (L. 2-3), o conector como estabelece, com a oração seguinte, uma relação semântica de</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>Funções Sintáticas</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J127" t="inlineStr">
+        <is>
+          <t>causa</t>
+        </is>
+      </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>condição</t>
+        </is>
+      </c>
+      <c r="L127" t="inlineStr">
+        <is>
+          <t>contraste</t>
+        </is>
+      </c>
+      <c r="M127" t="inlineStr">
+        <is>
+          <t>comparação</t>
+        </is>
+      </c>
+      <c r="N127" t="inlineStr">
+        <is>
+          <t>consequência</t>
+        </is>
+      </c>
+      <c r="O127" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P127" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q127" t="n">
+        <v>0</v>
+      </c>
+      <c r="R127" t="inlineStr">
+        <is>
+          <t>3f318563-40ba-46fa-af95-0bc5f6427870.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>128</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Ao contrário do período composto por coordenação, o período composto por subordinação apresenta ao menos uma oração sintaticamente dependente de outra.
+O seguinte período configura-se como composto por subordinação:</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>Funções Sintáticas</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J128" t="inlineStr">
+        <is>
+          <t>“Como o aquecimento global está atrapalhando a aviação”</t>
+        </is>
+      </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>“No mês passado, dezenas de voos foram cancelados nos EUA por causa do calor.”</t>
+        </is>
+      </c>
+      <c r="L128" t="inlineStr">
+        <is>
+          <t>“Por lá, as temperaturas altas não impactam só as contas de luz.”</t>
+        </is>
+      </c>
+      <c r="M128" t="inlineStr">
+        <is>
+          <t>“A sustentação que as asas do avião garantem depende da densidade do ar.”</t>
+        </is>
+      </c>
+      <c r="N128" t="inlineStr">
+        <is>
+          <t>“Os efeitos dessa restrição de peso podem pesar no bolso das companhias aéreas e mudar operações pelo mundo todo.”</t>
+        </is>
+      </c>
+      <c r="O128" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P128" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q128" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>129</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>UNIRIO</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;O suor e a lágrima&lt;/b&gt;
+Fazia calor no Rio, 40 graus e qualquer coisa, quase 41. No dia seguinte, os jornais diriam que fora o mais quente deste verão que inaugura o século e o milênio. Cheguei ao Santos Dumont, o vôo estava atrasado, decidi engraxar os sapatos. Pelo menos aqui no Rio, são raros esses engraxates, só existem nos aeroportos e em poucos lugares avulsos. (...) A predominância de orações e períodos coordenados no primeiro parágrafo do texto</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>Funções Sintáticas</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J129" t="inlineStr">
+        <is>
+          <t>torna a contextualização da narrativa mais dinâmica.</t>
+        </is>
+      </c>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>contribui para a dispersão das imagens apresentadas.</t>
+        </is>
+      </c>
+      <c r="L129" t="inlineStr">
+        <is>
+          <t>insere um tom de mistério aos acontecimentos relatados.</t>
+        </is>
+      </c>
+      <c r="M129" t="inlineStr">
+        <is>
+          <t>foca a atenção do leitor apenas ao calor que fazia no Rio.</t>
+        </is>
+      </c>
+      <c r="N129" t="inlineStr">
+        <is>
+          <t>gera um encadeamento entre cenas que se excluem.</t>
+        </is>
+      </c>
+      <c r="O129" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P129" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q129" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>130</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Petrobrás</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>No trecho “as transformações em direção &lt;u&gt;à sociedade da informação&lt;/u&gt;, em estágio avançado nos países industrializados”, a expressão em destaque tem a função de completar o sentido da palavra &lt;u&gt;direção&lt;/u&gt;, sendo, portanto, essencial à construção da frase.
+A mesma função pode ser observada na expressão destacada em:</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>Funções Sintáticas</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J130" t="inlineStr">
+        <is>
+          <t>“alcançando, de forma conceitualmente imprecisa, o universo vocabular&lt;u&gt; do cidadão&lt;/u&gt;.”</t>
+        </is>
+      </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>“decidir que composição do conjunto de tecnologias educacionais mobilizar para atingir suas metas &lt;u&gt;de desenvolvimento&lt;/u&gt;.”</t>
+        </is>
+      </c>
+      <c r="L130" t="inlineStr">
+        <is>
+          <t>“A Unesco tem atuado de forma sistemática no sentido de apoiar as iniciativas &lt;u&gt;dos Estados Membros&lt;/u&gt;”</t>
+        </is>
+      </c>
+      <c r="M130" t="inlineStr">
+        <is>
+          <t>“as ações &lt;u&gt;desse organismo internacional&lt;/u&gt; estão concentradas em duas áreas principais:”</t>
+        </is>
+      </c>
+      <c r="N130" t="inlineStr">
+        <is>
+          <t>“métodos e estratégias para a construção &lt;u&gt;de uma sociedade&lt;/u&gt; de informação global e justa.”</t>
+        </is>
+      </c>
+      <c r="O130" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P130" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q130" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>131</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>IBGE</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Há omissão do agente da ação verbal pelo recurso à voz passiva em:</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>Funções Sintáticas</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>“o comércio ambulante é visto como política compensatória, reservada a alguns grupos”</t>
+        </is>
+      </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>“Há políticas que reconhecem a informalidade como exceção permanente do capitalismo”</t>
+        </is>
+      </c>
+      <c r="L131" t="inlineStr">
+        <is>
+          <t>“Nessa concepção, ‘gerenciar’ a informalidade significa tolerá-la”</t>
+        </is>
+      </c>
+      <c r="M131" t="inlineStr">
+        <is>
+          <t>“‘domesticar’ a informalidade significa destinar ao comércio ambulante apenas alguns espaços na cidade”</t>
+        </is>
+      </c>
+      <c r="N131" t="inlineStr">
+        <is>
+          <t>“quando, na verdade, são instrumentos de exclusão dos trabalhadores das ruas”</t>
+        </is>
+      </c>
+      <c r="O131" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P131" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q131" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>132</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Nível Superior</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Dialética da mudança &lt;/b&gt;
+Certamente porque não é fácil compreender certas questões, as pessoas tendem a aceitar algumas afirmações como verdades indiscutíveis e até mesmo a irritar-se quando alguém insiste em discuti-las. É natural que isso aconteça, quando mais não seja porque as certezas nos dão segurança e tranquilidade. Pô-las em questão equivale a tirar o chão de sob nossos pés. Não necessito dizer que, para mim, não há verdades indiscutíveis, embora acredite em determinados valores e princípios que me parecem consistentes. De fato, é muito difícil, senão impossível, viver sem nenhuma certeza, sem valor algum.
+No passado distante, quando os valores religiosos se impunham à quase totalidade das pessoas, poucos eram os que questionavam, mesmo porque, dependendo da ocasião, pagavam com a vida seu inconformismo.
+Com o desenvolvimento do pensamento objetivo e da ciência, aquelas certezas inquestionáveis passaram a segundo plano, dando lugar a um novo modo de lidar com as certezas e os valores.
+Questioná-los, reavaliá-los, negá-los, propor mudanças às vezes radicais tornou-se frequente e inevitável, dando-se início a uma nova época da sociedade humana. Introduziram-se as ideias não só de evolução como de revolução.
+Naturalmente, essas mudanças não se deram do dia para a noite, nem tampouco se impuseram à maioria da sociedade. O que ocorreu de fato foi um processo difícil e conflituado em que, pouco a pouco, a visão inovadora veio ganhando terreno e, mais do que isso, conquistando posições estratégicas, o que tornou possível influir na formação de novas gerações, menos resistentes a visões questionadoras.
+A certa altura desse processo, os defensores das mudanças acreditavam-se senhores de novas verdades, mais consistentes porque eram fundadas no conhecimento objetivo das leis que governam o mundo material e social. Mas esse conhecimento era ainda precário e limitado.
+Inúmeras descobertas reafirmam a tese de que a mudança é inerente à realidade tanto material quanto espiritual, e que, portanto, o conceito de imutabilidade é destituído de fundamento.
+Ocorre, porém, que essa certeza pode induzir a outros erros: o de achar que quem defende determinados valores estabelecidos está indiscutivelmente errado. Em outras palavras, bastaria apresentar-se como inovador para estar certo. Será isso verdade? Os fatos demonstram que tanto pode ser como não.
+Mas também pode estar errado quem defende os valores consagrados e aceitos. Só que, em muitos casos, não há alternativa senão defendê-los. E sabem por quê? Pela simples razão de que toda sociedade é, por definição, conservadora, uma vez que, sem princípios e valores estabelecidos, seria impossível o convívio social. Uma comunidade cujos princípios e normas mudassem a cada dia seria caótica e, por isso mesmo, inviável.
+Por outro lado, como a vida muda e a mudança é inerente à existência, impedir a mudança é impossível. Daí resulta que a sociedade termina por aceitar as mudanças, mas apenas aquelas que de algum modo atendem a suas necessidades e a fazem avançar.
+GULLAR,Ferreira.Dialéticadamudança.FolhadeSãoPaulo,6maio2012,p.E10.
+Na frase “Não necessito dizer que, para mim, não há verdades indiscutíveis, embora acredite em determinados valores e princípios que me parecem consistentes.” (L. 6-7) podem ser identificados diferentes tipos de orações subordinadas (substantivas, adjetivas e adverbiais), que nela exercem distintas funções.
+Uma oração com função de expressar uma noção adjetiva é também encontrada em:</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>Funções Sintáticas</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t>“Certamente porque não é fácil compreender certas questões, as pessoas tendem a aceitar algumas afirmações” (L. 1-2)</t>
+        </is>
+      </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>“É natural que isso aconteça, quando mais não seja porque as certezas nos dão segurança e tranquilidade.” (L. 3-5)</t>
+        </is>
+      </c>
+      <c r="L132" t="inlineStr">
+        <is>
+          <t>“No passado distante, quando os valores religiosos se impunham à quase totalidade das pessoas,” (L. 10-11)</t>
+        </is>
+      </c>
+      <c r="M132" t="inlineStr">
+        <is>
+          <t>“Os fatos demonstram que tanto pode ser como não.” (L. 35)</t>
+        </is>
+      </c>
+      <c r="N132" t="inlineStr">
+        <is>
+          <t>“Uma comunidade cujos princípios e normas mudassem a cada dia seria caótica e, por isso mesmo, inviável.” (L. 40-41)</t>
+        </is>
+      </c>
+      <c r="O132" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P132" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q132" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>133</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Banco do Brasil</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>Um exemplo famoso disso foi o então auxiliar técnico do Brasil, Zagallo, que foi para a Copa do Mundo de (19)94 (a soma dá 13) dizendo que o Mundial ia terminar com o Brasil campeão devido a uma série de coincidências envolvendo o número.
+A oração “envolvendo o número” pode ser substituída, sem prejuízo do sentido original, pela seguinte oração:</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>Funções Sintáticas</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J133" t="inlineStr">
+        <is>
+          <t>por envolver o número.</t>
+        </is>
+      </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>que envolviam o número.</t>
+        </is>
+      </c>
+      <c r="L133" t="inlineStr">
+        <is>
+          <t>se envolvessem o número.</t>
+        </is>
+      </c>
+      <c r="M133" t="inlineStr">
+        <is>
+          <t>já que envolvem o número.</t>
+        </is>
+      </c>
+      <c r="N133" t="inlineStr">
+        <is>
+          <t>quando envolveram o número.</t>
+        </is>
+      </c>
+      <c r="O133" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P133" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q133" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>134</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>O marciano encontrou-me na rua e teve medo de minha impossibilidade humana. Como pode existir, pensou consigo, um ser que no existir põe tamanha anulação de existência? Afastou-se o marciano, e persegui-o. Precisava dele como de um testemunho. Mas, recusando o colóquio, desintegrou-se no ar constelado de problemas.
+E fiquei só em mim, de mim ausente.
+ANDRADE,CarlosDrummondde.Sciencefiction.Poesiaeprosa.RiodeJaneiro:NovaAguilar,1988,p.330-331.
+De acordo com a norma-padrão, há indeterminação do sujeito em:</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>Funções Sintáticas</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J134" t="inlineStr">
+        <is>
+          <t>Olharam-se com cumplicidade.</t>
+        </is>
+      </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>Barbearam-se todos antes da festa.</t>
+        </is>
+      </c>
+      <c r="L134" t="inlineStr">
+        <is>
+          <t>Trata-se de resolver questões econômicas.</t>
+        </is>
+      </c>
+      <c r="M134" t="inlineStr">
+        <is>
+          <t>Vendem-se artigos de qualidade naquela loja.</t>
+        </is>
+      </c>
+      <c r="N134" t="inlineStr">
+        <is>
+          <t>Compra-se muita mercadoria em época de festas.</t>
+        </is>
+      </c>
+      <c r="O134" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P134" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q134" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>135</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>BNDES</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Vista cansada&lt;/b&gt;
+Acho que foi o Hemingway quem disse que olhava cada coisa à sua volta como se a visse pela última vez. Pela última ou pela primeira vez? Pela primeira vez foi outro escritor quem disse. Essa ideia de olhar pela última vez tem algo de deprimente. Olhar de despedida, de quem não crê que a vida continua, não admira que o Hemingway tenha acabado como acabou.
+Se eu morrer, morre comigo um certo modo de ver, disse o poeta. Um poeta é só isto: um certo modo de ver. O diabo é que, de tanto ver, a gente banaliza o olhar. Vê não vendo. Experimente ver pela primeira vez o que você vê todo dia, sem ver. Parece fácil, mas não é. O que nos cerca, o que nos é familiar, já não desperta curiosidade. O campo visual da nossa rotina é como um vazio.
+Você sai todo dia, por exemplo, pela mesma porta. Se alguém lhe perguntar o que é que você vê no seu caminho, você não sabe. De tanto ver, você não vê. Sei de um profissional que passou 32 anos a fio pelo mesmo hall do prédio do seu escritório. Lá estava sempre, pontualíssimo, o mesmo porteiro. Dava-lhe bom-dia e às vezes lhe passava um recado ou uma correspondência.
+Um dia o porteiro cometeu a descortesia de falecer.
+Como era ele? Sua cara? Sua voz? Como se vestia? Não fazia a mínima ideia. Em 32 anos, nunca o viu. Para ser notado, o porteiro teve que morrer. Se um dia no seu lugar estivesse uma girafa, cumprindo o rito, pode ser também que ninguém desse por sua ausência. O hábito suja os olhos e lhes baixa a voltagem. Mas há sempre o que ver. Gente, coisas, bichos. E vemos? Não, não vemos.
+Uma criança vê o que o adulto não vê. Tem olhos atentos e limpos para o espetáculo do mundo.
+O poeta é capaz de ver pela primeira vez o que, de fato, ninguém vê. Há pai que nunca viu o próprio filho. Marido que nunca viu a própria mulher, isso existe às pampas. Nossos olhos se gastam no dia a dia, opacos. É por aí que se instala no coração o monstro da indiferença.
+A oração cuja classificação está INCORRETA é:</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>Funções Sintáticas</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J135" t="inlineStr">
+        <is>
+          <t>“Se eu morrer,” (L. 6) – oração subordinada adverbial condicional</t>
+        </is>
+      </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>“mas não é.” (L. 09) – oração coordenada sindética adversativa</t>
+        </is>
+      </c>
+      <c r="L135" t="inlineStr">
+        <is>
+          <t>“O campo visual da nossa rotina é como um vazio.” (L. 10-11) – oração principal</t>
+        </is>
+      </c>
+      <c r="M135" t="inlineStr">
+        <is>
+          <t>“Você sai todo dia, por exemplo, pela mesma porta.” (L. 12) – oração absoluta</t>
+        </is>
+      </c>
+      <c r="N135" t="inlineStr">
+        <is>
+          <t>“O hábito suja os olhos...” (L. 21) – oração coordenada assindética</t>
+        </is>
+      </c>
+      <c r="O135" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P135" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q135" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>136</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Banco do Brasil</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Empreendedorismo social: um caminho para quem quer mudar o mundo&lt;/b&gt;
+Ainda que não exista uma concepção única sobre o empreendedorismo social, de forma geral, o conceito está relacionado ao ato de empreender ou inovar com o objetivo de alavancar causas sociais e ambientais. A meta é transformar uma realidade, promover o bem-estar da sociedade e agregar valor com cunho social.
+Um empreendedor social produz bens e serviços que irão impactar positivamente a comunidade em que ele está inserido e solucionar algum problema ou necessidade daquele grupo. Apesar de poder ter retorno financeiro, os empreendimentos sociais analisam seu desempenho a partir do impacto social gerado por sua atuação.
+Vale ressaltar que, apesar de apresentarem muitas similaridades, empreendedorismo social e negócio social não são sinônimos. O empreendedorismo social cria valor por meio da inovação, que gera uma transformação social. O foco não é o retorno financeiro, mas a resolução de problemas sociais e o impacto positivo. Enquanto isso, os negócios sociais seguem a lógica tradicional do mercado, porém com a ambição de gerar valor social.
+Cinco características também são essenciais para a iniciativa: ser inovadora; realizável; autossustentável; contar com a participação de diversos segmentos da sociedade, incluindo as pessoas impactadas; e promover impacto social com resultados mensuráveis.
+Quem tem interesse de atuar nessa área precisa trabalhar em grupo e formar parcerias, saber lidar bem com as pessoas e buscar formas de trazer resultados de impacto social.
+Além disso, o profissional precisa ter flexibilidade e vontade de explorar, pois é possível que ele acabe exercendo um papel que não seja necessariamente na sua área de formação, ou que sua atuação se transforme rapidamente, por conta do dinamismo e das necessidades do negócio.
+(MENDES,T.Empreendedorismosocial:umcaminhoparaquemquermudaromundo.Naprática,7jul.2022.
+Disponívelem:https://www.napratica.org.br/empreendedorismo-social/.Acessoem:2set.2022.Adaptado).
+No trecho “&lt;u&gt;Ainda que&lt;/u&gt; não exista uma concepção única sobre o empreendedorismo social”, a expressão destacada pode ser substituída, sem prejuízo do sentido do texto, por</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>Orações Adverbiais</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>Fácil</t>
+        </is>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J136" t="inlineStr">
+        <is>
+          <t>À medida que</t>
+        </is>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>Contanto que</t>
+        </is>
+      </c>
+      <c r="L136" t="inlineStr">
+        <is>
+          <t>De modo que</t>
+        </is>
+      </c>
+      <c r="M136" t="inlineStr">
+        <is>
+          <t>Mesmo que</t>
+        </is>
+      </c>
+      <c r="N136" t="inlineStr">
+        <is>
+          <t>Por causa de</t>
+        </is>
+      </c>
+      <c r="O136" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P136" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q136" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>137</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;A história do método braile&lt;/b&gt;
+Ler no escuro. Quem já tentou sabe que é impossível. Mas foi exatamente a isso que um francês chamado Louis Braille dedicou a vida. Nascido em Coupvray, uma pequena aldeia nos arredores de Paris, em 1809, desde cedo ele mostrou muito interesse pelo trabalho do pai. Seus olhos azuis brilhavam da admiração de vê-lo cortar, com extrema perícia, selas e arreios. Pouco depois de completar 3 anos, o menino começou a brincar na selaria do pai, cortando pequenas tiras de couro. Uma tarde, uma sovela, instrumento usado para perfurar o couro, escapou-lhe da mão e atingiu o seu olho esquerdo. O resultado foi uma infecção que, seis meses depois, afetaria também o olho direito. Aos 5 anos, o garoto estava completamente cego.
+A tragédia não o impediu, porém, de frequentar a escola por dois anos e de se tornar ainda um aluno brilhante. Por essa razão, ele ganhou uma bolsa de estudos no Instituto Nacional para Jovens Cegos, em Paris, um colégio interno fundado por Valentin Haüy (1745-182. Além do currículo normal, Haüy introduzira um sistema especial de alfabetização, no qual letras de forma impressas em relevo, em papelão, eram reconhecidas pelos contornos. Desde o início do curso, Braille destacou-se como o melhor aluno da turma e logo começou a ajudar os colegas. Em 1821, aos 12 anos, conheceu um método inventado pouco antes por Charles Barbier de La Serre, oficial do Exército francês.
+O método Barbier, também chamado escrita noturna, era um código de pontos e traços em relevo impressos também em papelão. Destinava-se a enviar ordens cifradas a sentinelas em postos avançados. Estes decodificariam a mensagem até no escuro. Mas, como a ideia não pegou na tropa, Barbier adaptou o método para a leitura de cegos, com o nome de grafia sonora. O sistema permitia a comunicação entre os cegos, pois com ele era possível escrever, algo que o método de Haüy não possibilitava. O de Barbier era fonético: registrava sons e não letras. Dessa forma, as palavras não podiam ser soletradas. Além disso, o fato de um grande número de sinais ser usado para uma única palavra tornava o sistema muito complicado. Apesar dos inconvenientes, foi adotado como método auxiliar por Haüy.
+Pesquisando a fundo a grafia sonora, Braille percebeu suas limitações e pôs-se a aperfeiçoá-la.
+Em 1824, seu método estava pronto. Primeiro, eliminou os traços, para evitar erros de leitura: em seguida, criou uma célula de seis pontos, divididos em duas colunas de três pontos cada, que podem ser combinados de 63 maneiras diferentes. A posição dos pontos na célula está ao lado.
+Em 1826, aos 17 anos, ainda estudante, Braille começou a dar aulas. Embora seu método fizesse sucesso entre os alunos, não podia ensiná-lo na sala de aula, pois ainda não era reconhecido oficialmente. Por isso, Braille dava aulas do revolucionário sistema escondido no quarto, que logo se transformou numa segunda sala de aula.
+O braile é lido passando-se a ponta dos dedos sobre os sinais de relevo. Normalmente se usa a mão direita com um ou mais dedos, conforme a habilidade do leitor, enquanto a mão esquerda procura o início da outra linha. Aplica-se a qualquer língua, sem exceção, e também à estenografia, à música – Braille, por sinal, era ainda exímio pianista – e às notações científicas em geral. A escrita é feita mediante o uso da reglete, também idealizada por Braille: trata-se de uma régua especial, de duas linhas, com uma série de janelas de seis furos cada, correspondentes às células braile.
+Louis Braille morreu de tuberculose em 1852, com apenas 43 anos. Temia que seu método desaparecesse com ele, mas, finalmente, em 1854 foi oficializado pelo governo francês. No ano seguinte, foi apresentado ao mundo, na Exposição Internacional de Paris, por ordem do imperador Napoleão III (1808-187, que programou ainda uma série de concertos de piano com ex-alunos de Braille. O sucesso foi imediato, e o sistema se espalhou pelo mundo. Em 1952, o governo francês transferiu os restos mortais de Braille para o Panthéon, em Paris, onde estão sepultados os heróis nacionais.
+(ATANES,Silvio.SuperInteressante.Disponívelem:https://super.abril.]com.br/historia/.Acessoem:23out.2022.
+Adaptado.) Em “Mas, &lt;u&gt;como a ideia não pegou na tropa&lt;/u&gt;, Barbier adaptou o método para a leitura de cegos”, a oração destacada apresenta o valor semântico de</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>Orações Adverbiais</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J137" t="inlineStr">
+        <is>
+          <t>fim</t>
+        </is>
+      </c>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>causa</t>
+        </is>
+      </c>
+      <c r="L137" t="inlineStr">
+        <is>
+          <t>tempo</t>
+        </is>
+      </c>
+      <c r="M137" t="inlineStr">
+        <is>
+          <t>proporção</t>
+        </is>
+      </c>
+      <c r="N137" t="inlineStr">
+        <is>
+          <t>consequência</t>
+        </is>
+      </c>
+      <c r="O137" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P137" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q137" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>138</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>AgeRIO</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Floresta amazônica vai virar savana&lt;/b&gt;
+&lt;i&gt;Pesquisadores afirmam que mudança no ecossistema da Amazônia é iminente&lt;/i&gt;
+Se a Amazônia perder mais de 20% de sua área para o desmatamento, ela pode se descaracterizar de tal forma que deixaria de ser uma floresta e se transformaria em área de savana, alertam dois conceituados pesquisadores da área, em um artigo publicado recentemente.
+Hoje, o desmatamento acumulado está em 17%.
+Os cientistas acreditam que as sinergias negativas entre desmatamento, mudanças climáticas e uso indiscriminado de incêndios florestais indicam um tipping point (ponto crítico), um ponto sem volta, para transformar as partes Sul, Leste e central da Amazônia em um ecossistema não florestal se o desmatamento chegar a entre 20% e 25%.
+Os pesquisadores partiram do conceito da “savanização” da Amazônia, que surgiu após a descoberta de que as florestas interferem no regime de chuvas. Na Amazônia, por exemplo, estima-se que metade das chuvas na região é resultado da umidade produzida pela evapotranspiração (a transpiração das árvores), que “recicla” as correntes de ar úmido provenientes do Oceano Atlântico.
+Caso perca uma quantidade grande de árvores, a floresta recicla menos chuva, ficando mais suscetível a incêndios. O fogo altera a vegetação, favorecendo o avanço de gramíneas onde antes havia espécies florestais. O resultado desse processo ecológico é que grandes fragmentos de florestas se transformam em savanas ou cerrados, descaracterizando a Amazônia como a conhecemos hoje.
+A primeira estimativa de qual seria o tipping point para a Amazônia virar savana foi feita em um estudo em 2007, e chegou à conclusão de que esse valor era de 40% de florestas derrubadas. Só que esse estudo avaliou apenas uma variável, o desmatamento. Segundo um dos autores, quando se consideram outros fatores, como os incêndios florestais e o aquecimento global, essa margem diminui consideravelmente. Os focos de incêndio têm aumentado. O aquecimento global já está acontecendo, com um aumento de 1 grau Celsius na temperatura média da Amazônia.
+De acordo com uma especialista em ciência e Amazônia, a hipótese de savanização precisa ser encarada com seriedade, porque a floresta amazônica tem resiliência, ela consegue resistir a algum desmatamento. Mas essa possibilidade não é infinita, chega a um ponto que não tem retorno. Além disso, é preciso considerar a população da região, investindo na produção com sustentabilidade.
+Uma das propostas para que se possa evitar o tipping point é o reflorestamento. Com esse objetivo, o Brasil se comprometeu, na Conferência da ONU sobre Clima em Paris, em 2015, a reflorestar 12 milhões de hectares até 2030.
+(CALIXTO,B.OGlobo.Sociedade.RiodeJaneiro,22fev.2018.Adaptado.) O trecho do texto em que se estabelece uma relação lógica de condição entre as ideias, marcada pela presença da palavra ou expressão destacada, é:</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>Orações Adverbiais</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>“Caso perca uma quantidade grande de árvores, a floresta recicla menos chuva, ficando mais suscetível a incêndios.” (parágrafo 4)</t>
+        </is>
+      </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>“quando se consideram outros fatores, como os incêndios florestais e o aquecimento global, essa margem diminui consideravelmente.” (parágrafo 5)</t>
+        </is>
+      </c>
+      <c r="L138" t="inlineStr">
+        <is>
+          <t>“a hipótese de savanização precisa ser encarada com seriedade, porque a floresta amazônica tem resiliência, ela consegue resistir a algum desmatamento.” (parágrafo 6)</t>
+        </is>
+      </c>
+      <c r="M138" t="inlineStr">
+        <is>
+          <t>“Mas essa possibilidade não é infinita, chega a um ponto que não tem retorno.” (parágrafo 6)</t>
+        </is>
+      </c>
+      <c r="N138" t="inlineStr">
+        <is>
+          <t>“Uma das propostas para que se possa evitar o tipping point é o reflorestamento.” (parágrafo 7)</t>
+        </is>
+      </c>
+      <c r="O138" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P138" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q138" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>139</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>ELETRONUCLEAR</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Entulho eletrônico: risco iminente para a saúde e o ambiente&lt;/b&gt;
+Os resíduos de equipamentos eletroeletrônicos (lixo eletroeletrônico) são, por definição, produtos que têm componentes elétricos e eletrônicos e que, por razões de obsolescência (perspectiva ou programadA) e impossibilidade de conserto, são descartados pelos consumidores. Os exemplos mais comuns são televisores e equipamentos de informática e telefonia, mas a lista inclui eletrodomésticos, equipamentos médicos, brinquedos, sistemas de alarme, automação e controle.
+Obsolescência programada é a decisão intencional de fabricar um produto que se torne obsoleto ou não funcional após certo tempo, para forçar o consumidor a comprar uma nova geração desse produto. Já a obsolescência perspectiva é uma forma de reduzir a vida útil de produtos ainda funcionais. Nesse caso, são lançadas novas gerações com aparência inovadora e pequenas mudanças funcionais, dando à geração em uso aspecto de ultrapassada, o que induz o consumidor à troca.
+O lixo eletroeletrônico é mais um desafio que se soma aos problemas ambientais da atualidade.
+O consumidor raramente reflete sobre as consequências do consumo crescente desses produtos, preocupando- se em satisfazer suas necessidades. Afinal, eletroeletrônicos são tidos como sinônimos de melhor qualidade de vida, e a explosão da indústria da informação é uma força motriz da sociedade, oferecendo ferramentas para rápidos avanços na economia e no desenvolvimento social. O mundo globalizado impõe uma constante busca de informações em tempo real, e a sua interação com novas tecnologias traz maiores oportunidades e benefícios, segundo estudo da Organização das Nações Unidas (ONU). Tudo isso exerce um fascínio irresistível para os jovens.
+Dois aspectos justificam a inclusão dos eletroeletrônicos entre as preocupações da ONU: as vendas crescentes, em especial nos mercados emergentes (inclusive o Brasil), e a presença de metais e substâncias tóxicas em muitos componentes, trazendo risco à saúde e ao meio ambiente. Segundo a ONU, são gerados hoje 150 milhões de toneladas de lixo eletroeletrônico por ano, e esse tipo de resíduo cresce a uma velocidade três a cinco vezes maior que a do lixo urbano.
+(AFONSO,J.C.RevistaCiênciaHoje,n.314,maio2014.SãoPaulo:SBPC.Disponívelem: https://cienciahoje.periodicos.capes.gov.br/storage/acervo/ch/ch_314.pdf.Adaptado).
+No trecho do 3o parágrafo “segundo estudo da Organização das Nações Unidas”, a palavra destacada expressa ideia de</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>Orações Adverbiais</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J139" t="inlineStr">
+        <is>
+          <t>condição</t>
+        </is>
+      </c>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>concessão</t>
+        </is>
+      </c>
+      <c r="L139" t="inlineStr">
+        <is>
+          <t>conformidade</t>
+        </is>
+      </c>
+      <c r="M139" t="inlineStr">
+        <is>
+          <t>causalidade</t>
+        </is>
+      </c>
+      <c r="N139" t="inlineStr">
+        <is>
+          <t>temporalidade</t>
+        </is>
+      </c>
+      <c r="O139" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P139" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q139" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>140</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>ELETROBRÁS</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Entulho eletrônico: risco iminente para a saúde e o ambiente&lt;/b&gt;
+Os resíduos de equipamentos eletroeletrônicos (lixo eletroeletrônico) são, por definição, produtos que têm componentes elétricos e eletrônicos e que, por razões de obsolescência (perspectiva ou programadA) e impossibilidade de conserto, são descartados pelos consumidores. Os exemplos mais comuns são televisores e equipamentos de informática e telefonia, mas a lista inclui eletrodomésticos, equipamentos médicos, brinquedos, sistemas de alarme, automação e controle.
+Obsolescência programada é a decisão intencional de fabricar um produto que se torne obsoleto ou não funcional após certo tempo, para forçar o consumidor a comprar uma nova geração desse produto. Já a obsolescência perspectiva é uma forma de reduzir a vida útil de produtos ainda funcionais. Nesse caso, são lançadas novas gerações com aparência inovadora e pequenas mudanças funcionais, dando à geração em uso aspecto de ultrapassada, o que induz o consumidor à troca.
+O lixo eletroeletrônico é mais um desafio que se soma aos problemas ambientais da atualidade.
+O consumidor raramente reflete sobre as consequências do consumo crescente desses produtos, preocupando- se em satisfazer suas necessidades. Afinal, eletroeletrônicos são tidos como sinônimos de melhor qualidade de vida, e a explosão da indústria da informação é uma força motriz da sociedade, oferecendo ferramentas para rápidos avanços na economia e no desenvolvimento social. O mundo globalizado impõe uma constante busca de informações em tempo real, e a sua interação com novas tecnologias traz maiores oportunidades e benefícios, segundo estudo da Organização das Nações Unidas (ONU). Tudo isso exerce um fascínio irresistível para os jovens.
+Dois aspectos justificam a inclusão dos eletroeletrônicos entre as preocupações da ONU: as vendas crescentes, em especial nos mercados emergentes (inclusive o Brasil), e a presença de metais e substâncias tóxicas em muitos componentes, trazendo risco à saúde e ao meio ambiente. Segundo a ONU, são gerados hoje 150 milhões de toneladas de lixo eletroeletrônico por ano, e esse tipo de resíduo cresce a uma velocidade três a cinco vezes maior que a do lixo urbano.
+(AFONSO,J.C.RevistaCiênciaHoje,n.314,maio2014.SãoPaulo:SBPC.Disponívelem: https://cienciahoje.periodicos.capes.gov.br/storage/acervo/ch/ch_314.pdf.Adaptado).
+No trecho do 2° parágrafo “fabricar um produto que se torne obsoleto ou não funcional após certo tempo, &lt;u&gt;para &lt;/u&gt;forçar o consumidor a comprar uma nova geração desse produto”, a palavra destacada pode ser substituída, mantendo-se a mesma circunstância, pela expressão</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>Orações Adverbiais</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J140" t="inlineStr">
+        <is>
+          <t>de modo a</t>
+        </is>
+      </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>por causa de</t>
+        </is>
+      </c>
+      <c r="L140" t="inlineStr">
+        <is>
+          <t>na condição de</t>
+        </is>
+      </c>
+      <c r="M140" t="inlineStr">
+        <is>
+          <t>apesar de</t>
+        </is>
+      </c>
+      <c r="N140" t="inlineStr">
+        <is>
+          <t>em vez de</t>
+        </is>
+      </c>
+      <c r="O140" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P140" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q140" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>141</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>No trecho “Às organizações, cabe o desafio de orientar seus clientes,&lt;u&gt; já que&lt;/u&gt;, na maioria das vezes, eles não sabem quais são os limites da privacidade digital” (parágrafo 8), a expressão destacada expressa a noção de</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>Orações Adverbiais</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J141" t="inlineStr">
+        <is>
+          <t>condição</t>
+        </is>
+      </c>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>finalidade</t>
+        </is>
+      </c>
+      <c r="L141" t="inlineStr">
+        <is>
+          <t>concessão</t>
+        </is>
+      </c>
+      <c r="M141" t="inlineStr">
+        <is>
+          <t>causalidade</t>
+        </is>
+      </c>
+      <c r="N141" t="inlineStr">
+        <is>
+          <t>comparação</t>
+        </is>
+      </c>
+      <c r="O141" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P141" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q141" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>142</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>CAIXA ECONÔMICA</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>O paralelismo sintático é uma das convenções estabelecidas para a escrita oficial. A frase cuja organização sintática está plenamente de acordo com essa convenção é:</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>Paralelismo</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J142" t="inlineStr">
+        <is>
+          <t>É muito salutar que as pessoas se programem em relação à saúde e financeiramente.</t>
+        </is>
+      </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>O mundo financeiro, hoje, facilita o acesso ao crédito e leva ao endividamento progressivo.</t>
+        </is>
+      </c>
+      <c r="L142" t="inlineStr">
+        <is>
+          <t>Nossa vida financeira é saudável quando possibilita equilíbrio, segurança e que realizemos nossos sonhos.</t>
+        </is>
+      </c>
+      <c r="M142" t="inlineStr">
+        <is>
+          <t>A educação financeira orienta-nos na revisão de gastos excessivos e que comprometem nosso orçamento.</t>
+        </is>
+      </c>
+      <c r="N142" t="inlineStr">
+        <is>
+          <t>Os especialistas aconselham as escolas a promoverem momentos de discussão sobre educação financeira com os pais dos alunos e que ofereçam aulas sobre o tema para os alunos.</t>
+        </is>
+      </c>
+      <c r="O142" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P142" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q142" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>143</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>AgeRIO</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Floresta amazônica vai virar savana&lt;/b&gt;
+&lt;i&gt;Pesquisadores afirmam que mudança no ecossistema da Amazônia é iminente&lt;/i&gt;
+Se a Amazônia perder mais de 20% de sua área para o desmatamento, ela pode se descaracterizar de tal forma que deixaria de ser uma floresta e se transformaria em área de savana, alertam dois conceituados pesquisadores da área, em um artigo publicado recentemente.
+Hoje, o desmatamento acumulado está em 17%.
+Os cientistas acreditam que as sinergias negativas entre desmatamento, mudanças climáticas e uso indiscriminado de incêndios florestais indicam um tipping point (ponto crítico), um ponto sem volta, para transformar as partes Sul, Leste e central da Amazônia em um ecossistema não florestal se o desmatamento chegar a entre 20% e 25%.
+Os pesquisadores partiram do conceito da “savanização” da Amazônia, que surgiu após a descoberta de que as florestas interferem no regime de chuvas. Na Amazônia, por exemplo, estima-se que metade das chuvas na região é resultado da umidade produzida pela evapotranspiração (a transpiração das árvores), que “recicla” as correntes de ar úmido provenientes do Oceano Atlântico.
+Caso perca uma quantidade grande de árvores, a floresta recicla menos chuva, ficando mais suscetível a incêndios. O fogo altera a vegetação, favorecendo o avanço de gramíneas onde antes havia espécies florestais. O resultado desse processo ecológico é que grandes fragmentos de florestas se transformam em savanas ou cerrados, descaracterizando a Amazônia como a conhecemos hoje.
+A primeira estimativa de qual seria o tipping point para a Amazônia virar savana foi feita em um estudo em 2007, e chegou à conclusão de que esse valor era de 40% de florestas derrubadas. Só que esse estudo avaliou apenas uma variável, o desmatamento. Segundo um dos autores, quando se consideram outros fatores, como os incêndios florestais e o aquecimento global, essa margem diminui consideravelmente. Os focos de incêndio têm aumentado. O aquecimento global já está acontecendo, com um aumento de 1 grau Celsius na temperatura média da Amazônia.
+De acordo com uma especialista em ciência e Amazônia, a hipótese de savanização precisa ser encarada com seriedade, porque a floresta amazônica tem resiliência, ela consegue resistir a algum desmatamento. Mas essa possibilidade não é infinita, chega a um ponto que não tem retorno. Além disso, é preciso considerar a população da região, investindo na produção com sustentabilidade.
+Uma das propostas para que se possa evitar o tipping point é o reflorestamento. Com esse objetivo, o Brasil se comprometeu, na Conferência da ONU sobre Clima em Paris, em 2015, a reflorestar 12 milhões de hectares até 2030.
+(CALIXTO,B.OGlobo.Sociedade.RiodeJaneiro,22fev.2018.Adaptado).
+No trecho “ela pode se descaracterizar de tal forma que deixaria de ser uma floresta e se transformaria em área de savana” (parágrafo , os elementos destacados são responsáveis por expressar a ideia de</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>Palavra Que</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J143" t="inlineStr">
+        <is>
+          <t>adição</t>
+        </is>
+      </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>concessão</t>
+        </is>
+      </c>
+      <c r="L143" t="inlineStr">
+        <is>
+          <t>condição</t>
+        </is>
+      </c>
+      <c r="M143" t="inlineStr">
+        <is>
+          <t>consequência</t>
+        </is>
+      </c>
+      <c r="N143" t="inlineStr">
+        <is>
+          <t>temporalidade</t>
+        </is>
+      </c>
+      <c r="O143" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P143" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q143" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>144</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Banco da Amazônia</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>A ideia a que o pronome destacado se refere está adequadamente explicitada entre colchetes em:</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>Palavra Que</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J144" t="inlineStr">
+        <is>
+          <t>“Ela é produzida de forma descentralizada por milhares de computadores, mantidos por pessoas &lt;u&gt;que &lt;/u&gt;´emprestam´ a capacidade de suas máquinas para criar bitcoins” [computadores]</t>
+        </is>
+      </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>“No processo de nascimento de uma bitcoin, &lt;u&gt;que &lt;/u&gt;é chamado de ´mineração´, os computadores conectados à rede competem entre si” [bitcoin]</t>
+        </is>
+      </c>
+      <c r="L144" t="inlineStr">
+        <is>
+          <t>“O nível de dificuldade dos desafios é ajustado pela rede, para que a moeda cresça dentro de uma faixa limitada, &lt;u&gt;que &lt;/u&gt;é de até 21 milhões de unidades” [rede]</t>
+        </is>
+      </c>
+      <c r="M144" t="inlineStr">
+        <is>
+          <t>“Elas são guardadas em uma espécie de carteira, &lt;u&gt;que &lt;/u&gt;é criada quando o usuário se cadastra no software.” [espécie].</t>
+        </is>
+      </c>
+      <c r="N144" t="inlineStr">
+        <is>
+          <t>“Críticos afirmam que a moeda vive uma bolha &lt;u&gt;que &lt;/u&gt;em algum momento deve estourar.” [bolha].</t>
+        </is>
+      </c>
+      <c r="O144" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P144" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q144" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>145</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Téc. de Enfermagem</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>De acordo com a norma-padrão da língua portuguesa, o pronome que faz referência à palavra ou expressão entre colchetes em:</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>Palavra Que</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J145" t="inlineStr">
+        <is>
+          <t>“Energia, derivada de energia, que em grego significa ‘em ação’, é a propriedade de um sistema que lhe permite existir” [propriedade de um sistema]</t>
+        </is>
+      </c>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>“Existem fontes de energia alternativas que, adequadamente utilizadas, podem substituir os combustíveis fósseis” [alternativas]</t>
+        </is>
+      </c>
+      <c r="L145" t="inlineStr">
+        <is>
+          <t>“reservando-os para aquelas situações em que a substituição ainda não é possível” [combustíveis fósseis]</t>
+        </is>
+      </c>
+      <c r="M145" t="inlineStr">
+        <is>
+          <t>“...usinas eólicas não promovem queima de combustível, nem geram dejetos que poluem o ar, o solo ou a água” [usinas eólicas]</t>
+        </is>
+      </c>
+      <c r="N145" t="inlineStr">
+        <is>
+          <t>“o impacto visual causado pelas imensas hélices que provocam certas sombras e reflexos desagradáveis em áreas residenciais” [impacto visual]</t>
+        </is>
+      </c>
+      <c r="O145" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P145" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q145" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>146</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>O pronome se destacado apresenta a mesma função e classificação que exerce em “Automatiza-&lt;u&gt;se &lt;/u&gt;facilmente qualquer função que envolva detectar padrões nos dados [...]” (parágrafo 5) no seguinte período:</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>Palavra Se</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J146" t="inlineStr">
+        <is>
+          <t>Alguns trabalhadores mais velhos arrependem-&lt;u&gt;se &lt;/u&gt;de não procurar entender a nova realidade do mercado de trabalho.</t>
+        </is>
+      </c>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>Acostumar-&lt;u&gt;se &lt;/u&gt;com as novas exigências do mundo do trabalho é condição para sobreviver no mercado hoje.</t>
+        </is>
+      </c>
+      <c r="L146" t="inlineStr">
+        <is>
+          <t>O mercado vem mudando: trata-&lt;u&gt;se &lt;/u&gt;agora de valorizar flexibilidade, curiosidade, coragem e resiliência.</t>
+        </is>
+      </c>
+      <c r="M146" t="inlineStr">
+        <is>
+          <t>Ainda &lt;u&gt;se &lt;/u&gt;hesita diante da escolha entre habilidades medidas pelo QI e aquelas medidas pelo QA.</t>
+        </is>
+      </c>
+      <c r="N146" t="inlineStr">
+        <is>
+          <t>Ao longo do tempo, verificam-&lt;u&gt;se &lt;/u&gt;mudanças nas habilidades exigidas diante de novas maneiras de trabalhar.</t>
+        </is>
+      </c>
+      <c r="O146" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P146" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q146" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>147</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Petrobrás</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>“Anunciata se mostrava péssima cabeleireira” é uma oração que contém o pronome se com o mesmo valor presente em:</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>Palavra Se</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J147" t="inlineStr">
+        <is>
+          <t>A benzedeira &lt;u&gt;se &lt;/u&gt;fartou com o bolo de fubá.</t>
+        </is>
+      </c>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>Já &lt;u&gt;se &lt;/u&gt;sabia que o dr. Albano ia receitar Veganin.</t>
+        </is>
+      </c>
+      <c r="L147" t="inlineStr">
+        <is>
+          <t>A ferida da perna de Virgínia &lt;u&gt;se &lt;/u&gt;foi em três dias.</t>
+        </is>
+      </c>
+      <c r="M147" t="inlineStr">
+        <is>
+          <t>Minha mãe não &lt;u&gt;se &lt;/u&gt;queixou de nada com ninguém.</t>
+        </is>
+      </c>
+      <c r="N147" t="inlineStr">
+        <is>
+          <t>Falava-&lt;u&gt;se&lt;/u&gt; na ferida de Virgínia como algo misterioso.</t>
+        </is>
+      </c>
+      <c r="O147" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P147" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q147" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>148</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>Considere a ocorrência da palavra se no trecho “O opaco da enganação &lt;u&gt;se &lt;/u&gt;torna transparente”. A frase em que a palavra destacada pertence a uma classe gramatical diferente da do trecho mencionado é:</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>Palavra Se</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J148" t="inlineStr">
+        <is>
+          <t>Lemos com compreensão, &lt;u&gt;se &lt;/u&gt;conferimos sentido ao texto.</t>
+        </is>
+      </c>
+      <c r="K148" t="inlineStr">
+        <is>
+          <t>Alguns &lt;u&gt;se &lt;/u&gt;arrependem de não terem lido mais na infância.</t>
+        </is>
+      </c>
+      <c r="L148" t="inlineStr">
+        <is>
+          <t>Leem-&lt;u&gt;se &lt;/u&gt;narrativas literárias para desenvolver a criticidade.</t>
+        </is>
+      </c>
+      <c r="M148" t="inlineStr">
+        <is>
+          <t>Aprende-&lt;u&gt;se &lt;/u&gt;muito lendo textos literários de todos os gêneros.</t>
+        </is>
+      </c>
+      <c r="N148" t="inlineStr">
+        <is>
+          <t>Os jovens mais cultos são os que &lt;u&gt;se &lt;/u&gt;movem na direção dos livros.</t>
+        </is>
+      </c>
+      <c r="O148" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P148" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q148" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>149</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>A palavra &lt;u&gt;se &lt;/u&gt;destacada contém a ideia de condição em:</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>Palavra Se</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J149" t="inlineStr">
+        <is>
+          <t>“e os mecanismos com os quais podemos minimizá-los têm pouquíssimo destaque &lt;u&gt;se &lt;/u&gt;comparados aos de outros tipos de poluição.”</t>
+        </is>
+      </c>
+      <c r="K149" t="inlineStr">
+        <is>
+          <t>“Mais de perto, a poluição luminosa pode ser notada quando &lt;u&gt;se &lt;/u&gt;observa uma ‘aura’ de luz no horizonte”</t>
+        </is>
+      </c>
+      <c r="L149" t="inlineStr">
+        <is>
+          <t>“Mariposas e besouros têm seus ciclos de vida alterados e são atraídos e desorientados pela luz, tornando-&lt;u&gt;se &lt;/u&gt;vítimas fáceis de aves, morcegos e outros predadores.”</t>
+        </is>
+      </c>
+      <c r="M149" t="inlineStr">
+        <is>
+          <t>“mudanças na duração dos dias causadas por luminárias provocam confusão em relação à estação do ano em que &lt;u&gt;se &lt;/u&gt;encontram.”</t>
+        </is>
+      </c>
+      <c r="N149" t="inlineStr">
+        <is>
+          <t>“Com o desenvolvimento tecnológico das lâmpadas LED (sigla em inglês para diodo emissor de luz), a iluminação artificial torna-&lt;u&gt;se &lt;/u&gt;mais eficiente energeticamente”.</t>
+        </is>
+      </c>
+      <c r="O149" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P149" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q149" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>150</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Liquigás</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>A opção por uma linguagem informal, em algumas passagens de texto, permite jogos de palavras como o que se verifica no emprego de Se nas seguintes frases: “&lt;u&gt;Se &lt;/u&gt;o cinema está cheio, a gente senta na primeira fila e torce um pouco o pescoço.” “&lt;u&gt;Se &lt;/u&gt;acostuma para evitar feridas, sangramentos.” Nos trechos acima, as palavras em destaque classificam-se, respectivamente, como</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>Palavra Se</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J150" t="inlineStr">
+        <is>
+          <t>conjunção e pronome</t>
+        </is>
+      </c>
+      <c r="K150" t="inlineStr">
+        <is>
+          <t>conjunção e preposição</t>
+        </is>
+      </c>
+      <c r="L150" t="inlineStr">
+        <is>
+          <t>pronome e preposição</t>
+        </is>
+      </c>
+      <c r="M150" t="inlineStr">
+        <is>
+          <t>pronome e conjunção</t>
+        </is>
+      </c>
+      <c r="N150" t="inlineStr">
+        <is>
+          <t>conjunção e conjunção</t>
+        </is>
+      </c>
+      <c r="O150" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P150" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q150" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>151</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;À moda brasileira&lt;/b&gt;
+1 Estou me vendo debaixo de uma árvore, lendo a pequena história da literatura brasileira.
+2 Olavo Bilac! – eu disse em voz alta e de repente parei quase num susto depois que li os primeiros versos do soneto à língua portuguesa: Última flor do Lácio, inculta e bela / És, a um tempo, esplendor e sepultura.
+3 Fiquei pensando, mas o poeta disse sepultura?! O tal de Lácio eu não sabia onde ficava, mas de sepultura eu entendia bem, disso eu entendia, repensei baixando o olhar para a terra. Se escrevia (e já escrevia) pequenos contos nessa língua, quer dizer que era a sepultura que esperava por esses meus escritos?
+4 Fui falar com meu pai. Comecei por aquelas minhas sondagens antes de chegar até onde queria, os tais rodeios que ele ia ouvindo com paciência enquanto enrolava o cigarro de palha, fumava nessa época esses cigarros. Comecei por perguntar se minha mãe e ele não tinham viajado para o exterior.
+5 Meu pai fixou em mim o olhar verde. Viagens, só pelo Brasil, meus avós é que tinham feito aquelas longas viagens de navio, Portugal, França, Itália... Não esquecer que a minha avó, Pedrina Perucchi, era italiana, ele acrescentou. Mas por que essa curiosidade?
+6 Sentei-me ao lado dele, respirei fundo e comecei a gaguejar, é que seria tão bom se ambos tivessem nascido lá longe e assim eu estaria hoje escrevendo em italiano, italiano! – fiquei repetindo e abri o livro que trazia na mão: Olha aí, pai, o poeta escreveu com todas as letras, nossa língua é sepultura mesmo, tudo o que a gente fizer vai para debaixo da terra, desaparece!
+7 Calmamente ele pousou o cigarro no cinzeiro ao lado. Pegou os óculos. O soneto é muito bonito, disse me encarando com severidade. Feio é isso, filha, isso de querer renegar a própria língua. Se você chegar a escrever bem, não precisa ser em italiano ou espanhol ou alemão, você ficará na nossa língua mesmo, está me compreendendo? E as traduções? Renegar a língua é renegar o país, guarde isso nessa cabecinha. E depois (ele voltou a abrir o livro), olha que beleza o que o poeta escreveu em seguida, Amo-te assim, desconhecida e obscura, veja que confissão de amor ele fez à nossa língua! Tem mais, ele precisava da rima para sepultura e calhou tão bem essa obscura, entendeu agora? – acrescentou e levantou-se. Deu alguns passos e ficou olhando a borboleta que entrou na varanda: Já fez a sua lição de casa?
+8 Fechei o livro e recuei. Sempre que meu pai queria mudar de assunto ele mudava de lugar: saía da poltrona e ia para a cadeira de vime. Saía da cadeira de vime e ia para a rede ou simplesmente começava a andar. Era o sinal, Não quero falar nisso, chega. Então a gente falava noutra coisa ou ficava quieta.
+9 Tantos anos depois, quando me avisaram lá do pequeno hotel em Jacareí que ele tinha morrido, fiquei pensando nisso, ah! se quando a morte entrou, se nesse instante ele tivesse mudado de lugar. Mudar depressa de lugar e de assunto. Depressa, pai, saia da cama e fique na cadeira ou vá pra rua e feche a porta!
+(TELLES,LygiaFagundes.Duranteaqueleestranhochá:perdidoseachados.RiodeJaneiro:Rocco,2002,p.109-111.
+Fragmentoadaptado).
+A frase em que as vírgulas estão empregadas com a mesma função que em “Não esquecer que a minha avó, Pedrina Perucchi, era italiana” (parágrafo 5) é:</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>Fácil</t>
+        </is>
+      </c>
+      <c r="I151" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J151" t="inlineStr">
+        <is>
+          <t>Mude de lugar, meu pai, porque a morte vai chegar.</t>
+        </is>
+      </c>
+      <c r="K151" t="inlineStr">
+        <is>
+          <t>A filha, preocupada e triste, questionava a própria língua materna.</t>
+        </is>
+      </c>
+      <c r="L151" t="inlineStr">
+        <is>
+          <t>A língua portuguesa, embora inculta, constrói belos textos literários.</t>
+        </is>
+      </c>
+      <c r="M151" t="inlineStr">
+        <is>
+          <t>Os poemas, textos de uma beleza sem igual, encantam seus leitores.</t>
+        </is>
+      </c>
+      <c r="N151" t="inlineStr">
+        <is>
+          <t>Colocou os óculos e, caminhando pela sala, revelou a beleza do poema.</t>
+        </is>
+      </c>
+      <c r="O151" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P151" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q151" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>152</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>BANRISUL</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Implantação do código de ética nas empresas&lt;/b&gt;
+Desde a infância, estamos sujeitos à influência de nosso meio social, por intermédio da família, da escola, dos amigos, dos meios de comunicação de massa. Ao nascer, o homem já se defronta com um conjunto de regras, normas e valores aceitos em seu grupo social. As palavras “ética” e “moral” indicam costumes acumulados — conjunto de normas e valores dos grupos sociais em um contexto.
+A ética é um conjunto de princípios e disposições cujo objetivo é balizar as ações humanas. A ética existe como uma referência para os seres humanos em sociedade, de modo tal que a sociedade possa se tornar cada vez mais humana. Ela pode e deve ser incorporada pelos indivíduos, sob a forma de uma atitude diante da vida cotidiana. Mas ela não é um conjunto de verdades fixas, imutáveis. A ética se move historicamente, se amplia e se adensa. Para entendermos como isso acontece na história da humanidade, basta lembrarmos que, um dia, a escravidão foi considerada "natural". Ética é o que diz respeito à ação quando ela é refletida, pensada. A ética preocupa-se com o certo e com o errado, mas não é um conjunto simples de normas de conduta como a moral. Ela promove um estilo de ação que procura refletir sobre o melhor modo de agir que não abale a vida em sociedade e não desrespeite a individualidade dos outros.
+As empresas precisam desenvolver-se de tal forma que a conduta ética de seus integrantes, bem como os valores e convicções primários da organização, se tornem parte de sua cultura. Assim, a ética vem sendo vista como uma espécie de requisito para a sobrevivência das empresas no mundo moderno e pode ser definida como a transparência nas relações e a preocupação com o impacto das suas atividades na sociedade.
+Muitos exemplos poderiam ser citados de empresas que estão começando a valorizar e a alertar seus funcionários sobre a ética. Algumas empresas já implantaram, inclusive, um comitê de ética, o qual se destina à proteção da imagem da companhia. É preciso, portanto, que haja uma conscientização da importância de uma conduta ética ou mesmo a implantação de um código de ética nas organizações, pois a cada dia que passa a ética tem mostrado ser um dos caminhos para o sucesso e para o bem comum, agregando valor moral ao patrimônio da organização.
+O Código de Ética é um instrumento de realização dos princípios, da visão e da missão da empresa. Serve para orientar as ações de seus colaboradores e explicitar a postura social da empresa em face dos diferentes públicos com os quais interage. É da máxima importância que seu conteúdo seja refletido nas atitudes das pessoas a que se dirige e encontre respaldo na alta administração da empresa, que, tanto quanto o último empregado contratado, tem a responsabilidade de vivenciá-lo.
+As relações com os funcionários, desde o processo de contratação, desenvolvimento profissional, lealdade mútua, respeito entre chefes e subordinados, saúde e segurança, propriedade da informação, assédio profissional e sexual, alcoolismo, uso de drogas, entre outros, são aspectos que costumam ser abordados em um Código de Ética. Cumprir horários, entregar o trabalho no prazo, dar o seu melhor ao executar uma tarefa e manter a palavra dada são exemplos de atitudes que mostram aos superiores e aos colegas que o funcionário valoriza os princípios éticos da empresa ou da instituição.
+O Código também pode envolver situações de relacionamento com clientes, fornecedores, acionistas, investidores, comunidade vizinha, concorrentes e mídia. O Código de Ética pode estabelecer ações de responsabilidade social dirigidas ao desenvolvimento social de comunidades vizinhas, bem como apoio a projetos de educação voltados ao crescimento pessoal e profissional de jovens carentes. Também pode fazer referência à participação da empresa na comunidade, dando diretrizes sobre as relações com os sindicatos, outros órgãos da esfera pública, relações com o governo, entre outras.
+Portanto, conclui-se que o Código de Ética se fundamenta em deveres para com os colegas, clientes, profissão, sociedade e para consigo próprio.
+(MARTINS,Rosemir.UFPR,2003.Disponívelem:https://acervodigital.ufpr.br.Acessoem:16nov.2022.Adaptado.) O emprego da vírgula está plenamente de acordo com as exigências da norma-padrão da língua portuguesa em:</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J152" t="inlineStr">
+        <is>
+          <t>A capacidade do empresário de manter um bom relacionamento entre gerentes, funcionários, clientes e fornecedores de produtos, é uma das condições para uma organização conseguir o êxito esperado.</t>
+        </is>
+      </c>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>A preocupação com o comportamento dos funcionários deve ser constante, para assegurar que eles tenham seus direitos, garantidos.</t>
+        </is>
+      </c>
+      <c r="L152" t="inlineStr">
+        <is>
+          <t>O gerente daquela organização admitiu que, durante o período de maior contaminação da pandemia do coronavírus precisou contratar novos digitadores para realizarem serviços urgentes em sua instituição.</t>
+        </is>
+      </c>
+      <c r="M152" t="inlineStr">
+        <is>
+          <t>Os administradores da empresa reconheceram a importância de realizarem com muito cuidado, a inspeção em todos os espaços destinados ao atendimento dos clientes.</t>
+        </is>
+      </c>
+      <c r="N152" t="inlineStr">
+        <is>
+          <t>Os empregados das instituições, considerando o seu compromisso como cidadãos, procuram respeitar as leis estabelecidas para o bom comportamento no meio social em que vivem.</t>
+        </is>
+      </c>
+      <c r="O152" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P152" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q152" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>153</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Banco do Brasil</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;A história do método braile&lt;/b&gt;
+Ler no escuro. Quem já tentou sabe que é impossível. Mas foi exatamente a isso que um francês chamado Louis Braille dedicou a vida. Nascido em Coupvray, uma pequena aldeia nos arredores de Paris, em 1809, desde cedo ele mostrou muito interesse pelo trabalho do pai. Seus olhos azuis brilhavam da admiração de vê-lo cortar, com extrema perícia, selas e arreios. Pouco depois de completar 3 anos, o menino começou a brincar na selaria do pai, cortando pequenas tiras de couro. Uma tarde, uma sovela, instrumento usado para perfurar o couro, escapou-lhe da mão e atingiu o seu olho esquerdo. O resultado foi uma infecção que, seis meses depois, afetaria também o olho direito. Aos 5 anos, o garoto estava completamente cego.
+A tragédia não o impediu, porém, de frequentar a escola por dois anos e de se tornar ainda um aluno brilhante. Por essa razão, ele ganhou uma bolsa de estudos no Instituto Nacional para Jovens Cegos, em Paris, um colégio interno fundado por Valentin Haüy (1745-182. Além do currículo normal, Haüy introduzira um sistema especial de alfabetização, no qual letras de forma impressas em relevo, em papelão, eram reconhecidas pelos contornos. Desde o início do curso, Braille destacou-se como o melhor aluno da turma e logo começou a ajudar os colegas. Em 1821, aos 12 anos, conheceu um método inventado pouco antes por Charles Barbier de La Serre, oficial do Exército francês.
+O método Barbier, também chamado escrita noturna, era um código de pontos e traços em relevo impressos também em papelão. Destinava-se a enviar ordens cifradas a sentinelas em postos avançados. Estes decodificariam a mensagem até no escuro. Mas, como a ideia não pegou na tropa, Barbier adaptou o método para a leitura de cegos, com o nome de grafia sonora. O sistema permitia a comunicação entre os cegos, pois com ele era possível escrever, algo que o método de Haüy não possibilitava. O de Barbier era fonético: registrava sons e não letras. Dessa forma, as palavras não podiam ser soletradas. Além disso, o fato de um grande número de sinais ser usado para uma única palavra tornava o sistema muito complicado. Apesar dos inconvenientes, foi adotado como método auxiliar por Haüy.
+Pesquisando a fundo a grafia sonora, Braille percebeu suas limitações e pôs-se a aperfeiçoá-la.
+Em 1824, seu método estava pronto. Primeiro, eliminou os traços, para evitar erros de leitura: em seguida, criou uma célula de seis pontos, divididos em duas colunas de três pontos cada, que podem ser combinados de 63 maneiras diferentes. A posição dos pontos na célula está ao lado.
+Em 1826, aos 17 anos, ainda estudante, Braille começou a dar aulas. Embora seu método fizesse sucesso entre os alunos, não podia ensiná-lo na sala de aula, pois ainda não era reconhecido oficialmente. Por isso, Braille dava aulas do revolucionário sistema escondido no quarto, que logo se transformou numa segunda sala de aula.
+O braile é lido passando-se a ponta dos dedos sobre os sinais de relevo. Normalmente se usa a mão direita com um ou mais dedos, conforme a habilidade do leitor, enquanto a mão esquerda procura o início da outra linha. Aplica-se a qualquer língua, sem exceção, e também à estenografia, à música – Braille, por sinal, era ainda exímio pianista – e às notações científicas em geral. A escrita é feita mediante o uso da reglete, também idealizada por Braille: trata-se de uma régua especial, de duas linhas, com uma série de janelas de seis furos cada, correspondentes às células braile.
+Louis Braille morreu de tuberculose em 1852, com apenas 43 anos. Temia que seu método desaparecesse com ele, mas, finalmente, em 1854 foi oficializado pelo governo francês. No ano seguinte, foi apresentado ao mundo, na Exposição Internacional de Paris, por ordem do imperador Napoleão III (1808-187, que programou ainda uma série de concertos de piano com ex-alunos de Braille. O sucesso foi imediato, e o sistema se espalhou pelo mundo. Em 1952, o governo francês transferiu os restos mortais de Braille para o Panthéon, em Paris, onde estão sepultados os heróis nacionais.
+(ATANES, Silvio. Super Interessante. Disponível em: https://super.abril.]com.br/historia/. Acesso em: 23 out. 2022.
+Adaptado.) No trecho do parágrafo, “conheceu um método inventado pouco antes por Charles Barbier de La Serre, oficial do Exército francês”, a vírgula está empregada com a mesma função que em:</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J153" t="inlineStr">
+        <is>
+          <t>A cegueira não o impediu, no entanto, de estudar.</t>
+        </is>
+      </c>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>Perspicaz, Braille percebeu falhas no método de Barbier.</t>
+        </is>
+      </c>
+      <c r="L153" t="inlineStr">
+        <is>
+          <t>A infecção, seis meses depois, afetou o segundo olho de Braille.</t>
+        </is>
+      </c>
+      <c r="M153" t="inlineStr">
+        <is>
+          <t>Escrita noturna, método de Barbier, não teve sucesso quando criado.</t>
+        </is>
+      </c>
+      <c r="N153" t="inlineStr">
+        <is>
+          <t>No Instituto Nacional para Jovens Cegos, Braille desenvolveu seus estudos.</t>
+        </is>
+      </c>
+      <c r="O153" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P153" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q153" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>154</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Banco do Brasil</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Entenda o que é &lt;i&gt;deep fake&lt;/i&gt; e saiba como se proteger&lt;/b&gt;
+Vídeos que viralizam nas redes sociais mostrando figuras públicas em situações quase inacreditáveis são verdadeiros? Afinal de contas tudo parece tão real... A resposta é não, pois se trata de uma “deepfake”,“falsificação profunda” em português, que, como a tradução indica, é tão bem feita que pode enganar até os mais atentos. Segundo estudo de uma empresa de segurança, 65% dos brasileiros ignoram a sua existência e 71% não reconhecem quando um vídeo foi editado digitalmente usando essa técnica.
+O que muita gente não sabe, porém, é que esse tipo de golpe, além de manipular vídeos com celebridades e políticos famosos, também prejudica empresas e cidadãos comuns, que podem ser envolvidos em fraudes de identidade e extorsões. “Deepfakepode ser definida como a criação de vídeos e áudios falsos por meio de inteligência artificial”, explica um especialista de segurança cibernética e fraude. A prática costuma utilizar um vídeo de referência e a face (ou corpo) de outra pessoa, que não fazia parte do vídeo original.
+Criam-se áudios falsos, fazendo a inteligência artificial aprender como uma pessoa fala e, a partir daí, obter uma montagem com outras falas, inclusive alterando os lábios para acompanhar as palavras que são ditas.
+Esse processo vem evoluindo rapidamente, tornando cada vez mais difícil a sua identificação.
+Isso ocorre porque as novas redes neurais (sistemas de computação que funcionam como neurônios do cérebro humano), a evolução da capacidade de processamento e a redução de custos da computação em nuvem têm facilitado o acesso a essa tecnologia, contribuindo para aumentar a qualidade dos vídeos.
+No entanto, os criminosos não precisam de tanto conhecimento e tecnologia para aplicar seus golpes.
+Isso porque deepfakes criadas para serem distribuídas por appsde mensagens não exigem tanta qualidade. O perigo é que, para o cidadão comum, a deepfake pode ser o ponto de partida para uma fraude financeira, entre outros problemas.
+A recomendação para pessoas físicas se protegerem é diminuir a exposição de fotos com rostos e vídeos pessoais na internet. “As redes sociais devem se manter configuradas como privadas, já que fotos, áudios ou vídeos disponíveis publicamente podem ser utilizados para alimentar a inteligência artificial e engendrardeepfakes.” Além disso, ao receber um vídeo suspeito, observe se o rosto e os lábios da pessoa se movem em conjunto com o que ela diz. Preste atenção se a fala parece contínua ou se em algum momento apresenta cortes entre uma palavra e outra. E considere o contexto — ainda que tecnicamente o vídeo esteja muito bem manipulado, avalie se faz sentido que aquela pessoa diga o que parece dizer naquele momento.
+(Disponívelem:https://estudio.folha.uol.com.br/unico.Acessoem:20out.2022.Adaptado.) De acordo com a norma-padrão da língua portuguesa, o emprego da vírgula está correto em:</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J154" t="inlineStr">
+        <is>
+          <t>Os produtos comercializados nos mercados deverão apresentar embalagens adaptadas em seus rótulos até o próximo ano atendendo, à expectativa do cliente na busca de uma dieta saudável.</t>
+        </is>
+      </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>A tabela de informação nutricional, passará a conter informações gráficas nítidas e legíveis com o objetivo de preservar a compreensão das informações.</t>
+        </is>
+      </c>
+      <c r="L154" t="inlineStr">
+        <is>
+          <t>As indústrias alimentícias estão sendo obrigadas, pelos órgãos fiscalizadores a se adequarem à legislação em vigor para que não sejam multadas.</t>
+        </is>
+      </c>
+      <c r="M154" t="inlineStr">
+        <is>
+          <t>A partir da promulgação de lei no próximo ano, os rótulos de alimentos e bebidas deverão esclarecer os consumidores sobre a existência de substâncias alergênicas.</t>
+        </is>
+      </c>
+      <c r="N154" t="inlineStr">
+        <is>
+          <t>Vários economistas recomendam, que os consumidores tenham precaução ao utilizar seus cartões de crédito devido à possibilidade de aumentarem seu endividamento.</t>
+        </is>
+      </c>
+      <c r="O154" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P154" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q154" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>155</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Esc BB</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Pix: é o fim do dinheiro em espécie?&lt;/b&gt;
+O Pix muda a forma como realizamos transações financeiras. Representará realmente o fim do DOC e da TED? O boleto bancário está ainda mais ameaçado de extinção? E o velho cheque vai resistir a esses novos tempos?
+Abrangente como é, o Pix pode reduzir ou acabar com a circulação das notas de real? Essa é uma pergunta sem resposta fácil. O fato é que o avanço das transações financeiras eletrônicas, em detrimento do uso do dinheiro em papel, pode ser benéfico para o Brasil, em vários sentidos.
+O Pix tem tudo para ser o empurrãozinho que nos falta para chegarmos a esse cenário.
+E por que o dinheiro em espécie resiste? Talvez você esteja entre aqueles que compram no supermercado com cartão de crédito ou usam QR Code para pagar a farmácia. Mas a feira da semana e os churros na esquina você paga com “dinheiro vivo”, certo? Um dos fatores que escoram a circulação de papel-moeda no Brasil é a informalidade.
+Atrelada a isso está a situação dos desbancarizados. A dificuldade que muita gente teve para receber o auxílio emergencial, durante a pandemia, jogou luz sobre um problema notado há tempos: a enorme quantidade de brasileiros que não têm acesso a serviços bancários. O pouco de dinheiro que entra no orçamento dessas pessoas precisa ser gasto rapidamente para subsistência.
+Não há base financeira suficiente para justificar movimentações bancárias. Também pesa para o time dos “sem-banco” o baixo nível de educação ou a falta de familiaridade com a tecnologia.
+O fator cultural também favorece a circulação do dinheiro em espécie. É provável que você conheça alguém que, mesmo tendo boa renda, prefere pagar boletos ou receber pagamentos com cédulas simplesmente por estar acostumado a elas. Para muita gente que faz parte dessa turma, dinheiro vivo é dinheiro recebido ou pago na hora. Não é preciso esperar a TED cair ou o dia virar para o boleto ser compensado. Isso pesa mais do que a conveniência de se livrar da fila da lotérica.
+Embora o Brasil tenha um sistema bancário que suporta vários tipos de transações, o país estava ficando para trás no que diz respeito a pagamentos instantâneos. O Pix veio para preencher essa lacuna.
+A modalidade permite transações em qualquer horário e dia, incluindo finais de semana e feriados.
+Essa característica, por si só, já é capaz de mudar a forma como lidamos com o dinheiro, pois implica envio ou recebimento imediato: as transações via Pix são concluídas rapidamente. É o fim do papel-moeda? Não é tão simples assim. O Pix não foi idealizado com o propósito exclusivo de acabar com os meios de pagamento e transferência atuais, muito menos com o papelmoeda, mas para fazer o sistema financeiro do Brasil evoluir e ficar mais competitivo.
+Apesar disso, não é exagero esperar que, à medida que a população incorpore o sistema à sua rotina, o uso de DOC, TED, boletos e cartões caia. Eventualmente, algum desses meios poderá ser descontinuado, mas isso não acontecerá tão cedo — vide o exemplo do cheque, que não “morreu” com a chegada do cartão.
+No caso das cédulas, especialistas do mercado financeiro apontam para uma diminuição de circulação, mas não para um futuro próximo em que o papel-moeda deixará de existir. Para que esse cenário se torne realidade, é necessário, sobretudo, atacar a desbancarização. O medo ou a pouca familiaridade com a tecnologia podem ser obstáculos, mas o Pix é tão interessante para o país que o próprio comércio incentiva o público mais resistente a aderir a ele.
+(ALECRIM,E.Disponívelem:https://tecnoblog.net/especiais/pix-fim-dinheiro-especie-brasil/.Publicadoem novembrode2020.Acessoem:2dez.2022.Adaptado.) O emprego da vírgula está plenamente observado, de acordo com as exigências da norma-padrão da língua portuguesa, em:</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J155" t="inlineStr">
+        <is>
+          <t>A implantação do Pix trouxe novidades importantes para os usuários que em outra época, não conseguiam pagar suas contas com tanta facilidade.</t>
+        </is>
+      </c>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>A utilização de cheques por pessoas que possuem contas bancárias tem apresentado uma redução quantitativa por ser um instrumento, pouco confiável e facilmente falsificado.</t>
+        </is>
+      </c>
+      <c r="L155" t="inlineStr">
+        <is>
+          <t>Na aprovação da abertura de novas contas é importante, diagnosticar o público considerado vulnerável por ser composto por pessoas ou famílias que estão em processo de exclusão social.</t>
+        </is>
+      </c>
+      <c r="M155" t="inlineStr">
+        <is>
+          <t>No caso de ocorrerem roubo e perda do cartão de crédito, a primeira providência é comunicar o fato à administradora do cartão e pedir o seu bloqueio ou cancelamento.</t>
+        </is>
+      </c>
+      <c r="N155" t="inlineStr">
+        <is>
+          <t>O comportamento dos funcionários de uma instituição, seja ela particular ou pública requer um cuidado permanente para identificar pontos fortes e fracos no relacionamento com o público.</t>
+        </is>
+      </c>
+      <c r="O155" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P155" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q155" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>156</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Esc BB</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Empreendedorismo social: um caminho para quem quer mudar o mundo&lt;/b&gt;
+Ainda que não exista uma concepção única sobre o empreendedorismo social, de forma geral, o conceito está relacionado ao ato de empreender ou inovar com o objetivo de alavancar causas sociais e ambientais. A meta é transformar uma realidade, promover o bem-estar da sociedade e agregar valor com cunho social.
+Um empreendedor social produz bens e serviços que irão impactar positivamente a comunidade em que ele está inserido e solucionar algum problema ou necessidade daquele grupo. Apesar de poder ter retorno financeiro, os empreendimentos sociais analisam seu desempenho a partir do impacto social gerado por sua atuação.
+Vale ressaltar que, apesar de apresentarem muitas similaridades, empreendedorismo social e negócio social não são sinônimos. O empreendedorismo social cria valor por meio da inovação, que gera uma transformação social. O foco não é o retorno financeiro, mas a resolução de problemas sociais e o impacto positivo. Enquanto isso, os negócios sociais seguem a lógica tradicional do mercado, porém com a ambição de gerar valor social.
+Cinco características também são essenciais para a iniciativa: ser inovadora; realizável; autossustentável; contar com a participação de diversos segmentos da sociedade, incluindo as pessoas impactadas; e promover impacto social com resultados mensuráveis.
+Quem tem interesse de atuar nessa área precisa trabalhar em grupo e formar parcerias, saber lidar bem com as pessoas e buscar formas de trazer resultados de impacto social.
+Além disso, o profissional precisa ter flexibilidade e vontade de explorar, pois é possível que ele acabe exercendo um papel que não seja necessariamente na sua área de formação, ou que sua atuação se transforme rapidamente, por conta do dinamismo e das necessidades do negócio.
+(MENDES,T.Empreendedorismosocial:umcaminhoparaquemquermudaromundo.Naprática,7jul.2022.
+Disponívelem:https://www.napratica.org.br/empreendedorismo-social/.Acessoem:2set.2022.Adaptado) O emprego da vírgula atende às exigências da norma-padrão da língua portuguesa em:</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J156" t="inlineStr">
+        <is>
+          <t>A execução de novas tarefas em um supermercado, envolve a disposição dos funcionários de aceitarem as mudanças propostas pelo RH.</t>
+        </is>
+      </c>
+      <c r="K156" t="inlineStr">
+        <is>
+          <t>Ao consultar os fornecedores de produtos para suas lojas, os responsáveis por esse departamento devem ser cuidadosos.</t>
+        </is>
+      </c>
+      <c r="L156" t="inlineStr">
+        <is>
+          <t>A escolha do funcionário para proferir uma palestra em nome da empresa, compete à administração da instituição.</t>
+        </is>
+      </c>
+      <c r="M156" t="inlineStr">
+        <is>
+          <t>O profissional interessado em mudanças na sua área de atuação deve estudar, com antecedência as suas possibilidades de crescimento.</t>
+        </is>
+      </c>
+      <c r="N156" t="inlineStr">
+        <is>
+          <t>Para desenvolver projetos cabe ao gerente da organização, a iniciativa de implementar novas técnicas à disposição dos empreendedores.</t>
+        </is>
+      </c>
+      <c r="O156" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P156" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q156" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>157</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>AgeRIO</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>O emprego da vírgula está plenamente de acordo com a norma-padrão no seguinte período:</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J157" t="inlineStr">
+        <is>
+          <t>A agricultura depende, de serviços para combater pragas e manter a disponibilidade de água.</t>
+        </is>
+      </c>
+      <c r="K157" t="inlineStr">
+        <is>
+          <t>A água é uma das maiores dádivas, que o planeta nos concede e um dos recursos naturais mais lembrados quando se considera o futuro da humanidade.</t>
+        </is>
+      </c>
+      <c r="L157" t="inlineStr">
+        <is>
+          <t>Apesar de nosso país apresentar inúmeros atrativos naturais, a maioria das áreas de proteção ambiental ainda precisa cuidar da infraestrutura básica.</t>
+        </is>
+      </c>
+      <c r="M157" t="inlineStr">
+        <is>
+          <t>O Brasil tem a maior diversidade, de todas as partes do planeta Terra onde existe ou pode existir vida e ampla variedade de paisagens.</t>
+        </is>
+      </c>
+      <c r="N157" t="inlineStr">
+        <is>
+          <t>O fato de que devemos nos preocupar com o meio ambiente e economizar água deixou de ser, há muito tempo um simples conceito.</t>
+        </is>
+      </c>
+      <c r="O157" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P157" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q157" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>158</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>BASA</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;“Maior fronteira agrícola do mundo está no bioma amazônico”,&lt;/b&gt;
+diz pesquisador da Embrapa
+O Brasil é um dos poucos países no mundo com a possibilidade de ampliar áreas com a agropecuária. De fato, um estudo da ONU mostra que o país será o grande responsável por produzir os alimentos necessários para atender os mais de 9 bilhões de pessoas que habitarão o planeta em 2050. De acordo com pesquisadores da Embrapa, a região possui potencial e áreas para ampliação sustentável da agricultura. Portanto, a responsabilidade do agricultor brasileiro é muito grande.
+A região amazônica se mostra promissora para a agricultura, pois ela é rica em um insumo fundamental, a água. Estados como Rondônia e Acre têm municípios que recebem até 2.800 milímetros de chuvas por ano. E isso proporciona a qualidade e a possibilidade de semear mais de uma cultura por ano.
+Entretanto, as críticas internacionais, quanto ao uso e à ampliação da agricultura na região amazônica, são um limitante para a exploração dessas áreas. Para cada nova área aberta para a agricultura, parte deveria ser obrigatoriamente destinada à preservação ambiental, segundo as exigências dos países que compram nossos produtos agrícolas.
+POPOV,Daniel.CanalRural.Disponívelem:https://www.canalrural.com.br/projeto-soja-brasil/noticia/ maior-fronteira-agricola--mundo-amazonia-embrapa/.19set.2019.Acessoem:30nov.2021.Adaptado.
+De acordo com a norma-padrão da língua portuguesa, o emprego adequado da vírgula está plenamente atendido em:</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J158" t="inlineStr">
+        <is>
+          <t>A criação de animais para a produção de alimentos, é de grande importância para o sustento de milhares de famílias.</t>
+        </is>
+      </c>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>A floresta Amazônica, apesar de parecer homogênea, possui muitas diferenças na sua vegetação.</t>
+        </is>
+      </c>
+      <c r="L158" t="inlineStr">
+        <is>
+          <t>A melhor maneira de proteger as povoações situadas nas margens dos rios, é procurar soluções que impeçam o comércio ilegal.</t>
+        </is>
+      </c>
+      <c r="M158" t="inlineStr">
+        <is>
+          <t>O estado do Amazonas apresenta, a maior população indígena do Brasil com aproximadamente trinta mil habitantes.</t>
+        </is>
+      </c>
+      <c r="N158" t="inlineStr">
+        <is>
+          <t>O número de estudiosos preocupados com o futuro do planeta, aumentou devido ao aquecimento global.</t>
+        </is>
+      </c>
+      <c r="O158" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P158" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q158" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>159</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>ELETRONUCLEAR</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Maria José&lt;/b&gt;
+&lt;i&gt;Paulo Mendes Campos&lt;/i&gt;
+Faz um ano que Maria José morreu. Era meiga quase sempre, violenta quando necessário. Eu era menino e apanhava de um companheiro maior, quando ela me gritou da sacada se eu não via a pedra que marcava o gol. Dei uma pedrada no outro e acabei com a briga por milagre.
+Visitava os miseráveis, internava indigentes enfermos, devotava-se ao alívio de misérias físicas e morais do próximo, estudava o mistério teológico, exigia sempre o mais difícil de si mesma, comungava todos os dias, ingressou na Ordem Terceira de São Francisco. Mas nunca deixou de ter na gaveta o revólver que havia recebido, menina-e-moça, das mãos do pai, e que empunhou no quintal noturno, perseguindo um ladrão, para espanto de meus cinco anos.
+Já perto dos setenta anos, ela explicava para um amigo meu que tinha chegado à humildade da velhice; já não se importava com quem tentasse ofendê-la, mas conservava o revólver para a defesa dos filhos e dos netos.
+Tratou-me com a dureza e o carinho que mereciam a rebeldia e o verdor da minha meninice.
+Ensinou- me a ler as primeiras sentenças; me falava do Cura d’Ars e nos dois Franciscos, o de Sales e o de Assis; apresentou-me aos contos de Edgar Poe e aos poemas de Baudelaire; dizia-me sorrindo versos de Antônio Nobre que havia decorado quando menina; discutia comigo as ideias finais de Tolstoi; escutava maternalmente meus contos toscos. Quando me desgarrei nos primeiros envolvimentos adolescentes, Maria José, com irônico afeto, me repetia a advertência de Drummond: “Paulo, sossegue, o amor é isso que você está vendo: hoje beija, amanhã não beija, depois de amanhã é domingo e segunda-feira ninguém sabe o que será”.
+Logo que me fiz homenzinho, deixou a dureza e se fez minha amiga: nada me perguntava, adivinhava tudo.
+Terna e firme, nunca lhe vi a fraqueza da pieguice. Com o gosto espontâneo da qualidade das coisas, renunciou às vaidades mais singelas. Sensível, alegre, aprendeu a encarar o sofrimento de olhos lúcidos. Fiel à disciplina religiosa, compreendia celestialmente as almas que perdiam o rumo. Fé, Esperança e Caridade eram para ela a flecha e o alvo das criaturas.
+Tornara-se tão íntima da substância terrestre – a dor – que se fazia difícil para o médico saber o que sentia; acabava dizendo que doía um pouco, por delicadeza.
+Capaz de longos jejuns e abstinências, já no final da vida, podia acompanhar um casal amigo a Copacabana, passar do bar da moda ao restaurante diferente, beber dois cafés ou três uísques em santa serenidade e aceitar com alegria o prato exótico.
+Gostava das pessoas erradas, consumidas de paixão, admirava São Paulo e Santo Agostinho, acreditava que era preciso se fazer violência para entrar no reino celeste.
+Poucas horas antes de morrer, pediu um conhaque e sorriu, destemida e doce, como quem vai partir para o céu. Santificara-se. Deus era o dia e a noite de seu coração, o Pai, a piedade, o fogo do espírito. Perdi quem me amava e perdoava, quem me encomendava à compaixão do Criador e me defendia contra o mundo de revólver na mão.
+(Disponívelem:https://cronicabrasileira.org.br/cronicas/7173/maria-jose.Acessoem:05fev.2022).
+Considerando-se o emprego da vírgula, a frase que está de acordo com o padrão formal escrito da língua é</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J159" t="inlineStr">
+        <is>
+          <t>Eu que era frágil, sentia-me seguro, em sua presença.</t>
+        </is>
+      </c>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>Todos os dias, Maria José lia poemas para seu filho.</t>
+        </is>
+      </c>
+      <c r="L159" t="inlineStr">
+        <is>
+          <t>Seu desejo, era sempre, estar por perto para me proteger.</t>
+        </is>
+      </c>
+      <c r="M159" t="inlineStr">
+        <is>
+          <t>Maria José era uma mulher terna e, ao mesmo tempo firme.</t>
+        </is>
+      </c>
+      <c r="N159" t="inlineStr">
+        <is>
+          <t>Nem ela, nem o médico, nem eu, esperávamos aquele desfecho, triste.</t>
+        </is>
+      </c>
+      <c r="O159" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P159" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q159" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>160</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>ELETRONUCLEAR</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>O emprego da vírgula está plenamente de acordo com as exigências da norma-padrão da Língua Portuguesa em:</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J160" t="inlineStr">
+        <is>
+          <t>Caso sejam priorizadas medidas de proteção ao meio ambiente, a substituição dos lixões por uma forma adequada para tratar o lixo será benéfica.</t>
+        </is>
+      </c>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>Em todo o mundo há uma preocupação com a maneira de descartar o lixo por isso, é sempre preferível corrigir nossos hábitos.</t>
+        </is>
+      </c>
+      <c r="L160" t="inlineStr">
+        <is>
+          <t>O aterro sanitário apresenta inúmeras vantagens, como a redução da poluição porém, há desvantagens, como o seu alto custo.</t>
+        </is>
+      </c>
+      <c r="M160" t="inlineStr">
+        <is>
+          <t>O lixo eletrônico encontrado, em televisores, rádios, geladeiras, celulares, pilhas compromete a saúde pública.</t>
+        </is>
+      </c>
+      <c r="N160" t="inlineStr">
+        <is>
+          <t>O lixo hospitalar decorrente do atendimento médico a seres humanos ou animais, acarreta muitos problemas de saúde pública.</t>
+        </is>
+      </c>
+      <c r="O160" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P160" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q160" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>161</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>BANCO DA AMAZÔNIA</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>De acordo com a norma-padrão da língua portuguesa, o emprego adequado da vírgula está plenamente atendido em:</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J161" t="inlineStr">
+        <is>
+          <t>O outono que o Rio nos oferece, tem um ar fino, quase frio.</t>
+        </is>
+      </c>
+      <c r="K161" t="inlineStr">
+        <is>
+          <t>Uma senhora de cabelos muito brancos, ficava sentada, em uma cadeira.</t>
+        </is>
+      </c>
+      <c r="L161" t="inlineStr">
+        <is>
+          <t>Ele se incomodou, com as grades do Rio.</t>
+        </is>
+      </c>
+      <c r="M161" t="inlineStr">
+        <is>
+          <t>Todos os dias que passo pelo Aterro vejo, as árvores cada vez mais crescidas.</t>
+        </is>
+      </c>
+      <c r="N161" t="inlineStr">
+        <is>
+          <t>O porteiro, que prende passarinhos em gaiolas, não vê que o outono fica mais lindo quando estamos livres.</t>
+        </is>
+      </c>
+      <c r="O161" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P161" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q161" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>162</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>CAIXA ECONÔMICA</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>As vírgulas estão plenamente empregadas de acordo com o padrão formal da língua escrita em:</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J162" t="inlineStr">
+        <is>
+          <t>Há algumas décadas, se alguém falasse, em educação financeira, causaria um certo estranhamento.</t>
+        </is>
+      </c>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>Relacionar-se bem com o dinheiro de acordo com os especialistas, é uma forma de levar uma vida mais saudável, sem percalços.</t>
+        </is>
+      </c>
+      <c r="L162" t="inlineStr">
+        <is>
+          <t>É preciso criar uma cultura de discutir, na família, na escola, com os amigos, sobre como usar melhor os recursos financeiros.</t>
+        </is>
+      </c>
+      <c r="M162" t="inlineStr">
+        <is>
+          <t>A educação financeira, apesar de não resolver o problema da falta de dinheiro pode auxiliar, com um controle maior, de seu gasto.</t>
+        </is>
+      </c>
+      <c r="N162" t="inlineStr">
+        <is>
+          <t>Não gastar em demasia, não acumular dívidas, refletir sobre seus ganhos, e gastos, poupar são estratégias para gerir melhor suas finanças.</t>
+        </is>
+      </c>
+      <c r="O162" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P162" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q162" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>163</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>BANCO DA AMAZÔNIA</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>A frase que apresenta todas as vírgulas corretamente empregadas, de acordo com a norma-padrão da língua portuguesa, é:</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J163" t="inlineStr">
+        <is>
+          <t>A menina que descobriu o chicle, também experimentou, a possibilidade da eternidade.</t>
+        </is>
+      </c>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>São consideradas maravilhosas, aquelas histórias de príncipes e fadas, que vivem eternamente.</t>
+        </is>
+      </c>
+      <c r="L163" t="inlineStr">
+        <is>
+          <t>Aproveitou, a textura, o sabor docinho do chicle, e ainda o comparou com o mundo impossível da eternidade.</t>
+        </is>
+      </c>
+      <c r="M163" t="inlineStr">
+        <is>
+          <t>Muitas crianças, quando se deparam com o desconhecido, passam a fantasiar sobre ele na tentativa de entendê-lo.</t>
+        </is>
+      </c>
+      <c r="N163" t="inlineStr">
+        <is>
+          <t>Quando as crianças sonham, em serem príncipes, princesas e fadas, elas fantasiam sobre viverem felizes para sempre.</t>
+        </is>
+      </c>
+      <c r="O163" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P163" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q163" t="n">
+        <v>0</v>
+      </c>
+      <c r="R163" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
:up : ultimo commit antes de implementar a sincronização das listas suspensas com o banco de dados
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R163"/>
+  <dimension ref="A1:R176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14259,7 +14259,1067 @@
       <c r="Q163" t="n">
         <v>0</v>
       </c>
-      <c r="R163" t="inlineStr"/>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>164</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>De acordo com a norma-padrão da língua portuguesa, o emprego adequado da vírgula está plenamente atendido em:</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J164" t="inlineStr">
+        <is>
+          <t>O ensino remoto, com a pandemia de Covid-19 passou a fazer parte do processo de escolarização em todo o Brasil.</t>
+        </is>
+      </c>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>A melhor fase do ensino on-line tem sido vivida, atualmente embora permaneça a dúvida se é possível ensinar às crianças de forma remota.</t>
+        </is>
+      </c>
+      <c r="L164" t="inlineStr">
+        <is>
+          <t>Como o país não tinha experiências significativas no ensino remoto, precisou aderir à prática de forma emergencial.</t>
+        </is>
+      </c>
+      <c r="M164" t="inlineStr">
+        <is>
+          <t>A qualidade do ensino remoto era questionada, no passado porém o aprendizado conta com tecnologias que garantem ótimos resultados.</t>
+        </is>
+      </c>
+      <c r="N164" t="inlineStr">
+        <is>
+          <t>Um grande número de pesquisadores tem procurado avaliar, quais são as vantagens e desvantagens da educação a distância.</t>
+        </is>
+      </c>
+      <c r="O164" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P164" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q164" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>165</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>UNIRIO</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>Considere o trecho: “Diolino bolou então o sistema de atendimento direto aos veículos”. Caso fosse necessário reescrevê-lo empregando alguma vírgula e mantendo o sentido original, o resultado, de acordo com as normas pontuação, seria:</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J165" t="inlineStr">
+        <is>
+          <t>Diolino, bolou então o sistema de atendimento direto, aos veículos.</t>
+        </is>
+      </c>
+      <c r="K165" t="inlineStr">
+        <is>
+          <t>Diolino bolou então, o sistema, de atendimento direto aos veículos.</t>
+        </is>
+      </c>
+      <c r="L165" t="inlineStr">
+        <is>
+          <t>Diolino bolou então o sistema, de atendimento direto aos veículos.</t>
+        </is>
+      </c>
+      <c r="M165" t="inlineStr">
+        <is>
+          <t>Diolino bolou, então, o sistema de atendimento direto aos veículos.</t>
+        </is>
+      </c>
+      <c r="N165" t="inlineStr">
+        <is>
+          <t>Diolino bolou, então o sistema de atendimento direto aos veículos.</t>
+        </is>
+      </c>
+      <c r="O165" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P165" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q165" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>166</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>UNIRIO</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>A frase em que a vírgula está empregada adequadamente é:</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J166" t="inlineStr">
+        <is>
+          <t>A tela do computador, é a janela que descortina o mundo.</t>
+        </is>
+      </c>
+      <c r="K166" t="inlineStr">
+        <is>
+          <t>O investimento deve ser feito na área que, pode salvar vidas.</t>
+        </is>
+      </c>
+      <c r="L166" t="inlineStr">
+        <is>
+          <t>A vaga é para programador, que tem salário acima da média.</t>
+        </is>
+      </c>
+      <c r="M166" t="inlineStr">
+        <is>
+          <t>Concluíram, que não há mais como parar o avanço tecnológico.</t>
+        </is>
+      </c>
+      <c r="N166" t="inlineStr">
+        <is>
+          <t>É muito importante, que os investimentos na área tecnológica continuem.</t>
+        </is>
+      </c>
+      <c r="O166" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P166" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q166" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>167</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>Considere a seguinte passagem: “Dentro do amplo território portuário, os planejadores urbanos que idealizaram o Plano Porto do Rio haviam concentrado investimentos simbólicos e materiais nos arredores da praça Mauá, situada na convergência do bairro da Saúde com a avenida Rio Branco”.
+A reescritura que mantém os aspectos informacionais do trecho e respeita as normas de emprego dos sinais de pontuação é a seguinte:</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J167" t="inlineStr">
+        <is>
+          <t>Os planejadores urbanos, que idealizaram dentro do amplo território portuário o Plano Porto do Rio haviam concentrado investimentos simbólicos e materiais nos arredores da praça Mauá, situada na convergência do bairro da Saúde com a avenida Rio Branco.</t>
+        </is>
+      </c>
+      <c r="K167" t="inlineStr">
+        <is>
+          <t>Dentro do amplo território portuário, os planejadores urbanos que idealizaram o Plano Porto do Rio, haviam concentrado investimentos simbólicos e materiais nos arredores da praça Mauá, situada na convergência do bairro da Saúde com a avenida Rio Branco.</t>
+        </is>
+      </c>
+      <c r="L167" t="inlineStr">
+        <is>
+          <t>Os planejadores urbanos que idealizaram, dentro do amplo território portuário, o Plano Porto do Rio haviam concentrado, investimentos simbólicos e materiais nos arredores da praça Mauá, situada na convergência do bairro da Saúde com a avenida Rio Branco.</t>
+        </is>
+      </c>
+      <c r="M167" t="inlineStr">
+        <is>
+          <t>Os planejadores urbanos que idealizaram, dentro do amplo território portuário, o Plano Porto do Rio haviam concentrado investimentos simbólicos e materiais nos arredores da praça Mauá, situada na convergência do bairro da Saúde com a avenida Rio Branco.</t>
+        </is>
+      </c>
+      <c r="N167" t="inlineStr">
+        <is>
+          <t>Dentro do amplo, território portuário, os planejadores urbanos que idealizaram o Plano Porto do Rio haviam concentrado investimentos simbólicos e materiais nos arredores da praça Mauá situada na convergência do bairro da Saúde com a avenida Rio Branco.</t>
+        </is>
+      </c>
+      <c r="O167" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P167" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q167" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>168</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>Considere-se o emprego da primeira vírgula no trecho transcrito abaixo. “Naquele momento, quem o visse de perto perceberia o suor escorrendo frio por seu rosto”. A vírgula é empregada pelo mesmo motivo em:</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J168" t="inlineStr">
+        <is>
+          <t>A falta não foi dentro da área, mas o juiz deu pênalti.</t>
+        </is>
+      </c>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>O atacante passou pelo zagueiro, passou pelo goleiro e fez o gol.</t>
+        </is>
+      </c>
+      <c r="L168" t="inlineStr">
+        <is>
+          <t>Lúcio, atrase a bola para o goleiro!</t>
+        </is>
+      </c>
+      <c r="M168" t="inlineStr">
+        <is>
+          <t>O juiz verificou as balizas, a bola, as marcações do campo e deu início à partida.</t>
+        </is>
+      </c>
+      <c r="N168" t="inlineStr">
+        <is>
+          <t>No campo de jogo, Lúcio se sentia livre.</t>
+        </is>
+      </c>
+      <c r="O168" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P168" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q168" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>169</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>A vírgula está empregada corretamente em:</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J169" t="inlineStr">
+        <is>
+          <t>A divulgação de histórias falsas pode ter consequências reais desastrosas: prejuízos, financeiros e constrangimentos às empresas.</t>
+        </is>
+      </c>
+      <c r="K169" t="inlineStr">
+        <is>
+          <t>As novas tecnologias, criaram um abismo ao separar quem está conectado de quem não faz parte do mundo digital.</t>
+        </is>
+      </c>
+      <c r="L169" t="inlineStr">
+        <is>
+          <t>As pessoas tendem a aceitar apenas as declarações que confirmam aquilo que corresponde, às suas crenças.</t>
+        </is>
+      </c>
+      <c r="M169" t="inlineStr">
+        <is>
+          <t>Os jornalistas devem verificar as fontes citadas, cruzar dados e checar se as informações refletem a realidade.</t>
+        </is>
+      </c>
+      <c r="N169" t="inlineStr">
+        <is>
+          <t>Os consumidores de notícias não agem como cientistas porque não estão preocupados em conferir, pontos de vista alternativos.</t>
+        </is>
+      </c>
+      <c r="O169" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P169" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q169" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>170</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>A vírgula está empregada de acordo com a norma-padrão da língua portuguesa em:</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J170" t="inlineStr">
+        <is>
+          <t>A acessibilidade é a possibilidade que as pessoas, têm de atingir o destino desejado.</t>
+        </is>
+      </c>
+      <c r="K170" t="inlineStr">
+        <is>
+          <t>A mobilidade urbana tem, forte impacto, sobre o espaço e os recursos naturais.</t>
+        </is>
+      </c>
+      <c r="L170" t="inlineStr">
+        <is>
+          <t>As políticas públicas, devem priorizar os meios de transporte coletivo, nas cidades.</t>
+        </is>
+      </c>
+      <c r="M170" t="inlineStr">
+        <is>
+          <t>Como alertam os pesquisadores, é preciso discutir estratégias de mobilidade urbana.</t>
+        </is>
+      </c>
+      <c r="N170" t="inlineStr">
+        <is>
+          <t>Nos últimos anos aumentou, a insatisfação das pessoas com os engarrafamentos.</t>
+        </is>
+      </c>
+      <c r="O170" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P170" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q170" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>171</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>Considere o trecho “Num mundo em que as notícias são plantadas pela internet, em que muitos sites servem a qualquer mentira.”.
+A única reescritura que, além de conservar o conteúdo informacional, emprega os sinais de pontuação de acordo com a norma-padrão é:</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J171" t="inlineStr">
+        <is>
+          <t>Num mundo em que as notícias, são plantadas pela internet, em que muitos sites servem a qualquer mentira.</t>
+        </is>
+      </c>
+      <c r="K171" t="inlineStr">
+        <is>
+          <t>Num mundo em que muitos sites servem a qualquer mentira, em que as notícias são plantadas pela internet.</t>
+        </is>
+      </c>
+      <c r="L171" t="inlineStr">
+        <is>
+          <t>Num mundo em que, pela internet, as notícias são plantadas em que muitos sites, servem a qualquer mentira.</t>
+        </is>
+      </c>
+      <c r="M171" t="inlineStr">
+        <is>
+          <t>Num mundo, em que as notícias são plantadas pela internet em muitos sites que servem a qualquer mentira.</t>
+        </is>
+      </c>
+      <c r="N171" t="inlineStr">
+        <is>
+          <t>Num mundo em que, as notícias são plantadas pela internet e em que, muitos sites servem a qualquer mentira.</t>
+        </is>
+      </c>
+      <c r="O171" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P171" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q171" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>172</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>Observe atentamente o uso dos sinais de pontuação do trecho abaixo: “Há, de igual forma, entre os mais afortunados, aqueles ligados à indústria, voltados para a construção civil, o mobiliário, a ourivesaria e o fabrico de bebidas.” Qual das reescrituras desse trecho emprega corretamente os sinais de pontuação?</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J172" t="inlineStr">
+        <is>
+          <t>Há, entre os mais afortunados de igual forma, aqueles ligados à indústria voltados para a construção civil, o mobiliário, a ourivesaria, e o fabrico de bebidas.</t>
+        </is>
+      </c>
+      <c r="K172" t="inlineStr">
+        <is>
+          <t>De igual forma, há, entre os mais afortunados, aqueles ligados à indústria, voltados para a construção civil, o mobiliário, a ourivesaria e o fabrico de bebidas.</t>
+        </is>
+      </c>
+      <c r="L172" t="inlineStr">
+        <is>
+          <t>Entre os mais afortunados, há de igual forma, aqueles ligados à indústria, voltados para a construção civil, o mobiliário, a ourivesaria, e o fabrico de bebidas.</t>
+        </is>
+      </c>
+      <c r="M172" t="inlineStr">
+        <is>
+          <t>Há entre os mais afortunados de igual forma, aqueles ligados à indústria, voltados para a construção civil, o mobiliário, a ourivesaria e o fabrico de bebidas.</t>
+        </is>
+      </c>
+      <c r="N172" t="inlineStr">
+        <is>
+          <t>De igual forma, entre os mais afortunados, há, aqueles, ligados à indústria, voltados para a construção civil, o mobiliário, a ourivesaria e o fabrico de bebidas.</t>
+        </is>
+      </c>
+      <c r="O172" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P172" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q172" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>173</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>A vírgula está empregada corretamente em:</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J173" t="inlineStr">
+        <is>
+          <t>As grandes metrópoles que se destacaram no apoio à sustentabilidade, foram premiadas pelo mundo inteiro.</t>
+        </is>
+      </c>
+      <c r="K173" t="inlineStr">
+        <is>
+          <t>É preciso que futuramente, as cidades tenham melhores condições de vida: habitação, alimentação, saúde, emprego, transporte, educação.</t>
+        </is>
+      </c>
+      <c r="L173" t="inlineStr">
+        <is>
+          <t>Não é só o território que acelera o seu processo de urbanização, mas é a própria sociedade brasileira que se transforma cada vez mais em urbana.</t>
+        </is>
+      </c>
+      <c r="M173" t="inlineStr">
+        <is>
+          <t>Os estados que possuem os menores percentuais de população vivendo em áreas urbanas, estão concentrados nas regiões Norte e Nordeste.</t>
+        </is>
+      </c>
+      <c r="N173" t="inlineStr">
+        <is>
+          <t>Os passageiros, que dependem do transporte coletivo esperam que o futuro lhes ofereça mais comodidade do que o presente.</t>
+        </is>
+      </c>
+      <c r="O173" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P173" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q173" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>174</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>A vírgula foi plenamente empregada de acordo com as exigências da norma-padrão da língua portuguesa em:</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>Vírgula</t>
+        </is>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J174" t="inlineStr">
+        <is>
+          <t>A conexão é feita por meio de uma plataforma específica, e os conteúdos, podem ser acessados pelos dispositivos móveis dos passageiros.</t>
+        </is>
+      </c>
+      <c r="K174" t="inlineStr">
+        <is>
+          <t>O mercado brasileiro de automóveis, ainda é muito grande, porém não é capaz de absorver uma presença maior de produtos vindos do exterior.</t>
+        </is>
+      </c>
+      <c r="L174" t="inlineStr">
+        <is>
+          <t>Depois de chegarem às telas dos computadores e celulares, as notícias estarão disponíveis em voos internacionais.</t>
+        </is>
+      </c>
+      <c r="M174" t="inlineStr">
+        <is>
+          <t>Os últimos dados mostram que, muitas economias apresentam crescimento e inflação baixa, fazendo com que os juros cresçam pouco.</t>
+        </is>
+      </c>
+      <c r="N174" t="inlineStr">
+        <is>
+          <t>Pode ser que haja uma grande procura de carros importados, mas as montadoras vão fazer os cálculos e ver, se a importação vale a pena.</t>
+        </is>
+      </c>
+      <c r="O174" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P174" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q174" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>175</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>O período em que o sinal de dois pontos é empregado para introduzir uma enumeração, como no trecho que segue “demanda garantida” (parágrafo 2), é:</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>Dois</t>
+        </is>
+      </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I175" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J175" t="inlineStr">
+        <is>
+          <t>A remuneração faz parte do conjunto de ganhos de um prestador de serviço; ou seja: todos os ganhos auferidos pela pessoa compõem sua remuneração.</t>
+        </is>
+      </c>
+      <c r="K175" t="inlineStr">
+        <is>
+          <t>As horas extras, o vale-transporte e o plano de saúde podem fazer parte da remuneração: muitos trabalhadores escolhem seus empregos com base nessas vantagens.</t>
+        </is>
+      </c>
+      <c r="L175" t="inlineStr">
+        <is>
+          <t>O gerente informou aos candidatos como seria a remuneração pelos serviços: “O valor mensal vai depender de diversos itens, a serem combinados.”</t>
+        </is>
+      </c>
+      <c r="M175" t="inlineStr">
+        <is>
+          <t>Muitos itens já fizeram papel de dinheiro: o sal, usado até hoje por tribos da Etiópia, a cachaça, utilizada no Brasil colonial, e o bacalhau, antes usado na Escandinávia.</t>
+        </is>
+      </c>
+      <c r="N175" t="inlineStr">
+        <is>
+          <t>O tabaco também já foi usado como moeda de troca: no século XVIII, o estado americano de Virginia adotou esse método.</t>
+        </is>
+      </c>
+      <c r="O175" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P175" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q175" t="n">
+        <v>0</v>
+      </c>
+      <c r="R175" t="inlineStr">
+        <is>
+          <t>6833f320-6441-4318-89ab-c90bb9f149e6.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>176</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>Em “Posso intensamente desejar que o problema mais urgente se resolva: o da fome.", os dois-pontos cumprem o papel de introduzir uma</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>Dois</t>
+        </is>
+      </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I176" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J176" t="inlineStr">
+        <is>
+          <t>enumeração</t>
+        </is>
+      </c>
+      <c r="K176" t="inlineStr">
+        <is>
+          <t>explanação</t>
+        </is>
+      </c>
+      <c r="L176" t="inlineStr">
+        <is>
+          <t>retificação</t>
+        </is>
+      </c>
+      <c r="M176" t="inlineStr">
+        <is>
+          <t>especificação</t>
+        </is>
+      </c>
+      <c r="N176" t="inlineStr">
+        <is>
+          <t>contradição.</t>
+        </is>
+      </c>
+      <c r="O176" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P176" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q176" t="n">
+        <v>0</v>
+      </c>
+      <c r="R176" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
:up: mudadas alguns dados no db
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -514,21 +514,25 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cesgranrio</t>
+          <t>CESGRANRIO</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Banco da Amazônia</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>2021</v>
+          <t>BANCO DA AMAZÔNIA</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -595,12 +599,14 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Cesgranrio</t>
+          <t>CESGRANRIO</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -608,8 +614,10 @@
           <t>UNIRIO</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>2019</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -675,12 +683,14 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cesgranrio</t>
+          <t>CESGRANRIO</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -688,8 +698,10 @@
           <t>Liquigás</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>2018</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -754,12 +766,14 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cesgranrio</t>
+          <t>CESGRANRIO</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -767,8 +781,10 @@
           <t>Transpetro</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>2018</v>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -833,12 +849,14 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Cesgranrio</t>
+          <t>CESGRANRIO</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -846,8 +864,10 @@
           <t>IBGE</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>2016</v>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -912,12 +932,14 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cesgranrio</t>
+          <t>CESGRANRIO</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -925,8 +947,10 @@
           <t>UNIRIO</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>2016</v>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -991,12 +1015,14 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Cesgranrio</t>
+          <t>CESGRANRIO</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1004,8 +1030,10 @@
           <t>ANP</t>
         </is>
       </c>
-      <c r="D8" t="n">
-        <v>2016</v>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1070,12 +1098,14 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cesgranrio</t>
+          <t>CESGRANRIO</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1083,8 +1113,10 @@
           <t>ANP</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>2016</v>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1149,12 +1181,14 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Cesgranrio</t>
+          <t>CESGRANRIO</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1162,8 +1196,10 @@
           <t>Petrobras</t>
         </is>
       </c>
-      <c r="D10" t="n">
-        <v>2015</v>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1228,12 +1264,14 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Cesgranrio</t>
+          <t>CESGRANRIO</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1241,8 +1279,10 @@
           <t>Liquigás</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>2014</v>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1307,12 +1347,14 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Cesgranrio</t>
+          <t>CESGRANRIO</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1320,8 +1362,10 @@
           <t>UNIRIO</t>
         </is>
       </c>
-      <c r="D12" t="n">
-        <v>2019</v>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1386,12 +1430,14 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Cesgranrio</t>
+          <t>CESGRANRIO</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1399,8 +1445,10 @@
           <t>Liquigás</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>2018</v>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1465,12 +1513,14 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Cesgranrio</t>
+          <t>CESGRANRIO</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1478,8 +1528,10 @@
           <t>Liquigás</t>
         </is>
       </c>
-      <c r="D14" t="n">
-        <v>2014</v>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1544,21 +1596,25 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Cesgranrio</t>
+          <t>CESGRANRIO</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Liquigás</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>2018</v>
+          <t>LIQUIGÁS</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -15319,7 +15375,6 @@
       <c r="Q176" t="n">
         <v>0</v>
       </c>
-      <c r="R176" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
:release :up: listas integradas com o db finalizadas
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -6152,8 +6152,10 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="n">
-        <v>67</v>
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -6162,7 +6164,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>LIQUIGÁS DISTRIBUIDORA S. A</t>
+          <t>LIQUIGÁS</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -6233,8 +6235,10 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="n">
-        <v>68</v>
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -6243,7 +6247,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>PETRÓLEO BRASILEIRO S. A</t>
+          <t>PETROBRAS</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -9821,8 +9825,10 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="n">
-        <v>111</v>
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
@@ -9831,7 +9837,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>TRANSPETRO / SEGUN. OFICIAL</t>
+          <t>TRANSPETRO</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -11402,8 +11408,10 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" t="n">
-        <v>130</v>
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
@@ -11412,7 +11420,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Petrobrás</t>
+          <t>PETROBRAS</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -11565,8 +11573,10 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" t="n">
-        <v>132</v>
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>132</t>
+        </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
@@ -11575,7 +11585,7 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Nível Superior</t>
+          <t>BNDES</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -12697,8 +12707,10 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" t="n">
-        <v>145</v>
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>145</t>
+        </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
@@ -12707,7 +12719,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Téc. de Enfermagem</t>
+          <t>PETROBRAS</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -12859,8 +12871,10 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" t="n">
-        <v>147</v>
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
@@ -12869,7 +12883,7 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Petrobrás</t>
+          <t>PETROBRAS</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -13547,8 +13561,10 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" t="n">
-        <v>155</v>
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
@@ -13557,7 +13573,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Esc BB</t>
+          <t>BANCO DO BRASIL</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -13641,8 +13657,10 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" t="n">
-        <v>156</v>
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>156</t>
+        </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
@@ -13651,7 +13669,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Esc BB</t>
+          <t>BANCO DO BRASIL</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -15210,8 +15228,10 @@
       </c>
     </row>
     <row r="175">
-      <c r="A175" t="n">
-        <v>175</v>
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>175</t>
+        </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
@@ -15240,7 +15260,7 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>Dois</t>
+          <t>Dois-Pontos</t>
         </is>
       </c>
       <c r="H175" t="inlineStr">
@@ -15296,8 +15316,10 @@
       </c>
     </row>
     <row r="176">
-      <c r="A176" t="n">
-        <v>176</v>
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>176</t>
+        </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
@@ -15326,7 +15348,7 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>Dois</t>
+          <t>Dois-Pontos</t>
         </is>
       </c>
       <c r="H176" t="inlineStr">

</xml_diff>

<commit_message>
:up: ultimo commit antes de tentar resolver bug qu fica voltando o site para a pagina inicial
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R176"/>
+  <dimension ref="A1:R178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15398,6 +15398,170 @@
         <v>0</v>
       </c>
     </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>177</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>Os sinais de pontuação contribuem para a construção dos sentidos dos textos. No fragmento “Escriturei-me; deram-me um papel que... mas para que o estou a fatigar com isso? Deixe-me ficar com as minhas amofinações”, as reticências são usadas para demarcar a</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>Reticências</t>
+        </is>
+      </c>
+      <c r="H177" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I177" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J177" t="inlineStr">
+        <is>
+          <t>interrupção de uma ideia.</t>
+        </is>
+      </c>
+      <c r="K177" t="inlineStr">
+        <is>
+          <t>insinuação de uma ameaça.</t>
+        </is>
+      </c>
+      <c r="L177" t="inlineStr">
+        <is>
+          <t>hesitação comum na oralidade.</t>
+        </is>
+      </c>
+      <c r="M177" t="inlineStr">
+        <is>
+          <t>continuidade de uma ação ou fato.</t>
+        </is>
+      </c>
+      <c r="N177" t="inlineStr">
+        <is>
+          <t>omissão proposital de algo que se devia dizer.</t>
+        </is>
+      </c>
+      <c r="O177" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P177" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q177" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>178</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>As reticências utilizadas pelo autor no trecho “desabotoava a blusa até o estômago, enfiava a mão dentro dela e puxava para fora um seio lindo, liso, branco, aquele mamilo atrevido... E nós, meninos, de boca aberta...” assinalam uma determinada sensação.
+O trecho em que semelhante sensação se verifica é:</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>Reticências</t>
+        </is>
+      </c>
+      <c r="H178" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I178" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J178" t="inlineStr">
+        <is>
+          <t>“Se estou com fome e gosto de queijo, eu como queijo...”</t>
+        </is>
+      </c>
+      <c r="K178" t="inlineStr">
+        <is>
+          <t>“Procuro outra coisa de que goste: banana, pão com manteiga, chocolate...”</t>
+        </is>
+      </c>
+      <c r="L178" t="inlineStr">
+        <is>
+          <t>“Enquanto varria e limpava, sofria ouvindo o pianista tocando uma música horrível: Bach, Brahms, Debussy...”</t>
+        </is>
+      </c>
+      <c r="M178" t="inlineStr">
+        <is>
+          <t>“Mas eu comprava um mata-fome e ia para casa comendo o mata-fome bem devagarzinho...”</t>
+        </is>
+      </c>
+      <c r="N178" t="inlineStr">
+        <is>
+          <t>“Ridendo dicere severum: rindo, dizer as coisas sérias...”</t>
+        </is>
+      </c>
+      <c r="O178" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P178" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q178" t="n">
+        <v>0</v>
+      </c>
+      <c r="R178" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
:lady_beetle: bug de ficar voltando a pagina inicial corrigido
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R178"/>
+  <dimension ref="A1:R179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15560,7 +15560,88 @@
       <c r="Q178" t="n">
         <v>0</v>
       </c>
-      <c r="R178" t="inlineStr"/>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>179</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>BANCO DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>O uso de sinais (aspas e travessão) está adequado à norma-padrão, que deve ser observada em uma correspondência oficial, na seguinte frase:</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>Aspas</t>
+        </is>
+      </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I179" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J179" t="inlineStr">
+        <is>
+          <t>O artigo sobre o “processo de desregulamentação</t>
+        </is>
+      </c>
+      <c r="K179" t="inlineStr">
+        <is>
+          <t>As chuvas de verão — fenômenos que se repetem desde há muito tempo podem ser previstas.</t>
+        </is>
+      </c>
+      <c r="L179" t="inlineStr">
+        <is>
+          <t>“Mutatis mutandis</t>
+        </is>
+      </c>
+      <c r="M179" t="inlineStr">
+        <is>
+          <t>O cuidado com a saúde — meta prioritária do governo, será ainda maior.</t>
+        </is>
+      </c>
+      <c r="N179" t="inlineStr">
+        <is>
+          <t>— O diretor disse: Demita-se o funcionário.</t>
+        </is>
+      </c>
+      <c r="O179" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P179" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q179" t="n">
+        <v>0</v>
+      </c>
+      <c r="R179" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
:lady_beetl: consertado layout quebrado nas alternativas
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -9657,10 +9657,10 @@
         </is>
       </c>
       <c r="P108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
@@ -16136,10 +16136,10 @@
         </is>
       </c>
       <c r="P185" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q185" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186">

</xml_diff>

<commit_message>
:lady_beetle: ultimo commit antes de tentar corrigir quebra de paragrafo nao aparecendo
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -676,10 +676,10 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -4509,10 +4509,10 @@
         </is>
       </c>
       <c r="P50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -11568,7 +11568,7 @@
         </is>
       </c>
       <c r="P131" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q131" t="n">
         <v>0</v>
@@ -14817,10 +14817,10 @@
         </is>
       </c>
       <c r="P169" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q169" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170">

</xml_diff>

<commit_message>
:lady_beetle: correção de falha de captura de ano feita
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -5047,10 +5047,10 @@
         </is>
       </c>
       <c r="P56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -10409,7 +10409,7 @@
         </is>
       </c>
       <c r="P117" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q117" t="n">
         <v>0</v>
@@ -14907,10 +14907,10 @@
         </is>
       </c>
       <c r="P170" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q170" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171">
@@ -15070,7 +15070,7 @@
         </is>
       </c>
       <c r="P172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q172" t="n">
         <v>0</v>
@@ -15403,10 +15403,10 @@
         </is>
       </c>
       <c r="P176" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q176" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177">
@@ -15484,7 +15484,7 @@
         </is>
       </c>
       <c r="P177" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q177" t="n">
         <v>0</v>
@@ -16226,10 +16226,10 @@
         </is>
       </c>
       <c r="P186" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q186" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187">
@@ -18924,7 +18924,7 @@
         </is>
       </c>
       <c r="P218" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q218" t="n">
         <v>0</v>
@@ -23506,10 +23506,10 @@
         </is>
       </c>
       <c r="P272" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q272" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="273">
@@ -23587,10 +23587,10 @@
         </is>
       </c>
       <c r="P273" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q273" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R273" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
:release: códigos do frontend separados
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -1751,7 +1751,7 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q16" t="n">
         <v>0</v>
@@ -5985,10 +5985,10 @@
         </is>
       </c>
       <c r="P64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -6476,10 +6476,10 @@
         </is>
       </c>
       <c r="P70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -8262,10 +8262,10 @@
         </is>
       </c>
       <c r="P91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -8586,10 +8586,10 @@
         </is>
       </c>
       <c r="P95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -9993,7 +9993,7 @@
         </is>
       </c>
       <c r="P112" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q112" t="n">
         <v>0</v>
@@ -12018,10 +12018,10 @@
         </is>
       </c>
       <c r="P136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137">
@@ -15484,10 +15484,10 @@
         </is>
       </c>
       <c r="P177" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q177" t="n">
         <v>1</v>
-      </c>
-      <c r="Q177" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="178">
@@ -15813,7 +15813,7 @@
         </is>
       </c>
       <c r="P181" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q181" t="n">
         <v>0</v>
@@ -16501,10 +16501,10 @@
         </is>
       </c>
       <c r="P189" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q189" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190">
@@ -22701,8 +22701,10 @@
       </c>
     </row>
     <row r="264">
-      <c r="A264" t="n">
-        <v>264</v>
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>264</t>
+        </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
@@ -22731,7 +22733,7 @@
 Isso porque deepfakes criadas para serem distribuídas por appsde mensagens não exigem tanta qualidade. O perigo é que, para o cidadão comum, a deepfake pode ser o ponto de partida para uma fraude financeira, entre outros problemas.
 A recomendação para pessoas físicas se protegerem é diminuir a exposição de fotos com rostos e vídeos pessoais na internet. “As redes sociais devem se manter configuradas como privadas, já que fotos, áudios ou vídeos disponíveis publicamente podem ser utilizados para alimentar a inteligência artificial e engendrardeepfakes.” Além disso, ao receber um vídeo suspeito, observe se o rosto e os lábios da pessoa se movem em conjunto com o que ela diz. Preste atenção se a fala parece contínua ou se em algum momento apresenta cortes entre uma palavra e outra. E considere o contexto — ainda que tecnicamente o vídeo esteja muito bem manipulado, avalie se faz sentido que aquela pessoa diga o que parece dizer naquele momento.
 (Disponívelem:https://estudio.folha.uol.com.br/unico.Acessoem:20out.2022.Adaptado)
-No trecho “alimentar a inteligência artificial e engendrar deepfakes”, a palavra destacada pode ser substituída, sem prejuízo do sentido do texto, por</t>
+No trecho “alimentar a inteligência artificial e &lt;u&gt;engendrar&lt;/u&gt; deepfakes”, a palavra destacada pode ser substituída, sem prejuízo do sentido do texto, por</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">

</xml_diff>

<commit_message>
:up: todas as questoes do pdf 2 de CE cadastradas
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R378"/>
+  <dimension ref="A1:R406"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -32568,8 +32568,10 @@
       </c>
     </row>
     <row r="377">
-      <c r="A377" t="n">
-        <v>377</v>
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>377</t>
+        </is>
       </c>
       <c r="B377" t="inlineStr">
         <is>
@@ -32635,7 +32637,7 @@
       <c r="N377" t="inlineStr"/>
       <c r="O377" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="P377" t="n">
@@ -32651,8 +32653,10 @@
       </c>
     </row>
     <row r="378">
-      <c r="A378" t="n">
-        <v>378</v>
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>378</t>
+        </is>
       </c>
       <c r="B378" t="inlineStr">
         <is>
@@ -32717,16 +32721,2227 @@
       <c r="N378" t="inlineStr"/>
       <c r="O378" t="inlineStr">
         <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P378" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q378" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="n">
+        <v>379</v>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Banca D</t>
+        </is>
+      </c>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E379" t="inlineStr">
+        <is>
+          <t>Em relação a critérios qualificadores de pedidos e critérios ganhadores de pedidos, julgue o item abaixo.
+Em serviços especializados preço pode ser considerado um critério qualificador de pedido e rapidez um critério ganhador de pedidos.</t>
+        </is>
+      </c>
+      <c r="F379" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G379" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H379" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I379" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J379" t="inlineStr"/>
+      <c r="K379" t="inlineStr"/>
+      <c r="L379" t="inlineStr"/>
+      <c r="M379" t="inlineStr"/>
+      <c r="N379" t="inlineStr"/>
+      <c r="O379" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P379" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q379" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="n">
+        <v>380</v>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>2009</t>
+        </is>
+      </c>
+      <c r="E380" t="inlineStr">
+        <is>
+          <t>No nível estratégico, os objetivos de desempenho podem se relacionar e materializar os interesses dos stakeholders das operações. Os cinco objetivos de desempenho são: custo, confiabilidade, flexibilidade, qualidade e rapidez.
+Nesse sentido, é correto afirmar que</t>
+        </is>
+      </c>
+      <c r="F380" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G380" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H380" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I380" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J380" t="inlineStr">
+        <is>
+          <t>a qualidade é o grau de certeza de que os produtos oferecidos cumprirão suas funções conforme estabelecido.</t>
+        </is>
+      </c>
+      <c r="K380" t="inlineStr">
+        <is>
+          <t>a representação polar é muito útil em planejamentos estratégicos que solicitam análises comparativas considerando os objetivos de desempenho.</t>
+        </is>
+      </c>
+      <c r="L380" t="inlineStr">
+        <is>
+          <t>a produção confirma a flexibilidade dos bens e dos serviços oferecidos pela instituição, ao fornecer produtos isentos de erros e dentro das especificações.</t>
+        </is>
+      </c>
+      <c r="M380" t="inlineStr">
+        <is>
+          <t>um incremento em qualquer dos objetivos de desempenho, normalmente, implica uma redução dos custos de produção e de operações.</t>
+        </is>
+      </c>
+      <c r="N380" t="inlineStr">
+        <is>
+          <t>rapidez é a capacidade de adaptar os bens e os serviços oferecidos a uma gama de necessidades diferentes.</t>
+        </is>
+      </c>
+      <c r="O380" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P380" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q380" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="n">
+        <v>381</v>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="E381" t="inlineStr">
+        <is>
+          <t>Sistemas de Produção podem ser definidos como conjuntos de pessoas, equipamentos e procedimentos organizados para a realização de operações de manufatura ou serviços em uma empresa. Os principais Sistemas de Produção em manufatura são:</t>
+        </is>
+      </c>
+      <c r="F381" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G381" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H381" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I381" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J381" t="inlineStr">
+        <is>
+          <t>Sistema de Produção em Massa - Sistema de Produção de Posição Fixa</t>
+        </is>
+      </c>
+      <c r="K381" t="inlineStr">
+        <is>
+          <t>Sistema de Produção por Lotes ou Encomendas - Sistema de Produção de Serviços Funcionais</t>
+        </is>
+      </c>
+      <c r="L381" t="inlineStr">
+        <is>
+          <t>Sistema de Produção em Massa - Sistema de Produção de Posição Fixa - Sistema de Produção para Pequenas Quantidades</t>
+        </is>
+      </c>
+      <c r="M381" t="inlineStr">
+        <is>
+          <t>Sistema de Produção por Lotes ou Encomendas - Sistema de Produção em Massa - Sistema de Produção para Médios ou Pequenos Projetos</t>
+        </is>
+      </c>
+      <c r="N381" t="inlineStr">
+        <is>
+          <t>Sistema de Produção para Grandes Projetos - Sistema de Produção por Lotes ou Encomendas Sistema de Produção em Massa</t>
+        </is>
+      </c>
+      <c r="O381" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P381" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q381" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="n">
+        <v>382</v>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>FGV</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>Câmara de Salvador</t>
+        </is>
+      </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E382" t="inlineStr">
+        <is>
+          <t>A definição de estoque pode ser dada como a acumulação armazenada de materiais em um sistema de transformação. Um dos métodos para a sua reposição é o de previsão de demanda.
+A técnica de previsão de demanda realizada por meio de informações qualitativas é definida como:</t>
+        </is>
+      </c>
+      <c r="F382" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G382" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H382" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I382" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J382" t="inlineStr">
+        <is>
+          <t>Explicação</t>
+        </is>
+      </c>
+      <c r="K382" t="inlineStr">
+        <is>
+          <t>Predileção</t>
+        </is>
+      </c>
+      <c r="L382" t="inlineStr">
+        <is>
+          <t>Projeção</t>
+        </is>
+      </c>
+      <c r="M382" t="inlineStr">
+        <is>
+          <t>Ponderação</t>
+        </is>
+      </c>
+      <c r="N382" t="inlineStr">
+        <is>
+          <t>Mínimos Quadrados</t>
+        </is>
+      </c>
+      <c r="O382" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P382" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q382" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="n">
+        <v>383</v>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>INSTITUTO AOCP</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>EBSERH</t>
+        </is>
+      </c>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="E383" t="inlineStr">
+        <is>
+          <t>Assinale a alternativa que apresenta grupos de técnicas de previsão do consumo, tendo em vista a determinação dos níveis de estoques de materiais.</t>
+        </is>
+      </c>
+      <c r="F383" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G383" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H383" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I383" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J383" t="inlineStr">
+        <is>
+          <t>Aleatoriedade, racionalização e ativação.</t>
+        </is>
+      </c>
+      <c r="K383" t="inlineStr">
+        <is>
+          <t>Evolução, exponenciação e potenciação.</t>
+        </is>
+      </c>
+      <c r="L383" t="inlineStr">
+        <is>
+          <t>Projeção, explicação e predileção.</t>
+        </is>
+      </c>
+      <c r="M383" t="inlineStr">
+        <is>
+          <t>Combinação, arranjo e validação.</t>
+        </is>
+      </c>
+      <c r="N383" t="inlineStr">
+        <is>
+          <t>Confirmação, comparação e modelação.</t>
+        </is>
+      </c>
+      <c r="O383" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P383" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q383" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="n">
+        <v>384</v>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>UFES</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>UFES</t>
+        </is>
+      </c>
+      <c r="D384" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="E384" t="inlineStr">
+        <is>
+          <t>De acordo com a bibliografia do concurso, as técnicas de previsão de consumo podem ser classificadas em projeção, explicação e predileção. Sobre as técnicas é INCORRETO afirmar:</t>
+        </is>
+      </c>
+      <c r="F384" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G384" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H384" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I384" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J384" t="inlineStr">
+        <is>
+          <t>Na projeção, a base de cálculo utilizada é de natureza essencialmente quantitativa.</t>
+        </is>
+      </c>
+      <c r="K384" t="inlineStr">
+        <is>
+          <t>Na projeção, admite-se que as vendas evoluirão no tempo futuro da mesma forma que ocorreram no passado.</t>
+        </is>
+      </c>
+      <c r="L384" t="inlineStr">
+        <is>
+          <t>Na explicação, procura-se compreender as vendas do passado mediante leis que relacionem essas vendas com outras variáveis cuja evolução é conhecida ou previsível.</t>
+        </is>
+      </c>
+      <c r="M384" t="inlineStr">
+        <is>
+          <t>Na explicação, são utilizadas basicamente as técnicas de regressão e correlação.</t>
+        </is>
+      </c>
+      <c r="N384" t="inlineStr">
+        <is>
+          <t>Na predileção, os funcionários do setor estabelecem a evolução das vendas futuras com base na sua preferência pelos produtos.</t>
+        </is>
+      </c>
+      <c r="O384" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P384" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q384" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="n">
+        <v>385</v>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Consulplan</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>Prefeitura de Cascavel</t>
+        </is>
+      </c>
+      <c r="D385" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E385" t="inlineStr">
+        <is>
+          <t>O que é o método Delphi ?</t>
+        </is>
+      </c>
+      <c r="F385" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G385" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H385" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I385" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J385" t="inlineStr">
+        <is>
+          <t>Método através do qual o pesquisador capta a realidade observada. Vários tipos de profissionais, entre eles o médico, o psicólogo e o publicitário, apesar de normalmente utilizarem uma diversidade de métodos de coleta de informação, fazem uso frequente deste método.</t>
+        </is>
+      </c>
+      <c r="K385" t="inlineStr">
+        <is>
+          <t>Método de pesquisa das ciências sociais que pode ser descrito como a obtenção de dados ou informações sobre características, ações ou opiniões de determinado grupo de pessoas, indicado como representante de uma população-alvo, por meio de um instrumento de pesquisa, que pode ser um questionário.</t>
+        </is>
+      </c>
+      <c r="L385" t="inlineStr">
+        <is>
+          <t>Método que coleta dados sobre estudos de usuários sem interrogá-los ou observá-los de uma forma direta. Nesse método, os dados são coletados através de documentos já existentes, como estatísticas de bibliotecas, referência de obras citadas, anotações, textos etc. É utilizado em estudo de usuários.</t>
+        </is>
+      </c>
+      <c r="M385" t="inlineStr">
+        <is>
+          <t>Método que faz uso do questionário para obter um consenso sobre determinado assunto sendo sua principal área de aplicação a de previsão tecnológica; consiste em uma sucessão de rounds em que são colhidas as opiniões de um grupo de especialistas, para levantar seus conhecimentos e capacidade de julgamento.</t>
+        </is>
+      </c>
+      <c r="N385" t="inlineStr">
+        <is>
+          <t>Método para mapear necessidade de informação sob a ótica do usuário; consiste em pontuações de premissas teóricas e conceituais e outras metodologias relacionadas, para avaliar como audiências, usuários, clientes e cidadãos percebem, compreendem e sentem suas interações com instituições, mídias, mensagens e como usam a informação e outros recursos nesse processo.</t>
+        </is>
+      </c>
+      <c r="O385" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P385" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q385" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="n">
+        <v>386</v>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D386" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="E386" t="inlineStr">
+        <is>
+          <t>Com base nos sistemas de previsão qualitativa e quantitativa se estabelecem políticas de controle para sistemas de estoques. Os sistemas podem ser alimentados por dados históricos e experiência gerencial. Também é necessário definir a periodicidade com que o modelo de decisão será revisto e atualizado.
+O modelo quantitativo que se apoia nos componentes tendência, ciclicidade e aleatoriedade é o(a)</t>
+        </is>
+      </c>
+      <c r="F386" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G386" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H386" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I386" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J386" t="inlineStr">
+        <is>
+          <t>Delphi</t>
+        </is>
+      </c>
+      <c r="K386" t="inlineStr">
+        <is>
+          <t>mini-delphi</t>
+        </is>
+      </c>
+      <c r="L386" t="inlineStr">
+        <is>
+          <t>de analogia histórica</t>
+        </is>
+      </c>
+      <c r="M386" t="inlineStr">
+        <is>
+          <t>de séries temporais</t>
+        </is>
+      </c>
+      <c r="N386" t="inlineStr">
+        <is>
+          <t>de suavização exponencial.</t>
+        </is>
+      </c>
+      <c r="O386" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P386" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q386" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="n">
+        <v>387</v>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D387" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="E387" t="inlineStr">
+        <is>
+          <t>O consumo de determinado item de estoque foi acompanhado durante 6 meses, de acordo com a tabela a seguir.
+Para prever a demanda do sétimo mês, o analista decidiu usar, isoladamente, 3 métodos:
+1 - média móvel simples para 4 períodos;
+2 - média móvel simples para 3 períodos; e
+3 - média móvel ponderada para 3 períodos, assumindo-se os pesos 0,5 para o período mais recente, 0,3 para o período anterior e 0,2 para o período restante.
+Se a demanda real do sétimo mês foi 200 unidades conclui-se que o</t>
+        </is>
+      </c>
+      <c r="F387" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G387" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H387" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I387" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J387" t="inlineStr">
+        <is>
+          <t>método 1 forneceu uma previsão com menor erro absoluto que o método 2.</t>
+        </is>
+      </c>
+      <c r="K387" t="inlineStr">
+        <is>
+          <t>método 2 forneceu uma previsão com menor erro absoluto que o método 3.</t>
+        </is>
+      </c>
+      <c r="L387" t="inlineStr">
+        <is>
+          <t>maior erro absoluto foi obtido pelo método 2.</t>
+        </is>
+      </c>
+      <c r="M387" t="inlineStr">
+        <is>
+          <t>menor erro absoluto foi obtido pelo método 1.</t>
+        </is>
+      </c>
+      <c r="N387" t="inlineStr">
+        <is>
+          <t>menor erro absoluto foi obtido pelo método 3.</t>
+        </is>
+      </c>
+      <c r="O387" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P387" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q387" t="n">
+        <v>0</v>
+      </c>
+      <c r="R387" t="inlineStr">
+        <is>
+          <t>b1fe8b00-ecc9-4526-8ad9-bdebf18127fe.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="n">
+        <v>388</v>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Cespe</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>STF</t>
+        </is>
+      </c>
+      <c r="D388" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="E388" t="inlineStr">
+        <is>
+          <t>Considerando que os estoques de uma organização, pública ou privada, devem ser bem administrados, pois o desperdício de recursos onera os resultados da organização, julgue os itens seguintes.
+A média com suavização exponencial é uma técnica para previsão de demanda de curto prazo adaptável, ou seja, se autocorrige de acordo com as alterações no comportamento das vendas.</t>
+        </is>
+      </c>
+      <c r="F388" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G388" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H388" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I388" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J388" t="inlineStr"/>
+      <c r="K388" t="inlineStr"/>
+      <c r="L388" t="inlineStr"/>
+      <c r="M388" t="inlineStr"/>
+      <c r="N388" t="inlineStr"/>
+      <c r="O388" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P388" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q388" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="n">
+        <v>389</v>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Quadrix</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>CREF 11ª Região</t>
+        </is>
+      </c>
+      <c r="D389" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E389" t="inlineStr">
+        <is>
+          <t>A partir dos dados apresentados na tabela acima, julgue o item.
+Suponha‐se que, por meio do método da média móvel exponencialmente ponderada, a previsão para o mês de março/2019 tenha sido de 35 unidades e o coeficiente de ajuste igual a 0,2. Nesse caso, a previsão para o mês de abril/2019, por meio do método da média móvel exponencialmente ponderada, será de 33 unidades.</t>
+        </is>
+      </c>
+      <c r="F389" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G389" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H389" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I389" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J389" t="inlineStr"/>
+      <c r="K389" t="inlineStr"/>
+      <c r="L389" t="inlineStr"/>
+      <c r="M389" t="inlineStr"/>
+      <c r="N389" t="inlineStr"/>
+      <c r="O389" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P389" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q389" t="n">
+        <v>0</v>
+      </c>
+      <c r="R389" t="inlineStr">
+        <is>
+          <t>76485393-72dc-480a-b64a-0ac98b1884f6.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="n">
+        <v>390</v>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>Hemobrás</t>
+        </is>
+      </c>
+      <c r="D390" t="inlineStr">
+        <is>
+          <t>2008</t>
+        </is>
+      </c>
+      <c r="E390" t="inlineStr">
+        <is>
+          <t>Considerando que a direção de um hospital decida aumentar a capacidade em 500 pacientes por dia, julgue os itens que se seguem, relativos ao planejamento e controle dessa situação.
+O planejamento e controle de capacidade é a tarefa de determinar a capacidade efetiva da operação produtiva necessária para que possa responder à demanda.</t>
+        </is>
+      </c>
+      <c r="F390" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G390" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H390" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I390" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J390" t="inlineStr"/>
+      <c r="K390" t="inlineStr"/>
+      <c r="L390" t="inlineStr"/>
+      <c r="M390" t="inlineStr"/>
+      <c r="N390" t="inlineStr"/>
+      <c r="O390" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P390" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q390" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>391</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Banca D</t>
+        </is>
+      </c>
+      <c r="D391" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E391" t="inlineStr">
+        <is>
+          <t>Considerando os tipos de capacidades produtivas marque a alternativa correta</t>
+        </is>
+      </c>
+      <c r="F391" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G391" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H391" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I391" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J391" t="inlineStr">
+        <is>
+          <t>A capacidade produtiva instalada diária e a capacidade produtiva disponível diária podem ser alcançadas apenas multiplicando a quantidade de itens produzidos por hora e depois multiplicar o valor encontrado por 24h.</t>
+        </is>
+      </c>
+      <c r="K391" t="inlineStr">
+        <is>
+          <t>A melhor forma de alinhar a capacidade produtiva à demanda é encontrando a capacidade produtiva disponível.</t>
+        </is>
+      </c>
+      <c r="L391" t="inlineStr">
+        <is>
+          <t>Considerando que uma empresa tenha uma capacidade produtiva efetiva de 90 mesas por dia, que tem horário de trabalho das 08:00 às 17:00 e que as paradas programadas no planejamento correspondem a 10% do tempo total disponível, a capacidade produtiva disponível é de 100 mesas por dia.</t>
+        </is>
+      </c>
+      <c r="M391" t="inlineStr">
+        <is>
+          <t>A capacidade produtiva efetiva leva em consideração paradas não planejadas como falta de energia ou quebra de equipamentos.</t>
+        </is>
+      </c>
+      <c r="N391" t="inlineStr">
+        <is>
+          <t>A capacidade produtiva realizada diária é medida calculando o total de itens produzidos por hora e depois multiplicando o resultado por 24h.</t>
+        </is>
+      </c>
+      <c r="O391" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P391" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q391" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="n">
+        <v>392</v>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>PREFEITURA DO RJ</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>PREFEITURA DO RJ</t>
+        </is>
+      </c>
+      <c r="D392" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E392" t="inlineStr">
+        <is>
+          <t>O sistema de planejamento de necessidades de materiais que trabalha com um conjunto de informações básicas, tais como o plano mestre de produção, a estrutura do produto com base em uma lista de materiais e a situação geral dos estoques dos itens, é o conhecido como:</t>
+        </is>
+      </c>
+      <c r="F392" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G392" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H392" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I392" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J392" t="inlineStr">
+        <is>
+          <t>ERP</t>
+        </is>
+      </c>
+      <c r="K392" t="inlineStr">
+        <is>
+          <t>JIT</t>
+        </is>
+      </c>
+      <c r="L392" t="inlineStr">
+        <is>
+          <t>CRP</t>
+        </is>
+      </c>
+      <c r="M392" t="inlineStr">
+        <is>
+          <t>MRP</t>
+        </is>
+      </c>
+      <c r="N392" t="inlineStr"/>
+      <c r="O392" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P392" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q392" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="n">
+        <v>393</v>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D393" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E393" t="inlineStr">
+        <is>
+          <t>MRP I e MRP II são insumos importantes para a área de logística ao fornecerem algumas informações. O impacto dessas informações está mais relacionado com a área de:</t>
+        </is>
+      </c>
+      <c r="F393" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G393" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H393" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I393" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J393" t="inlineStr">
+        <is>
+          <t>Embalagem</t>
+        </is>
+      </c>
+      <c r="K393" t="inlineStr">
+        <is>
+          <t>Gestão do estoque</t>
+        </is>
+      </c>
+      <c r="L393" t="inlineStr">
+        <is>
+          <t>Gestão da frota</t>
+        </is>
+      </c>
+      <c r="M393" t="inlineStr">
+        <is>
+          <t>Manuseio de materiais</t>
+        </is>
+      </c>
+      <c r="N393" t="inlineStr">
+        <is>
+          <t>Picking</t>
+        </is>
+      </c>
+      <c r="O393" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P393" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q393" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>394</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>FUNDEP</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>IFSP</t>
+        </is>
+      </c>
+      <c r="D394" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E394" t="inlineStr">
+        <is>
+          <t>Como incremento produtivo, a empresa Mega está implantando um sistema de Planejamento de Necessidades de Materiais (MRP). Sobre o MRP, assinale a alternativa CORRETA.</t>
+        </is>
+      </c>
+      <c r="F394" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G394" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H394" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I394" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J394" t="inlineStr">
+        <is>
+          <t>É o resultado de ações coordenadas de compartilhamento de informações de produtividade entre a gerência de materiais e a gerência financeira.</t>
+        </is>
+      </c>
+      <c r="K394" t="inlineStr">
+        <is>
+          <t>É um programa de operações com dados sobre tempo/máquina, custos, homem hora e consumo de materiais, para perfazimento de quantidades finais.</t>
+        </is>
+      </c>
+      <c r="L394" t="inlineStr">
+        <is>
+          <t>É uma rotina de escalas produtivas com redução dos tempos Inter processos e aumento dos lead times internos em função de uma redução de custos.</t>
+        </is>
+      </c>
+      <c r="M394" t="inlineStr">
+        <is>
+          <t>É um processo de definição de escalas de produção voltadas para minimização de estoques internos e favorecimento de um Just in time.</t>
+        </is>
+      </c>
+      <c r="N394" t="inlineStr"/>
+      <c r="O394" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P394" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q394" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="n">
+        <v>395</v>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D395" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E395" t="inlineStr">
+        <is>
+          <t>O planejamento agregado é parte integrante do processo de planejamento e controle da produção. Planejar determina o que se pretende que aconteça em algum momento no futuro. Controlar é o processo de se ajustar quando os fatos não acontecem como o esperado.
+Qual dos seguintes fatores difere por ocasião do estabelecimento do planejamento agregado em um serviço e em uma manufatura?</t>
+        </is>
+      </c>
+      <c r="F395" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G395" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H395" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I395" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J395" t="inlineStr">
+        <is>
+          <t>Incerteza na demanda</t>
+        </is>
+      </c>
+      <c r="K395" t="inlineStr">
+        <is>
+          <t>Perecibilidade da capacidade</t>
+        </is>
+      </c>
+      <c r="L395" t="inlineStr">
+        <is>
+          <t>Custo de armazenamento de estoque</t>
+        </is>
+      </c>
+      <c r="M395" t="inlineStr">
+        <is>
+          <t>Custo das horas extras</t>
+        </is>
+      </c>
+      <c r="N395" t="inlineStr">
+        <is>
+          <t>Custo da contratação</t>
+        </is>
+      </c>
+      <c r="O395" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P395" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q395" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="n">
+        <v>396</v>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D396" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E396" t="inlineStr">
+        <is>
+          <t>Produtos organizacionais são comercializados entre empresas para uso na gestão dos negócios. Uma de suas variações engloba os bens de capital, que incluem</t>
+        </is>
+      </c>
+      <c r="F396" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G396" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H396" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I396" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J396" t="inlineStr">
+        <is>
+          <t>matérias-primas e artigos para serem manufaturados.</t>
+        </is>
+      </c>
+      <c r="K396" t="inlineStr">
+        <is>
+          <t>instalações e equipamentos destinados à produção.</t>
+        </is>
+      </c>
+      <c r="L396" t="inlineStr">
+        <is>
+          <t>material para uso operacional, tais como lubrificante e itens de manutenção.</t>
+        </is>
+      </c>
+      <c r="M396" t="inlineStr">
+        <is>
+          <t>serviços de crédito, tais como empréstimos e financiamentos.</t>
+        </is>
+      </c>
+      <c r="N396" t="inlineStr">
+        <is>
+          <t>assessoria nas áreas financeira e contábil, entre outras.</t>
+        </is>
+      </c>
+      <c r="O396" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P396" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q396" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="n">
+        <v>397</v>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D397" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E397" t="inlineStr">
+        <is>
+          <t>É uma ferramenta de lean manufacturing que auxilia o controle da produção e consiste na utilização de sinais sonoros ou luminosos com o intuito de avisar o operador da ocorrência de uma falha na linha de produção. Essa ferramenta é denominada</t>
+        </is>
+      </c>
+      <c r="F397" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G397" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H397" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I397" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J397" t="inlineStr">
+        <is>
+          <t>Andon</t>
+        </is>
+      </c>
+      <c r="K397" t="inlineStr">
+        <is>
+          <t>Kaizen</t>
+        </is>
+      </c>
+      <c r="L397" t="inlineStr">
+        <is>
+          <t>Just-in-time</t>
+        </is>
+      </c>
+      <c r="M397" t="inlineStr">
+        <is>
+          <t>Just-in-sequence</t>
+        </is>
+      </c>
+      <c r="N397" t="inlineStr">
+        <is>
+          <t>Poka-Yoke</t>
+        </is>
+      </c>
+      <c r="O397" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="P378" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q378" t="n">
-        <v>0</v>
-      </c>
-      <c r="R378" t="inlineStr"/>
+      <c r="P397" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q397" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="n">
+        <v>398</v>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>EPE</t>
+        </is>
+      </c>
+      <c r="D398" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E398" t="inlineStr">
+        <is>
+          <t>A dimensão associada à exposição das atividades do processo produtivo aos consumidores é denominada</t>
+        </is>
+      </c>
+      <c r="F398" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G398" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H398" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I398" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J398" t="inlineStr">
+        <is>
+          <t>volume</t>
+        </is>
+      </c>
+      <c r="K398" t="inlineStr">
+        <is>
+          <t>variação</t>
+        </is>
+      </c>
+      <c r="L398" t="inlineStr">
+        <is>
+          <t>variedade</t>
+        </is>
+      </c>
+      <c r="M398" t="inlineStr">
+        <is>
+          <t>visibilidade</t>
+        </is>
+      </c>
+      <c r="N398" t="inlineStr">
+        <is>
+          <t>variabilidade.</t>
+        </is>
+      </c>
+      <c r="O398" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P398" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q398" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="n">
+        <v>399</v>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D399" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E399" t="inlineStr">
+        <is>
+          <t>A análise de valor é uma das abordagens utilizadas na engenharia de operações e processos de produção que visa</t>
+        </is>
+      </c>
+      <c r="F399" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G399" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H399" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I399" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J399" t="inlineStr">
+        <is>
+          <t>identificar e eliminar os custos desnecessários ou as atividades que não agregam valor aos produtos ou serviços.</t>
+        </is>
+      </c>
+      <c r="K399" t="inlineStr">
+        <is>
+          <t>representar e analisar o comportamento dos sistemas produtivos sob diferentes condições, por meio da utilização de modelos matemáticos, computacionais ou físicos.</t>
+        </is>
+      </c>
+      <c r="L399" t="inlineStr">
+        <is>
+          <t>definir e padronizar os melhores métodos para executar as tarefas nos sistemas produtivos, por meio da aplicação de técnicas como o estudo de tempos e movimentos, o diagrama de operações e o balanceamento de linhas.</t>
+        </is>
+      </c>
+      <c r="M399" t="inlineStr">
+        <is>
+          <t>adaptar os sistemas produtivos às características físicas, psicológicas e sociais dos trabalhadores, por meio da aplicação de técnicas como a análise postural, a análise biomecânica e a análise cognitiva.</t>
+        </is>
+      </c>
+      <c r="N399" t="inlineStr">
+        <is>
+          <t>indicar o volume máximo de produtos ou serviços que podem ser gerados pelos sistemas produtivos em um determinado período de tempo.</t>
+        </is>
+      </c>
+      <c r="O399" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P399" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q399" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="n">
+        <v>400</v>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D400" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E400" t="inlineStr">
+        <is>
+          <t>O Poka Yoke é uma das técnicas utilizadas na engenharia de operações e processos de produção que tem como objetivo</t>
+        </is>
+      </c>
+      <c r="F400" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G400" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H400" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I400" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J400" t="inlineStr">
+        <is>
+          <t>eliminar os desperdícios e aumentar o valor dos produtos ou serviços, por meio da aplicação dos princípios da produção enxuta.</t>
+        </is>
+      </c>
+      <c r="K400" t="inlineStr">
+        <is>
+          <t>reduzir a variabilidade e os defeitos nos processos, por meio da aplicação de ferramentas estatísticas e da melhoria contínua.</t>
+        </is>
+      </c>
+      <c r="L400" t="inlineStr">
+        <is>
+          <t>prevenir ou detectar os erros nos processos, por meio da utilização de dispositivos à prova de falhas.</t>
+        </is>
+      </c>
+      <c r="M400" t="inlineStr">
+        <is>
+          <t>promover a melhoria contínua dos processos, envolvendo todos os funcionários da organização.</t>
+        </is>
+      </c>
+      <c r="N400" t="inlineStr">
+        <is>
+          <t>estabelecer os requisitos e as diretrizes para a gestão de ativos físicos, para otimizar o valor, o desempenho e os riscos dos ativos ao longo do seu ciclo de vida.</t>
+        </is>
+      </c>
+      <c r="O400" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P400" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q400" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="n">
+        <v>401</v>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D401" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E401" t="inlineStr">
+        <is>
+          <t>Qual é a principal diferença entre just-in-time e just-in-sequence?</t>
+        </is>
+      </c>
+      <c r="F401" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G401" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H401" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I401" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J401" t="inlineStr">
+        <is>
+          <t>Just-in-time é uma técnica de gestão da produção, enquanto just-in-sequence é uma técnica de gestão do estoque.</t>
+        </is>
+      </c>
+      <c r="K401" t="inlineStr">
+        <is>
+          <t>Just-in-time é uma técnica de gestão do estoque, enquanto just-in-sequence é uma técnica de gestão da produção.</t>
+        </is>
+      </c>
+      <c r="L401" t="inlineStr">
+        <is>
+          <t>Just-in-time é uma técnica de gestão da produção que visa reduzir os estoques e os custos, enquanto just-in-sequence é uma técnica de gestão da produção que visa sincronizar a entrega dos componentes com a montagem dos produtos.</t>
+        </is>
+      </c>
+      <c r="M401" t="inlineStr">
+        <is>
+          <t>Just-in-time é uma técnica de gestão da produção que visa aumentar a eficiência e a qualidade dos produtos, enquanto just-in-sequence é uma técnica de gestão da produção que visa adaptar a produção à demanda dos clientes.</t>
+        </is>
+      </c>
+      <c r="N401" t="inlineStr">
+        <is>
+          <t>Just-in-time é uma técnica de gestão da produção que visa eliminar os desperdícios e melhorar os processos, enquanto just-in-sequence é uma técnica de gestão da produção que visa integrar os fornecedores e os distribuidores.</t>
+        </is>
+      </c>
+      <c r="O401" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P401" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q401" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="n">
+        <v>402</v>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D402" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E402" t="inlineStr">
+        <is>
+          <t>Um engenheiro estava fazendo o planejamento da produção de uma fábrica de bicicletas. Foi-lhe pedido que utilizasse o software de planejamento da produção para calcular quanto e quando comprar componentes para montar a linha de bicicletas produzidas por essa fábrica. As heurísticas de reposição de estoque sob demanda variável no tempo buscam comprar as menores quantidades de componentes, ao menor custo e no momento certo da montagem. Dentre as heurísticas de reposição de demanda determinística variável no tempo, o engenheiro decidiu escolher a de menor custo, que é a seguinte:</t>
+        </is>
+      </c>
+      <c r="F402" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G402" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H402" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I402" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J402" t="inlineStr">
+        <is>
+          <t>reposição lote a lote</t>
+        </is>
+      </c>
+      <c r="K402" t="inlineStr">
+        <is>
+          <t>lote econômico de compras</t>
+        </is>
+      </c>
+      <c r="L402" t="inlineStr">
+        <is>
+          <t>pedidos periódicos</t>
+        </is>
+      </c>
+      <c r="M402" t="inlineStr">
+        <is>
+          <t>menor custo unitário</t>
+        </is>
+      </c>
+      <c r="N402" t="inlineStr">
+        <is>
+          <t>heurística de Silver Meal</t>
+        </is>
+      </c>
+      <c r="O402" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P402" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q402" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="n">
+        <v>403</v>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D403" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E403" t="inlineStr">
+        <is>
+          <t>Buscando atender à demanda de clientes, a manufatura utiliza três principais estratégias: antecipação da demanda, aumentando a capacidade produtiva antes que a demanda ocorra; seguimento da demanda, aguardando que a demanda ultrapasse a capacidade produtiva para aumentar a capacidade; e uma estratégia mista, combinando antecipação e seguimento da demanda.
+Em indústrias de fluxo contínuo de produção, como siderúrgicas ou fábricas de celulose, a estratégia mais utilizada é a de seguir a demanda, pois nesse tipo de indústria</t>
+        </is>
+      </c>
+      <c r="F403" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G403" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H403" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I403" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J403" t="inlineStr">
+        <is>
+          <t>a complexidade do processo produtivo em fluxo contínuo exige maior tempo de planejamento para expandir.</t>
+        </is>
+      </c>
+      <c r="K403" t="inlineStr">
+        <is>
+          <t>a demanda tem uma grande elasticidade, e os clientes aguardam as expansões.</t>
+        </is>
+      </c>
+      <c r="L403" t="inlineStr">
+        <is>
+          <t>os tempos de realização da expansão são demasiadamente longos.</t>
+        </is>
+      </c>
+      <c r="M403" t="inlineStr">
+        <is>
+          <t>os valores financeiros necessários para a expansão são muito altos, tornando a antecipação inviável.</t>
+        </is>
+      </c>
+      <c r="N403" t="inlineStr">
+        <is>
+          <t>os fornecedores de máquinas e equipamentos para a indústria de fluxo contínuo demandam maior tempo de entrega.</t>
+        </is>
+      </c>
+      <c r="O403" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P403" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q403" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="n">
+        <v>404</v>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>BR DISTRIBUIDORA</t>
+        </is>
+      </c>
+      <c r="D404" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="E404" t="inlineStr">
+        <is>
+          <t>O processo de Planejamento e Controle da Produção (PCP) é responsável por planejar estoques de matérias-primas, semiacabados e acabados, controlar prazos de entrega e controlar a utilização dos recursos de produção. Sobre as etapas do PCP, é INCORRETO afirmar que</t>
+        </is>
+      </c>
+      <c r="F404" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G404" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H404" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I404" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J404" t="inlineStr">
+        <is>
+          <t>No Planejamento das Necessidades de Materais (MRP – Material Requirement Planning), os componentes (matérias-primas e semiacabados) do produto acabado são planejados de acordo com a lista de materiais (BOM – Bill of Materials), estoques disponíveis e prazos de fabricação ou aquisição de cada componente.</t>
+        </is>
+      </c>
+      <c r="K404" t="inlineStr">
+        <is>
+          <t>Na etapa Planejamento de Recursos de Capacidade (CRP – Capacity Resource Planning), analisam-se os resultados dos cálculos da etapa MRP e seus impactos sobre a capacidade dos recursos de produção, no curto prazo.</t>
+        </is>
+      </c>
+      <c r="L404" t="inlineStr">
+        <is>
+          <t>A Programação Mestre de Produção (MPS – Master Production Schedule) é responsável por planejar datas de entrega dos produtos acabados, de acordo com as previsões de vendas e estoques disponíveis de produtos acabados.</t>
+        </is>
+      </c>
+      <c r="M404" t="inlineStr">
+        <is>
+          <t>a etapa de Planejamento Grosseiro de Capacidade (RCCP – Rough Cut Capacity Planning) é utilizada, com foco principalmente nos impactos sobre os gargalos da produção, para avaliar os resultados dos cálculos da etapa MPS.</t>
+        </is>
+      </c>
+      <c r="N404" t="inlineStr">
+        <is>
+          <t>A etapa de planejamento agregado consiste em estabelecer os níveis de produção e estoques para cada família de produtos, com horizonte de planejamento de curto prazo, e seu objetivo é garantir que os principais recursos de produção estarão disponíveis.</t>
+        </is>
+      </c>
+      <c r="O404" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P404" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q404" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="n">
+        <v>405</v>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>PBIO</t>
+        </is>
+      </c>
+      <c r="D405" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="E405" t="inlineStr">
+        <is>
+          <t>Planejamento e Controle da Produção (PCP) é composto por etapas hierárquicas cujo objetivo é garantir que os recursos necessários para a produção estarão disponíveis no momento certo. Para isso, são elaborados planejamentos de nível estratégico, tático e operacional.
+Associe as características à esquerda com as etapas do PCP, que se encontram à direita.
+Características
+I - Explosão de necessidades de materiais e componentes
+II - Planejamento de estoques e prazos de entrega dos produtos finais
+III - Planejamento de capacidade dos recursos críticos (gargalos)
+IV - Planejamento de produção e estoques por famílias de produtos
+Etapas do PCP
+P - SOP (Sales and Operations Planning) - Planejamento de Vendas e Operações
+Q - RCCP (Rough Cut Capacity Planning) - Planejamento Grosseiro de Capacidade
+R - MPS (Master Production Schedule) - Planejamento Mestre da Produção
+S - CRP (Capacity Requirements Planning) - Planejamento de Capacidade de Curto Prazo
+T - MRP (Material Requirements Planning) - Planejamento das Necessidades de Materiais
+A associação correta é</t>
+        </is>
+      </c>
+      <c r="F405" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G405" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H405" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I405" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J405" t="inlineStr">
+        <is>
+          <t>I - T, II - R, III - Q, IV - P</t>
+        </is>
+      </c>
+      <c r="K405" t="inlineStr">
+        <is>
+          <t>I - R, II - T, III - Q, IV - S</t>
+        </is>
+      </c>
+      <c r="L405" t="inlineStr">
+        <is>
+          <t>I - R, II - T, III - S, IV - Q</t>
+        </is>
+      </c>
+      <c r="M405" t="inlineStr">
+        <is>
+          <t>I - R, II - T, III - P, IV -S</t>
+        </is>
+      </c>
+      <c r="N405" t="inlineStr">
+        <is>
+          <t>I - S, II - R, III - P, IV - T.</t>
+        </is>
+      </c>
+      <c r="O405" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P405" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q405" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="n">
+        <v>406</v>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>ELETRONUCLEAR</t>
+        </is>
+      </c>
+      <c r="D406" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="E406" t="inlineStr">
+        <is>
+          <t>Numa empresa que compete no mercado aberto, a produção visa a disponibilizar seus produtos com a melhor qualidade, a custos competitivos, com menores tempos de entrega e com flexibilidade para aumentar e diminuir a quantidade de produtos, de acordo com a demanda. Qualidade, custos, tempos e flexibilidade são chamados de prioridades competitivas.
+A teoria de trade off afirma que a estratégia de uma empresa face à concorrência deve ser</t>
+        </is>
+      </c>
+      <c r="F406" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G406" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H406" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I406" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J406" t="inlineStr">
+        <is>
+          <t>aumentar a qualidade de seus produtos, antes de competir em custos, tempos e flexibilidade.</t>
+        </is>
+      </c>
+      <c r="K406" t="inlineStr">
+        <is>
+          <t>aumentar a qualidade e reduzir os custos, antes de competir em tempos e flexibilidade.</t>
+        </is>
+      </c>
+      <c r="L406" t="inlineStr">
+        <is>
+          <t>escolher uma prioridade competitiva e desenvolver uma a uma, de forma sucessiva, em qualquer ordem.</t>
+        </is>
+      </c>
+      <c r="M406" t="inlineStr">
+        <is>
+          <t>escolher uma prioridade competitiva e desenvolver uma a uma, de forma sucessiva, necessariamente nesta ordem: qualidade, tempos, flexibilidade e custos.</t>
+        </is>
+      </c>
+      <c r="N406" t="inlineStr">
+        <is>
+          <t>reduzir os custos de produção, antes de competir em qualidade, tempos e flexibilidade.</t>
+        </is>
+      </c>
+      <c r="O406" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P406" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q406" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
:up: questoes do pdf pesquisa operacional de CE cadastradas
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R406"/>
+  <dimension ref="A1:R468"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -33189,7 +33189,7 @@
         </is>
       </c>
       <c r="P384" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q384" t="n">
         <v>0</v>
@@ -34943,6 +34943,4825 @@
         <v>0</v>
       </c>
     </row>
+    <row r="407">
+      <c r="A407" t="n">
+        <v>407</v>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D407" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E407" t="inlineStr">
+        <is>
+          <t>O diagrama de rede abaixo apresenta o encadeamento das tarefas de um dado projeto, juntamente com os tempos necessários para a sua execução.
+Considerando que o prazo total para a conclusão do projeto, uma vez iniciado, é de dezesseis dias e que, contratualmente, não se admite atraso, verifica-se que o(</t>
+        </is>
+      </c>
+      <c r="F407" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G407" t="inlineStr">
+        <is>
+          <t>Gestão de Projetos</t>
+        </is>
+      </c>
+      <c r="H407" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I407" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J407" t="inlineStr">
+        <is>
+          <t>conjunto de tarefas 3 e 4 apresenta folga de até quatro dias.</t>
+        </is>
+      </c>
+      <c r="K407" t="inlineStr">
+        <is>
+          <t>tarefa 2 não apresenta folga.</t>
+        </is>
+      </c>
+      <c r="L407" t="inlineStr">
+        <is>
+          <t>folga total do projeto é nula.</t>
+        </is>
+      </c>
+      <c r="M407" t="inlineStr">
+        <is>
+          <t>tarefa 4 pode iniciar até quatro dias depois do término da tarefa 3, caso a tarefa 3 comece no mesmo dia em que a tarefa 1.</t>
+        </is>
+      </c>
+      <c r="N407" t="inlineStr">
+        <is>
+          <t>folga da tarefa 4 será de quatro dias, caso a tarefa 3 comece um dia depois da tarefa 1.</t>
+        </is>
+      </c>
+      <c r="O407" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P407" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q407" t="n">
+        <v>0</v>
+      </c>
+      <c r="R407" t="inlineStr">
+        <is>
+          <t>bbd68495-0dde-494a-a87d-6991991a6c2f.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="n">
+        <v>408</v>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D408" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E408" t="inlineStr">
+        <is>
+          <t>O ciclo de vida de um dado projeto, já completado, é representado pelo gráfico abaixo.
+Com base nesse gráfico, conclui-se que o(</t>
+        </is>
+      </c>
+      <c r="F408" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G408" t="inlineStr">
+        <is>
+          <t>Gestão de Projetos</t>
+        </is>
+      </c>
+      <c r="H408" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I408" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J408" t="inlineStr">
+        <is>
+          <t>esforço máximo foi executado no início do projeto (até o tempo t1), quando ainda se desenvolvia o seu conceito, e os processos a serem aplicados estavam em seleção.</t>
+        </is>
+      </c>
+      <c r="K408" t="inlineStr">
+        <is>
+          <t>maior volume de recursos foi aplicado a partir do momento em que 50% do projeto já tinha sido executado.</t>
+        </is>
+      </c>
+      <c r="L408" t="inlineStr">
+        <is>
+          <t>faixa entre 15% e 85% de execução representa as fases nas quais existem um mínimo de planejamento e predominam as tarefas de desenvolvimento.</t>
+        </is>
+      </c>
+      <c r="M408" t="inlineStr">
+        <is>
+          <t>faixa a partir de 85% indica uma aceleração da velocidade de execução do projeto.</t>
+        </is>
+      </c>
+      <c r="N408" t="inlineStr">
+        <is>
+          <t>faixa entre 15% e 85% indica uma diminuição da velocidade de execução do projeto.</t>
+        </is>
+      </c>
+      <c r="O408" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P408" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q408" t="n">
+        <v>0</v>
+      </c>
+      <c r="R408" t="inlineStr">
+        <is>
+          <t>ba337bb0-13fa-40b2-9a75-d1864dafa8ac.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="n">
+        <v>409</v>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D409" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E409" t="inlineStr">
+        <is>
+          <t>Em um determinado projeto, o lançamento de um novo produto foi programado, de acordo com o tempo necessário para sua execução. A Figura abaixo representa a rede PERT desse projeto, com as atividades e as respectivas durações (em dias). A fase 1 representa a etapa inicial, e a fase 6 diz respeito ao lançamento do produto.
+Com base no conceito do caminho crítico, a sequência de atividades a que o gestor do projeto deve dispensar maior atenção, a fim de lançar o produto no prazo previsto é</t>
+        </is>
+      </c>
+      <c r="F409" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G409" t="inlineStr">
+        <is>
+          <t>Gestão de Projetos</t>
+        </is>
+      </c>
+      <c r="H409" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I409" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J409" t="inlineStr">
+        <is>
+          <t>A – G – I</t>
+        </is>
+      </c>
+      <c r="K409" t="inlineStr">
+        <is>
+          <t>B – D – G – I</t>
+        </is>
+      </c>
+      <c r="L409" t="inlineStr">
+        <is>
+          <t>B – E – H – I</t>
+        </is>
+      </c>
+      <c r="M409" t="inlineStr">
+        <is>
+          <t>C – H – I</t>
+        </is>
+      </c>
+      <c r="N409" t="inlineStr">
+        <is>
+          <t>B – F – I</t>
+        </is>
+      </c>
+      <c r="O409" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P409" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q409" t="n">
+        <v>0</v>
+      </c>
+      <c r="R409" t="inlineStr">
+        <is>
+          <t>003c39c0-804a-480f-b0be-36cd9987e530.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="n">
+        <v>410</v>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D410" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E410" t="inlineStr">
+        <is>
+          <t>O diretor de uma empresa de produtos químicos deseja identificar demandas que devem ser implementadas através de projetos. Ao receber a lista, ele verifica que NÃO poderá tratar como projeto a:</t>
+        </is>
+      </c>
+      <c r="F410" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G410" t="inlineStr">
+        <is>
+          <t>Gestão de Projetos</t>
+        </is>
+      </c>
+      <c r="H410" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I410" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J410" t="inlineStr">
+        <is>
+          <t>Ampliação do depósito de drogas</t>
+        </is>
+      </c>
+      <c r="K410" t="inlineStr">
+        <is>
+          <t>Substituição do software de controle de processos</t>
+        </is>
+      </c>
+      <c r="L410" t="inlineStr">
+        <is>
+          <t>Criação de um sistema de informação gerencial</t>
+        </is>
+      </c>
+      <c r="M410" t="inlineStr">
+        <is>
+          <t>Descontaminação semanal do reator de fermentação</t>
+        </is>
+      </c>
+      <c r="N410" t="inlineStr">
+        <is>
+          <t>Automação do setor de embalagem de produtos</t>
+        </is>
+      </c>
+      <c r="O410" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P410" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q410" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="n">
+        <v>411</v>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Quadrix</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>CRF-PR</t>
+        </is>
+      </c>
+      <c r="D411" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E411" t="inlineStr">
+        <is>
+          <t>O projeto é um empreendimento que faz parte, consciente ou inconscientemente, do dia a dia de qualquer organização. A visão da empresa influenciará sensivelmente no sucesso do projeto. Acerca desse tema, assinale a alternativa correta.</t>
+        </is>
+      </c>
+      <c r="F411" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G411" t="inlineStr">
+        <is>
+          <t>Gestão de Projetos</t>
+        </is>
+      </c>
+      <c r="H411" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I411" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J411" t="inlineStr">
+        <is>
+          <t>É temporário, pois é dividido em começo, meio e fim, com datas que determinam sua duração.</t>
+        </is>
+      </c>
+      <c r="K411" t="inlineStr">
+        <is>
+          <t>Poderá começar sem um objetivo específico e, ao longo de seu desenvolvimento, a equipe definirá o que se pretende com ele</t>
+        </is>
+      </c>
+      <c r="L411" t="inlineStr">
+        <is>
+          <t>Não poderá coexistir com nenhum outro projeto, pois perderá o foco nas execuções e consequentemente sua eficácia.</t>
+        </is>
+      </c>
+      <c r="M411" t="inlineStr">
+        <is>
+          <t>Uma característica interessante sobre projeto é que ele não possui restrição de recursos, o que aumenta a qualidade de sua execução.</t>
+        </is>
+      </c>
+      <c r="N411" t="inlineStr">
+        <is>
+          <t>Para que haja a execução de um bom projeto, é necessário que ele nunca seja inédito, ou seja, quanto mais mudanças ocorrerem, mais desafiadora se tornará a gestão do projeto.</t>
+        </is>
+      </c>
+      <c r="O411" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P411" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q411" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="n">
+        <v>412</v>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>IBFC</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>Câmara Municipal de Araraquara - SP</t>
+        </is>
+      </c>
+      <c r="D412" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E412" t="inlineStr">
+        <is>
+          <t>É difícil definir um conjunto de indicadores que possa ser usado por qualquer gestor de projetos. Cada organização possui características únicas e os indicadores que funcionam bem para um projeto podem não ser adequados para outros. Apesar disso, é possível estabelecer alguns requisitos genéricos que podem ser particularizados conforme cada projeto. A esse respeito, analise as afirmativas abaixo e assinale a alternativa correta:
+I. Cumprir o cronograma e respeitar o orçamento.
+II. Utilizar sem desperdícios todos os recursos alocados.
+III. Alcançar os requisitos de qualidade especificados no projeto.
+IV. Elaborar um conjunto de boas práticas para mitigar cada fase do projeto.
+V. Passar pelo maior número possível de alterações no escopo.</t>
+        </is>
+      </c>
+      <c r="F412" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G412" t="inlineStr">
+        <is>
+          <t>Gestão de Projetos</t>
+        </is>
+      </c>
+      <c r="H412" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I412" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J412" t="inlineStr">
+        <is>
+          <t>Apenas as afirmativas I, II e III estão corretas</t>
+        </is>
+      </c>
+      <c r="K412" t="inlineStr">
+        <is>
+          <t>Apenas as afirmativas IV e V estão corretas</t>
+        </is>
+      </c>
+      <c r="L412" t="inlineStr">
+        <is>
+          <t>Apenas as afirmativas III e IV estão corretas</t>
+        </is>
+      </c>
+      <c r="M412" t="inlineStr">
+        <is>
+          <t>Apenas as afirmativas I e II estão corretas</t>
+        </is>
+      </c>
+      <c r="N412" t="inlineStr">
+        <is>
+          <t>Apenas as afirmativas I, IV e V estão corretas</t>
+        </is>
+      </c>
+      <c r="O412" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P412" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q412" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="n">
+        <v>413</v>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>FGV</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>SEE-PE</t>
+        </is>
+      </c>
+      <c r="D413" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E413" t="inlineStr">
+        <is>
+          <t>Uma importante ferramenta utilizada no planejamento e controle de projetos complexos é PERT/CPM. Utilizando modelagem e programação em rede, uma dos principais objetivos do PERT/CPM é determinar o caminho crítico e sua duração.
+Na figura a seguir, as atividades de um determinado projeto são representadas por letras maiúsculas localizadas nos arcos; a duração das atividades, expressa em dias, são números também apresentados nos arcos.
+A duração do caminho crítico é de:</t>
+        </is>
+      </c>
+      <c r="F413" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G413" t="inlineStr">
+        <is>
+          <t>Gestão de Projetos</t>
+        </is>
+      </c>
+      <c r="H413" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I413" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J413" t="inlineStr">
+        <is>
+          <t>16 dias</t>
+        </is>
+      </c>
+      <c r="K413" t="inlineStr">
+        <is>
+          <t>14 dias</t>
+        </is>
+      </c>
+      <c r="L413" t="inlineStr">
+        <is>
+          <t>12 dias</t>
+        </is>
+      </c>
+      <c r="M413" t="inlineStr">
+        <is>
+          <t>10 dias</t>
+        </is>
+      </c>
+      <c r="N413" t="inlineStr">
+        <is>
+          <t>8 dias</t>
+        </is>
+      </c>
+      <c r="O413" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P413" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q413" t="n">
+        <v>0</v>
+      </c>
+      <c r="R413" t="inlineStr">
+        <is>
+          <t>ada9ef2c-4378-4f1c-9068-3ef291065d72.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="n">
+        <v>414</v>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Cebraspe</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>Empresa Maranhense de Administração Portuária</t>
+        </is>
+      </c>
+      <c r="D414" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E414" t="inlineStr">
+        <is>
+          <t>Julgue o próximo item, referente a rede de suprimentos.
+O ERP e o CRM são tecnologias utilizadas para a gestão da rede de suprimentos de uma empresa.</t>
+        </is>
+      </c>
+      <c r="F414" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G414" t="inlineStr">
+        <is>
+          <t>Gestão da Cadeia de Suprimentos</t>
+        </is>
+      </c>
+      <c r="H414" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I414" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J414" t="inlineStr"/>
+      <c r="K414" t="inlineStr"/>
+      <c r="L414" t="inlineStr"/>
+      <c r="M414" t="inlineStr"/>
+      <c r="N414" t="inlineStr"/>
+      <c r="O414" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P414" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q414" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="n">
+        <v>415</v>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Cebraspe</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>SERPRO</t>
+        </is>
+      </c>
+      <c r="D415" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="E415" t="inlineStr">
+        <is>
+          <t>Julgue o item, acerca de suprimento de materiais.
+Uma empresa que atua como intermediário comerciante, vendendo suprimentos ao consumidor final é caracterizada como atacadista.</t>
+        </is>
+      </c>
+      <c r="F415" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G415" t="inlineStr">
+        <is>
+          <t>Gestão da Cadeia de Suprimentos</t>
+        </is>
+      </c>
+      <c r="H415" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I415" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J415" t="inlineStr"/>
+      <c r="K415" t="inlineStr"/>
+      <c r="L415" t="inlineStr"/>
+      <c r="M415" t="inlineStr"/>
+      <c r="N415" t="inlineStr"/>
+      <c r="O415" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P415" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q415" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="n">
+        <v>416</v>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Cebraspe</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>SERPRO</t>
+        </is>
+      </c>
+      <c r="D416" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="E416" t="inlineStr">
+        <is>
+          <t>Julgue o item que se segue, referente à gestão de materiais.
+A gestão da cadeia de suprimento estabelece um compartilhamento de informações entre fornecedores, produtores, distribuidores e clientes em um processo integrado, não existindo foco em um cliente direto ou imediato.</t>
+        </is>
+      </c>
+      <c r="F416" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G416" t="inlineStr">
+        <is>
+          <t>Gestão da Cadeia de Suprimentos</t>
+        </is>
+      </c>
+      <c r="H416" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I416" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J416" t="inlineStr"/>
+      <c r="K416" t="inlineStr"/>
+      <c r="L416" t="inlineStr"/>
+      <c r="M416" t="inlineStr"/>
+      <c r="N416" t="inlineStr"/>
+      <c r="O416" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P416" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q416" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="n">
+        <v>417</v>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>TRT 10ª Região</t>
+        </is>
+      </c>
+      <c r="D417" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="E417" t="inlineStr">
+        <is>
+          <t>Julgue o item que se segue, relativos à gestão de materiais.
+Denomina-se verticalização o processo em que a empresa se torna seu próprio fornecedor, passando ela própria a produzir internamente suas matérias-primas, para evitar a dependência de fornecedores externos.</t>
+        </is>
+      </c>
+      <c r="F417" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G417" t="inlineStr">
+        <is>
+          <t>Gestão da Cadeia de Suprimentos</t>
+        </is>
+      </c>
+      <c r="H417" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I417" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J417" t="inlineStr"/>
+      <c r="K417" t="inlineStr"/>
+      <c r="L417" t="inlineStr"/>
+      <c r="M417" t="inlineStr"/>
+      <c r="N417" t="inlineStr"/>
+      <c r="O417" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P417" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q417" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="n">
+        <v>418</v>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>ANP</t>
+        </is>
+      </c>
+      <c r="D418" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="E418" t="inlineStr">
+        <is>
+          <t>A logística pode ser entendida como a competência que vincula a empresa a seus clientes e a seus fornecedores. Segundo os conceitos de logística integrada, e considerando as etapas de suprimento, manufatura e distribuição, julgue o item a seguir.
+A etapa de suprimento abrange a compra e a organização da movimentação de materiais entre a empresa e os seus clientes finais.</t>
+        </is>
+      </c>
+      <c r="F418" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G418" t="inlineStr">
+        <is>
+          <t>Gestão da Cadeia de Suprimentos</t>
+        </is>
+      </c>
+      <c r="H418" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I418" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J418" t="inlineStr"/>
+      <c r="K418" t="inlineStr"/>
+      <c r="L418" t="inlineStr"/>
+      <c r="M418" t="inlineStr"/>
+      <c r="N418" t="inlineStr"/>
+      <c r="O418" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P418" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q418" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="n">
+        <v>419</v>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>PEFOCE</t>
+        </is>
+      </c>
+      <c r="D419" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="E419" t="inlineStr">
+        <is>
+          <t>Acerca de logística, julgue o item abaixo.
+O longo caminho que se estende desde as fontes de matéria-prima, passando pelas fábricas dos componentes, pela manufatura do produto, pelos distribuidores e chegando finalmente ao consumidor por meio do varejista constitui uma cadeia de suprimento.</t>
+        </is>
+      </c>
+      <c r="F419" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G419" t="inlineStr">
+        <is>
+          <t>Gestão da Cadeia de Suprimentos</t>
+        </is>
+      </c>
+      <c r="H419" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I419" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J419" t="inlineStr"/>
+      <c r="K419" t="inlineStr"/>
+      <c r="L419" t="inlineStr"/>
+      <c r="M419" t="inlineStr"/>
+      <c r="N419" t="inlineStr"/>
+      <c r="O419" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P419" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q419" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="n">
+        <v>420</v>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>Anatel</t>
+        </is>
+      </c>
+      <c r="D420" t="inlineStr">
+        <is>
+          <t>2004</t>
+        </is>
+      </c>
+      <c r="E420" t="inlineStr">
+        <is>
+          <t>Julgue o item subsequente, relativo à cadeia de suprimentos.
+Cadeia produtiva é o conjunto de atividades econômicas que se articulam progressivamente desde o início da elaboração de um produto — incluindo-se as matérias-primas, as máquinas, os equipamentos e os produtos intermediários — até o resultado final. A distribuição e a comercialização não fazem parte da cadeia produtiva.</t>
+        </is>
+      </c>
+      <c r="F420" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G420" t="inlineStr">
+        <is>
+          <t>Gestão da Cadeia de Suprimentos</t>
+        </is>
+      </c>
+      <c r="H420" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I420" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J420" t="inlineStr"/>
+      <c r="K420" t="inlineStr"/>
+      <c r="L420" t="inlineStr"/>
+      <c r="M420" t="inlineStr"/>
+      <c r="N420" t="inlineStr"/>
+      <c r="O420" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P420" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q420" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="n">
+        <v>421</v>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>Anatel</t>
+        </is>
+      </c>
+      <c r="D421" t="inlineStr">
+        <is>
+          <t>2004</t>
+        </is>
+      </c>
+      <c r="E421" t="inlineStr">
+        <is>
+          <t>Julgue o item subsequente, relativo à cadeia de suprimentos.
+Devido às similaridades em suas atividades, o canal de suprimento físico — também denominado administração de materiais — e o canal de distribuição física compreendem atividades integradas na logística empresarial, cujo gerenciamento é conhecido como gerenciamento da cadeia de suprimentos.</t>
+        </is>
+      </c>
+      <c r="F421" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G421" t="inlineStr">
+        <is>
+          <t>Gestão da Cadeia de Suprimentos</t>
+        </is>
+      </c>
+      <c r="H421" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I421" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J421" t="inlineStr"/>
+      <c r="K421" t="inlineStr"/>
+      <c r="L421" t="inlineStr"/>
+      <c r="M421" t="inlineStr"/>
+      <c r="N421" t="inlineStr"/>
+      <c r="O421" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P421" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q421" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="n">
+        <v>422</v>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Cebraspe</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>IFB</t>
+        </is>
+      </c>
+      <c r="D422" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="E422" t="inlineStr">
+        <is>
+          <t>Julgue os itens seguintes, relativos a rede de suprimentos.
+As cadeias de suprimentos de alta velocidade e baixo custo são a melhor escolha para responder com agilidade a mudanças inesperadas de demanda ou de suprimento.</t>
+        </is>
+      </c>
+      <c r="F422" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G422" t="inlineStr">
+        <is>
+          <t>Gestão da Cadeia de Suprimentos</t>
+        </is>
+      </c>
+      <c r="H422" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I422" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J422" t="inlineStr"/>
+      <c r="K422" t="inlineStr"/>
+      <c r="L422" t="inlineStr"/>
+      <c r="M422" t="inlineStr"/>
+      <c r="N422" t="inlineStr"/>
+      <c r="O422" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P422" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q422" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="n">
+        <v>423</v>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Cebraspe</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>IFB</t>
+        </is>
+      </c>
+      <c r="D423" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="E423" t="inlineStr">
+        <is>
+          <t>Julgue os itens seguintes, referentes a rede de suprimentos.
+Redes de suprimento de ciclo fechado são aquelas compostas por fluxos diretos e reversos, formando ciclos que fazem materiais usados retornarem a pontos anteriores da rede para reutilização ou reprocessamento para nova utilização.</t>
+        </is>
+      </c>
+      <c r="F423" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G423" t="inlineStr">
+        <is>
+          <t>Gestão da Cadeia de Suprimentos</t>
+        </is>
+      </c>
+      <c r="H423" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I423" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J423" t="inlineStr"/>
+      <c r="K423" t="inlineStr"/>
+      <c r="L423" t="inlineStr"/>
+      <c r="M423" t="inlineStr"/>
+      <c r="N423" t="inlineStr"/>
+      <c r="O423" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P423" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q423" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="n">
+        <v>424</v>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>BIORIO</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>ELETROBRAS</t>
+        </is>
+      </c>
+      <c r="D424" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E424" t="inlineStr">
+        <is>
+          <t>Na análise das demonstrações financeiras são muito adotados como indicadores de liquidez contábil o índice de liquidez corrente e o índice de liquidez seca que são dados, respectivamente, por:</t>
+        </is>
+      </c>
+      <c r="F424" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G424" t="inlineStr">
+        <is>
+          <t>Gestão de Investimentos e Risco</t>
+        </is>
+      </c>
+      <c r="H424" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I424" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J424" t="inlineStr">
+        <is>
+          <t>(Ativos totais)/(passivo total) e (ativos de conversão rápida)/ (passivo total).</t>
+        </is>
+      </c>
+      <c r="K424" t="inlineStr">
+        <is>
+          <t>(Ativos de conversão rápida)/(passivo total) e (ativos circulantes totais)/(passivo total)</t>
+        </is>
+      </c>
+      <c r="L424" t="inlineStr">
+        <is>
+          <t>(Ativos circulantes totais)/(passivo total) e (ativos de conversão rápida)/(passivo total)</t>
+        </is>
+      </c>
+      <c r="M424" t="inlineStr">
+        <is>
+          <t>(Ativos circulantes totais/(passivos circulantes totais) e (ativos de conversão rápida)/(passivos circulantes totais)</t>
+        </is>
+      </c>
+      <c r="N424" t="inlineStr">
+        <is>
+          <t>(Ativos de conversão rápida)/(passivos circulantes totais) e (ativos circulantes totais)/(passivos circulantes totais).</t>
+        </is>
+      </c>
+      <c r="O424" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P424" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q424" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="n">
+        <v>425</v>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>CEBRASPE</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>FUB</t>
+        </is>
+      </c>
+      <c r="D425" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E425" t="inlineStr">
+        <is>
+          <t>Considerando que a tabela acima, cujos valores estão descritos em R$ milhões, tenha sido extraída da contabilidade de determinada empresa ao longo de dois exercícios consecutivos, julgue o item subsequente.
+O índice de liquidez geral do ano 1 foi superior ao índice de liquidez geral do ano</t>
+        </is>
+      </c>
+      <c r="F425" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G425" t="inlineStr">
+        <is>
+          <t>Gestão de Investimentos e Risco</t>
+        </is>
+      </c>
+      <c r="H425" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I425" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J425" t="inlineStr"/>
+      <c r="K425" t="inlineStr"/>
+      <c r="L425" t="inlineStr"/>
+      <c r="M425" t="inlineStr"/>
+      <c r="N425" t="inlineStr"/>
+      <c r="O425" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P425" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q425" t="n">
+        <v>0</v>
+      </c>
+      <c r="R425" t="inlineStr">
+        <is>
+          <t>48307916-16fa-49c6-811f-1f161b2b6419.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="n">
+        <v>426</v>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>UFC</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>UFC</t>
+        </is>
+      </c>
+      <c r="D426" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E426" t="inlineStr">
+        <is>
+          <t>O ROI (Return On Investment ou, em português, Retorno Sobre Investimento) é uma das maneiras mais tradicionais de se fazer a previsão dos prováveis proventos auferidos num projeto social. Com relação a essa métrica, temos que:</t>
+        </is>
+      </c>
+      <c r="F426" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G426" t="inlineStr">
+        <is>
+          <t>Gestão de Investimentos e Risco</t>
+        </is>
+      </c>
+      <c r="H426" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I426" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J426" t="inlineStr">
+        <is>
+          <t>Ela é a taxa de desconto que zera o valor presente líquido dos fluxos de caixa de um projeto, ou seja, faz com que todas as entradas igualem todas as saídas de caixa do projeto social</t>
+        </is>
+      </c>
+      <c r="K426" t="inlineStr">
+        <is>
+          <t>É definido como o número de períodos (anos, meses, semanas etc.) para se recuperar o investimento inicial. Seu cálculo requer que se some os valores dos fluxos de caixa descontados pela taxa mínima de atratividade.</t>
+        </is>
+      </c>
+      <c r="L426" t="inlineStr">
+        <is>
+          <t>Consiste em uma métrica utilizada para mensurar o rendimento obtido com uma dada quantia de recursos. O ROI é dado pela razão entre o lucro líquido alcançado e o investimento efetuado dentro de um dado período.</t>
+        </is>
+      </c>
+      <c r="M426" t="inlineStr">
+        <is>
+          <t>Por definição, esse método consiste em trazer para a data zero, usando como taxa de desconto a Taxa Mínima de Atratividade do projeto, todos os fluxos de caixa do investimento e somá-los ao valor do investimento inicial.</t>
+        </is>
+      </c>
+      <c r="N426" t="inlineStr">
+        <is>
+          <t>É definido como o número de períodos (anos, meses, semanas etc.) para se recuperar o investimento inicial. Seu cálculo requer que se some os valores dos fluxos de caixa auferidos, período a período, até que essa soma se iguale ao valor do investimento inicial.</t>
+        </is>
+      </c>
+      <c r="O426" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P426" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q426" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="n">
+        <v>427</v>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>IBFC</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>EBSERH</t>
+        </is>
+      </c>
+      <c r="D427" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E427" t="inlineStr">
+        <is>
+          <t>Retorno sobre investimento - ROI é a relação entre o dinheiro ganho ou perdido através de um investimento, e o montante de dinheiro investido. Existem três formulações possíveis de taxa de retorno:
+I. O retorno efetivo: é o que permite determinar o valor de um investimento.
+II. O retomo previsto: serve como medida de avaliação do desempenho de um investimento.
+III. O retorno exigido: serve como medida ante o desempenho de um investimento.
+Das afirmações acima:</t>
+        </is>
+      </c>
+      <c r="F427" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G427" t="inlineStr">
+        <is>
+          <t>Gestão de Investimentos e Risco</t>
+        </is>
+      </c>
+      <c r="H427" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I427" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J427" t="inlineStr">
+        <is>
+          <t>Todas as afirmações estão corretas.</t>
+        </is>
+      </c>
+      <c r="K427" t="inlineStr">
+        <is>
+          <t>Apenas I e II estão corretas.</t>
+        </is>
+      </c>
+      <c r="L427" t="inlineStr">
+        <is>
+          <t>Apenas II e III estão corretas.</t>
+        </is>
+      </c>
+      <c r="M427" t="inlineStr">
+        <is>
+          <t>Nenhuma afirmativa está correta.</t>
+        </is>
+      </c>
+      <c r="N427" t="inlineStr">
+        <is>
+          <t>Apenas I e III estão corretas.</t>
+        </is>
+      </c>
+      <c r="O427" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P427" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q427" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="n">
+        <v>428</v>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>AOCP</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>BRDE</t>
+        </is>
+      </c>
+      <c r="D428" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E428" t="inlineStr">
+        <is>
+          <t>O Fluxo de Caixa Descontado (FCD) é uma das metodologias utilizadas na avaliação de empresas. A esse respeito, assinale a alternativa INCORRETA.</t>
+        </is>
+      </c>
+      <c r="F428" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G428" t="inlineStr">
+        <is>
+          <t>Gestão de Investimentos e Risco</t>
+        </is>
+      </c>
+      <c r="H428" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I428" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J428" t="inlineStr">
+        <is>
+          <t>Pelo FCD, o valor de uma empresa é determinado pelo fluxo de caixa projetado, descontado por uma taxa que reflita o risco associado ao investimento.</t>
+        </is>
+      </c>
+      <c r="K428" t="inlineStr">
+        <is>
+          <t>O investimento será considerado viável se o valor presente do fluxo de entradas superar o valor presente do fluxo de saídas.</t>
+        </is>
+      </c>
+      <c r="L428" t="inlineStr">
+        <is>
+          <t>O método FCD pode necessitar de adaptações em função de circunstâncias especiais, tais como: empresas com dificuldades financeiras; empresas em processo de reestruturação; empresas de capital fechado; empresas cíclicas.</t>
+        </is>
+      </c>
+      <c r="M428" t="inlineStr">
+        <is>
+          <t>A metodologia FCD baseia-se no conceito de que uma empresa que gera retorno mais alto precisará investir menos para gerar fluxos de caixa mais altos.</t>
+        </is>
+      </c>
+      <c r="N428" t="inlineStr">
+        <is>
+          <t>A avaliação de empresas, pelo método do FCD, não deve considerar o cálculo do valor residual e o cálculo do valor da empresa.</t>
+        </is>
+      </c>
+      <c r="O428" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P428" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q428" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="n">
+        <v>429</v>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>AOCP</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>Prefeitura de Juiz de Fora - MG</t>
+        </is>
+      </c>
+      <c r="D429" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E429" t="inlineStr">
+        <is>
+          <t>Qual é o critério utilizado para a avaliação econômicofinanceira de investimentos que levam em conta o valor do dinheiro no tempo?</t>
+        </is>
+      </c>
+      <c r="F429" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G429" t="inlineStr">
+        <is>
+          <t>Gestão de Investimentos e Risco</t>
+        </is>
+      </c>
+      <c r="H429" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I429" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J429" t="inlineStr">
+        <is>
+          <t>Fluxo de caixa contábil.</t>
+        </is>
+      </c>
+      <c r="K429" t="inlineStr">
+        <is>
+          <t>Fluxo de caixa econômico.</t>
+        </is>
+      </c>
+      <c r="L429" t="inlineStr">
+        <is>
+          <t>Fluxo de caixa histórico.</t>
+        </is>
+      </c>
+      <c r="M429" t="inlineStr">
+        <is>
+          <t>Fluxo de caixa descontado.</t>
+        </is>
+      </c>
+      <c r="N429" t="inlineStr">
+        <is>
+          <t>Fluxo de caixa futuro.</t>
+        </is>
+      </c>
+      <c r="O429" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P429" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q429" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="n">
+        <v>430</v>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>ANATEL</t>
+        </is>
+      </c>
+      <c r="D430" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E430" t="inlineStr">
+        <is>
+          <t>A tabela acima apresenta dados de fluxos de caixa esperados dos investimentos relativos aos projetos A, B e C. Considerando a taxa de atratividade definida para investimento igual a 5% a.a. e que 1,10 e 1,15 sejam valores aproximados para (1,05)² e (1,05)³ , respectivamente, julgue os próximos itens.
+De acordo com o método do valor presente líquido, a melhor alternativa de investimento é o projeto A.</t>
+        </is>
+      </c>
+      <c r="F430" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G430" t="inlineStr">
+        <is>
+          <t>Gestão de Investimentos e Risco</t>
+        </is>
+      </c>
+      <c r="H430" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I430" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J430" t="inlineStr"/>
+      <c r="K430" t="inlineStr"/>
+      <c r="L430" t="inlineStr"/>
+      <c r="M430" t="inlineStr"/>
+      <c r="N430" t="inlineStr"/>
+      <c r="O430" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P430" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q430" t="n">
+        <v>0</v>
+      </c>
+      <c r="R430" t="inlineStr">
+        <is>
+          <t>1117c73d-2c61-4478-8af9-8a5e9905ec44.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="n">
+        <v>431</v>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>CEBRASPE</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>INMETRO</t>
+        </is>
+      </c>
+      <c r="D431" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E431" t="inlineStr">
+        <is>
+          <t>A fim de construir uma nova planta industrial para a produção de e-books, uma empresa estimou que os investimentos necessários sejam de 10 milhões de reais e que a construção da fábrica e a instalação dos equipamentos levem um ano, mas, que, em razão de questões contratuais, todo o investimento será realizado imediatamente.
+Nessa situação, para uma taxa de desconto de 10%, o valor presente líquido, em reais, será de</t>
+        </is>
+      </c>
+      <c r="F431" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G431" t="inlineStr">
+        <is>
+          <t>Gestão de Investimentos e Risco</t>
+        </is>
+      </c>
+      <c r="H431" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I431" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J431" t="inlineStr">
+        <is>
+          <t>8 milhões.</t>
+        </is>
+      </c>
+      <c r="K431" t="inlineStr">
+        <is>
+          <t>10 milhões.</t>
+        </is>
+      </c>
+      <c r="L431" t="inlineStr">
+        <is>
+          <t>12 milhões.</t>
+        </is>
+      </c>
+      <c r="M431" t="inlineStr">
+        <is>
+          <t>20 milhões.</t>
+        </is>
+      </c>
+      <c r="N431" t="inlineStr">
+        <is>
+          <t>22 milhões.</t>
+        </is>
+      </c>
+      <c r="O431" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P431" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q431" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="n">
+        <v>432</v>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>FUNIVERSA</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>EMBRATUR</t>
+        </is>
+      </c>
+      <c r="D432" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E432" t="inlineStr">
+        <is>
+          <t>Com relação aos estudos de viabilidade de um projeto de investimento, assinale a alternativa correta.</t>
+        </is>
+      </c>
+      <c r="F432" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G432" t="inlineStr">
+        <is>
+          <t>Gestão de Investimentos e Risco</t>
+        </is>
+      </c>
+      <c r="H432" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I432" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J432" t="inlineStr">
+        <is>
+          <t>Quando o valor presente líquido for maior que zero, rejeita-se o projeto.</t>
+        </is>
+      </c>
+      <c r="K432" t="inlineStr">
+        <is>
+          <t>Quando a taxa interna de retorno for menor que a taxa mínima de atratividade, aceita-se o projeto.</t>
+        </is>
+      </c>
+      <c r="L432" t="inlineStr">
+        <is>
+          <t>Quando o valor presente líquido for menor que zero, aceita-se o projeto.</t>
+        </is>
+      </c>
+      <c r="M432" t="inlineStr">
+        <is>
+          <t>Quando a taxa interna de retorno for maior que a taxa mínima de atratividade, aceita-se o projeto.</t>
+        </is>
+      </c>
+      <c r="N432" t="inlineStr">
+        <is>
+          <t>Quando a taxa interna de retorno for maior que a taxa mínima de atratividade, rejeita-se o projeto.</t>
+        </is>
+      </c>
+      <c r="O432" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P432" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q432" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="n">
+        <v>433</v>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>ANP</t>
+        </is>
+      </c>
+      <c r="D433" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E433" t="inlineStr">
+        <is>
+          <t>A taxa interna de retorno (TIR) do fluxo financeiro de qualquer projeto de investimento é</t>
+        </is>
+      </c>
+      <c r="F433" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G433" t="inlineStr">
+        <is>
+          <t>Gestão de Investimentos e Risco</t>
+        </is>
+      </c>
+      <c r="H433" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I433" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J433" t="inlineStr">
+        <is>
+          <t>sempre positiva.</t>
+        </is>
+      </c>
+      <c r="K433" t="inlineStr">
+        <is>
+          <t>igual à taxa de juros do mercado.</t>
+        </is>
+      </c>
+      <c r="L433" t="inlineStr">
+        <is>
+          <t>igual ao custo de capital para o investidor.</t>
+        </is>
+      </c>
+      <c r="M433" t="inlineStr">
+        <is>
+          <t>a taxa de desconto que anula o valor presente líquido (VPL) do fluxo financeiro.</t>
+        </is>
+      </c>
+      <c r="N433" t="inlineStr">
+        <is>
+          <t>o único critério válido para determinar se vale a pena fazer o investimento.</t>
+        </is>
+      </c>
+      <c r="O433" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P433" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q433" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="n">
+        <v>434</v>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>TERMOBAHIA</t>
+        </is>
+      </c>
+      <c r="D434" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="E434" t="inlineStr">
+        <is>
+          <t>Os modais de transporte podem ser classificados por diversas características operacionais, entre as quais a capacidade, velocidade, disponibilidade, confiabilidade e frequência.
+Em qual destas características o modal aquaviário apresenta uma melhor performance que os modais ferroviário, rodoviário, dutoviário e aéreo?</t>
+        </is>
+      </c>
+      <c r="F434" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G434" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="H434" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I434" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J434" t="inlineStr">
+        <is>
+          <t>capacidade</t>
+        </is>
+      </c>
+      <c r="K434" t="inlineStr">
+        <is>
+          <t>velocidade</t>
+        </is>
+      </c>
+      <c r="L434" t="inlineStr">
+        <is>
+          <t>disponibilidade</t>
+        </is>
+      </c>
+      <c r="M434" t="inlineStr">
+        <is>
+          <t>confiabilidade</t>
+        </is>
+      </c>
+      <c r="N434" t="inlineStr">
+        <is>
+          <t>frequência</t>
+        </is>
+      </c>
+      <c r="O434" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P434" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q434" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="n">
+        <v>435</v>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>Câmara dos Deputados</t>
+        </is>
+      </c>
+      <c r="D435" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="E435" t="inlineStr">
+        <is>
+          <t>Julgue os itens subsequentes, referentes às características das modalidades de transporte.
+O transporte ferroviário, embora eficiente no consumo de combustível, demanda custos fixos elevados em relação à ferrovia.</t>
+        </is>
+      </c>
+      <c r="F435" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G435" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="H435" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I435" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J435" t="inlineStr"/>
+      <c r="K435" t="inlineStr"/>
+      <c r="L435" t="inlineStr"/>
+      <c r="M435" t="inlineStr"/>
+      <c r="N435" t="inlineStr"/>
+      <c r="O435" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P435" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q435" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="n">
+        <v>436</v>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D436" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="E436" t="inlineStr">
+        <is>
+          <t>Sobre o modal ferroviário, seus equipamentos e características de desempenho é INCORRETO afirmar que:</t>
+        </is>
+      </c>
+      <c r="F436" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G436" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="H436" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I436" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J436" t="inlineStr">
+        <is>
+          <t>apresenta o menor custo fixo dentre todos os modais e maior custo variável.</t>
+        </is>
+      </c>
+      <c r="K436" t="inlineStr">
+        <is>
+          <t>oferece capacidade de transportar grandes volumes de carga em longas distâncias, com média a alta variabilidade de tempo de trânsito.</t>
+        </is>
+      </c>
+      <c r="L436" t="inlineStr">
+        <is>
+          <t>é indicado para transportar matérias-primas como carvão, madeira e produtos químicos e também produtos de baixo valor agregado, como alimentos, papel e produtos de madeira.</t>
+        </is>
+      </c>
+      <c r="M436" t="inlineStr">
+        <is>
+          <t>há redução do tempo exigido no intercâmbio de vagões com o uso de vagões articulados com chassi estendido para carregar diversos contêineres em uma única unidade flexível.</t>
+        </is>
+      </c>
+      <c r="N436" t="inlineStr">
+        <is>
+          <t>há duplicação da capacidade de cada vagão ao se utilizarem vagões-plataforma construídos para transportar dois níveis de contêineres.</t>
+        </is>
+      </c>
+      <c r="O436" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P436" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q436" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="n">
+        <v>437</v>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D437" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="E437" t="inlineStr">
+        <is>
+          <t>A escolha do modal de transporte mais adequado para o transporte de cargas é uma das decisões-chave na Logística. A escolha dependerá das características do produto, prazo da entrega, riscos envolvidos e do custo total do transporte. Em relação às características de desempenho, o modal de transporte</t>
+        </is>
+      </c>
+      <c r="F437" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G437" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="H437" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I437" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J437" t="inlineStr">
+        <is>
+          <t>ferroviário é adequado para transportar cargas de alto valor agregado.</t>
+        </is>
+      </c>
+      <c r="K437" t="inlineStr">
+        <is>
+          <t>ferroviário é apropriado para cargas a granel, sendo considerado o mais lento dentre todos os modais.</t>
+        </is>
+      </c>
+      <c r="L437" t="inlineStr">
+        <is>
+          <t>aéreo apresenta a menor variabilidade de tempo de entrega e o maior custo por toneladaquilômetro.</t>
+        </is>
+      </c>
+      <c r="M437" t="inlineStr">
+        <is>
+          <t>dutoviário apresenta grande flexibilidade de transporte de produtos em relação aos outros modais, sendo indicado para transporte de produtos de alto valor agregado.</t>
+        </is>
+      </c>
+      <c r="N437" t="inlineStr">
+        <is>
+          <t>rodoviário será sempre mais rápido, considerando o tempo de entrega porta a porta.</t>
+        </is>
+      </c>
+      <c r="O437" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P437" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q437" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="n">
+        <v>438</v>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D438" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E438" t="inlineStr">
+        <is>
+          <t>Os cinco principais tipos de modais de transporte são: o ferroviário, o rodoviário, o aquaviário, o dutoviário e o aéreo. Cada tipo de modal é mais adaptado para um tipo de carga. O modal rodoviário é mais adaptado para transportar</t>
+        </is>
+      </c>
+      <c r="F438" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G438" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="H438" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I438" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J438" t="inlineStr">
+        <is>
+          <t>produtos da indústria extrativa, pesada e commodities agrícolas</t>
+        </is>
+      </c>
+      <c r="K438" t="inlineStr">
+        <is>
+          <t>produtos leves e médios, entre distribuidores e atacadistas</t>
+        </is>
+      </c>
+      <c r="L438" t="inlineStr">
+        <is>
+          <t>commodities de mineração, básicos a granel, produtos químicos, cimento e alguns produtos agrícolas</t>
+        </is>
+      </c>
+      <c r="M438" t="inlineStr">
+        <is>
+          <t>petróleo e misturas semifluidas de carvão</t>
+        </is>
+      </c>
+      <c r="N438" t="inlineStr">
+        <is>
+          <t>todos os tipos de commodities e envios de urgência</t>
+        </is>
+      </c>
+      <c r="O438" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P438" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q438" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="n">
+        <v>439</v>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>UFMT</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>UFSBA</t>
+        </is>
+      </c>
+      <c r="D439" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="E439" t="inlineStr">
+        <is>
+          <t>Em relação aos tipos de Logística de Transportes, analise as assertivas.
+I - O transporte aquaviário, é todo e qualquer tipo de transporte e movimentação realizado em vias aquáticas. É dividido em: transporte marítimo, transporte fluvial e transporte lacustre.
+II - O modal lacustre tem as mesmas características do fluvial, porém o transporte é em lagos. Essa modalidade no Brasil é muito pequena, podendo ser considerada como desprezível, não tendo importância relativa no transporte de cargas.
+III - O transporte fluvial é realizado em rios, a utilização no Brasil ainda é muito pequena. É um transporte de baixo custo. O grande volume de mercadorias transportadas por esse modal é de produtos agrícolas, minérios, derivados de petróleo, álcool e assemelhados.
+IV - O transporte aéreo diferencia-se dos demais com as seguintes características: maior agilidade no transporte; remessa de mercadorias de pouco volume/peso e muito valor; mercadorias com prioridade de entrega (urgência).
+Está correto o que se afirma em:</t>
+        </is>
+      </c>
+      <c r="F439" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G439" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="H439" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I439" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J439" t="inlineStr">
+        <is>
+          <t>I, II e IV, apenas.</t>
+        </is>
+      </c>
+      <c r="K439" t="inlineStr">
+        <is>
+          <t>I, II, III e IV.</t>
+        </is>
+      </c>
+      <c r="L439" t="inlineStr">
+        <is>
+          <t>I e IV, apenas.</t>
+        </is>
+      </c>
+      <c r="M439" t="inlineStr">
+        <is>
+          <t>II e III, apenas.</t>
+        </is>
+      </c>
+      <c r="N439" t="inlineStr"/>
+      <c r="O439" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P439" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q439" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="n">
+        <v>440</v>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>UEG</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>TJ-GO</t>
+        </is>
+      </c>
+      <c r="D440" t="inlineStr">
+        <is>
+          <t>2006</t>
+        </is>
+      </c>
+      <c r="E440" t="inlineStr">
+        <is>
+          <t>As três atividades logísticas primárias são:</t>
+        </is>
+      </c>
+      <c r="F440" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G440" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="H440" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I440" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J440" t="inlineStr">
+        <is>
+          <t>Transportes, manutenção de estoque, processamento de pedidos</t>
+        </is>
+      </c>
+      <c r="K440" t="inlineStr">
+        <is>
+          <t>Transportes, localização, processamento de pedidos</t>
+        </is>
+      </c>
+      <c r="L440" t="inlineStr">
+        <is>
+          <t>Transportes, manutenção de estoque, localização</t>
+        </is>
+      </c>
+      <c r="M440" t="inlineStr">
+        <is>
+          <t>Transportes, localização, compras</t>
+        </is>
+      </c>
+      <c r="N440" t="inlineStr"/>
+      <c r="O440" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P440" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q440" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="n">
+        <v>441</v>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Colégio Pedro II</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>Colégio Pedro II</t>
+        </is>
+      </c>
+      <c r="D441" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E441" t="inlineStr">
+        <is>
+          <t>O transporte é o elemento mais importante nos custos logísticos para a maioria das empresas. O usuário do transporte tem uma larga faixa de serviços à sua disposição, todos girando em torno dos cinco modais básicos (aquaviário, ferroviário, rodoviário, aeroviário e dutoviário).
+No que se refere a esses modais de transporte básicos, é correto afirmar que</t>
+        </is>
+      </c>
+      <c r="F441" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G441" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="H441" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I441" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J441" t="inlineStr">
+        <is>
+          <t>o transporte rodoviário é semelhante ao ferroviário, mas movimenta fretes médios, em extensões médias e com a vantagem de serviços porta a porta.</t>
+        </is>
+      </c>
+      <c r="K441" t="inlineStr">
+        <is>
+          <t>o modal aquaviário é mais veloz que o ferroviário, mas tem capacidade de transporte reduzida.</t>
+        </is>
+      </c>
+      <c r="L441" t="inlineStr">
+        <is>
+          <t>a ferrovia é uma boa opção para pequenas distâncias e movimentação lenta de produtos de alto valor</t>
+        </is>
+      </c>
+      <c r="M441" t="inlineStr">
+        <is>
+          <t>o transporte por dutovias é veloz e oferece uma extensa faixa de serviços e capacidades.</t>
+        </is>
+      </c>
+      <c r="N441" t="inlineStr"/>
+      <c r="O441" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P441" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q441" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="n">
+        <v>442</v>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D442" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="E442" t="inlineStr">
+        <is>
+          <t>Uma empresa que transporte uma mercadoria por vias urbanas não exclusivas e depois por via de cabotagem está utilizando, respectivamente, os seguintes modais:</t>
+        </is>
+      </c>
+      <c r="F442" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G442" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="H442" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I442" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J442" t="inlineStr">
+        <is>
+          <t>rodoviário e metroviário</t>
+        </is>
+      </c>
+      <c r="K442" t="inlineStr">
+        <is>
+          <t>rodoviário e ferroviário</t>
+        </is>
+      </c>
+      <c r="L442" t="inlineStr">
+        <is>
+          <t>rodoviário e marítimo</t>
+        </is>
+      </c>
+      <c r="M442" t="inlineStr">
+        <is>
+          <t>metroviário e ferroviário</t>
+        </is>
+      </c>
+      <c r="N442" t="inlineStr">
+        <is>
+          <t>metroviário e marítimo</t>
+        </is>
+      </c>
+      <c r="O442" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P442" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q442" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="n">
+        <v>443</v>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>UFLA</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>UFLA</t>
+        </is>
+      </c>
+      <c r="D443" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E443" t="inlineStr">
+        <is>
+          <t>Analise as proposições a seguir, referentes à especificação e à codificação de materiais:
+I. A especificação de materiais propicia, entre outras, facilidades às tarefas de coleta de preços, cuidados no transporte, na identificação, na inspeção, na armazenagem e na preservação de materiais.
+II. A codificação de materiais tem o objetivo de diminuir o número de itens no estoque, evitando a variedade de materiais de mesma classe.
+III. Os planos de codificação seguem, de um modo geral, o mesmo princípio, dividindo os materiais em grupos e classes de materiais.
+IV. O sistema de codificação decimal dos materiais divide o universo de materiais em grandes grupos, de acordo com sua estrutura, e é composta por 11 dígitos, sendo os últimos 4 dígitos para indicar a classe do material.
+Assinale a alternativa CORRETA:</t>
+        </is>
+      </c>
+      <c r="F443" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G443" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="H443" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I443" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J443" t="inlineStr">
+        <is>
+          <t>Somente as proposições I e IV estão corretas.</t>
+        </is>
+      </c>
+      <c r="K443" t="inlineStr">
+        <is>
+          <t>Somente as proposições II e III estão corretas.</t>
+        </is>
+      </c>
+      <c r="L443" t="inlineStr">
+        <is>
+          <t>Somente as proposições III e IV estão corretas.</t>
+        </is>
+      </c>
+      <c r="M443" t="inlineStr">
+        <is>
+          <t>Somente as proposições I e III estão corretas.</t>
+        </is>
+      </c>
+      <c r="N443" t="inlineStr"/>
+      <c r="O443" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P443" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q443" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="n">
+        <v>444</v>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>QUADRIX</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>CRO-GO</t>
+        </is>
+      </c>
+      <c r="D444" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="E444" t="inlineStr">
+        <is>
+          <t>Almoxarifado é o local destinado à guarda e conservação de materiais, em recinto coberto ou não, adequado à sua natureza, tendo a função de destinar espaços onde cada item permanecerá aguardando a necessidade de seu uso, ficando a localização, a disposição interna e os equipamentos acondicionados à política geral de estoques da organização. Um sistema de classificação e codificação de materiais é fundamental para que existam procedimentos de armazenagem apropriados, um controle eficiente dos estoques e uma operacionalização correta do almoxarifado. Quando dois ou mais itens de estoque podem ser usados para o mesmo fim, recomenda-se a escolha pelo uso de um deles. Essa redução da diversidade de itens empregados para uma mesma finalidade é conhecida por:</t>
+        </is>
+      </c>
+      <c r="F444" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G444" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="H444" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I444" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J444" t="inlineStr">
+        <is>
+          <t>Padronização.</t>
+        </is>
+      </c>
+      <c r="K444" t="inlineStr">
+        <is>
+          <t>Normalização.</t>
+        </is>
+      </c>
+      <c r="L444" t="inlineStr">
+        <is>
+          <t>Simplificação.</t>
+        </is>
+      </c>
+      <c r="M444" t="inlineStr">
+        <is>
+          <t>Especificação.</t>
+        </is>
+      </c>
+      <c r="N444" t="inlineStr">
+        <is>
+          <t>Catalogação.</t>
+        </is>
+      </c>
+      <c r="O444" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P444" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q444" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="n">
+        <v>445</v>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>FMP Concursos</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>PROCEMPA</t>
+        </is>
+      </c>
+      <c r="D445" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="E445" t="inlineStr">
+        <is>
+          <t>Sobre o Transportation Management System – TMS, assinale V para as assertivas verdadeiras ou F para as falsas.
+( ) Redução nos custos de transportes, melhoria do nível de serviço e a utilização dos recursos de transportes.
+( ) É um sistema que contempla as várias áreas de uma empresa, desde o chão de fábrica até a alta direção, permitindo um maior controle de todo o processo produtivo e disponibilizando elementos que podem facilitar a tomada de decisão.
+( ) Melhoria na composição de cargas (consolidação), rotas, menor tempo necessário para planejar a distribuição e a montagem de cargas.
+( ) Disponibilidade de dados acurados dos custos de frete mostrado de várias formas, como por exemplos por cliente ou por produto.
+( ) Acompanhamento da evolução dos custos com transportes.
+Assinale a alternativa que apresenta a sequência correta.</t>
+        </is>
+      </c>
+      <c r="F445" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G445" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="H445" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I445" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J445" t="inlineStr">
+        <is>
+          <t>A sequência correta é: F – F – V – V – V.</t>
+        </is>
+      </c>
+      <c r="K445" t="inlineStr">
+        <is>
+          <t>A sequência correta é: F – F – V – F – V.</t>
+        </is>
+      </c>
+      <c r="L445" t="inlineStr">
+        <is>
+          <t>A sequência correta é: V – V – F – V – F.</t>
+        </is>
+      </c>
+      <c r="M445" t="inlineStr">
+        <is>
+          <t>A sequência correta é: V – F – V – V – V.</t>
+        </is>
+      </c>
+      <c r="N445" t="inlineStr">
+        <is>
+          <t>A sequência correta é: F – V – F – V – F.</t>
+        </is>
+      </c>
+      <c r="O445" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P445" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q445" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="n">
+        <v>446</v>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Vunesp</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>TJ-SP</t>
+        </is>
+      </c>
+      <c r="D446" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E446" t="inlineStr">
+        <is>
+          <t>O instrumento de desenvolvimento econômico e social caracterizado por um conjunto de ações, procedimentos e meios destinados a viabilizar a coleta e a restituição dos resíduos sólidos ao setor empresarial, para reaproveitamento, em seu ciclo ou em outros ciclos produtivos, ou outra destinação final ambientalmente adequada, e que permite o descarte apropriado de materiais e principalmente a preservação ambiental, é</t>
+        </is>
+      </c>
+      <c r="F446" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G446" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="H446" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I446" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J446" t="inlineStr">
+        <is>
+          <t>logística reversa.</t>
+        </is>
+      </c>
+      <c r="K446" t="inlineStr">
+        <is>
+          <t>monitoramento ambiental.</t>
+        </is>
+      </c>
+      <c r="L446" t="inlineStr">
+        <is>
+          <t>monitoramento de desempenho ambiental.</t>
+        </is>
+      </c>
+      <c r="M446" t="inlineStr">
+        <is>
+          <t>trade-off logístico.</t>
+        </is>
+      </c>
+      <c r="N446" t="inlineStr">
+        <is>
+          <t>logística integrada.</t>
+        </is>
+      </c>
+      <c r="O446" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P446" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q446" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="n">
+        <v>447</v>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D447" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E447" t="inlineStr">
+        <is>
+          <t>O modelo de lote econômico assume diversos aspectos para facilitar o cálculo para a quantidade a ser pedida por lote.
+Dentre essas hipóteses NÃO se encontra a</t>
+        </is>
+      </c>
+      <c r="F447" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G447" t="inlineStr">
+        <is>
+          <t>Gestão de Estoques</t>
+        </is>
+      </c>
+      <c r="H447" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I447" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J447" t="inlineStr">
+        <is>
+          <t>variabilidade de demanda</t>
+        </is>
+      </c>
+      <c r="K447" t="inlineStr">
+        <is>
+          <t>saída de estoque de forma linear</t>
+        </is>
+      </c>
+      <c r="L447" t="inlineStr">
+        <is>
+          <t>saída de estoque de forma linear</t>
+        </is>
+      </c>
+      <c r="M447" t="inlineStr">
+        <is>
+          <t>existência de um custo de manutenção de estoque unitário fixo</t>
+        </is>
+      </c>
+      <c r="N447" t="inlineStr">
+        <is>
+          <t>proporcionalidade entre o custo de manutenção e a quantidade de estoque</t>
+        </is>
+      </c>
+      <c r="O447" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P447" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q447" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="n">
+        <v>448</v>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>BNDES</t>
+        </is>
+      </c>
+      <c r="D448" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="E448" t="inlineStr">
+        <is>
+          <t>Um revendedor de tintas obtém seu produto principal de um único fornecedor, sendo a demanda por esse produto aproximadamente constante ao longo do ano. No ano passado, o revendedor vendeu 400 litros do produto. Os custos estimados de colocação de um pedido são de cerca de R$ 12,50 cada vez que um pedido é colocado, e os custos anuais de manutenção de estoque por litro são equivalentes a 25% do custo de aquisição.
+Se o revendedor adquire o produto a R$ 36,00 por litro, quantos litros a loja deve pedir por vez, considerando a fórmula do Lote Econômico de Compra (LEC)?</t>
+        </is>
+      </c>
+      <c r="F448" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G448" t="inlineStr">
+        <is>
+          <t>Gestão de Estoques</t>
+        </is>
+      </c>
+      <c r="H448" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I448" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J448" t="inlineStr">
+        <is>
+          <t>3,00</t>
+        </is>
+      </c>
+      <c r="K448" t="inlineStr">
+        <is>
+          <t>3,33</t>
+        </is>
+      </c>
+      <c r="L448" t="inlineStr">
+        <is>
+          <t>30,00</t>
+        </is>
+      </c>
+      <c r="M448" t="inlineStr">
+        <is>
+          <t>33,33</t>
+        </is>
+      </c>
+      <c r="N448" t="inlineStr">
+        <is>
+          <t>60,00</t>
+        </is>
+      </c>
+      <c r="O448" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P448" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q448" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="n">
+        <v>449</v>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D449" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E449" t="inlineStr">
+        <is>
+          <t>A empresa ALFA está tentando reduzir custos na aquisição de determinados insumos de produção. Ela decidiu utilizar o modelo de Lote Econômico de Compra – LEC – para estimar o volume a ser comprado da peça B17. Sabe-se que a sua demanda anual é de 200 peças, o custo para manter uma unidade dessa peça em estoque durante um ano é de R$ 1,00, e o custo médio para emitir um pedido de compra é de R$ 4,00.
+Qual o LEC de peças B17?</t>
+        </is>
+      </c>
+      <c r="F449" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G449" t="inlineStr">
+        <is>
+          <t>Gestão de Estoques</t>
+        </is>
+      </c>
+      <c r="H449" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I449" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J449" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="K449" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="L449" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="M449" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="N449" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="O449" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P449" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q449" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="n">
+        <v>450</v>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>IESES</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>IESES</t>
+        </is>
+      </c>
+      <c r="D450" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E450" t="inlineStr">
+        <is>
+          <t>Uma das restrições para utilização do Modelo de Lote Econômico de Compra é que:</t>
+        </is>
+      </c>
+      <c r="F450" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G450" t="inlineStr">
+        <is>
+          <t>Gestão de Estoques</t>
+        </is>
+      </c>
+      <c r="H450" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I450" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J450" t="inlineStr">
+        <is>
+          <t>O item ser nacional.</t>
+        </is>
+      </c>
+      <c r="K450" t="inlineStr">
+        <is>
+          <t>Ter um acordo de nível de serviço.</t>
+        </is>
+      </c>
+      <c r="L450" t="inlineStr">
+        <is>
+          <t>Ele só funciona em ambientes milk run.</t>
+        </is>
+      </c>
+      <c r="M450" t="inlineStr">
+        <is>
+          <t>O fornecedor ser próximo a fábrica.</t>
+        </is>
+      </c>
+      <c r="N450" t="inlineStr">
+        <is>
+          <t>A demanda tem que ser linear.</t>
+        </is>
+      </c>
+      <c r="O450" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P450" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q450" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="n">
+        <v>451</v>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>Transpetro</t>
+        </is>
+      </c>
+      <c r="D451" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E451" t="inlineStr">
+        <is>
+          <t>A função de cálculo do lote econômico de compras (LEC) é derivada de duas equações.
+Essas equações são as de custos</t>
+        </is>
+      </c>
+      <c r="F451" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G451" t="inlineStr">
+        <is>
+          <t>Gestão de Estoques</t>
+        </is>
+      </c>
+      <c r="H451" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I451" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J451" t="inlineStr">
+        <is>
+          <t>de estocar e do capital de giro</t>
+        </is>
+      </c>
+      <c r="K451" t="inlineStr">
+        <is>
+          <t>de estocar e do pedido</t>
+        </is>
+      </c>
+      <c r="L451" t="inlineStr">
+        <is>
+          <t>do pedido e do capital de giro</t>
+        </is>
+      </c>
+      <c r="M451" t="inlineStr">
+        <is>
+          <t>do lote e da unidade</t>
+        </is>
+      </c>
+      <c r="N451" t="inlineStr">
+        <is>
+          <t>do capital de giro e de custo médio de estoque</t>
+        </is>
+      </c>
+      <c r="O451" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P451" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q451" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="n">
+        <v>452</v>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>VUNESP</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>Prefeitura de Guararapes - SP</t>
+        </is>
+      </c>
+      <c r="D452" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E452" t="inlineStr">
+        <is>
+          <t>Ponto de ressuprimento é :</t>
+        </is>
+      </c>
+      <c r="F452" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G452" t="inlineStr">
+        <is>
+          <t>Gestão de Estoques</t>
+        </is>
+      </c>
+      <c r="H452" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I452" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J452" t="inlineStr">
+        <is>
+          <t>um parâmetro de alerta no dimensionamento de estoques.</t>
+        </is>
+      </c>
+      <c r="K452" t="inlineStr">
+        <is>
+          <t>um nível de estoque que, ao ser atingido, sinaliza o momento de se fazer a previsão de nova compra.</t>
+        </is>
+      </c>
+      <c r="L452" t="inlineStr">
+        <is>
+          <t>a quantidade de cada item que deve ser mantida como reserva para garantir a continuidade do atendimento em caso de ocorrência não prevista, como elevação brusca no consumo e atraso no suprimento</t>
+        </is>
+      </c>
+      <c r="M452" t="inlineStr">
+        <is>
+          <t>o nível do estoque de segurança que evita ruptura do atendimento.</t>
+        </is>
+      </c>
+      <c r="N452" t="inlineStr">
+        <is>
+          <t>uma técnica quantitativa que utiliza dados históricos de consumo como base para determinação de padrões que podem se repetir no futuro.</t>
+        </is>
+      </c>
+      <c r="O452" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P452" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q452" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="n">
+        <v>453</v>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>FUNDEP</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>IFSP</t>
+        </is>
+      </c>
+      <c r="D453" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E453" t="inlineStr">
+        <is>
+          <t>Newson, o novo encarregado de produção, está com dificuldades de estabelecer os lotes de produção em função da sua inabilidade em calcular o ponto de ressuprimento. Os valores observados por Newson são os seguintes: DM = 1.250; TR = 12h.
+De acordo com os dados acima, assinale a alternativa que apresenta CORRETAMENTE o ponto de ressuprimento.</t>
+        </is>
+      </c>
+      <c r="F453" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G453" t="inlineStr">
+        <is>
+          <t>Gestão de Estoques</t>
+        </is>
+      </c>
+      <c r="H453" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I453" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J453" t="inlineStr">
+        <is>
+          <t>105 unidades.</t>
+        </is>
+      </c>
+      <c r="K453" t="inlineStr">
+        <is>
+          <t>2.500 unidades.</t>
+        </is>
+      </c>
+      <c r="L453" t="inlineStr">
+        <is>
+          <t>12.500 unidades.</t>
+        </is>
+      </c>
+      <c r="M453" t="inlineStr">
+        <is>
+          <t>15.000 unidades.</t>
+        </is>
+      </c>
+      <c r="N453" t="inlineStr"/>
+      <c r="O453" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P453" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q453" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="n">
+        <v>454</v>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>ANCINE</t>
+        </is>
+      </c>
+      <c r="D454" t="inlineStr">
+        <is>
+          <t>2006</t>
+        </is>
+      </c>
+      <c r="E454" t="inlineStr">
+        <is>
+          <t>Com referência à administração de bens materiais, julgue o item que se segue.
+Entre as técnicas não-matemáticas de previsão de consumo, a projeção que admite que o futuro será
+repetição do passado e a explicação que relaciona os quantitativos com alguma variável cuja evolução
+é conhecida ou previsível são as mais utilizadas.</t>
+        </is>
+      </c>
+      <c r="F454" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G454" t="inlineStr">
+        <is>
+          <t>Previsão da Demanda</t>
+        </is>
+      </c>
+      <c r="H454" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I454" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J454" t="inlineStr"/>
+      <c r="K454" t="inlineStr"/>
+      <c r="L454" t="inlineStr"/>
+      <c r="M454" t="inlineStr"/>
+      <c r="N454" t="inlineStr"/>
+      <c r="O454" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P454" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q454" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="n">
+        <v>455</v>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>CNMP</t>
+        </is>
+      </c>
+      <c r="D455" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="E455" t="inlineStr">
+        <is>
+          <t>Na gestão de riscos, o método Delphi é usado para</t>
+        </is>
+      </c>
+      <c r="F455" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G455" t="inlineStr">
+        <is>
+          <t>Previsão da Demanda</t>
+        </is>
+      </c>
+      <c r="H455" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I455" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J455" t="inlineStr">
+        <is>
+          <t>identificação dos riscos. Trata-se de uma técnica de coleta de informações que objetiva alcançar um consenso de especialistas em um assunto.</t>
+        </is>
+      </c>
+      <c r="K455" t="inlineStr">
+        <is>
+          <t>avaliação dos riscos. Trata-se de um quadro de pontuação que prioriza os riscos e as tomadas de decisão para cada situação.</t>
+        </is>
+      </c>
+      <c r="L455" t="inlineStr">
+        <is>
+          <t>análise dos riscos. Trata-se de uma técnica de avaliação de causas-raiz de um problema e propõe uma solução bem definida para cada situação de risco.</t>
+        </is>
+      </c>
+      <c r="M455" t="inlineStr">
+        <is>
+          <t>identificação dos riscos. Trata-se de um workflow de soluções direcionadas para a mitigação dos riscos</t>
+        </is>
+      </c>
+      <c r="N455" t="inlineStr">
+        <is>
+          <t>análise dos riscos. Trata-se de um diagrama do tipo “espinha de peixe” que serve para melhorar os processos.</t>
+        </is>
+      </c>
+      <c r="O455" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P455" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q455" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>456</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>FGV</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>IBGE</t>
+        </is>
+      </c>
+      <c r="D456" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E456" t="inlineStr">
+        <is>
+          <t>Os métodos estatísticos mais comuns para previsão de demandas, de acordo com o tamanho, a complexidade e o tipo de demanda são: (1) média aritmética; (2) média móvel; (3) média ponderada exponencialmente; (4) regressão; e (5) modelos econométricos. Entre essas variedades, o conceito mais preciso para a média móvel é:</t>
+        </is>
+      </c>
+      <c r="F456" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G456" t="inlineStr">
+        <is>
+          <t>Previsão da Demanda</t>
+        </is>
+      </c>
+      <c r="H456" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I456" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J456" t="inlineStr">
+        <is>
+          <t>forma de média aritmética empregada para prever demandas sazonais;</t>
+        </is>
+      </c>
+      <c r="K456" t="inlineStr">
+        <is>
+          <t>média que aplica dados empíricos, incorporando termos residuais diversos, não disponíveis na série histórica;</t>
+        </is>
+      </c>
+      <c r="L456" t="inlineStr">
+        <is>
+          <t>média aritmética, calculada período a período, empregada, principalmente, para a projeção de demandas;</t>
+        </is>
+      </c>
+      <c r="M456" t="inlineStr">
+        <is>
+          <t>medida de tendência central, obtida a partir de uma massa dispersa de dados;</t>
+        </is>
+      </c>
+      <c r="N456" t="inlineStr">
+        <is>
+          <t>média aritmética, de uma série de dados, com a substituição, a cada período, do dado mais antigo pelo mais recente.</t>
+        </is>
+      </c>
+      <c r="O456" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P456" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q456" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="n">
+        <v>457</v>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>BR Distribuidora</t>
+        </is>
+      </c>
+      <c r="D457" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="E457" t="inlineStr">
+        <is>
+          <t>Uma companhia comercial que controla seus estoques pelo inventário permanente apresentou as seguintes informações relativas à movimentação de mercadorias no mês novembro de 2012
+Considerando-se exclusivamente os dados informados e adotando-se o método da Média Ponderada
+Móvel, o estoque final de mercadorias, no mês de novembro/2012, em reais, é um número entre:</t>
+        </is>
+      </c>
+      <c r="F457" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G457" t="inlineStr">
+        <is>
+          <t>Previsão da Demanda</t>
+        </is>
+      </c>
+      <c r="H457" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I457" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J457" t="inlineStr">
+        <is>
+          <t>5.000 e 6.000</t>
+        </is>
+      </c>
+      <c r="K457" t="inlineStr">
+        <is>
+          <t>6.000 e 7.000</t>
+        </is>
+      </c>
+      <c r="L457" t="inlineStr">
+        <is>
+          <t>7.000 e 8.000</t>
+        </is>
+      </c>
+      <c r="M457" t="inlineStr">
+        <is>
+          <t>8.000 e 9.000</t>
+        </is>
+      </c>
+      <c r="N457" t="inlineStr">
+        <is>
+          <t>9.000 e 10.000</t>
+        </is>
+      </c>
+      <c r="O457" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P457" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q457" t="n">
+        <v>0</v>
+      </c>
+      <c r="R457" t="inlineStr">
+        <is>
+          <t>8d8ea1fc-a37e-4b0d-af4e-2be03f86a70a.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="n">
+        <v>458</v>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>FGV</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>IBGE</t>
+        </is>
+      </c>
+      <c r="D458" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E458" t="inlineStr">
+        <is>
+          <t>A média móvel ponderada exponencialmente consiste em um método semelhante ao da média móvel clássica, contudo com cálculo mais simples. Dessa forma, é correto afirmar que o coeficiente de ajustamento α – alfa – utilizado no método de média móvel ponderada exponencialmente apresenta um valor inversamente proporcional:</t>
+        </is>
+      </c>
+      <c r="F458" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G458" t="inlineStr">
+        <is>
+          <t>Previsão da Demanda</t>
+        </is>
+      </c>
+      <c r="H458" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I458" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J458" t="inlineStr">
+        <is>
+          <t>ao número n empregado para o cálculo da média móvel;</t>
+        </is>
+      </c>
+      <c r="K458" t="inlineStr">
+        <is>
+          <t>ao número de dados da série histórica empregada;</t>
+        </is>
+      </c>
+      <c r="L458" t="inlineStr">
+        <is>
+          <t>à média calculada no período de previsão anterior;</t>
+        </is>
+      </c>
+      <c r="M458" t="inlineStr">
+        <is>
+          <t>à correlação dos dados;</t>
+        </is>
+      </c>
+      <c r="N458" t="inlineStr">
+        <is>
+          <t>à 50% do número de dados da série histórica empregada.</t>
+        </is>
+      </c>
+      <c r="O458" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P458" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q458" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="n">
+        <v>459</v>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>UFG</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>CS-UFG</t>
+        </is>
+      </c>
+      <c r="D459" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E459" t="inlineStr">
+        <is>
+          <t>O processo estocástico é definido como:</t>
+        </is>
+      </c>
+      <c r="F459" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G459" t="inlineStr">
+        <is>
+          <t>Pesquisa Operacional</t>
+        </is>
+      </c>
+      <c r="H459" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I459" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J459" t="inlineStr">
+        <is>
+          <t>um processo estacionário de variáveis contínuas relacionado a cadeias de valores fixos ao longo do tempo.</t>
+        </is>
+      </c>
+      <c r="K459" t="inlineStr">
+        <is>
+          <t>uma família de variáveis aleatórias que representam a evolução do estado de um sistema de valores com o tempo.</t>
+        </is>
+      </c>
+      <c r="L459" t="inlineStr">
+        <is>
+          <t>um processo de formação e controle de estoques físicos em um sistema com capacidade finita.</t>
+        </is>
+      </c>
+      <c r="M459" t="inlineStr">
+        <is>
+          <t>um conjunto de sistemas estáticos e reacionários que dependem de análise de variância estatística.</t>
+        </is>
+      </c>
+      <c r="N459" t="inlineStr"/>
+      <c r="O459" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P459" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q459" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="n">
+        <v>460</v>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>UPE</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>Prefeitura de Olinda</t>
+        </is>
+      </c>
+      <c r="D460" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E460" t="inlineStr">
+        <is>
+          <t>A Pesquisa Operacional (PO) é uma ciência que objetiva fornecer ferramentas quantitativas ao processo de tomada de decisões. Um dos modelos utilizados na PO é o modelo de programa linear. Assinale a opção incorreta no que diz respeito a esse modelo de otimização.</t>
+        </is>
+      </c>
+      <c r="F460" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G460" t="inlineStr">
+        <is>
+          <t>Pesquisa Operacional</t>
+        </is>
+      </c>
+      <c r="H460" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I460" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J460" t="inlineStr">
+        <is>
+          <t>Os problemas de programação linear (PL) tentam otimizar (maximizar ou minimizar) uma função linear das variáveis de decisão, chamada de função-objetivo.</t>
+        </is>
+      </c>
+      <c r="K460" t="inlineStr">
+        <is>
+          <t>As variáveis de decisão compõem tanto a função-objetivo como as restrições e são, em geral, designadas por letras como x, y, z, etc. ou por uma letra indexada como x1, x2, etc</t>
+        </is>
+      </c>
+      <c r="L460" t="inlineStr">
+        <is>
+          <t>A Programação Linear é uma programação matemática utilizada na determinação de valores possíveis para variáveis de decisão.</t>
+        </is>
+      </c>
+      <c r="M460" t="inlineStr">
+        <is>
+          <t>Na Programação Linear, assume-se que a função-objetivo é linear e que as restrições são expressas através de equações ou inequações não lineares.</t>
+        </is>
+      </c>
+      <c r="N460" t="inlineStr">
+        <is>
+          <t>Dentre os métodos utilizados para resolver os problemas de programação linear, pode-se citar a solução gráfica e o método Simplex.</t>
+        </is>
+      </c>
+      <c r="O460" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P460" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q460" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="n">
+        <v>461</v>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>IBADE</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>Prefeitura de Jaru - RO</t>
+        </is>
+      </c>
+      <c r="D461" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E461" t="inlineStr">
+        <is>
+          <t>Na Programação Linear, a tarefa primordial é o reconhecimento e a formulação do problema de forma tal que ele possa ser trabalhado e, assim, fornecer um objetivo desejável a ser otimizado. O Método Gráfico da Programação Linear consiste em um sistema:</t>
+        </is>
+      </c>
+      <c r="F461" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G461" t="inlineStr">
+        <is>
+          <t>Pesquisa Operacional</t>
+        </is>
+      </c>
+      <c r="H461" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I461" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J461" t="inlineStr">
+        <is>
+          <t>não coordenado, onde se mostra um polígono convexo que contém os pontos representativos das possibilidades.</t>
+        </is>
+      </c>
+      <c r="K461" t="inlineStr">
+        <is>
+          <t>de coordenadas perpendiculares, onde se mostra um polígono côncavo que contém os pontos representativos das possibilidades.</t>
+        </is>
+      </c>
+      <c r="L461" t="inlineStr">
+        <is>
+          <t>de coordenadas ortogonais, onde se mostra um polígono convexo que contém os pontos representativos das possibilidades.</t>
+        </is>
+      </c>
+      <c r="M461" t="inlineStr">
+        <is>
+          <t>não coordenado, onde se mostra um polígono côncavo que contém os pontos representativos das possibilidades.</t>
+        </is>
+      </c>
+      <c r="N461" t="inlineStr">
+        <is>
+          <t>de coordenadas ortogonais, onde se mostra um polígono convexo que não contém os pontos representativos das possibilidades.</t>
+        </is>
+      </c>
+      <c r="O461" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P461" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q461" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="n">
+        <v>462</v>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>TRT23ª Região</t>
+        </is>
+      </c>
+      <c r="D462" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E462" t="inlineStr">
+        <is>
+          <t>Um estudo apresentou em seu relatório um problema de programação linear que é descrito abaixo.
+Os valores de x e y são, respectivamente,</t>
+        </is>
+      </c>
+      <c r="F462" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G462" t="inlineStr">
+        <is>
+          <t>Pesquisa Operacional</t>
+        </is>
+      </c>
+      <c r="H462" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I462" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J462" t="inlineStr">
+        <is>
+          <t>3,0 e 2,0.</t>
+        </is>
+      </c>
+      <c r="K462" t="inlineStr">
+        <is>
+          <t>1,0 e 3,0.</t>
+        </is>
+      </c>
+      <c r="L462" t="inlineStr">
+        <is>
+          <t>1,2 e 2,6.</t>
+        </is>
+      </c>
+      <c r="M462" t="inlineStr">
+        <is>
+          <t>1,0 e 2,5.</t>
+        </is>
+      </c>
+      <c r="N462" t="inlineStr">
+        <is>
+          <t>2,0 e 3,0.</t>
+        </is>
+      </c>
+      <c r="O462" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P462" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q462" t="n">
+        <v>0</v>
+      </c>
+      <c r="R462" t="inlineStr">
+        <is>
+          <t>becccfca-950b-41a0-bb75-e2be4b5af29c.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="n">
+        <v>463</v>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>EPE</t>
+        </is>
+      </c>
+      <c r="D463" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E463" t="inlineStr">
+        <is>
+          <t>O método simplex é um procedimento iterativo para resolver problemas de programação linear. Os procedimentos para a solução exigem que a sua formulação esteja expressa na forma padrão.
+Sobre essa forma, analise as afirmações a seguir.
+I – Todas as restrições são expressas por desigualdades.
+II – A função objetivo é de maximização ou de minimização.
+III – Todas as variáveis são não negativas.
+É correto APENAS o que se afirma em</t>
+        </is>
+      </c>
+      <c r="F463" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G463" t="inlineStr">
+        <is>
+          <t>Pesquisa Operacional</t>
+        </is>
+      </c>
+      <c r="H463" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I463" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J463" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="K463" t="inlineStr">
+        <is>
+          <t>II</t>
+        </is>
+      </c>
+      <c r="L463" t="inlineStr">
+        <is>
+          <t>III</t>
+        </is>
+      </c>
+      <c r="M463" t="inlineStr">
+        <is>
+          <t>I e II</t>
+        </is>
+      </c>
+      <c r="N463" t="inlineStr">
+        <is>
+          <t>II e III</t>
+        </is>
+      </c>
+      <c r="O463" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P463" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q463" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="n">
+        <v>464</v>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>UECE</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>Metrô/DF</t>
+        </is>
+      </c>
+      <c r="D464" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E464" t="inlineStr">
+        <is>
+          <t>Os modelos de programação linear são um tipo especial de modelos de otimização. Para representar um sistema por meio de um modelo de programação linear, ele deve possuir algumas características. Quanto a esse assunto, assinale a alternativa que descreve corretamente uma característica de um modelo de programação linear.</t>
+        </is>
+      </c>
+      <c r="F464" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G464" t="inlineStr">
+        <is>
+          <t>Pesquisa Operacional</t>
+        </is>
+      </c>
+      <c r="H464" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I464" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J464" t="inlineStr">
+        <is>
+          <t>Proporcionalidade: a quantidade de recurso utilizado por uma dada atividade deve ser proporcional ao nível dessa atividade na solução do problema.</t>
+        </is>
+      </c>
+      <c r="K464" t="inlineStr">
+        <is>
+          <t>Negatividade: deve ser sempre possível realizar uma determinada atividade em qualquer nível não negativo.</t>
+        </is>
+      </c>
+      <c r="L464" t="inlineStr">
+        <is>
+          <t>Não negatividade: deve ser sempre possível realizar uma determinada atividade em qualquer nível negativo.</t>
+        </is>
+      </c>
+      <c r="M464" t="inlineStr">
+        <is>
+          <t>Separabilidade: o custo total é a soma das parcelas associadas a cada atividade.</t>
+        </is>
+      </c>
+      <c r="N464" t="inlineStr">
+        <is>
+          <t>Aditividade: pode-se identificar, de forma separada, o custo (ou consumo de recursos) específico das operações de cada atividade.</t>
+        </is>
+      </c>
+      <c r="O464" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P464" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q464" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="n">
+        <v>465</v>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>FUNCAB</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>Prefeitura Municipal de Chapéu - BA</t>
+        </is>
+      </c>
+      <c r="D465" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E465" t="inlineStr">
+        <is>
+          <t>O dono de uma camioneta transporta caixas com 30kg de bananas e caixas com 40kg de laranjas. O valor de cada caixa de bananas é R$40,00 e o valor de cada caixa de laranjas é R$50,00. A camioneta tem capacidade de transportar 2 toneladas e o dono da camioneta tem 40 caixas de bananas e 40 caixas de laranjas para transportar. Quantas caixas de laranjas devem ser transportadas para que o dono da camioneta receba o maior valor possível?</t>
+        </is>
+      </c>
+      <c r="F465" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G465" t="inlineStr">
+        <is>
+          <t>Pesquisa Operacional</t>
+        </is>
+      </c>
+      <c r="H465" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I465" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J465" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="K465" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="L465" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="M465" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N465" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="O465" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P465" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q465" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="n">
+        <v>466</v>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>FCM</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>IF Farroupilha</t>
+        </is>
+      </c>
+      <c r="D466" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E466" t="inlineStr">
+        <is>
+          <t>O método das duas fases é um procedimento que pode ser utilizado para obter uma solução ótima viável, usando a lógica de funcionamento do método simplex quando a determinação de uma solução básica viável inicial não é óbvia.
+Em relação à lógica de funcionamento do método das duas fases, aplicado à resolução de problemas de programação linear, é correto afirmar que:</t>
+        </is>
+      </c>
+      <c r="F466" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G466" t="inlineStr">
+        <is>
+          <t>Pesquisa Operacional</t>
+        </is>
+      </c>
+      <c r="H466" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I466" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J466" t="inlineStr">
+        <is>
+          <t>O método fornece, ao final da primeira fase, uma solução básica viável ótima.</t>
+        </is>
+      </c>
+      <c r="K466" t="inlineStr">
+        <is>
+          <t>O método fornece, ao final da segunda fase, uma solução básica degenerada.</t>
+        </is>
+      </c>
+      <c r="L466" t="inlineStr">
+        <is>
+          <t>A primeira fase do método fornece uma solução básica inviável que deve ser viabilizada na segunda fase do método.</t>
+        </is>
+      </c>
+      <c r="M466" t="inlineStr">
+        <is>
+          <t>A segunda fase do método tem como objetivo encontrar uma solução básica viável ótima a partir de uma solução básica viável, obtida ao final da primeira fase.</t>
+        </is>
+      </c>
+      <c r="N466" t="inlineStr">
+        <is>
+          <t>Se o problema de programação linear for viável, então, ao final da segunda fase do método, as variáveis artificiais adicionadas deverão permanecer na base.</t>
+        </is>
+      </c>
+      <c r="O466" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P466" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q466" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="n">
+        <v>467</v>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>IADES</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>SEAD/df</t>
+        </is>
+      </c>
+      <c r="D467" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E467" t="inlineStr">
+        <is>
+          <t>A pesquisa operacional pode ser definida como um método científico de tomada de decisões. De maneira geral, consiste na descrição de um sistema organizado com o auxílio de um modelo e, através da experimentação com o modelo, na descoberta da melhor maneira de operar o sistema. Acerca desse tema, assinale a alternativa que apresenta as fases de um estudo em pesquisa operacional.</t>
+        </is>
+      </c>
+      <c r="F467" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G467" t="inlineStr">
+        <is>
+          <t>Pesquisa Operacional</t>
+        </is>
+      </c>
+      <c r="H467" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I467" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J467" t="inlineStr">
+        <is>
+          <t>Coleta de informações, análise das informações e resultados.</t>
+        </is>
+      </c>
+      <c r="K467" t="inlineStr">
+        <is>
+          <t>Formulação do problema, construção do modelo do sistema, cálculo da solução através do modelo, teste do modelo e da solução, estabelecimento de controles de solução e implantação e acompanhamento.</t>
+        </is>
+      </c>
+      <c r="L467" t="inlineStr">
+        <is>
+          <t>Planejamento, coleta de dados, análise dos dados e estudo dos resultados.</t>
+        </is>
+      </c>
+      <c r="M467" t="inlineStr">
+        <is>
+          <t>Estabelecimento de metas, planejamento, coleta de dados, análise de dados e estudo dos resultados.</t>
+        </is>
+      </c>
+      <c r="N467" t="inlineStr">
+        <is>
+          <t>Formulação do planejamento, análise de dados e apresentação dos resultados.</t>
+        </is>
+      </c>
+      <c r="O467" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P467" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q467" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="n">
+        <v>468</v>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Comperve</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>IFRN</t>
+        </is>
+      </c>
+      <c r="D468" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E468" t="inlineStr">
+        <is>
+          <t>É correto afirmar que um Modelo de Programação Linear</t>
+        </is>
+      </c>
+      <c r="F468" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G468" t="inlineStr">
+        <is>
+          <t>Pesquisa Operacional</t>
+        </is>
+      </c>
+      <c r="H468" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I468" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J468" t="inlineStr">
+        <is>
+          <t>é um algoritmo de um problema real descrito em termos de equações e inequações, ou seja, em linguagem matemática, no qual existem variáveis de decisão e uma função-objetivo, que se tenta otimizar.</t>
+        </is>
+      </c>
+      <c r="K468" t="inlineStr">
+        <is>
+          <t>é um algoritmo que representa um problema real descrito em termos de equações, em linguagem matemática, e neste existem variáveis de decisão, restrições e uma função-objetivo, que se tenta otimizar.</t>
+        </is>
+      </c>
+      <c r="L468" t="inlineStr">
+        <is>
+          <t>é uma representação de um problema real descrito em termos de equações e in equações lineares, ou seja, em linguagem matemática, no qual existem variáveis de decisão, restrições e uma funçãoobjetivo, que se tenta otimizar.</t>
+        </is>
+      </c>
+      <c r="M468" t="inlineStr">
+        <is>
+          <t>é uma representação espacial de um problema real descrito em termos de equações e inequações lineares, ou seja, em linguagem matemática, no qual existem variáveis de decisão e uma funçãoobjetivo, que se tenta otimizar.</t>
+        </is>
+      </c>
+      <c r="N468" t="inlineStr"/>
+      <c r="O468" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P468" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q468" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
:up: questoes de engenharia organizacional cadastradas
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R468"/>
+  <dimension ref="A1:R506"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -39762,6 +39762,3171 @@
         <v>0</v>
       </c>
     </row>
+    <row r="469">
+      <c r="A469" t="n">
+        <v>469</v>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>TRANSPETRO)</t>
+        </is>
+      </c>
+      <c r="D469" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E469" t="inlineStr">
+        <is>
+          <t>Segundo o modelo administrativo de tomada de decisão, existe um processo que consiste em analisar alternativas apenas até que seja encontrada uma solução que apresente um mínimo de requisitos e, então, encerrar a procura por uma melhor solução. Esse processo é denominado</t>
+        </is>
+      </c>
+      <c r="F469" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G469" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H469" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I469" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J469" t="inlineStr">
+        <is>
+          <t>subotimização</t>
+        </is>
+      </c>
+      <c r="K469" t="inlineStr">
+        <is>
+          <t>incubação</t>
+        </is>
+      </c>
+      <c r="L469" t="inlineStr">
+        <is>
+          <t>heurística</t>
+        </is>
+      </c>
+      <c r="M469" t="inlineStr">
+        <is>
+          <t>estruturação</t>
+        </is>
+      </c>
+      <c r="N469" t="inlineStr">
+        <is>
+          <t>maldição do conhecimento</t>
+        </is>
+      </c>
+      <c r="O469" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P469" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q469" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="n">
+        <v>470</v>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D470" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E470" t="inlineStr">
+        <is>
+          <t>O processo de tomada de decisão, na maioria das organizações, envolve alguns passos.
+Esses passos, ordenados do primeiro para o último, são:</t>
+        </is>
+      </c>
+      <c r="F470" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G470" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H470" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I470" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J470" t="inlineStr">
+        <is>
+          <t>identificação e estudo do problema; formulação de alternativas; tomada de decisão sobre a solução mais adequada; implementação dessa solução; avaliação do impacto da intervenção.</t>
+        </is>
+      </c>
+      <c r="K470" t="inlineStr">
+        <is>
+          <t>tomada de decisão sobre a solução mais adequada; identificação do problema; implementação dessa solução; avaliação do impacto da intervenção; formulação de alternativas.</t>
+        </is>
+      </c>
+      <c r="L470" t="inlineStr">
+        <is>
+          <t>identificação e estudo do problema; tomada de decisão sobre a solução mais adequada; avaliação do impacto da intervenção; implementação dessa solução.</t>
+        </is>
+      </c>
+      <c r="M470" t="inlineStr">
+        <is>
+          <t>avaliação do impacto da intervenção; tomada de decisão sobre a solução mais adequada; implementação dessa solução; avaliação dos resultados.</t>
+        </is>
+      </c>
+      <c r="N470" t="inlineStr">
+        <is>
+          <t>identificação e estudo da solução mais adequada; implementação dessa solução; avaliação do impacto da intervenção; avaliação do problema; tomada de decisão sobre a solução mais adequada.</t>
+        </is>
+      </c>
+      <c r="O470" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P470" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q470" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="n">
+        <v>471</v>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D471" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E471" t="inlineStr">
+        <is>
+          <t>A empresa de operação logística W, diante da necessidade de aumentar o nível de serviço ao cliente, precisa deliberar sobre duas soluções projetadas por sua equipe técnica, a saber: automatizar a montagem de pedidos, com valor de implantação de R$10.000.000,00, ou reajustar os contratos com transportadoras, com valor de R$5.000.000,00. Quando implementadas, ambas as soluções podem gerar ganhos elevados ou pequenos com o aumento de nível de serviço. Para tomar essa decisão, a cúpula executiva da empresa optou por aplicar a análise de Valor Monetário Esperado (Expected Monetary Value - EMV), um método para análise quantitativa de risco. Os fatores a serem considerados nesse processo decisório são representados na árvore de decisão que segue:
+A primeira solução, que consiste em automatizar a montagem de pedidos, apresenta probabilidade de 85% de gerar R$ 20.000.000,00 em ganho por aumento do nível de serviço e 15% de probabilidade de ganho de R$ 2.000.000,00.
+A segunda solução, que consiste em reajustar os contratos com transportadoras, apresenta probabilidade de 60% de gerar R$ 30.000.000,00 em ganho por aumento do nível de serviço e 40% de probabilidade de ganho de R$ 10.000.000,00.
+Portanto, seguindo o método adotado para tomada de decisão, a solução a ser implantada por W é</t>
+        </is>
+      </c>
+      <c r="F471" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G471" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H471" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I471" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J471" t="inlineStr">
+        <is>
+          <t>automatizar a montagem de pedidos, por apresentar um VME de 17 milhões.</t>
+        </is>
+      </c>
+      <c r="K471" t="inlineStr">
+        <is>
+          <t>automatizar a montagem de pedidos, por apresentar um VME de 7,3 milhões.</t>
+        </is>
+      </c>
+      <c r="L471" t="inlineStr">
+        <is>
+          <t>automatizar a montagem de pedidos, por apresentar um VME superior ao VME da solução de ajustar os contratos com as transportadoras.</t>
+        </is>
+      </c>
+      <c r="M471" t="inlineStr">
+        <is>
+          <t>reajustar os contratos com as transportadoras, por apresentar um VME de 12 milhões.</t>
+        </is>
+      </c>
+      <c r="N471" t="inlineStr">
+        <is>
+          <t>reajustar os contratos com as transportadoras, por apresentar um VME de 17 milhões.</t>
+        </is>
+      </c>
+      <c r="O471" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P471" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q471" t="n">
+        <v>0</v>
+      </c>
+      <c r="R471" t="inlineStr">
+        <is>
+          <t>976429d4-a404-41e6-8c95-9abc0de1aaaa.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="n">
+        <v>472</v>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>BR DISTRIBUIDORA</t>
+        </is>
+      </c>
+      <c r="D472" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="E472" t="inlineStr">
+        <is>
+          <t>Existem três classes de modelos decisórios em relação à natureza: decisões com certeza, decisões com risco e decisões com incerteza.
+Para decisões com incerteza, o método mais conservador de tomar decisões, que avalia cada decisão pelo mínimo retorno possível associado a ela, é o critério</t>
+        </is>
+      </c>
+      <c r="F472" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G472" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H472" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I472" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J472" t="inlineStr">
+        <is>
+          <t>maximin</t>
+        </is>
+      </c>
+      <c r="K472" t="inlineStr">
+        <is>
+          <t>maximax</t>
+        </is>
+      </c>
+      <c r="L472" t="inlineStr">
+        <is>
+          <t>de arrependimento minimax</t>
+        </is>
+      </c>
+      <c r="M472" t="inlineStr">
+        <is>
+          <t>de Laplace</t>
+        </is>
+      </c>
+      <c r="N472" t="inlineStr">
+        <is>
+          <t>de Fourier</t>
+        </is>
+      </c>
+      <c r="O472" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P472" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q472" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="n">
+        <v>473</v>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>BR DISTRIBUIDORA</t>
+        </is>
+      </c>
+      <c r="D473" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="E473" t="inlineStr">
+        <is>
+          <t>Considere as seguintes características sobre processo decisório.
+I - dados repetitivos;
+II - imprevisibilidade;
+III - condições estáticas;
+IV - condições dinâmicas.
+São características de decisões não programadas APENAS</t>
+        </is>
+      </c>
+      <c r="F473" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G473" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H473" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I473" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J473" t="inlineStr">
+        <is>
+          <t>I e II.</t>
+        </is>
+      </c>
+      <c r="K473" t="inlineStr">
+        <is>
+          <t>II e III.</t>
+        </is>
+      </c>
+      <c r="L473" t="inlineStr">
+        <is>
+          <t>II e IV.</t>
+        </is>
+      </c>
+      <c r="M473" t="inlineStr">
+        <is>
+          <t>I, II e IV.</t>
+        </is>
+      </c>
+      <c r="N473" t="inlineStr">
+        <is>
+          <t>I, III e IV.</t>
+        </is>
+      </c>
+      <c r="O473" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P473" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q473" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="n">
+        <v>474</v>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D474" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="E474" t="inlineStr">
+        <is>
+          <t>A avaliação de projetos de investimento em situação de futuro indeterminado é uma atividade rotineira da maioria dos dirigentes de empresas. Diversos critérios podem ser adotados para a tomada de decisão.
+Considere que um dirigente quer aumentar a participação de mercado de sua empresa seguindo uma das quatro estratégias disponíveis (E1, E2, E3 ou E4), e que uma análise da concorrência indicou que a reação poderia ocorrer de três formas diferentes (A1, A2 ou A3), mas, sem condições de determinar qualquer probabilidade de ocorrência de cada reação. Analisando cada um dos possíveis estados da natureza, o dirigente elaborou a matriz de ganhos abaixo.
+Orientado por um consultor, o dirigente deverá adotar o critério de Wald, também conhecido como
+Maximin. Nessa situação, conclui-se que a estratégia adotada foi</t>
+        </is>
+      </c>
+      <c r="F474" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G474" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H474" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I474" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J474" t="inlineStr">
+        <is>
+          <t>lançar um novo produto, pois apresenta o melhor resultado potencial.</t>
+        </is>
+      </c>
+      <c r="K474" t="inlineStr">
+        <is>
+          <t>lançar uma campanha publicitária, pois se identificou, para cada estratégia possível, o estado da natureza que conduzirá ao resultado menos desfavorável.</t>
+        </is>
+      </c>
+      <c r="L474" t="inlineStr">
+        <is>
+          <t>lançar uma promoção de vendas, pois apresentou a maior média ponderada entre o pior e melhor resultado potencial.</t>
+        </is>
+      </c>
+      <c r="M474" t="inlineStr">
+        <is>
+          <t>praticar uma política de baixa de preços, pois se efetuou uma média aritmética simples dos resultados esperados.</t>
+        </is>
+      </c>
+      <c r="N474" t="inlineStr">
+        <is>
+          <t>praticar uma política de baixa de preços, pois se identificou, para cada um dos estados da natureza, a estratégia mais favorável para que, então, se determinasse o quanto deixaria de ganhar.</t>
+        </is>
+      </c>
+      <c r="O474" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P474" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q474" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="n">
+        <v>475</v>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D475" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="E475" t="inlineStr">
+        <is>
+          <t>Todo processo de tomada de decisão começa pela identificação do problema. Após, os esforços devem ser concentrados em diagnosticar uma situação.
+Esse diagnóstico consiste em</t>
+        </is>
+      </c>
+      <c r="F475" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G475" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H475" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I475" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J475" t="inlineStr">
+        <is>
+          <t>identificar objetivos – analisar causas</t>
+        </is>
+      </c>
+      <c r="K475" t="inlineStr">
+        <is>
+          <t>identificar oportunidade – analisar os resultados finais</t>
+        </is>
+      </c>
+      <c r="L475" t="inlineStr">
+        <is>
+          <t>avaliar a situação – identificar os custos finais</t>
+        </is>
+      </c>
+      <c r="M475" t="inlineStr">
+        <is>
+          <t>analisar causas – identificar efeitos sociais</t>
+        </is>
+      </c>
+      <c r="N475" t="inlineStr">
+        <is>
+          <t>analisar a situação econômica – avaliar preços</t>
+        </is>
+      </c>
+      <c r="O475" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P475" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q475" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="n">
+        <v>476</v>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D476" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="E476" t="inlineStr">
+        <is>
+          <t>Com a competição cada vez maior entre as organizações e a necessidade de informações rápidas para auxiliar no processo de tomada de decisão, surgiu o Sistema de Apoio à Decisão. No Modelo de Simon, as decisões são diferenciadas em programadas e não programadas.
+As decisões programadas possuem as seguintes características:</t>
+        </is>
+      </c>
+      <c r="F476" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G476" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H476" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I476" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J476" t="inlineStr">
+        <is>
+          <t>incerteza e dados únicos</t>
+        </is>
+      </c>
+      <c r="K476" t="inlineStr">
+        <is>
+          <t>condições estáticas e dados inadequados</t>
+        </is>
+      </c>
+      <c r="L476" t="inlineStr">
+        <is>
+          <t>dados repetitivos e condições dinâmicas</t>
+        </is>
+      </c>
+      <c r="M476" t="inlineStr">
+        <is>
+          <t>dados repetitivos e condições estáticas</t>
+        </is>
+      </c>
+      <c r="N476" t="inlineStr">
+        <is>
+          <t>dados únicos e condições estáticas</t>
+        </is>
+      </c>
+      <c r="O476" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P476" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q476" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="n">
+        <v>477</v>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D477" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="E477" t="inlineStr">
+        <is>
+          <t>O ambiente de uma organização que atua na indústria petrolífera é dado por todas as condições e influências externas que afetam seu desenvolvimento, sendo relevantes à tomada de decisão, por exemplo, a construção de uma nova refinaria.
+Muitas podem ser as influências externas, EXCETO a</t>
+        </is>
+      </c>
+      <c r="F477" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G477" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H477" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I477" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J477" t="inlineStr">
+        <is>
+          <t>competência, porque a experiência de refinar e distribuir um produto pode servir como base para explorar uma descoberta e conviver com seu sucesso.</t>
+        </is>
+      </c>
+      <c r="K477" t="inlineStr">
+        <is>
+          <t>tecnologia, porque os avanços tecnológicos trazem mudanças aos processos produtivos, à concepção de novos produtos e ao nível de automação.</t>
+        </is>
+      </c>
+      <c r="L477" t="inlineStr">
+        <is>
+          <t>ecologia, porque a escolha da localização deve considerar a disponibilidade e o acesso a recursos, assim como impactos em água, ar, trânsito e qualidade de vida.</t>
+        </is>
+      </c>
+      <c r="M477" t="inlineStr">
+        <is>
+          <t>economia, porque o monitoramento de tendências econômicas evita que a empresa seja pega de surpresa para que seus investimentos alcancem o retorno esperado.</t>
+        </is>
+      </c>
+      <c r="N477" t="inlineStr">
+        <is>
+          <t>sociedade, porque os desenvolvimentos sociais são importantes devido a mudanças nos padrões de trabalho, na noção de diversidade e igualdade de grupos minoritários e de mulheres.</t>
+        </is>
+      </c>
+      <c r="O477" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P477" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q477" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="n">
+        <v>478</v>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>IBGE</t>
+        </is>
+      </c>
+      <c r="D478" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="E478" t="inlineStr">
+        <is>
+          <t>Com relação à figura acima e aos fundamentos da tomada de decisão, analise as afirmações abaixo.
+I - Alternativa é uma ação que pode ser escolhida pelo tomador da decisão, que, na figura, representa o mercado favorável ou desfavorável.
+II - Estado da natureza é uma ocorrência ou situação sobre a qual o tomador da decisão tem pouco controle.
+III - No nó de decisão podem sair vários estados da natureza
+É(São) correta(s) APENAS a(s) afirmativa(s)</t>
+        </is>
+      </c>
+      <c r="F478" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G478" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H478" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I478" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J478" t="inlineStr">
+        <is>
+          <t>I.</t>
+        </is>
+      </c>
+      <c r="K478" t="inlineStr">
+        <is>
+          <t>II.</t>
+        </is>
+      </c>
+      <c r="L478" t="inlineStr">
+        <is>
+          <t>I e II.</t>
+        </is>
+      </c>
+      <c r="M478" t="inlineStr">
+        <is>
+          <t>II e III.</t>
+        </is>
+      </c>
+      <c r="N478" t="inlineStr">
+        <is>
+          <t>I, II e III.</t>
+        </is>
+      </c>
+      <c r="O478" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P478" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q478" t="n">
+        <v>0</v>
+      </c>
+      <c r="R478" t="inlineStr">
+        <is>
+          <t>4475bb19-6273-4b7f-a9be-ec9d984029d6.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="n">
+        <v>479</v>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D479" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E479" t="inlineStr">
+        <is>
+          <t>O Design Thinking vem sendo frequentemente adotado nas empresas para diferentes aplicações, tendo como objetivo primordial a construção de soluções de problemas considerados complexos.
+A característica determinante do Design Thinking, enquanto ações mobilizadoras para resolução de problemas, se dá pela(o)</t>
+        </is>
+      </c>
+      <c r="F479" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G479" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H479" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I479" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J479" t="inlineStr">
+        <is>
+          <t>organização do trabalho colaborativo das pessoas envolvidas, em uma lógica que articula simultaneamente análise e síntese.</t>
+        </is>
+      </c>
+      <c r="K479" t="inlineStr">
+        <is>
+          <t>ausência de métodos, procedimentos e ferramentas, justamente para que não haja nenhum viés na busca por soluções.</t>
+        </is>
+      </c>
+      <c r="L479" t="inlineStr">
+        <is>
+          <t>modelagem de dados e informações em softwares de simulação, fazendo com que não seja necessária a imersão direta dos participantes nos problemas reais.</t>
+        </is>
+      </c>
+      <c r="M479" t="inlineStr">
+        <is>
+          <t>participação única de especialistas que, com suas competências e experiências, criarão diversas soluções alternativas para o problema.</t>
+        </is>
+      </c>
+      <c r="N479" t="inlineStr">
+        <is>
+          <t>planejamento estruturado no início da definição do problema, antes de se construir uma solução única e otimizada.</t>
+        </is>
+      </c>
+      <c r="O479" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P479" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q479" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="n">
+        <v>480</v>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>IBGE</t>
+        </is>
+      </c>
+      <c r="D480" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E480" t="inlineStr">
+        <is>
+          <t>Os indivíduos frequentemente cometem equívocos na tomada de decisão, causados por vieses cognitivos. Analise- se o seguinte exemplo: a maioria dos meninos de quinze anos de uma comunidade carioca se esforça para ser um jogador de futebol profissional, porque acredita que terá o sucesso do Neymar, e a maioria das meninas da mesma idade decide ser modelo inspirada na carreira de Gisele Bündchen.
+Esses dois grupos decidem embasados no viés</t>
+        </is>
+      </c>
+      <c r="F480" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G480" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H480" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I480" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J480" t="inlineStr">
+        <is>
+          <t>da confirmação</t>
+        </is>
+      </c>
+      <c r="K480" t="inlineStr">
+        <is>
+          <t>da ancoragem</t>
+        </is>
+      </c>
+      <c r="L480" t="inlineStr">
+        <is>
+          <t>da compreensão tardia</t>
+        </is>
+      </c>
+      <c r="M480" t="inlineStr">
+        <is>
+          <t>da representatividade</t>
+        </is>
+      </c>
+      <c r="N480" t="inlineStr">
+        <is>
+          <t>do comprometimento</t>
+        </is>
+      </c>
+      <c r="O480" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P480" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q480" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="n">
+        <v>481</v>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>EPE</t>
+        </is>
+      </c>
+      <c r="D481" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E481" t="inlineStr">
+        <is>
+          <t>O administrador, em suas atividades diárias, precisa fazer diversas escolhas para que os objetivos da organização sejam alcançados.
+Essas escolhas se constituem em decisões necessárias para a resolução de problemas ou para aproveitar alguma oportunidade.
+As decisões em uma organização são classificadas em duas categorias, a saber:</t>
+        </is>
+      </c>
+      <c r="F481" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G481" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H481" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I481" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J481" t="inlineStr">
+        <is>
+          <t>programadas e não programadas</t>
+        </is>
+      </c>
+      <c r="K481" t="inlineStr">
+        <is>
+          <t>cíclicas e lineares</t>
+        </is>
+      </c>
+      <c r="L481" t="inlineStr">
+        <is>
+          <t>cíclicas e programadas</t>
+        </is>
+      </c>
+      <c r="M481" t="inlineStr">
+        <is>
+          <t>lineares e estruturadas</t>
+        </is>
+      </c>
+      <c r="N481" t="inlineStr">
+        <is>
+          <t>programadas e estruturadas</t>
+        </is>
+      </c>
+      <c r="O481" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P481" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q481" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="n">
+        <v>482</v>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>IBGE</t>
+        </is>
+      </c>
+      <c r="D482" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E482" t="inlineStr">
+        <is>
+          <t>Especialistas em administração afirmam que a maioria das decisões significativas é tomada mais por meio de julgamentos subjetivos do que por um modelo prescritivo.
+Assim sendo, os decisores organizacionais</t>
+        </is>
+      </c>
+      <c r="F482" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G482" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H482" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I482" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J482" t="inlineStr">
+        <is>
+          <t>operam dentro de uma racionalidade limitada, buscando escolhas satisfatórias.</t>
+        </is>
+      </c>
+      <c r="K482" t="inlineStr">
+        <is>
+          <t>fazem escolhas coerentes, seguindo um modelo racional que busca agregar valor.</t>
+        </is>
+      </c>
+      <c r="L482" t="inlineStr">
+        <is>
+          <t>apegam-se a ações malsucedidas porque têm dificuldade para lidar com o acaso.</t>
+        </is>
+      </c>
+      <c r="M482" t="inlineStr">
+        <is>
+          <t>têm aversão ao risco e, por isso, tendem a julgar as coisas com base nas informações mais disponíveis.</t>
+        </is>
+      </c>
+      <c r="N482" t="inlineStr">
+        <is>
+          <t>buscam informações que corroborem escolhas anteriores porque acham que sabem antecipadamente o resultado de um evento.</t>
+        </is>
+      </c>
+      <c r="O482" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P482" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q482" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="n">
+        <v>483</v>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>CEFET-RJ</t>
+        </is>
+      </c>
+      <c r="D483" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E483" t="inlineStr">
+        <is>
+          <t>De acordo com as situações a que se aplicam, as decisões podem ser classificadas de diversas formas.
+As decisões que se aplicam a problemas repetitivos são denominadas</t>
+        </is>
+      </c>
+      <c r="F483" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G483" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H483" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I483" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J483" t="inlineStr">
+        <is>
+          <t>coletivas</t>
+        </is>
+      </c>
+      <c r="K483" t="inlineStr">
+        <is>
+          <t>individuais</t>
+        </is>
+      </c>
+      <c r="L483" t="inlineStr">
+        <is>
+          <t>maximizadas</t>
+        </is>
+      </c>
+      <c r="M483" t="inlineStr">
+        <is>
+          <t>programadas</t>
+        </is>
+      </c>
+      <c r="N483" t="inlineStr">
+        <is>
+          <t>administrativas</t>
+        </is>
+      </c>
+      <c r="O483" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P483" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q483" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="n">
+        <v>484</v>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>IBGE</t>
+        </is>
+      </c>
+      <c r="D484" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="E484" t="inlineStr">
+        <is>
+          <t>O gerente de operações de uma fábrica convoca uma reunião para resolver problemas operacionais. Em determinado momento da discussão, um analista da área de qualidade propõe a utilização de árvores de decisão, pois essa técnica de apoio à decisão permite.</t>
+        </is>
+      </c>
+      <c r="F484" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G484" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H484" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I484" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J484" t="inlineStr">
+        <is>
+          <t>monitorar a implementação da decisão e avaliar sua eficácia de acordo com as metas estabelecidas.</t>
+        </is>
+      </c>
+      <c r="K484" t="inlineStr">
+        <is>
+          <t>comparar e avaliar as alternativas de solução, permitindo a seleção da melhor.</t>
+        </is>
+      </c>
+      <c r="L484" t="inlineStr">
+        <is>
+          <t>identificar de forma mais eficiente o problema a ser resolvido.</t>
+        </is>
+      </c>
+      <c r="M484" t="inlineStr">
+        <is>
+          <t>analisar as causas que estão na origem do problema.</t>
+        </is>
+      </c>
+      <c r="N484" t="inlineStr">
+        <is>
+          <t>gerar alternativas de solução possível.</t>
+        </is>
+      </c>
+      <c r="O484" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P484" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q484" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="n">
+        <v>485</v>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>IBGE</t>
+        </is>
+      </c>
+      <c r="D485" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="E485" t="inlineStr">
+        <is>
+          <t>Num processo de seleção, muitas vezes os tomadores de decisões se valem excessivamente da própria experiência, de seus impulsos, instintos e regras de ‘senso comum’ para o julgamento de candidatos.
+Nesses vieses comuns à tomada de decisão, há uma tendência de incorrer no erro de:</t>
+        </is>
+      </c>
+      <c r="F485" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G485" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H485" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I485" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J485" t="inlineStr">
+        <is>
+          <t>viés da compreensão tardia: acreditar que somos melhores do que na verdade somos em fazer previsões, que nos torna falsamente confiantes.</t>
+        </is>
+      </c>
+      <c r="K485" t="inlineStr">
+        <is>
+          <t>aleatoriedade: julgar as coisas com base nas informações mais facilmente disponíveis.</t>
+        </is>
+      </c>
+      <c r="L485" t="inlineStr">
+        <is>
+          <t>escalada de comprometimento: ancorar o julgamento em uma informação inicial, o que dificulta o ajuste diante de informações posteriores.</t>
+        </is>
+      </c>
+      <c r="M485" t="inlineStr">
+        <is>
+          <t>aversão ao risco: buscar informações que corroborem escolhas anteriores e descartar as que contestem julgamentos prévios.</t>
+        </is>
+      </c>
+      <c r="N485" t="inlineStr">
+        <is>
+          <t>lógica: pressupor que as outras pessoas compartilham de seus valores e suas crenças.</t>
+        </is>
+      </c>
+      <c r="O485" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P485" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q485" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="n">
+        <v>486</v>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>BNDES</t>
+        </is>
+      </c>
+      <c r="D486" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="E486" t="inlineStr">
+        <is>
+          <t>A tomada de decisão é um processo natural a todos os seres humanos. Esse processo, nas organizações empresariais, tendem a ser racionais, estabelecendo-se metodologias que auxiliem a atingir os seus objetivos.
+As decisões são classificadas em dois tipos, quais sejam:</t>
+        </is>
+      </c>
+      <c r="F486" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G486" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H486" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I486" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J486" t="inlineStr">
+        <is>
+          <t>estratégicas, cujas variáveis são coletadas num ambiente estático; e operacionais, que têm regras estabelecidas, e as variáveis são reunidas com alto grau de incerteza.</t>
+        </is>
+      </c>
+      <c r="K486" t="inlineStr">
+        <is>
+          <t>fixas, que são tomadas em ambiente de incerteza; e variáveis, cujos elementos para a tomada de decisão são reunidos com dificuldade.</t>
+        </is>
+      </c>
+      <c r="L486" t="inlineStr">
+        <is>
+          <t>programadas, que são rotineiras e atendem a um conjunto de regras preestabelecidas; e não programadas, que não têm regras a seguir nem possuem um esquema específico para ser utilizado.</t>
+        </is>
+      </c>
+      <c r="M486" t="inlineStr">
+        <is>
+          <t>simples, que se referem às estratégias organizacionais; e complexas, que se referem às decisões que envolvem as atividades operacionais da empresa.</t>
+        </is>
+      </c>
+      <c r="N486" t="inlineStr">
+        <is>
+          <t>conceituais, referentes às decisões tomadas no nível operacional da organização; e técnicas, que se referem às decisões tomadas no nível técnico.</t>
+        </is>
+      </c>
+      <c r="O486" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P486" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q486" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="n">
+        <v>487</v>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>IBGE</t>
+        </is>
+      </c>
+      <c r="D487" t="inlineStr">
+        <is>
+          <t>2009</t>
+        </is>
+      </c>
+      <c r="E487" t="inlineStr">
+        <is>
+          <t>Dada a diversidade de lugares e pessoas com as quais vai trabalhar, Marcelo precisa tomar decisões fundamentais quase instantaneamente e com base em muitas variáveis, entre elas:
+I – condições de incerteza;
+II – influência da situação na qual se envolve;
+III – resultados que se deseja alcançar;
+IV – critérios de escolha.
+São presentes no processo decisório as variáveis:</t>
+        </is>
+      </c>
+      <c r="F487" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G487" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H487" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I487" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J487" t="inlineStr">
+        <is>
+          <t>I e II, apenas.</t>
+        </is>
+      </c>
+      <c r="K487" t="inlineStr">
+        <is>
+          <t>I e III, apenas.</t>
+        </is>
+      </c>
+      <c r="L487" t="inlineStr">
+        <is>
+          <t>II e IV, apenas.</t>
+        </is>
+      </c>
+      <c r="M487" t="inlineStr">
+        <is>
+          <t>I, III e IV, apenas.</t>
+        </is>
+      </c>
+      <c r="N487" t="inlineStr">
+        <is>
+          <t>I, II, III e IV.</t>
+        </is>
+      </c>
+      <c r="O487" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P487" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q487" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="n">
+        <v>488</v>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>DECEA)</t>
+        </is>
+      </c>
+      <c r="D488" t="inlineStr">
+        <is>
+          <t>2006</t>
+        </is>
+      </c>
+      <c r="E488" t="inlineStr">
+        <is>
+          <t>Herbert Simon, que escreveu um clássico da administração, teorizou que a racionalidade pressupõe a escolha, em um processo decisório, de alternativas possíveis.
+No entanto, alertou para o fato de que as pessoas tomam decisões baseadas apenas naqueles aspectos que conseguem perceber. Simon aponta, portanto, para a:</t>
+        </is>
+      </c>
+      <c r="F488" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G488" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H488" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I488" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J488" t="inlineStr">
+        <is>
+          <t>complementaridade das decisões.</t>
+        </is>
+      </c>
+      <c r="K488" t="inlineStr">
+        <is>
+          <t>racionalidade administrativa.</t>
+        </is>
+      </c>
+      <c r="L488" t="inlineStr">
+        <is>
+          <t>racionalidade limitada.</t>
+        </is>
+      </c>
+      <c r="M488" t="inlineStr">
+        <is>
+          <t>caracterização das decisões.</t>
+        </is>
+      </c>
+      <c r="N488" t="inlineStr">
+        <is>
+          <t>hierarquia das decisões.</t>
+        </is>
+      </c>
+      <c r="O488" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P488" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q488" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="n">
+        <v>489</v>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D489" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E489" t="inlineStr">
+        <is>
+          <t>Tomadores de decisão que fazem uso de um estilo voltado para a intuição se concentram em desenvolver abstrações e exemplos figurativos para que sejam utilizados na tomada de decisão, com ênfase na imaginação e nas possibilidades. Esse estilo voltado para a intuição pode mostrar-se valioso em situações específicas, quando há</t>
+        </is>
+      </c>
+      <c r="F489" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G489" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H489" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I489" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J489" t="inlineStr">
+        <is>
+          <t>um baixo nível de ambiguidade e várias alternativas de solução plausíveis, com bons argumentos para cada uma delas.</t>
+        </is>
+      </c>
+      <c r="K489" t="inlineStr">
+        <is>
+          <t>fatos ilimitados que indicam claramente o caminho a ser seguido.</t>
+        </is>
+      </c>
+      <c r="L489" t="inlineStr">
+        <is>
+          <t>tempo ilimitado e muitos precedentes que não favorecem decisões inovadoras e criativas.</t>
+        </is>
+      </c>
+      <c r="M489" t="inlineStr">
+        <is>
+          <t>várias alternativas de soluções plausíveis, com bons argumentos para cada uma delas.</t>
+        </is>
+      </c>
+      <c r="N489" t="inlineStr">
+        <is>
+          <t>um problema estruturado e uma situação com alto nível de certeza.</t>
+        </is>
+      </c>
+      <c r="O489" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P489" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q489" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="n">
+        <v>490</v>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D490" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E490" t="inlineStr">
+        <is>
+          <t>Os indivíduos frequentemente cometem equívocos na tomada de decisão por vieses cognitivos. A esse respeito, considere os três exemplos descritos a seguir:
+1. Um potencial empregador pergunta a um candidato a uma vaga qual era o seu salário anterior, e ele responde aumentando o real valor com a expectativa de uma oferta melhor.
+2. Alguém que tem habilidades intelectuais e interpessoais mais fracas do que outra pessoa apresenta maiores probabilidades de superestimar sua capacidade e desempenho.
+3. Uma moça estava namorando há seis anos. Embora ela própria afirmasse que o relacionamento não era satisfatório, marcou a data do casamento porque já havia investido muito na relação.
+Identificam-se nos três exemplos, respectivamente, o viés de:</t>
+        </is>
+      </c>
+      <c r="F490" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G490" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H490" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I490" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J490" t="inlineStr">
+        <is>
+          <t>autoconveniência, disponibilidade, representatividade</t>
+        </is>
+      </c>
+      <c r="K490" t="inlineStr">
+        <is>
+          <t>confirmação, aleatoriedade, compreensão tardia</t>
+        </is>
+      </c>
+      <c r="L490" t="inlineStr">
+        <is>
+          <t>ancoragem, excesso de confiança, escalada do comprometimento</t>
+        </is>
+      </c>
+      <c r="M490" t="inlineStr">
+        <is>
+          <t>informação coletiva, custo passado, facilidade de lembrança</t>
+        </is>
+      </c>
+      <c r="N490" t="inlineStr">
+        <is>
+          <t>consenso de problema, questionamento dialético, heurística</t>
+        </is>
+      </c>
+      <c r="O490" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P490" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q490" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="n">
+        <v>491</v>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D491" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E491" t="inlineStr">
+        <is>
+          <t>O diretor de uma empresa vê-se frente a uma difícil decisão: construir ou não a barragem que servirá para gerar energia elétrica para toda uma região. Como forma de definir o que fazer, ele calcula as consequências das possíveis decisões sobre cada um dos grupos envolvidos. Conclui que se a barragem for construída, o benefício a toda a comunidade será maior do que qualquer transtorno que possa vir a ser causado. Ele acredita que sua decisão sobre a construção da barragem trará mais satisfação para uma quantidade maior de pessoas.
+A abordagem para a tomada de decisão ética que descreve a estratégia desse diretor é a abordagem</t>
+        </is>
+      </c>
+      <c r="F491" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G491" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H491" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I491" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J491" t="inlineStr">
+        <is>
+          <t>utilitária</t>
+        </is>
+      </c>
+      <c r="K491" t="inlineStr">
+        <is>
+          <t>genérica</t>
+        </is>
+      </c>
+      <c r="L491" t="inlineStr">
+        <is>
+          <t>da justiça</t>
+        </is>
+      </c>
+      <c r="M491" t="inlineStr">
+        <is>
+          <t>do individualismo</t>
+        </is>
+      </c>
+      <c r="N491" t="inlineStr">
+        <is>
+          <t>da moral e dos direitos</t>
+        </is>
+      </c>
+      <c r="O491" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P491" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q491" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="n">
+        <v>492</v>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CESGRANRIO </t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D492" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="E492" t="inlineStr">
+        <is>
+          <t>O processo de tomada de decisão do consumidor tem início com o reconhecimento de uma necessidade, quando o consumidor percebe uma diferença entre seu estado real e algum estado desejado.
+PORQUE
+O consumidor pode obter informações através de fontes pessoais, comerciais, públicas ou experimentais.
+A esse respeito, conclui-se que</t>
+        </is>
+      </c>
+      <c r="F492" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G492" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H492" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I492" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J492" t="inlineStr">
+        <is>
+          <t>as duas afirmações são verdadeiras e a segunda justifica a primeira.</t>
+        </is>
+      </c>
+      <c r="K492" t="inlineStr">
+        <is>
+          <t>as duas afirmações são verdadeiras e a segunda não justifica a primeira.</t>
+        </is>
+      </c>
+      <c r="L492" t="inlineStr">
+        <is>
+          <t>a primeira afirmação é verdadeira e a segunda é falsa.</t>
+        </is>
+      </c>
+      <c r="M492" t="inlineStr">
+        <is>
+          <t>a primeira afirmação é falsa e a segunda é verdadeira.</t>
+        </is>
+      </c>
+      <c r="N492" t="inlineStr">
+        <is>
+          <t>as duas afirmações são falsas.</t>
+        </is>
+      </c>
+      <c r="O492" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P492" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q492" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="n">
+        <v>493</v>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D493" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E493" t="inlineStr">
+        <is>
+          <t>Uma empresa de navegação optou pela operação Ship to Ship (STS), com base numa informação inicial de que a eficiência aumentaria. Essa decisão foi afetada pelo viés de ancoragem, que é a tendência a um indivíduo</t>
+        </is>
+      </c>
+      <c r="F493" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G493" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H493" t="inlineStr">
+        <is>
+          <t>Fácil</t>
+        </is>
+      </c>
+      <c r="I493" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J493" t="inlineStr">
+        <is>
+          <t>buscar informações que corroborem escolhas anteriores e descartar as que contestem julgamentos prévios.</t>
+        </is>
+      </c>
+      <c r="K493" t="inlineStr">
+        <is>
+          <t>acreditar que é possível prever o resultado de eventos aleatórios, favorecendo o controle e a gestão do acaso.</t>
+        </is>
+      </c>
+      <c r="L493" t="inlineStr">
+        <is>
+          <t>preferir um ganho certo de uma quantidade moderada a um resultado mais arriscado, mesmo que este tenha uma compensação mais alta.</t>
+        </is>
+      </c>
+      <c r="M493" t="inlineStr">
+        <is>
+          <t>julgar as coisas com base nas informações mais facilmente disponíveis, levando a superestimar eventos improváveis.</t>
+        </is>
+      </c>
+      <c r="N493" t="inlineStr">
+        <is>
+          <t>fixar-se em uma informação como ponto de partida e a dificuldade de ajustar-se diante de informações posteriores.</t>
+        </is>
+      </c>
+      <c r="O493" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P493" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q493" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="n">
+        <v>494</v>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D494" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E494" t="inlineStr">
+        <is>
+          <t>Considere o texto a seguir.
+&lt;b&gt;Ludmilla dá o sangue&lt;/b&gt;
+A cantora Ludmilla prometeu dar um ingresso de seu show “Numanice” para cada pessoa que doasse sangue entre os dias 5 e 7 de julho, no Rio de Janeiro.
+Como resultado, recordes de doações foram batidos. Ao ver os números, eu pensei que este seria um belíssimo caso em que a economia comportamental pode explicar o fenômeno. Ela é uma disciplina que surge da incorporação, pela economia, de desenvolvimentos teóricos e descobertas empíricas no campo da psicologia, da neurociência e de outras ciência sociais.
+&lt;i&gt;SANTANA, Irapuã. Ludmilla dá o sangue. O Globo, Rio de Janeiro, ano XCVIII, n. 32.851, 17 jul. 2023. Opinião, p. 3. Adaptado.&lt;/i&gt;
+Para o autor do texto, o sucesso da campanha da cantora Ludmilla explica-se pela tomada de decisão intuitiva que pode ser caracterizada como um</t>
+        </is>
+      </c>
+      <c r="F494" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G494" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H494" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I494" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J494" t="inlineStr">
+        <is>
+          <t>modelo racional de tomada de decisão e escolhas coerentes e de valor maximizado dentro de certos limites e restrições.</t>
+        </is>
+      </c>
+      <c r="K494" t="inlineStr">
+        <is>
+          <t>modelo simplificado de racionalidade limitada que captura toda a complexidade da decisão.</t>
+        </is>
+      </c>
+      <c r="L494" t="inlineStr">
+        <is>
+          <t>processo de decisões significativas tomadas mais por meio de julgamentos objetivos do que por um modelo prescritivo.</t>
+        </is>
+      </c>
+      <c r="M494" t="inlineStr">
+        <is>
+          <t>processo cognitivo inconsciente, gerado pelas experiências vividas, que geralmente envolve emoções.</t>
+        </is>
+      </c>
+      <c r="N494" t="inlineStr">
+        <is>
+          <t>processo decisório no qual as pessoas se satisfazem, isto é, buscam soluções que sejam suficientes e satisfatórias, e não ótimas.</t>
+        </is>
+      </c>
+      <c r="O494" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P494" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q494" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="n">
+        <v>495</v>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D495" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E495" t="inlineStr">
+        <is>
+          <t>Um gerente está tentando decidir se deve construir um novo navio pequeno ou grande. A decisão depende muito da demanda futura que deverá surgir, que poderá ser baixa ou alta. O gerente pode fazer uma relação dos possíveis eventos, mas não pode estimar suas probabilidades, portanto, há uma tomada de decisão com incerteza. Nesse caso, o gerente opta por uma regra de decisão denominada “Laplace”, escolhendo a seguinte alternativa:</t>
+        </is>
+      </c>
+      <c r="F495" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G495" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H495" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I495" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J495" t="inlineStr">
+        <is>
+          <t>“melhor das melhores”, adotada por pessoas otimistas, que têm grandes expectativas e preferem arriscar tudo num esforço grande.</t>
+        </is>
+      </c>
+      <c r="K495" t="inlineStr">
+        <is>
+          <t>“melhor das piores”, adotada por pessoas pessimistas, que antecipa o pior caso para cada opção.</t>
+        </is>
+      </c>
+      <c r="L495" t="inlineStr">
+        <is>
+          <t>“melhor payoff ponderado”, adotada por pessoas realistas, que atribui igual importância a cada evento.</t>
+        </is>
+      </c>
+      <c r="M495" t="inlineStr">
+        <is>
+          <t>“melhor pior arrependimento”, que mostra, para cada evento, quanto é perdido ao selecionar uma alternativa para aquela que é melhor para esse evento.</t>
+        </is>
+      </c>
+      <c r="N495" t="inlineStr">
+        <is>
+          <t>“melhor pior perda de oportunidade”, que mostra a diferença entre um determinado payoff e o melhor payoff das mesmas alternativas e eventos.</t>
+        </is>
+      </c>
+      <c r="O495" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P495" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q495" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="n">
+        <v>496</v>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CESGRANRIO </t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PETROBRAS </t>
+        </is>
+      </c>
+      <c r="D496" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E496" t="inlineStr">
+        <is>
+          <t>Quando o administrador da empresa comparou o processo decisório de dois de seus subordinados, percebeu que X é mais lento para processar as informações, quase sempre demorando mais tempo para decidir do que Y, e que sua escolha final nem sempre é a melhor. Além disso, quando existe uma óbvia dimensão de risco associada à sua decisão, X sempre prefere assumir o risco.
+Dos diferentes estilos de tomada de decisões de X e Y conclui-se que enquanto Y tem estilo</t>
+        </is>
+      </c>
+      <c r="F496" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G496" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H496" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I496" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J496" t="inlineStr">
+        <is>
+          <t>diretivo, com alta tolerância à ambiguidade e busca a racionalidade, X tem um estilo analítico com pouca tolerância à ambiguidade.</t>
+        </is>
+      </c>
+      <c r="K496" t="inlineStr">
+        <is>
+          <t>conceitual, que considera um grande número de alternativas possíveis para o problema e dados de várias fontes, X tem um estilo comportamental focado no longo prazo e no uso de dados confiáveis.</t>
+        </is>
+      </c>
+      <c r="L496" t="inlineStr">
+        <is>
+          <t>analítico, que o leva ao desejo de mais informações e à consideração de número maior de alternativas, X tem um estilo conceitual com alta tolerância à ambiguidade e uma visão ampla dos fatos.</t>
+        </is>
+      </c>
+      <c r="M496" t="inlineStr">
+        <is>
+          <t>comportamental e gosta de conversar com as pessoas uma por uma para compreender seus sentimentos sobre o problema, X tem um estilo conceitual, preferindo soluções claras e eficientes, embasadas em regras e procedimentos.</t>
+        </is>
+      </c>
+      <c r="N496" t="inlineStr">
+        <is>
+          <t>utilitarista e toma decisões embasado em regras justas e imparciais, de maneira que exista uma distribuição equitativa de custos e de benefícios, X tem um estilo deontológico e toma decisões visando ao bem-estar da maioria.</t>
+        </is>
+      </c>
+      <c r="O496" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P496" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q496" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="n">
+        <v>497</v>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CESGRANRIO </t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D497" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E497" t="inlineStr">
+        <is>
+          <t>Um gerente de projeto recebe determinação para realizar uma análise de valor monetário esperado (VME) e, em consequência, sugerir à direção da empresa, uma entre duas alternativas para a realização de determinada fase de um projeto. Levanta, então, as seguintes informações:
+- Investimentos
+&lt;ul&gt;&lt;li&gt;Linha de ação acelerada: R$ 80.000,00&lt;/li&gt;&lt;li&gt;Procedimento padrão: R$ 40.000,00&lt;/li&gt;&lt;/ul&gt;
+- Receita prevista e probabilidade correspondente, no caso de haver bônus por bom desempenho
+&lt;ul&gt;&lt;li&gt;Linha de ação acelerada: R$ 430.000,00 e 70% de probabilidade de ocorrência&lt;/li&gt;&lt;li&gt;Procedimento padrão: R$ 400.000,00 e 70% de probabilidade de ocorrência&lt;/li&gt;&lt;/ul&gt;
+- Receita prevista e probabilidade correspondente, no caso de haver multa por mau desempenho
+&lt;ul&gt;&lt;li&gt;Linha de ação acelerada: R$ 300.000,00 e 30% de probabilidade de ocorrência&lt;/li&gt;&lt;li&gt;Procedimento padrão: R$ 280.000,00 e 30% de probabilidade de ocorrência&lt;/li&gt;&lt;/ul&gt;
+Qual foi o tipo de procedimento e o respectivo VME pelos quais decidiu o gerente de projeto?</t>
+        </is>
+      </c>
+      <c r="F497" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G497" t="inlineStr">
+        <is>
+          <t>Processos Decisórios</t>
+        </is>
+      </c>
+      <c r="H497" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I497" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J497" t="inlineStr">
+        <is>
+          <t>Procedimento padrão e R$ 280.000,00</t>
+        </is>
+      </c>
+      <c r="K497" t="inlineStr">
+        <is>
+          <t>Procedimento padrão e R$ 324.000,00</t>
+        </is>
+      </c>
+      <c r="L497" t="inlineStr">
+        <is>
+          <t>Linha de ação acelerada e R$ 245.000,00</t>
+        </is>
+      </c>
+      <c r="M497" t="inlineStr">
+        <is>
+          <t>Linha de ação acelerada e R$ 301.000,00</t>
+        </is>
+      </c>
+      <c r="N497" t="inlineStr">
+        <is>
+          <t>Linha de ação acelerada e R$ 350.000,00</t>
+        </is>
+      </c>
+      <c r="O497" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P497" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q497" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="n">
+        <v>498</v>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D498" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="E498" t="inlineStr">
+        <is>
+          <t>A possibilidade de descrição geral dos produtos que determinada empresa deseja fabricar e a definição dos mercados aos quais ela atenderá, usando suas competências essenciais básicas e sendo eficaz ao conseguir estabelecer a individualidade da empresa, referem-se, num planejamento estratégico, à etapa de</t>
+        </is>
+      </c>
+      <c r="F498" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G498" t="inlineStr">
+        <is>
+          <t>Engenharia Organizacional</t>
+        </is>
+      </c>
+      <c r="H498" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I498" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J498" t="inlineStr">
+        <is>
+          <t>declaração de missão empresarial.</t>
+        </is>
+      </c>
+      <c r="K498" t="inlineStr">
+        <is>
+          <t>visão organizacional.</t>
+        </is>
+      </c>
+      <c r="L498" t="inlineStr">
+        <is>
+          <t>avaliação do mercado interno.</t>
+        </is>
+      </c>
+      <c r="M498" t="inlineStr">
+        <is>
+          <t>descrição de cenários.</t>
+        </is>
+      </c>
+      <c r="N498" t="inlineStr">
+        <is>
+          <t>cultura organizacional.</t>
+        </is>
+      </c>
+      <c r="O498" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P498" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q498" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="n">
+        <v>499</v>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D499" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E499" t="inlineStr">
+        <is>
+          <t>No planejamento estratégico de uma empresa do setor energético está escrita a seguinte frase: “Ser referência no setor de energia, oferecendo produtos de qualidade aos clientes e atendendo aos interesses dos stakeholders”. Essa frase se refere a:</t>
+        </is>
+      </c>
+      <c r="F499" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G499" t="inlineStr">
+        <is>
+          <t>Engenharia Organizacional</t>
+        </is>
+      </c>
+      <c r="H499" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I499" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J499" t="inlineStr">
+        <is>
+          <t>composto de marketing</t>
+        </is>
+      </c>
+      <c r="K499" t="inlineStr">
+        <is>
+          <t>missão da empresa</t>
+        </is>
+      </c>
+      <c r="L499" t="inlineStr">
+        <is>
+          <t>visão da empresa</t>
+        </is>
+      </c>
+      <c r="M499" t="inlineStr">
+        <is>
+          <t>valores da empresa</t>
+        </is>
+      </c>
+      <c r="N499" t="inlineStr">
+        <is>
+          <t>estratégia operacional</t>
+        </is>
+      </c>
+      <c r="O499" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P499" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q499" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="n">
+        <v>500</v>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D500" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="E500" t="inlineStr">
+        <is>
+          <t>O desempenho satisfatório de uma organização não de- pende apenas de um processo de planejamento responsável por elaborar objetivos desafiadores e realistas de um desenho estrutural que permita a execução adequada de atividades e de uma direção que lidere e motive os funcionários; depende também de um sistema de controle eficaz, que seja responsável por identificar possíveis desvios e corrigi-los em tempo hábil.
+&lt;i&gt;SOBRAL, Filipe; PECI, Alketa. Administração, teoria e prática. São Paulo: Pearson, 2008. p. 231.&lt;/i&gt;
+Sabendo-se que o controle é um conceito aplicável a diferentes níveis organizacionais, a função que corresponde ao controle estratégico é:</t>
+        </is>
+      </c>
+      <c r="F500" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G500" t="inlineStr">
+        <is>
+          <t>Engenharia Organizacional</t>
+        </is>
+      </c>
+      <c r="H500" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I500" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J500" t="inlineStr">
+        <is>
+          <t>possibilitar decisões específicas dos gerentes para resolver problemas em suas áreas de atuação.</t>
+        </is>
+      </c>
+      <c r="K500" t="inlineStr">
+        <is>
+          <t>utilizar mecanismos de controle específicos, com foco em atividades operacionais.</t>
+        </is>
+      </c>
+      <c r="L500" t="inlineStr">
+        <is>
+          <t>garantir todos os recursos necessários à execução das atividades.</t>
+        </is>
+      </c>
+      <c r="M500" t="inlineStr">
+        <is>
+          <t>analisar a adequação da missão, visão, estratégias e objetivos organizacionais.</t>
+        </is>
+      </c>
+      <c r="N500" t="inlineStr">
+        <is>
+          <t>monitorar as atividades de acordo com os padrões definidos pela alta direção.</t>
+        </is>
+      </c>
+      <c r="O500" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P500" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q500" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="n">
+        <v>501</v>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D501" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E501" t="inlineStr">
+        <is>
+          <t>Em relação ao Balanced Scorecard (BSC), considere as afirmações a seguir.
+I – Na gestão estratégica competitiva, o BSC é utilizado como um sistema de controle estratégico que permite às organizações utilizarem o desdobramento da estratégia para fazerem o seu planejamento.
+II – O BSC é uma ferramenta gerencial e, portanto, deve ficar nas mãos da direção e não precisa ser compartilhada com os funcionários.
+III – Em oposição aos sistemas de avaliação de gestão estratégica dos anos sessenta, o BSC baseiase em indicadores financeiros e não financeiros.
+IV – O BSC realiza medições com indicadores para monitoramento em três dimensões-chave: clientes externos, processos internos e financeira.
+É correto o que se afirma em</t>
+        </is>
+      </c>
+      <c r="F501" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G501" t="inlineStr">
+        <is>
+          <t>Engenharia Organizacional</t>
+        </is>
+      </c>
+      <c r="H501" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I501" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J501" t="inlineStr">
+        <is>
+          <t>I e III, apenas</t>
+        </is>
+      </c>
+      <c r="K501" t="inlineStr">
+        <is>
+          <t>II e IV, apenas</t>
+        </is>
+      </c>
+      <c r="L501" t="inlineStr">
+        <is>
+          <t>I, II e III, apenas</t>
+        </is>
+      </c>
+      <c r="M501" t="inlineStr">
+        <is>
+          <t>II, III e IV, apenas</t>
+        </is>
+      </c>
+      <c r="N501" t="inlineStr">
+        <is>
+          <t>I, II, III e IV</t>
+        </is>
+      </c>
+      <c r="O501" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P501" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q501" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="n">
+        <v>502</v>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D502" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="E502" t="inlineStr">
+        <is>
+          <t>O planejamento estratégico é condição precípua para a sobrevivência das organizações modernas, dado que o dinamismo ambiental, sua flexibilidade e mutação constante contrastam com o ambiente organizacional estático de um passado recente.
+Planejar é palavra-chave para as organizações se ajustarem às mudanças globais.
+Analise as características listadas abaixo.
+I - Especifica o rumo da organização, permitindo direcionar esforços dos seus membros para um objetivo comum.
+II - Promove a integração e a coordenação das atividades dos membros organizacionais.
+III- Facilita a identificação das pessoas com a organização.
+IV – Serve de fundamento para o processo decisório.
+As características que correspondem às vantagens do planejamento estratégico quando relacionadas, respectivamente, ao senso de direção e ao foco nos esforços, são (</t>
+        </is>
+      </c>
+      <c r="F502" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G502" t="inlineStr">
+        <is>
+          <t>Engenharia Organizacional</t>
+        </is>
+      </c>
+      <c r="H502" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I502" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J502" t="inlineStr">
+        <is>
+          <t>I e II apenas (</t>
+        </is>
+      </c>
+      <c r="K502" t="inlineStr">
+        <is>
+          <t>III e IV, apenas (</t>
+        </is>
+      </c>
+      <c r="L502" t="inlineStr">
+        <is>
+          <t>I, II e III, apenas (</t>
+        </is>
+      </c>
+      <c r="M502" t="inlineStr">
+        <is>
+          <t>II, III e IV, apenas (</t>
+        </is>
+      </c>
+      <c r="N502" t="inlineStr">
+        <is>
+          <t>I, II, III, e IV</t>
+        </is>
+      </c>
+      <c r="O502" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P502" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q502" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="n">
+        <v>503</v>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>VUNESP</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>UFABC</t>
+        </is>
+      </c>
+      <c r="D503" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E503" t="inlineStr">
+        <is>
+          <t>O prefeito que recentemente assumiu um pequeno município constatou uma situação desafiadora: faltavam emprego e renda para mais de 30% da população economicamente ativa. O histórico desse município indicava um quadro de ausência de inovação na gestão pública nos últimos 20 anos. Por outro lado, o chefe do executivo acreditava no potencial desse município, pois havia recursos naturais em abundância – rios, peixes, extensa e rica fauna e flora –, uma população criativa e empreendora, enfim um contexto favorável para melhoria econômica. Assim, ele reuniu sua equipe da área de desenvolvimento econômico e solicitou um Planejamento Estratégico. Sua equipe, diante dessa situação e ciente da complexidade na elaboração desse planejamento estratégico, procedeu corretamente realizando:</t>
+        </is>
+      </c>
+      <c r="F503" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G503" t="inlineStr">
+        <is>
+          <t>Engenharia Organizacional</t>
+        </is>
+      </c>
+      <c r="H503" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I503" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J503" t="inlineStr">
+        <is>
+          <t>Um trabalho de intervenção sobre os pontos fracos e fortes desse município e uma pesquisa sobre o perfil dos moradores e da economia local para uma proposta de redesenho da estrutura municipal</t>
+        </is>
+      </c>
+      <c r="K503" t="inlineStr">
+        <is>
+          <t>Uma proposta de ação estratégica para o desenvolvimento de competências dos moradores, de tal forma a ampliar as oportunidades de emprego e renda da população economicamente ativa.</t>
+        </is>
+      </c>
+      <c r="L503" t="inlineStr">
+        <is>
+          <t>O mapeamento de oportunidades de emprego e renda nesse município de tal forma a otimizar os recursos existentes e também trabalhando no sentido de melhorar o transporte aos municípios vizinhos para a busca de trabalho.</t>
+        </is>
+      </c>
+      <c r="M503" t="inlineStr">
+        <is>
+          <t>Uma análise de municípios congêneres que conseguiram gerar emprego e renda a partir da sua realidade local, ou seja, a equipe foi em busca de potenciais oportunidades e ameaças, tendo em vista a ciência dos pontos fortes e fracos.</t>
+        </is>
+      </c>
+      <c r="N503" t="inlineStr">
+        <is>
+          <t>A análise situacional, pois pode-se prescindir da realidade local e do perfil dos moradores; além disso, buscou-se uma proposta de estímulo à inovação a partir de palestras e eventos com consultores e especialistas.</t>
+        </is>
+      </c>
+      <c r="O503" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P503" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q503" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="n">
+        <v>504</v>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D504" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E504" t="inlineStr">
+        <is>
+          <t>O Balanced Scorecard (BSC) é uma ferramenta da administração que pode ser usada para gerenciar o desempenho organizacional.
+Analisando-se essa ferramenta, verifica-se que ela:</t>
+        </is>
+      </c>
+      <c r="F504" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G504" t="inlineStr">
+        <is>
+          <t>Engenharia Organizacional</t>
+        </is>
+      </c>
+      <c r="H504" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I504" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J504" t="inlineStr">
+        <is>
+          <t>permite avaliar o posicionamento estratégico da empresa por meio da identificação das forças e fraquezas (ambiente interno) e das ameaças e oportunidades (ambiente externo).</t>
+        </is>
+      </c>
+      <c r="K504" t="inlineStr">
+        <is>
+          <t>pode ser considerada como um modelo de gestão estratégico, que permite às empresas priorizarem suas ações do dia a dia para atingirem os objetivos traçados em seus planos estratégicos.</t>
+        </is>
+      </c>
+      <c r="L504" t="inlineStr">
+        <is>
+          <t>é o conceito de gestão que aumenta o gap existente entre a estratégia e a parte operacional do negócio, alinhando a empresa aos seus objetivos estratégicos.</t>
+        </is>
+      </c>
+      <c r="M504" t="inlineStr">
+        <is>
+          <t>substitui as medidas financeiras por outras relacionadas aos aspectos subjetivos como satisfação dos clientes, aprendizagem e crescimento organizacional.</t>
+        </is>
+      </c>
+      <c r="N504" t="inlineStr">
+        <is>
+          <t>analisa os fatores que satisfaçam tanto clientes (internos e externos) quanto fornecedores, considerando a perspectiva dos clientes.</t>
+        </is>
+      </c>
+      <c r="O504" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P504" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q504" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="n">
+        <v>505</v>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D505" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E505" t="inlineStr">
+        <is>
+          <t>Sobre o Modelo das Cinco Forças Competitivas, considere as afirmações a seguir.
+I. São exemplos de ameaças a produtos substitutos os custos de mudança, a diferenciação do produto e as economias de escala.
+II. O maior poder de negociação dos compradores conduz à disputa entre fornecedores concorrentes e, consequentemente, à redução na rentabilidade do negócio.
+III. A ameaça de saída de um participante da indústria diz respeito à relação entre as barreiras de saída existentes e a reação dos concorrentes à saída deste participante.
+IV. A competição com produtos substitutos faz com que haja uma redução no retorno potencial das empresas deste mercado, uma vez que limita o preço que tais empresas podem fixar.
+É correto o que se afirma em:</t>
+        </is>
+      </c>
+      <c r="F505" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G505" t="inlineStr">
+        <is>
+          <t>Engenharia Organizacional</t>
+        </is>
+      </c>
+      <c r="H505" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I505" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J505" t="inlineStr">
+        <is>
+          <t>I e III, apenas</t>
+        </is>
+      </c>
+      <c r="K505" t="inlineStr">
+        <is>
+          <t>II e IV, apenas</t>
+        </is>
+      </c>
+      <c r="L505" t="inlineStr">
+        <is>
+          <t>I, II e III, apenas</t>
+        </is>
+      </c>
+      <c r="M505" t="inlineStr">
+        <is>
+          <t>II, III e IV, apenas</t>
+        </is>
+      </c>
+      <c r="N505" t="inlineStr">
+        <is>
+          <t>I, II, III e IV</t>
+        </is>
+      </c>
+      <c r="O505" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P505" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q505" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="n">
+        <v>506</v>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>IFMT</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>IFMT</t>
+        </is>
+      </c>
+      <c r="D506" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="E506" t="inlineStr">
+        <is>
+          <t>Sobre o Diagnóstico Estratégico, marque V para as afirmativas verdadeiras e F para as falsas.
+( ) O diagnóstico que corresponde a uma análise estratégica tem como uma das premissas básicas considerar o ambiente e suas variáveis relevantes no qual está inserida a empresa.
+( ) Um dos instrumentos administrativos que podem auxiliar o processo do diagnóstico estratégico é o benchmarking.
+( ) A análise interna tem por finalidade estudar a relação existente entre a organização e seu ambiente em termos de oportunidades e ameaças.
+( ) Os pontos fortes e fracos representam as variáveis controláveis, enquanto as oportunidades e ameaças representam as variáveis não controláveis pela organização.
+Assinale a sequência correta.</t>
+        </is>
+      </c>
+      <c r="F506" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G506" t="inlineStr">
+        <is>
+          <t>Engenharia Organizacional</t>
+        </is>
+      </c>
+      <c r="H506" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I506" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J506" t="inlineStr">
+        <is>
+          <t>V, V, F, V</t>
+        </is>
+      </c>
+      <c r="K506" t="inlineStr">
+        <is>
+          <t>V, F, V, F</t>
+        </is>
+      </c>
+      <c r="L506" t="inlineStr">
+        <is>
+          <t>F, V, F, V</t>
+        </is>
+      </c>
+      <c r="M506" t="inlineStr">
+        <is>
+          <t>F, F, V, F</t>
+        </is>
+      </c>
+      <c r="N506" t="inlineStr"/>
+      <c r="O506" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P506" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q506" t="n">
+        <v>0</v>
+      </c>
+      <c r="R506" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
:up: :checkered_flag: sistema agora é capaz de captar tb as questões de sintaxe '[número] - (', questões comentadas de engenharia de produto cadastradas
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R631"/>
+  <dimension ref="A1:R656"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -53401,7 +53401,1821 @@
       <c r="Q631" t="n">
         <v>0</v>
       </c>
-      <c r="R631" t="inlineStr"/>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>632</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>COMPERVE</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>UFRN</t>
+        </is>
+      </c>
+      <c r="D632" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="E632" t="inlineStr">
+        <is>
+          <t>O sistema logístico deve se adaptar ao ciclo de vida do produto, de maneira a atingir um equilíbrio entre custos logísticos e nível de serviço. Nesse contexto, é correto afirmar:</t>
+        </is>
+      </c>
+      <c r="F632" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G632" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H632" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I632" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J632" t="inlineStr">
+        <is>
+          <t>a fase de declínio requer que o produto esteja presente na totalidade de armazéns do sistema de distribuição a fim de alavancar as vendas.</t>
+        </is>
+      </c>
+      <c r="K632" t="inlineStr">
+        <is>
+          <t>o estágio de lançamento requer que o sistema logístico garanta disponibilidade ilimitada do produto para evitar perda de vendas.</t>
+        </is>
+      </c>
+      <c r="L632" t="inlineStr">
+        <is>
+          <t>no período de maturidade, o controle sobre a disponibilidade do produto se torna inviável devido às incertezas e às oscilações da demanda.</t>
+        </is>
+      </c>
+      <c r="M632" t="inlineStr">
+        <is>
+          <t>no estágio de crescimento, a disponibilidade do produto deve aumentar rapidamente numa ampla área geográfica, porém não se conhece a demanda com certo grau de confiabilidade.</t>
+        </is>
+      </c>
+      <c r="N632" t="inlineStr"/>
+      <c r="O632" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P632" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q632" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="n">
+        <v>633</v>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D633" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="E633" t="inlineStr">
+        <is>
+          <t>Com relação ao ciclo de vida de um produto no mercado, considere as seguintes afirmações:
+I – Na fase de introdução do produto no mercado, ocorre um crescimento relativamente lento das vendas, em comparação com as demais fases.
+II – Na fase de maturidade, ou saturação, as vendas são inferiores às registradas na fase de crescimento.
+III – Durante a fase de crescimento, em geral, o produto é retirado do mercado.
+IV – Na fase de renovação, o produto ganha acessórios. É correto APENAS o que se afirma em</t>
+        </is>
+      </c>
+      <c r="F633" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G633" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H633" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I633" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J633" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="K633" t="inlineStr">
+        <is>
+          <t>II</t>
+        </is>
+      </c>
+      <c r="L633" t="inlineStr">
+        <is>
+          <t>I e III</t>
+        </is>
+      </c>
+      <c r="M633" t="inlineStr">
+        <is>
+          <t>II e IV</t>
+        </is>
+      </c>
+      <c r="N633" t="inlineStr">
+        <is>
+          <t>III e IV</t>
+        </is>
+      </c>
+      <c r="O633" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P633" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q633" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="n">
+        <v>634</v>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D634" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E634" t="inlineStr">
+        <is>
+          <t>Após a introdução de um novo produto ou serviço, ocorrem mudanças tanto no próprio projeto do produto quanto no projeto do sistema de produção. Contudo, as inovações no produto ou no processo tendem a ter intensidades distintas, em função do estágio do ciclo de vida onde o produto esteja situado.
+Nesse âmbito, a quantidade de mudanças ou inovações no processo tende a começar a aumentar</t>
+        </is>
+      </c>
+      <c r="F634" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G634" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H634" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I634" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J634" t="inlineStr">
+        <is>
+          <t>no estágio de introdução do produto</t>
+        </is>
+      </c>
+      <c r="K634" t="inlineStr">
+        <is>
+          <t>no estágio de diversificação do produto</t>
+        </is>
+      </c>
+      <c r="L634" t="inlineStr">
+        <is>
+          <t>apenas a partir do estágio de maturidade do produto</t>
+        </is>
+      </c>
+      <c r="M634" t="inlineStr">
+        <is>
+          <t>a partir do estágio de declínio do produto</t>
+        </is>
+      </c>
+      <c r="N634" t="inlineStr">
+        <is>
+          <t>a partir do estágio de crescimento do produto</t>
+        </is>
+      </c>
+      <c r="O634" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P634" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q634" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="n">
+        <v>635</v>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D635" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="E635" t="inlineStr">
+        <is>
+          <t>A demanda de diversos produtos passa por fases que constituem o seu ciclo de vida. Os efeitos gerenciais na empresa exigem diferentes estratégias financeiras, de fabricação e de marketing para cada fase, durante o tempo em que o produto se encontra no mercado.
+A fase em que o produto final é elevado e que a flexibilidade é um dos objetivos das operações de produção é a de</t>
+        </is>
+      </c>
+      <c r="F635" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G635" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H635" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I635" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J635" t="inlineStr">
+        <is>
+          <t>crescimento</t>
+        </is>
+      </c>
+      <c r="K635" t="inlineStr">
+        <is>
+          <t>declínio</t>
+        </is>
+      </c>
+      <c r="L635" t="inlineStr">
+        <is>
+          <t>introdução</t>
+        </is>
+      </c>
+      <c r="M635" t="inlineStr">
+        <is>
+          <t>maturidade</t>
+        </is>
+      </c>
+      <c r="N635" t="inlineStr">
+        <is>
+          <t>saturação</t>
+        </is>
+      </c>
+      <c r="O635" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P635" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q635" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="n">
+        <v>636</v>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>UFES</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>UFES</t>
+        </is>
+      </c>
+      <c r="D636" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="E636" t="inlineStr">
+        <is>
+          <t>O ciclo de vida de produtos relaciona-se ao:</t>
+        </is>
+      </c>
+      <c r="F636" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G636" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H636" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I636" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J636" t="inlineStr">
+        <is>
+          <t>histórico do produto, desde sua criação até a sua retirada do mercado.</t>
+        </is>
+      </c>
+      <c r="K636" t="inlineStr">
+        <is>
+          <t>trabalho de criação do produto, desde o seu projeto até o término de sua produção na organização.</t>
+        </is>
+      </c>
+      <c r="L636" t="inlineStr">
+        <is>
+          <t>projeto de criação do produto na organização, bem como às eventuais revisões necessárias durante a sua produção.</t>
+        </is>
+      </c>
+      <c r="M636" t="inlineStr">
+        <is>
+          <t>ciclo de vida do produto, do ponto de vista dos clientes, que são a razão de existir dos produtos.</t>
+        </is>
+      </c>
+      <c r="N636" t="inlineStr">
+        <is>
+          <t>ciclo de produção propriamente dito.</t>
+        </is>
+      </c>
+      <c r="O636" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P636" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q636" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="n">
+        <v>637</v>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>CEBRASPE</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>FUB</t>
+        </is>
+      </c>
+      <c r="D637" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E637" t="inlineStr">
+        <is>
+          <t>Acerca das estratégias de produção, julgue o item a seguir.
+A maioria das curvas do ciclo de vida do produto, normalmente divididas em introdução, crescimento, maturidade e declínio, assume a forma de sino.</t>
+        </is>
+      </c>
+      <c r="F637" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G637" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H637" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I637" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J637" t="inlineStr"/>
+      <c r="K637" t="inlineStr"/>
+      <c r="L637" t="inlineStr"/>
+      <c r="M637" t="inlineStr"/>
+      <c r="N637" t="inlineStr"/>
+      <c r="O637" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P637" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q637" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="n">
+        <v>638</v>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Questão inédita</t>
+        </is>
+      </c>
+      <c r="D638" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E638" t="inlineStr">
+        <is>
+          <t>Com relação ao ciclo de vida de um produto no mercado, considere as seguintes afirmações:
+I – Na fase de crescimento do produto no mercado é onde há o maior pico de vendas.
+II – Na fase de maturidade, o produto deve buscar a flexibilidade enquanto objetivo de desempenho.
+III – Durante a fase de declínio, deve haver um número elevado de estoque.
+IV – Na fase de sustentabilidade, estuda-se como o produto pode afetar o meio ambiente.
+É correto APENAS o que se afirma em</t>
+        </is>
+      </c>
+      <c r="F638" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G638" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H638" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I638" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J638" t="inlineStr">
+        <is>
+          <t>I e II</t>
+        </is>
+      </c>
+      <c r="K638" t="inlineStr">
+        <is>
+          <t>II e III</t>
+        </is>
+      </c>
+      <c r="L638" t="inlineStr">
+        <is>
+          <t>I, II e III</t>
+        </is>
+      </c>
+      <c r="M638" t="inlineStr">
+        <is>
+          <t>I, II, III, e IV</t>
+        </is>
+      </c>
+      <c r="N638" t="inlineStr">
+        <is>
+          <t>Nenhuma das alternativas anteriores.</t>
+        </is>
+      </c>
+      <c r="O638" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P638" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q638" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="n">
+        <v>639</v>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>TRANSPETRO</t>
+        </is>
+      </c>
+      <c r="D639" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E639" t="inlineStr">
+        <is>
+          <t>Um processo típico de desenvolvimento de produto é dividido em macrofases, a saber: Pré-desenvolvimento, Desenvolvimento e Pós-desenvolvimento. A macrofase de Desenvolvimento, por sua vez, é dividida em diversas fases. Uma dessas fases tem como objetivo criar, a partir do Plano do Projeto, as chamadas Especificações-Meta, compostas pelos requisitos e informações qualitativas necessários para o desenvolvimento do futuro produto.
+O nome dessa fase é</t>
+        </is>
+      </c>
+      <c r="F639" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G639" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H639" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I639" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J639" t="inlineStr">
+        <is>
+          <t>Lançamento do Produto</t>
+        </is>
+      </c>
+      <c r="K639" t="inlineStr">
+        <is>
+          <t>Preparação da Produção</t>
+        </is>
+      </c>
+      <c r="L639" t="inlineStr">
+        <is>
+          <t>Projeto Conceitual</t>
+        </is>
+      </c>
+      <c r="M639" t="inlineStr">
+        <is>
+          <t>Projeto Detalhado</t>
+        </is>
+      </c>
+      <c r="N639" t="inlineStr">
+        <is>
+          <t>Projeto Informacional</t>
+        </is>
+      </c>
+      <c r="O639" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P639" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q639" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="n">
+        <v>640</v>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>UFTM</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>UFTM</t>
+        </is>
+      </c>
+      <c r="D640" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E640" t="inlineStr">
+        <is>
+          <t>Sobre a fase na qual se identificam as necessidades do consumidor para o desenvolvimento de produtos, é CORRETO afirmar que:</t>
+        </is>
+      </c>
+      <c r="F640" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G640" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H640" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I640" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J640" t="inlineStr">
+        <is>
+          <t>ocorre depois da fase de geração de conceitos.</t>
+        </is>
+      </c>
+      <c r="K640" t="inlineStr">
+        <is>
+          <t>ocorre antes da fase de geração de ideias.</t>
+        </is>
+      </c>
+      <c r="L640" t="inlineStr">
+        <is>
+          <t>busca identificar somente as necessidades explícitas.</t>
+        </is>
+      </c>
+      <c r="M640" t="inlineStr">
+        <is>
+          <t>provêm uma base para justificar as especificações.</t>
+        </is>
+      </c>
+      <c r="N640" t="inlineStr"/>
+      <c r="O640" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P640" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q640" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="n">
+        <v>641</v>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>FUB</t>
+        </is>
+      </c>
+      <c r="D641" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E641" t="inlineStr">
+        <is>
+          <t>Julgue o próximo item, acerca de planejamento e marketing do produto.
+O planejamento de produto, atividade que precede o desenvolvimento de um produto específico, envolve pesquisa de mercado, análise dos concorrentes e elaboração e especificações do projeto.</t>
+        </is>
+      </c>
+      <c r="F641" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G641" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H641" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I641" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J641" t="inlineStr"/>
+      <c r="K641" t="inlineStr"/>
+      <c r="L641" t="inlineStr"/>
+      <c r="M641" t="inlineStr"/>
+      <c r="N641" t="inlineStr"/>
+      <c r="O641" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P641" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q641" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="n">
+        <v>642</v>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Questão Inédita</t>
+        </is>
+      </c>
+      <c r="D642" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E642" t="inlineStr">
+        <is>
+          <t>Julgue o próximo item, acerca de planejamento e marketing do produto.
+Acerca da metodologia de desenvolvimento de produtos, julgue o item a seguir.
+Na fase pré-projeto, determina-se quais produtos a empresa deverá produzir somente com base na concorrência.</t>
+        </is>
+      </c>
+      <c r="F642" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G642" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H642" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I642" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J642" t="inlineStr"/>
+      <c r="K642" t="inlineStr"/>
+      <c r="L642" t="inlineStr"/>
+      <c r="M642" t="inlineStr"/>
+      <c r="N642" t="inlineStr"/>
+      <c r="O642" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P642" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q642" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="n">
+        <v>643</v>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>COMPERVE</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>UFRN</t>
+        </is>
+      </c>
+      <c r="D643" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="E643" t="inlineStr">
+        <is>
+          <t>No desenvolvimento de produto, a conversão das necessidades do consumidor em objetivos técnicos é fundamental para o controle de qualidade do projeto. Este, por sua vez, cumpre a dupla função de direcionar o processo de desenvolvimento do novo produto e de filtrar o desenvolvimento, deixando prosseguir apenas as alternativas que se aproximam da meta estabelecida.
+A opção que descreve a sequência correta de etapas desse processo é</t>
+        </is>
+      </c>
+      <c r="F643" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G643" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H643" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I643" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J643" t="inlineStr">
+        <is>
+          <t>planejamento do produto; projeto conceitual; configuração; detalhamento das especificações;</t>
+        </is>
+      </c>
+      <c r="K643" t="inlineStr">
+        <is>
+          <t>configuração das necessidades; projeto conceitual; planejamento do produto; detalhamento das especificações;</t>
+        </is>
+      </c>
+      <c r="L643" t="inlineStr">
+        <is>
+          <t>detalhamento das necessidades; planejamento do produto; configuração; projeto conceitual;</t>
+        </is>
+      </c>
+      <c r="M643" t="inlineStr">
+        <is>
+          <t>projeto conceitual; detalhamento das necessidades; planejamento do produto; configuração.</t>
+        </is>
+      </c>
+      <c r="N643" t="inlineStr"/>
+      <c r="O643" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P643" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q643" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="n">
+        <v>644</v>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>HEMOBRAS</t>
+        </is>
+      </c>
+      <c r="D644" t="inlineStr">
+        <is>
+          <t>2008</t>
+        </is>
+      </c>
+      <c r="E644" t="inlineStr">
+        <is>
+          <t>Uma equipe de projeto está desenvolvendo uma linha de produção para um novo produto. Nessa nova linha, haverá um maior grau de automação industrial, com a instalação de diversas máquinas cuja operação é controlada por computadores. Em determinado setor, um projetista pretende optar pela implantação de um sistema flexível de manufatura — flexible manufacturing system (FMS).
+Tendo a situação acima como referência inicial, julgue os itens que se seguem, acerca da utilização de computadores no projeto e na operação.
+A capacidade do CAD de facilitar a manipulação de detalhes do projeto pode aumentar a produtividade da atividade de projeto.</t>
+        </is>
+      </c>
+      <c r="F644" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G644" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H644" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I644" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J644" t="inlineStr"/>
+      <c r="K644" t="inlineStr"/>
+      <c r="L644" t="inlineStr"/>
+      <c r="M644" t="inlineStr"/>
+      <c r="N644" t="inlineStr"/>
+      <c r="O644" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P644" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q644" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="n">
+        <v>645</v>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>FUB</t>
+        </is>
+      </c>
+      <c r="D645" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E645" t="inlineStr">
+        <is>
+          <t>Com relação à metodologia de projeto do produto e à engenharia do produto, julgue o item a seguir.
+Embora a fabricação de novos produtos seja normalmente complexa, o desenvolvimento desses produtos constitui problema de fácil resolução, desde que se utilize um método adequado.</t>
+        </is>
+      </c>
+      <c r="F645" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G645" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H645" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I645" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J645" t="inlineStr"/>
+      <c r="K645" t="inlineStr"/>
+      <c r="L645" t="inlineStr"/>
+      <c r="M645" t="inlineStr"/>
+      <c r="N645" t="inlineStr"/>
+      <c r="O645" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P645" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q645" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="n">
+        <v>646</v>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>TJ-CE</t>
+        </is>
+      </c>
+      <c r="D646" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E646" t="inlineStr">
+        <is>
+          <t>Ainda que haja diferenças entre as empresas e seus produtos, existem etapas bem definidas no desenvolvimento do projeto de um produto, tais como</t>
+        </is>
+      </c>
+      <c r="F646" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G646" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H646" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I646" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J646" t="inlineStr">
+        <is>
+          <t>estabelecimento dos detalhes funcionais, identificação das necessidades técnicas e análise econômica.</t>
+        </is>
+      </c>
+      <c r="K646" t="inlineStr">
+        <is>
+          <t>geração e filtragem de ideias, projeto inicial, introdução, crescimento, maturidade e projeto final.</t>
+        </is>
+      </c>
+      <c r="L646" t="inlineStr">
+        <is>
+          <t>geração e filtragem de ideias, estabelecimento dos detalhes funcionais, identificação das necessidades técnicas e análise econômica.</t>
+        </is>
+      </c>
+      <c r="M646" t="inlineStr">
+        <is>
+          <t>geração e filtragem de ideias, projeto inicial, análise econômica, teste do protótipo e projeto final.</t>
+        </is>
+      </c>
+      <c r="N646" t="inlineStr">
+        <is>
+          <t>introdução, crescimento, maturidade, saturação e declínio.</t>
+        </is>
+      </c>
+      <c r="O646" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P646" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q646" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="n">
+        <v>647</v>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>HEMOBRAS</t>
+        </is>
+      </c>
+      <c r="D647" t="inlineStr">
+        <is>
+          <t>2008</t>
+        </is>
+      </c>
+      <c r="E647" t="inlineStr">
+        <is>
+          <t>A incerteza na atividade de projeto reduz-se à medida que o projeto evolui da concepção à especificação, com a escolha, por parte do projetista, da alternativa para se atingir os objetivos do projeto. Essa decisão deve ser tomada com base em uma avaliação do valor ou da importância de cada opção do projeto. A natureza da atividade de projeto em todos os aspectos da administração da produção pode ser caracterizada pelos quatro aspectos do projeto: criatividade, complexidade, compromisso e escolha.
+Acerca dos critérios e dos aspectos de projeto, julgue os itens a seguir.
+O aspecto de compromisso de um projeto emerge fortemente quando, em todos os níveis (desde o conceito básico até o menor detalhe), é necessário fazer-se escolhas entre diversas soluções possíveis para um problema.</t>
+        </is>
+      </c>
+      <c r="F647" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G647" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H647" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I647" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J647" t="inlineStr"/>
+      <c r="K647" t="inlineStr"/>
+      <c r="L647" t="inlineStr"/>
+      <c r="M647" t="inlineStr"/>
+      <c r="N647" t="inlineStr"/>
+      <c r="O647" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P647" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q647" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="n">
+        <v>648</v>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>UFG</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>UFG</t>
+        </is>
+      </c>
+      <c r="D648" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E648" t="inlineStr">
+        <is>
+          <t>Uma ferramenta amplamente utilizada no processo de desenvolvimento de produtos é o desdobramento da função qualidade (QFD). Essa ferramenta</t>
+        </is>
+      </c>
+      <c r="F648" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G648" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H648" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I648" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J648" t="inlineStr">
+        <is>
+          <t>é utilizada quando se deseja fazer uma análise de quais parâmetros do novo produto poderão atender às demandas dos clientes.</t>
+        </is>
+      </c>
+      <c r="K648" t="inlineStr">
+        <is>
+          <t>é conhecido como Casa da Qualidade, que é organizada em seis campos: os requisitos dos clientes; os requisitos do produto; a matriz de relacionamento; a importância dada pelo cliente a cada requisito; o benchmarking competitivo; a quantificação dos requisitos dos produtos.</t>
+        </is>
+      </c>
+      <c r="L648" t="inlineStr">
+        <is>
+          <t>analisa como os principais fornecedores dos componentes da empresa têm se comportado em relação a cada requisito do cliente por meio da matriz de correlação.</t>
+        </is>
+      </c>
+      <c r="M648" t="inlineStr">
+        <is>
+          <t>faz uma análise da interação de cada um dos requisitos dos clientes, por meio da matriz de correlação.</t>
+        </is>
+      </c>
+      <c r="N648" t="inlineStr"/>
+      <c r="O648" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P648" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q648" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="n">
+        <v>649</v>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>SLU-DF</t>
+        </is>
+      </c>
+      <c r="D649" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E649" t="inlineStr">
+        <is>
+          <t>O método desdobramento da função qualidade — QFD (Quality Function Deployment) —, também conhecido como método das matrizes, criado por japoneses no fim dos anos 60 do século passado, é considerado um dos mais importantes métodos utilizados no processo de desenvolvimento de produtos. Uma das matrizes que o compõem é a chamada casa da qualidade. A respeito de aspectos relacionados a esse método, julgue o item que se segue.
+O método QFD engloba, no total, quatro matrizes.</t>
+        </is>
+      </c>
+      <c r="F649" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G649" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H649" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I649" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J649" t="inlineStr"/>
+      <c r="K649" t="inlineStr"/>
+      <c r="L649" t="inlineStr"/>
+      <c r="M649" t="inlineStr"/>
+      <c r="N649" t="inlineStr"/>
+      <c r="O649" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P649" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q649" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="n">
+        <v>650</v>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>SLU-DF</t>
+        </is>
+      </c>
+      <c r="D650" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E650" t="inlineStr">
+        <is>
+          <t>O método desdobramento da função qualidade — QFD (Quality Function Deployment) —, também conhecido como método das matrizes, criado por japoneses no fim dos anos 60 do século passado, é considerado um dos mais importantes métodos utilizados no processo de desenvolvimento de produtos. Uma das matrizes que o compõem é a chamada casa da qualidade. A respeito de aspectos relacionados a esse método, julgue o item que se segue.
+No início do processo de aplicação do método QFD, na casa da qualidade, as necessidades dos clientes são convertidas em requisitos dos clientes.</t>
+        </is>
+      </c>
+      <c r="F650" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G650" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H650" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I650" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J650" t="inlineStr"/>
+      <c r="K650" t="inlineStr"/>
+      <c r="L650" t="inlineStr"/>
+      <c r="M650" t="inlineStr"/>
+      <c r="N650" t="inlineStr"/>
+      <c r="O650" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P650" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q650" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="n">
+        <v>651</v>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>SLU-DF</t>
+        </is>
+      </c>
+      <c r="D651" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E651" t="inlineStr">
+        <is>
+          <t>O método desdobramento da função qualidade — QFD (Quality Function Deployment) —, também conhecido como método das matrizes, criado por japoneses no fim dos anos 60 do século passado, é considerado um dos mais importantes métodos utilizados no processo de desenvolvimento de produtos. Uma das matrizes que o compõem é a chamada casa da qualidade. A respeito de aspectos relacionados a esse método, julgue o item que se segue.
+As características da qualidade do produto consistem em atributos do produto destinados a atender os requisitos dos clientes.</t>
+        </is>
+      </c>
+      <c r="F651" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G651" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H651" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I651" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J651" t="inlineStr"/>
+      <c r="K651" t="inlineStr"/>
+      <c r="L651" t="inlineStr"/>
+      <c r="M651" t="inlineStr"/>
+      <c r="N651" t="inlineStr"/>
+      <c r="O651" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P651" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q651" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="n">
+        <v>652</v>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>SLU-DF</t>
+        </is>
+      </c>
+      <c r="D652" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E652" t="inlineStr">
+        <is>
+          <t>O método desdobramento da função qualidade — QFD (Quality Function Deployment) —, também conhecido como método das matrizes, criado por japoneses no fim dos anos 60 do século passado, é considerado um dos mais importantes métodos utilizados no processo de desenvolvimento de produtos. Uma das matrizes que o compõem é a chamada casa da qualidade. A respeito de aspectos relacionados a esse método, julgue o item que se segue.
+As inter-relações entre os diversos requisitos dos clientes são identificadas no denominado telhado da casa da qualidade.</t>
+        </is>
+      </c>
+      <c r="F652" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G652" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H652" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I652" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J652" t="inlineStr"/>
+      <c r="K652" t="inlineStr"/>
+      <c r="L652" t="inlineStr"/>
+      <c r="M652" t="inlineStr"/>
+      <c r="N652" t="inlineStr"/>
+      <c r="O652" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P652" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q652" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="n">
+        <v>653</v>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>IFTO</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>IFTO</t>
+        </is>
+      </c>
+      <c r="D653" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="E653" t="inlineStr">
+        <is>
+          <t>Uma conversão das demandas dos consumidores em características de qualidade, desenvolvendo uma qualidade de projeto para o produto acabado pelos relacionamentos desdobrados sistematicamente entre as demandas e as características, começando com a qualidade de cada componente funcional e estendendo o desdobramento para a qualidade de cada parte e processo.
+Esta definição refere-se:</t>
+        </is>
+      </c>
+      <c r="F653" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G653" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H653" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I653" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J653" t="inlineStr">
+        <is>
+          <t>Engenharia de requisitos.</t>
+        </is>
+      </c>
+      <c r="K653" t="inlineStr">
+        <is>
+          <t>Teoria das Restrições.</t>
+        </is>
+      </c>
+      <c r="L653" t="inlineStr">
+        <is>
+          <t>Kanban.</t>
+        </is>
+      </c>
+      <c r="M653" t="inlineStr">
+        <is>
+          <t>Análise de SWOT.</t>
+        </is>
+      </c>
+      <c r="N653" t="inlineStr">
+        <is>
+          <t>Quality Function Deployment (QFD).</t>
+        </is>
+      </c>
+      <c r="O653" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P653" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q653" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="n">
+        <v>654</v>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>FUB</t>
+        </is>
+      </c>
+      <c r="D654" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E654" t="inlineStr">
+        <is>
+          <t>A respeito de gestão do produto, julgue o seguinte item.
+No desenvolvimento de um produto complexo, ainda que seja nas primeiras fases, devem-se incluir informações sobre oportunidades de mercado, movimentos competitivos e estudos quantificados relativos à necessidade de investimento e impactos financeiros, entre outros itens.</t>
+        </is>
+      </c>
+      <c r="F654" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G654" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H654" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I654" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J654" t="inlineStr"/>
+      <c r="K654" t="inlineStr"/>
+      <c r="L654" t="inlineStr"/>
+      <c r="M654" t="inlineStr"/>
+      <c r="N654" t="inlineStr"/>
+      <c r="O654" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P654" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q654" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="n">
+        <v>655</v>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>FEPESE</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>ABEPRO</t>
+        </is>
+      </c>
+      <c r="D655" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E655" t="inlineStr">
+        <is>
+          <t>O projeto de produto ou de serviço é uma importante atividade realizada na empresa, contribuindo para definir a sua posição competitiva.
+Analise as afirmativas abaixo sobre o projeto de produtos e serviços.
+1. O termo “pacote” corresponde à combinação de produtos e serviços que a empresa oferece aos seus clientes.
+2. O Quality Function Deployment (QFD) corresponde a uma técnica desenvolvida no Japão e usada amplamente pela Toyota para assegurar que o projeto final atenda às necessidades dos clientes.
+3. O método Taguchi consiste em uma técnica desenvolvida no Japão para o projeto de produtos com alto nível de customização e produzidos por mão de obra pouco qualificada, características comuns encontradas no Japão após a Segunda Guerra Mundial.
+Assinale a alternativa que indica todas as afirmativas corretas.</t>
+        </is>
+      </c>
+      <c r="F655" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G655" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H655" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I655" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J655" t="inlineStr">
+        <is>
+          <t>É correta apenas a afirmativa 1.</t>
+        </is>
+      </c>
+      <c r="K655" t="inlineStr">
+        <is>
+          <t>É correta apenas a afirmativa 2.</t>
+        </is>
+      </c>
+      <c r="L655" t="inlineStr">
+        <is>
+          <t>São corretas apenas as afirmativas 1 e 2.</t>
+        </is>
+      </c>
+      <c r="M655" t="inlineStr">
+        <is>
+          <t>São corretas apenas as afirmativas 1 e 3.</t>
+        </is>
+      </c>
+      <c r="N655" t="inlineStr">
+        <is>
+          <t>São corretas as afirmativas 1, 2 e 3.</t>
+        </is>
+      </c>
+      <c r="O655" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P655" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q655" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="n">
+        <v>656</v>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D656" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="E656" t="inlineStr">
+        <is>
+          <t>Um fabricante de cerveja constatou que os consumidores passaram a preferir a cerveja de outra empresa, apesar de ter gosto similar ao da sua, porque, uma vez colocada no copo, proporcionava o tradicional colarinho como o dos chopes. Ao inspecionar o produto da concorrência, ele descobriu um engenhoso dispositivo no fundo das latas que fazia uma injeção adicional de gás à bebida no momento de sua abertura. Assim, ele decidiu copiar o dispositivo e passou a colocá-lo em suas próprias latas. Esse caso é um exemplo de</t>
+        </is>
+      </c>
+      <c r="F656" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G656" t="inlineStr">
+        <is>
+          <t>Engenharia de Produto</t>
+        </is>
+      </c>
+      <c r="H656" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I656" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J656" t="inlineStr">
+        <is>
+          <t>engenharia reversa</t>
+        </is>
+      </c>
+      <c r="K656" t="inlineStr">
+        <is>
+          <t>engenharia de valor</t>
+        </is>
+      </c>
+      <c r="L656" t="inlineStr">
+        <is>
+          <t>engenharia simultânea</t>
+        </is>
+      </c>
+      <c r="M656" t="inlineStr">
+        <is>
+          <t>método de Taguchi</t>
+        </is>
+      </c>
+      <c r="N656" t="inlineStr">
+        <is>
+          <t>tentativa e erro</t>
+        </is>
+      </c>
+      <c r="O656" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P656" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q656" t="n">
+        <v>0</v>
+      </c>
+      <c r="R656" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
:up: ultimo commit antes de tentar consertar o sistema pegando a letra A de Alternativa nos gabaritos
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R656"/>
+  <dimension ref="A1:R714"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -55215,7 +55215,4647 @@
       <c r="Q656" t="n">
         <v>0</v>
       </c>
-      <c r="R656" t="inlineStr"/>
+    </row>
+    <row r="657">
+      <c r="A657" t="n">
+        <v>657</v>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t xml:space="preserve">VUNESP </t>
+        </is>
+      </c>
+      <c r="D657" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E657" t="inlineStr">
+        <is>
+          <t>A segurança e a saúde ocupacionais são regulamentadas no Brasil, como previsto na legislação trabalhista brasileira, na portaria n° 3.214 de 08 de junho de 1978, considerando o disposto no art. 200, da CLT, com redação dada pela Lei n° 6.514, de 22 de dezembro de 1977 do Ministério do Trabalho e Emprego, por intermédio da Norma Regulamentadora n° 4 (NR-4) e as normas da ABNT referentes à segurança no trabalho. O nome dos serviços desempenhados por uma equipe de profissionais especializados, contratados pelas empresas, com a finalidade de promover a saúde e proteger a integridade física dos trabalhadores é:</t>
+        </is>
+      </c>
+      <c r="F657" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G657" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H657" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I657" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J657" t="inlineStr">
+        <is>
+          <t>CIPA, ou Comissão Interna de Prevenção de Acidentes.</t>
+        </is>
+      </c>
+      <c r="K657" t="inlineStr">
+        <is>
+          <t>SPSTPS, ou Serviços de Promoção da Segurança no Trabalho e Promoção Social;</t>
+        </is>
+      </c>
+      <c r="L657" t="inlineStr">
+        <is>
+          <t>CSMT/CIRA, ou Comitê de Segurança e Medicina do Trabalho e Comissão Interna de Redução de Acidentes.</t>
+        </is>
+      </c>
+      <c r="M657" t="inlineStr">
+        <is>
+          <t>BRST, ou Brigada da Segurança do Trabalho.</t>
+        </is>
+      </c>
+      <c r="N657" t="inlineStr">
+        <is>
+          <t>SESMT, ou Serviços Especializados em Engenharia de Segurança e Medicina do Trabalho.</t>
+        </is>
+      </c>
+      <c r="O657" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P657" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q657" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="n">
+        <v>658</v>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>SABESP</t>
+        </is>
+      </c>
+      <c r="D658" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E658" t="inlineStr">
+        <is>
+          <t>De acordo com as disposições da NR-9, o Programa de Prevenção de Riscos Ambientais (PPRA) poderá ser elaborado, implementado, acompanhado e avaliado somente:</t>
+        </is>
+      </c>
+      <c r="F658" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G658" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H658" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I658" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J658" t="inlineStr">
+        <is>
+          <t>Pelo SESMT ou por pessoa ou equipe de pessoas, a critério do empregador, com capacidade para desenvolver o disposto na referida NR;</t>
+        </is>
+      </c>
+      <c r="K658" t="inlineStr">
+        <is>
+          <t>Por engenheiro de segurança do trabalho ou técnico em segurança do trabalho, com devida qualificação e habilitação;</t>
+        </is>
+      </c>
+      <c r="L658" t="inlineStr">
+        <is>
+          <t>Por engenheiro de segurança do trabalho com respectivo registro no Crea;</t>
+        </is>
+      </c>
+      <c r="M658" t="inlineStr">
+        <is>
+          <t>Pela CIPA, com anuência do SESMT;</t>
+        </is>
+      </c>
+      <c r="N658" t="inlineStr">
+        <is>
+          <t>Por profissional devidamente capacitado e autorizado pelo empregador.</t>
+        </is>
+      </c>
+      <c r="O658" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P658" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q658" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>659</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>SABESP</t>
+        </is>
+      </c>
+      <c r="D659" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E659" t="inlineStr">
+        <is>
+          <t>Durante uma inspeção no local de trabalho, um engenheiro de segurança do trabalho identificou riscos ambientais que, de acordo com a NR-9, são determinados por três agentes físicos, dois agentes químicos e três agentes biológicos, sendo eles:</t>
+        </is>
+      </c>
+      <c r="F659" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G659" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H659" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I659" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J659" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Agente Físico&lt;/b&gt;&lt;br&gt;&lt;ul&gt;&lt;li&gt;ruído&lt;/li&gt;&lt;li&gt;temperatura extrema&lt;/li&gt;&lt;li&gt;vibração&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;&lt;b&gt;Agente Químico&lt;/b&gt;&lt;br&gt;&lt;ul&gt;&lt;li&gt;gases&lt;/li&gt;&lt;li&gt;névoas&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;&lt;b&gt;Agente Biológico&lt;/b&gt;&lt;ul&gt;&lt;li&gt;fungos&lt;/li&gt;&lt;li&gt;parasitas&lt;/li&gt;&lt;li&gt;vírus&lt;/li&gt;&lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="K659" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Agente Físico&lt;/b&gt;&lt;br&gt;&lt;ul&gt;&lt;li&gt;poeiras&lt;/li&gt;&lt;li&gt;ruído&lt;/li&gt;&lt;li&gt;fumos&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;&lt;b&gt;Agente Químico&lt;/b&gt;&lt;br&gt;&lt;ul&gt;&lt;li&gt;temperatura extrema&lt;/li&gt;&lt;li&gt;gases&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;&lt;b&gt;Agente Biológico&lt;/b&gt;&lt;ul&gt;&lt;li&gt;bacilos&lt;/li&gt;&lt;li&gt;protozoários&lt;/li&gt;&lt;li&gt;névoas&lt;/li&gt;&lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="L659" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Agente Físico&lt;/b&gt;&lt;br&gt;&lt;ul&gt;&lt;li&gt;pressão anormal&lt;/li&gt;&lt;li&gt;temperatura extrema&lt;/li&gt;&lt;li&gt;poeiras&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;&lt;b&gt;Agente Químico&lt;/b&gt;&lt;br&gt;&lt;ul&gt;&lt;li&gt;gases&lt;/li&gt;&lt;li&gt;neblinas&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;&lt;b&gt;Agente Biológico&lt;/b&gt;&lt;ul&gt;&lt;li&gt;parasitas&lt;/li&gt;&lt;li&gt;vírus&lt;/li&gt;&lt;li&gt;vapores&lt;/li&gt;&lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="M659" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Agente Físico&lt;/b&gt;&lt;br&gt;&lt;ul&gt;&lt;li&gt;vapores&lt;/li&gt;&lt;li&gt;vibrações&lt;/li&gt;&lt;li&gt;poeiras&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;&lt;b&gt;Agente Químico&lt;/b&gt;&lt;br&gt;&lt;ul&gt;&lt;li&gt;neblinas&lt;/li&gt;&lt;li&gt;protozoários&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;&lt;b&gt;Agente Biológico&lt;/b&gt;&lt;ul&gt;&lt;li&gt;bacilos&lt;/li&gt;&lt;li&gt;fungos&lt;/li&gt;&lt;li&gt;fumos&lt;/li&gt;&lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="N659" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Agente Físico&lt;/b&gt;&lt;br&gt;&lt;ul&gt;&lt;li&gt;radiações ionizantes&lt;/li&gt;&lt;li&gt;fumos&lt;/li&gt;&lt;li&gt;temperaturas extremas&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;&lt;b&gt;Agente Químico&lt;/b&gt;&lt;br&gt;&lt;ul&gt;&lt;li&gt;neblinas&lt;/li&gt;&lt;li&gt;poeiras&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;&lt;b&gt;Agente Biológico&lt;/b&gt;&lt;ul&gt;&lt;li&gt;fumos&lt;/li&gt;&lt;li&gt;bacilos&lt;/li&gt;&lt;li&gt;vírus&lt;/li&gt;&lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="O659" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P659" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q659" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="n">
+        <v>660</v>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t xml:space="preserve">COPS </t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>UEL</t>
+        </is>
+      </c>
+      <c r="D660" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="E660" t="inlineStr">
+        <is>
+          <t>Sobre Equipamento de Proteção Individual (EPI), considere as afirmativas a seguir.
+I. Compete ao Serviço Especializado em Engenharia de Segurança e em Medicina do Trabalho (SESMT), ouvida a Comissão Interna de Prevenção de Acidentes (CIPA), assim como os trabalhadores usuários, recomendar ao empregador o EPI adequado ao risco existente em determinada atividade.
+II. Considera-se EPI todo dispositivo ou produto de uso individual utilizado pelo trabalhador destinado à proteção de riscos suscetíveis de ameaçar a segurança e a saúde no trabalho.
+III. Entende-se como Equipamento Conjugado de Proteção Individual todo aquele composto por vários dispositivos que o fabricante tenha associado contra um ou mais riscos que possam ocorrer simultaneamente e que sejam suscetíveis de ameaçar a segurança e a saúde no trabalho.
+IV. O EPI de fabricação nacional poderá ser colocado à venda após autorização e o importado, após nacionalização, e ambos só poderão ser utilizados com a indicação do Certificado de Aprovação (CA), expedido pelo INMETRO.
+Assinale a alternativa correta.</t>
+        </is>
+      </c>
+      <c r="F660" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G660" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H660" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I660" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J660" t="inlineStr">
+        <is>
+          <t>Somente as afirmativas I e II são corretas.</t>
+        </is>
+      </c>
+      <c r="K660" t="inlineStr">
+        <is>
+          <t>Somente as afirmativas I e IV são corretas.</t>
+        </is>
+      </c>
+      <c r="L660" t="inlineStr">
+        <is>
+          <t>Somente as afirmativas III e IV são corretas.</t>
+        </is>
+      </c>
+      <c r="M660" t="inlineStr">
+        <is>
+          <t>Somente as afirmativas I, II e III são corretas.</t>
+        </is>
+      </c>
+      <c r="N660" t="inlineStr">
+        <is>
+          <t>Somente as afirmativas II, III e IV são corretas.</t>
+        </is>
+      </c>
+      <c r="O660" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P660" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q660" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="n">
+        <v>661</v>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>COMPESA</t>
+        </is>
+      </c>
+      <c r="D661" t="inlineStr">
+        <is>
+          <t>2009</t>
+        </is>
+      </c>
+      <c r="E661" t="inlineStr">
+        <is>
+          <t>Quanto ao Programa de Condições e Meio Ambiente de Trabalho na Indústria da Construção – PCMAT, é incorreto afirmar:</t>
+        </is>
+      </c>
+      <c r="F661" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G661" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H661" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I661" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J661" t="inlineStr">
+        <is>
+          <t>Deve ser elaborado e executado por profissional legalmente habilitado na área de segurança do trabalho.</t>
+        </is>
+      </c>
+      <c r="K661" t="inlineStr">
+        <is>
+          <t>São obrigatórios a elaboração e o cumprimento do PCMAT em todos os estabelecimentos industriais.</t>
+        </is>
+      </c>
+      <c r="L661" t="inlineStr">
+        <is>
+          <t>O PCMAT deve contemplar as exigências contidas na NR 9 - Programa de Prevenção e Riscos Ambientais.</t>
+        </is>
+      </c>
+      <c r="M661" t="inlineStr">
+        <is>
+          <t>O PCMAT deve ser mantido no estabelecimento à disposição do órgão regional do Ministério do Trabalho e Emprego-MTE.</t>
+        </is>
+      </c>
+      <c r="N661" t="inlineStr">
+        <is>
+          <t>A implementação do PCMAT nos estabelecimentos é de responsabilidade do empregador ou condomínio.</t>
+        </is>
+      </c>
+      <c r="O661" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P661" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q661" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="n">
+        <v>662</v>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>COMPESA</t>
+        </is>
+      </c>
+      <c r="D662" t="inlineStr">
+        <is>
+          <t>2009</t>
+        </is>
+      </c>
+      <c r="E662" t="inlineStr">
+        <is>
+          <t>Os fornos que utilizarem combustíveis gasosos ou líquidos devem ter sistemas de proteção no sentido de evitar:</t>
+        </is>
+      </c>
+      <c r="F662" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G662" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H662" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I662" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J662" t="inlineStr">
+        <is>
+          <t>a formação de campos eletromagnéticos.</t>
+        </is>
+      </c>
+      <c r="K662" t="inlineStr">
+        <is>
+          <t>a formação de atmosfera IPVS.</t>
+        </is>
+      </c>
+      <c r="L662" t="inlineStr">
+        <is>
+          <t>retrocesso da chama.</t>
+        </is>
+      </c>
+      <c r="M662" t="inlineStr">
+        <is>
+          <t>a caracterização da insalubridade.</t>
+        </is>
+      </c>
+      <c r="N662" t="inlineStr">
+        <is>
+          <t>formação do arco voltaico.</t>
+        </is>
+      </c>
+      <c r="O662" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P662" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q662" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="n">
+        <v>663</v>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>VUNESP</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>MPSP</t>
+        </is>
+      </c>
+      <c r="D663" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E663" t="inlineStr">
+        <is>
+          <t>A Constituição Federal estabelece, entre os direitos sociais dos trabalhadores urbanos e rurais, alguns pertinentes à segurança e à saúde no trabalho, como o direito:
+(</t>
+        </is>
+      </c>
+      <c r="F663" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G663" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H663" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I663" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J663" t="inlineStr">
+        <is>
+          <t>à informação acerca dos riscos à saúde existentes em processos, substâncias e equipamentos utilizados em seu ambiente de trabalho.</t>
+        </is>
+      </c>
+      <c r="K663" t="inlineStr">
+        <is>
+          <t>à representação, na forma definida em lei específica, em comitês, grupos de trabalho ou afins que tenham como objetivo a definição e a implementação de política de segurança e saúde no trabalho no estabelecimento.</t>
+        </is>
+      </c>
+      <c r="L663" t="inlineStr">
+        <is>
+          <t>à percepção de adicional de remuneração para atividades penosas, insalubres ou perigosas, na forma da lei.</t>
+        </is>
+      </c>
+      <c r="M663" t="inlineStr">
+        <is>
+          <t>à recusa ou interrupção de atividade quando entender, por motivos razoáveis, que aquela situação de trabalho implica risco grave e iminente a sua saúde.</t>
+        </is>
+      </c>
+      <c r="N663" t="inlineStr">
+        <is>
+          <t>de livre acesso a todo e qualquer resultado de exame médico, avaliação psicológica ou teste de aptidão física a que tenha sido submetido por exigência do empregador.</t>
+        </is>
+      </c>
+      <c r="O663" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P663" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q663" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="n">
+        <v>664</v>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>CONSULPLAN</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>FSERJ</t>
+        </is>
+      </c>
+      <c r="D664" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="E664" t="inlineStr">
+        <is>
+          <t>Dentre outros, para efeito da Lei nº 8.213/91, equiparam-se também ao acidente do trabalho aquele sofrido pelo segurado no local e no horário do trabalho, em consequência de:
+I. Ato de agressão praticado por terceiro ou companheiro de trabalho.
+II. Ofensa física intencional, inclusive de terceiro, por motivo de disputa relacionada ao trabalho.
+III. Ato de imprudência, de negligência de terceiro ou de companheiro de trabalho.
+IV. Ato de pessoa privada do uso da razão.
+V. Incêndio e outros casos fortuitos ou decorrentes de força maior.
+VI. Ato de sabotagem ou terrorismo praticado por terceiro ou companheiro de trabalho.
+VII. Ato de imperícia de terceiro ou de companheiro de trabalho.
+VIII. Desabamento e inundação.
+Estão corretas as afirmativas</t>
+        </is>
+      </c>
+      <c r="F664" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G664" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H664" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I664" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J664" t="inlineStr">
+        <is>
+          <t>I, III, VI e VII, apenas.</t>
+        </is>
+      </c>
+      <c r="K664" t="inlineStr">
+        <is>
+          <t>II, III, IV e VI, apenas.</t>
+        </is>
+      </c>
+      <c r="L664" t="inlineStr">
+        <is>
+          <t>I, II, III, IV, V, VI, VII e VIII.</t>
+        </is>
+      </c>
+      <c r="M664" t="inlineStr">
+        <is>
+          <t>I, II, III, IV, VI e VII, apenas.</t>
+        </is>
+      </c>
+      <c r="N664" t="inlineStr"/>
+      <c r="O664" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P664" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q664" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="n">
+        <v>665</v>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>CONSULPLAN</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>FSERJ</t>
+        </is>
+      </c>
+      <c r="D665" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="E665" t="inlineStr">
+        <is>
+          <t>Conforme NR 9, “consideram-se riscos ambientais os agentes físicos, químicos e biológicos existentes nos ambientes de trabalho que, em função de sua natureza, concentração ou intensidade e tempo de exposição, são capazes de causar danos à saúde do trabalhador”. Radiações ionizantes, fumos, protozoários e pressões anormais, são considerados, respectivamente, agentes:</t>
+        </is>
+      </c>
+      <c r="F665" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G665" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H665" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I665" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J665" t="inlineStr">
+        <is>
+          <t>Físicos; químicos; biológicos; e, físicos.</t>
+        </is>
+      </c>
+      <c r="K665" t="inlineStr">
+        <is>
+          <t>Físicos; biológicos; químicos; e, físicos.</t>
+        </is>
+      </c>
+      <c r="L665" t="inlineStr">
+        <is>
+          <t>Físicos; físicos; químicos; e, biológicos.</t>
+        </is>
+      </c>
+      <c r="M665" t="inlineStr">
+        <is>
+          <t>Biológicos; físicos; físicos; e, químicos.</t>
+        </is>
+      </c>
+      <c r="N665" t="inlineStr"/>
+      <c r="O665" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P665" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q665" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="n">
+        <v>666</v>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>FUNDEP</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>FUNDEP</t>
+        </is>
+      </c>
+      <c r="D666" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E666" t="inlineStr">
+        <is>
+          <t>Na NR–9, o item 9.3.8.1 descreve que deverá ser mantido pelo empregador ou instituição um registro de dados estruturado, de forma a constituir um histórico técnico e administrativo do desenvolvimento do PPRA. O item 9.3.8.2 determina que esses dados devam ser mantidos por um período mínimo de:</t>
+        </is>
+      </c>
+      <c r="F666" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G666" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H666" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I666" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J666" t="inlineStr">
+        <is>
+          <t>um ano.</t>
+        </is>
+      </c>
+      <c r="K666" t="inlineStr">
+        <is>
+          <t>cinco anos.</t>
+        </is>
+      </c>
+      <c r="L666" t="inlineStr">
+        <is>
+          <t>dez anos</t>
+        </is>
+      </c>
+      <c r="M666" t="inlineStr">
+        <is>
+          <t>20 anos.</t>
+        </is>
+      </c>
+      <c r="N666" t="inlineStr"/>
+      <c r="O666" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P666" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q666" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="n">
+        <v>667</v>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>FUNDEP</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>FUNDEP</t>
+        </is>
+      </c>
+      <c r="D667" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E667" t="inlineStr">
+        <is>
+          <t>Os seguintes percentuais podem ser pagos ao trabalhador pelo exercício de trabalho em condições de insalubridade, incidente sobre o salário-mínimo da região, exceto:</t>
+        </is>
+      </c>
+      <c r="F667" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G667" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H667" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I667" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J667" t="inlineStr">
+        <is>
+          <t>40%.</t>
+        </is>
+      </c>
+      <c r="K667" t="inlineStr">
+        <is>
+          <t>30%.</t>
+        </is>
+      </c>
+      <c r="L667" t="inlineStr">
+        <is>
+          <t>20%.</t>
+        </is>
+      </c>
+      <c r="M667" t="inlineStr">
+        <is>
+          <t>10%.</t>
+        </is>
+      </c>
+      <c r="N667" t="inlineStr"/>
+      <c r="O667" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P667" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q667" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="n">
+        <v>668</v>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Desconhecida</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>SANECAP-MT</t>
+        </is>
+      </c>
+      <c r="D668" t="inlineStr">
+        <is>
+          <t>2009</t>
+        </is>
+      </c>
+      <c r="E668" t="inlineStr">
+        <is>
+          <t>A Portaria do Ministério do Trabalho nº 3.214, que entrou em vigor em 08 de junho de 1978, se refere às Normas Regulamentadoras de Segurança e Medicina do Trabalho. Sobre essas normas, assinale a afirmativa correta.</t>
+        </is>
+      </c>
+      <c r="F668" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G668" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H668" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I668" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J668" t="inlineStr">
+        <is>
+          <t>São de observância obrigatória apenas pelos órgãos públicos da administração direta e indireta.</t>
+        </is>
+      </c>
+      <c r="K668" t="inlineStr">
+        <is>
+          <t>São de observância obrigatória apenas pelos órgãos públicos da administração direta e indireta.</t>
+        </is>
+      </c>
+      <c r="L668" t="inlineStr">
+        <is>
+          <t>São de observância obrigatória pelas empresas privadas e públicas e pelos órgãos públicos da administração direta e indireta, bem como pelos órgãos dos Poderes Legislativo e Judiciário, que possuam empregados regidos pela Consolidação das Leis do Trabalho (CLT).</t>
+        </is>
+      </c>
+      <c r="M668" t="inlineStr">
+        <is>
+          <t>São de observância exclusiva dos órgãos dos Poderes Legislativo e Judiciário.</t>
+        </is>
+      </c>
+      <c r="N668" t="inlineStr"/>
+      <c r="O668" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P668" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q668" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="n">
+        <v>669</v>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>DESCONHECIDA</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>SANECAP-MT</t>
+        </is>
+      </c>
+      <c r="D669" t="inlineStr">
+        <is>
+          <t>2009</t>
+        </is>
+      </c>
+      <c r="E669" t="inlineStr">
+        <is>
+          <t>Sobre acidentes de trabalho, analise as afirmativas.
+I - Acidente pessoal: É aquele cuja caracterização depende de existir acidentado.
+II - Acidente de trajeto: É o acidente sofrido pelo empregado no percurso da residência para o trabalho ou deste para aquela.
+III - Acidente impessoal: É aquele cuja caracterização independe de existir acidentado, não podendo ser considerado como causador direto da lesão pessoal.
+IV - A doença profissional e a doença do trabalho são equiparadas ao acidente do trabalho.
+Estão corretas as afirmativas</t>
+        </is>
+      </c>
+      <c r="F669" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G669" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H669" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I669" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J669" t="inlineStr">
+        <is>
+          <t>I, II e IV, apenas.</t>
+        </is>
+      </c>
+      <c r="K669" t="inlineStr">
+        <is>
+          <t>I, III e IV, apenas.</t>
+        </is>
+      </c>
+      <c r="L669" t="inlineStr">
+        <is>
+          <t>I, II, III e IV.</t>
+        </is>
+      </c>
+      <c r="M669" t="inlineStr">
+        <is>
+          <t>II e IV, apenas.</t>
+        </is>
+      </c>
+      <c r="N669" t="inlineStr"/>
+      <c r="O669" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P669" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q669" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="n">
+        <v>670</v>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>DESCONHECIDA</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>SANECAP-MT</t>
+        </is>
+      </c>
+      <c r="D670" t="inlineStr">
+        <is>
+          <t>2009</t>
+        </is>
+      </c>
+      <c r="E670" t="inlineStr">
+        <is>
+          <t>A construção do Mapa de Riscos Ambientais é uma atribuição</t>
+        </is>
+      </c>
+      <c r="F670" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G670" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H670" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I670" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J670" t="inlineStr">
+        <is>
+          <t>dos membros da CIPA.</t>
+        </is>
+      </c>
+      <c r="K670" t="inlineStr">
+        <is>
+          <t>do Engenheiro de Segurança do Trabalho.</t>
+        </is>
+      </c>
+      <c r="L670" t="inlineStr">
+        <is>
+          <t>do Técnico em Segurança do Trabalho.</t>
+        </is>
+      </c>
+      <c r="M670" t="inlineStr">
+        <is>
+          <t>do Médico do Trabalho.</t>
+        </is>
+      </c>
+      <c r="N670" t="inlineStr"/>
+      <c r="O670" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P670" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q670" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="n">
+        <v>671</v>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t xml:space="preserve">UFPR </t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>UFPR</t>
+        </is>
+      </c>
+      <c r="D671" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E671" t="inlineStr">
+        <is>
+          <t>As Normas Regulamentadoras (NR) relativas à segurança e medicina do trabalho tratam de diversos aspectos relacionados às atividades laborativas. Com relação ao assunto, identifique como verdadeiras (V) ou falsas (F) as seguintes afirmativas:
+( ) A NR 23 trata das Condições Sanitárias e de Conforto nos Locais de Trabalho.
+( ) A NR 26 trata da Sinalização de Segurança.
+( ) A NR 28 trata da Fiscalização e Penalidades.
+( ) A NR 30 trata da Segurança e Saúde nos Trabalhos em Espaços Confinados.
+Assinale a alternativa que apresenta a sequência correta, de cima para baixo.</t>
+        </is>
+      </c>
+      <c r="F671" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G671" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H671" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I671" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J671" t="inlineStr">
+        <is>
+          <t>F – V – F – V.</t>
+        </is>
+      </c>
+      <c r="K671" t="inlineStr">
+        <is>
+          <t>V – F – F – V.</t>
+        </is>
+      </c>
+      <c r="L671" t="inlineStr">
+        <is>
+          <t>F – V – V – F.</t>
+        </is>
+      </c>
+      <c r="M671" t="inlineStr">
+        <is>
+          <t>F – F – V – V.</t>
+        </is>
+      </c>
+      <c r="N671" t="inlineStr">
+        <is>
+          <t>V – F – V – F.</t>
+        </is>
+      </c>
+      <c r="O671" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P671" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q671" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="n">
+        <v>672</v>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>MSCONCURSOS</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>MSCONCURSOS</t>
+        </is>
+      </c>
+      <c r="D672" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E672" t="inlineStr">
+        <is>
+          <t>Segundo o art. 58 da Lei nº 8.213, de 24 de julho de 1991, o Laudo Técnico de Condições Ambientais do Trabalho (LTCAT) tem como principal função:</t>
+        </is>
+      </c>
+      <c r="F672" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G672" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H672" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I672" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J672" t="inlineStr">
+        <is>
+          <t>Comprovar a existência de medidas de proteção coletivas.</t>
+        </is>
+      </c>
+      <c r="K672" t="inlineStr">
+        <is>
+          <t>Realizar análise quantitativa dos riscos do ambiente de trabalho.</t>
+        </is>
+      </c>
+      <c r="L672" t="inlineStr">
+        <is>
+          <t>Realizar análise qualitativa dos riscos do ambiente de trabalho.</t>
+        </is>
+      </c>
+      <c r="M672" t="inlineStr">
+        <is>
+          <t>Caracterizar a exposição do trabalhador a agentes/riscos nocivos à saúde.</t>
+        </is>
+      </c>
+      <c r="N672" t="inlineStr">
+        <is>
+          <t>Comprovar a existência de medidas de proteção individuais.</t>
+        </is>
+      </c>
+      <c r="O672" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P672" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q672" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="n">
+        <v>673</v>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>ASBESP</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>ASBESP</t>
+        </is>
+      </c>
+      <c r="D673" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E673" t="inlineStr">
+        <is>
+          <t>Considerando as recomendações da norma que regulamenta as questões ergonômicas do trabalho no que tange a sua organização, cabe ao engenheiro de segurança do trabalho considerar minimamente, ao inspecionar e avaliar riscos em um ambiente de produção:</t>
+        </is>
+      </c>
+      <c r="F673" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G673" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H673" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I673" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J673" t="inlineStr">
+        <is>
+          <t>o sistema de produção, as condições de temperatura, iluminação e ruído, a disposição dos postos de trabalho e os controles e mostradores das máquinas.</t>
+        </is>
+      </c>
+      <c r="K673" t="inlineStr">
+        <is>
+          <t>o sistema de produção, as condições ambientais, a quantidade de operadores, a segurança das máquinas e os EPIs que são utilizados.</t>
+        </is>
+      </c>
+      <c r="L673" t="inlineStr">
+        <is>
+          <t>os controles, os métodos de acionamento, as condições das instalações, os movimentos dos operadores e as ordens de serviço.</t>
+        </is>
+      </c>
+      <c r="M673" t="inlineStr">
+        <is>
+          <t>as normas, o modo operatório, a exigência de tempo, a determinação do conteúdo de tempo, o ritmo de trabalho e o conteúdo das tarefas.</t>
+        </is>
+      </c>
+      <c r="N673" t="inlineStr">
+        <is>
+          <t>as posturas exigidas, a qualidade do trabalho, as condições ambientais, as exigências dos superiores imediatos e as ordens de serviço.</t>
+        </is>
+      </c>
+      <c r="O673" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P673" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q673" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="n">
+        <v>674</v>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t xml:space="preserve">COPS </t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>UEL</t>
+        </is>
+      </c>
+      <c r="D674" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="E674" t="inlineStr">
+        <is>
+          <t>.Considere um motorista utilizando um veículo de transporte da empresa para serviços diários, cujo tempo de exposição ao ruído durante sua jornada de trabalho de 8 horas é o seguinte: 6 horas exposto a 85 dB(A) e 2 horas exposto a 90 dB(A). Sobre os limites de exposição a ruídos dados pela NR 15, do Ministério do Trabalho e Emprego (MTE), assinale a alternativa correta.</t>
+        </is>
+      </c>
+      <c r="F674" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G674" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H674" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I674" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J674" t="inlineStr">
+        <is>
+          <t>A dose de ruído está abaixo dos limites recomendados pela norma.</t>
+        </is>
+      </c>
+      <c r="K674" t="inlineStr">
+        <is>
+          <t>O trabalhador trabalha sob condições insalubres.</t>
+        </is>
+      </c>
+      <c r="L674" t="inlineStr">
+        <is>
+          <t>O trabalhador trabalha sob condições de periculosidade.</t>
+        </is>
+      </c>
+      <c r="M674" t="inlineStr">
+        <is>
+          <t>O uso de abafadores de concha cessaria a periculosidade.</t>
+        </is>
+      </c>
+      <c r="N674" t="inlineStr">
+        <is>
+          <t>Não há necessidade do uso de abafadores de ruído.</t>
+        </is>
+      </c>
+      <c r="O674" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P674" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q674" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="n">
+        <v>675</v>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>UNICENTRO</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>UNICENTRO</t>
+        </is>
+      </c>
+      <c r="D675" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E675" t="inlineStr">
+        <is>
+          <t>Selecione a alternativa que contenha apenas Riscos Ergonômicos:</t>
+        </is>
+      </c>
+      <c r="F675" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G675" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H675" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I675" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J675" t="inlineStr">
+        <is>
+          <t>Umidade, monotonia e arranjo físico inadequado;</t>
+        </is>
+      </c>
+      <c r="K675" t="inlineStr">
+        <is>
+          <t>Postura incorreta, vibrações e poeira;</t>
+        </is>
+      </c>
+      <c r="L675" t="inlineStr">
+        <is>
+          <t>Trabalho repetitivo, monotonia e postura incorreta;</t>
+        </is>
+      </c>
+      <c r="M675" t="inlineStr">
+        <is>
+          <t>Ritmo intenso, ruídos e calor.</t>
+        </is>
+      </c>
+      <c r="N675" t="inlineStr"/>
+      <c r="O675" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P675" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q675" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="n">
+        <v>676</v>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>UNICENTRO</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>UNICENTRO</t>
+        </is>
+      </c>
+      <c r="D676" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E676" t="inlineStr">
+        <is>
+          <t>. A NR-6 é a norma que regulamenta os equipamentos de proteção individual.
+Sobre as atribuições do empregador dispostas na NR-6, marque com V as alternativas verdadeiras e com F as alternativas falsas.
+( ) Cabe ao empregador comunicar ao INMETRO quaisquer alterações dos dados cadastrais fornecidos pelo fabricante do equipamento de proteção individual.
+( ) O empregador deve responsabilizar-se pela higienização e manutenção periódica dos equipamentos de proteção individual.
+( ) É responsabilidade do empregador orientar e treinar o trabalhador sobre o uso adequado, guarda e conservação dos equipamentos de proteção individual.
+( ) O empregador deve solicitar a renovação do CA quando vencido o prazo de validade.
+Assinale a alternativa que contém a sequência correta de afirmações verdadeiras e falsas, de cima para baixo.</t>
+        </is>
+      </c>
+      <c r="F676" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G676" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H676" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I676" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J676" t="inlineStr">
+        <is>
+          <t>F F F V;</t>
+        </is>
+      </c>
+      <c r="K676" t="inlineStr">
+        <is>
+          <t>F V V V;</t>
+        </is>
+      </c>
+      <c r="L676" t="inlineStr">
+        <is>
+          <t>V V F F;</t>
+        </is>
+      </c>
+      <c r="M676" t="inlineStr">
+        <is>
+          <t>F V V F.</t>
+        </is>
+      </c>
+      <c r="N676" t="inlineStr"/>
+      <c r="O676" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P676" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q676" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="n">
+        <v>677</v>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>UNICENTRO</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>UNICENTRO</t>
+        </is>
+      </c>
+      <c r="D677" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E677" t="inlineStr">
+        <is>
+          <t>Sobre a NR-15 - Atividades e Operações Insalubres é incorreto afirmar:</t>
+        </is>
+      </c>
+      <c r="F677" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G677" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H677" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I677" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J677" t="inlineStr">
+        <is>
+          <t>Nas perícias requeridas às Delegacias Regionais do Trabalho, desde que comprovada a insalubridade, o perito do Ministério do Trabalho indicará o adicional devido;</t>
+        </is>
+      </c>
+      <c r="K677" t="inlineStr">
+        <is>
+          <t>O percentual de adicional para insalubridade de grau mínimo é de 10% (dez por cento) sobre o salário do trabalhador;</t>
+        </is>
+      </c>
+      <c r="L677" t="inlineStr">
+        <is>
+          <t>A eliminação ou neutralização da insalubridade pode ser caracterizada apenas através de avaliação pericial por órgão competente, que comprove a inexistência de risco à saúde do trabalhador;</t>
+        </is>
+      </c>
+      <c r="M677" t="inlineStr">
+        <is>
+          <t>Os níveis de ruído contínuo ou intermitente devem ser medidos em decibéis (dB) com instrumento de nível de pressão sonora operando no circuito de compensação “A” e circuito de resposta lenta (SLOW).</t>
+        </is>
+      </c>
+      <c r="N677" t="inlineStr"/>
+      <c r="O677" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P677" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q677" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="n">
+        <v>678</v>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>DESCONHECIDA</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>DMAE-Uberlândia-MG</t>
+        </is>
+      </c>
+      <c r="D678" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="E678" t="inlineStr">
+        <is>
+          <t>O Perfil Profissiográfico Previdenciário (PPP) deverá ser atualizado por meio magnético ou físico (papel) juntamente com o PPRA, a cada:</t>
+        </is>
+      </c>
+      <c r="F678" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G678" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H678" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I678" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J678" t="inlineStr">
+        <is>
+          <t>três meses.</t>
+        </is>
+      </c>
+      <c r="K678" t="inlineStr">
+        <is>
+          <t>seis meses.</t>
+        </is>
+      </c>
+      <c r="L678" t="inlineStr">
+        <is>
+          <t>um ano.</t>
+        </is>
+      </c>
+      <c r="M678" t="inlineStr">
+        <is>
+          <t>dois anos.</t>
+        </is>
+      </c>
+      <c r="N678" t="inlineStr"/>
+      <c r="O678" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P678" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q678" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="n">
+        <v>679</v>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>DESCONHECIDA</t>
+        </is>
+      </c>
+      <c r="E679" t="inlineStr">
+        <is>
+          <t>Analise a afirmativa a seguir. O perfil profissiográfico previdenciário (PPP), deve ser emitido com base no laudo técnico de condições ambientais do trabalho (LTCAT) e continua sendo exigido das empresas, conforme o Art. 148 da Instrução Normativa Nº 84 e pelo _______.
+Assinale a alternativa que completa corretamente essa afirmativa.</t>
+        </is>
+      </c>
+      <c r="F679" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G679" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H679" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I679" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J679" t="inlineStr">
+        <is>
+          <t>PCMSO</t>
+        </is>
+      </c>
+      <c r="K679" t="inlineStr">
+        <is>
+          <t>PGR</t>
+        </is>
+      </c>
+      <c r="L679" t="inlineStr">
+        <is>
+          <t>PPRA</t>
+        </is>
+      </c>
+      <c r="M679" t="inlineStr">
+        <is>
+          <t>SESMT</t>
+        </is>
+      </c>
+      <c r="N679" t="inlineStr"/>
+      <c r="O679" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P679" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q679" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="n">
+        <v>680</v>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>FUNDATEC</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>FUNDATEC</t>
+        </is>
+      </c>
+      <c r="D680" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E680" t="inlineStr">
+        <is>
+          <t>Sobre o Laudo Técnico de Condições Ambientais do Trabalho (LTCAT), segundo o Manual de Aposentadoria Especial (setembro 2018), da Diretoria de Saúde do Trabalhador/INSS, analise as seguintes assertivas:
+I. O LTCAT pode ser coletivo ou individual.
+II. O LTCAT, previsto na Lei nº 8.213/1991, tem finalidade previdenciária na concessão da aposentadoria especial.
+III. O laudo (LTCAT) para fins previdenciários depende de duas definições básicas: a nocividade e a permanência.
+Quais estão corretas?</t>
+        </is>
+      </c>
+      <c r="F680" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G680" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H680" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I680" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J680" t="inlineStr">
+        <is>
+          <t>Apenas I.</t>
+        </is>
+      </c>
+      <c r="K680" t="inlineStr">
+        <is>
+          <t>Apenas II.</t>
+        </is>
+      </c>
+      <c r="L680" t="inlineStr">
+        <is>
+          <t>Apenas III.</t>
+        </is>
+      </c>
+      <c r="M680" t="inlineStr">
+        <is>
+          <t>Apenas II e III.</t>
+        </is>
+      </c>
+      <c r="N680" t="inlineStr">
+        <is>
+          <t>I, II e III.</t>
+        </is>
+      </c>
+      <c r="O680" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P680" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q680" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="n">
+        <v>681</v>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>AOCP</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>UEPS</t>
+        </is>
+      </c>
+      <c r="D681" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E681" t="inlineStr">
+        <is>
+          <t>Em relação à NR17, assinale a alternativa INCORRETA.</t>
+        </is>
+      </c>
+      <c r="F681" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G681" t="inlineStr">
+        <is>
+          <t>Engenharia do Trabalho</t>
+        </is>
+      </c>
+      <c r="H681" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I681" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J681" t="inlineStr">
+        <is>
+          <t>Com vistas a limitar ou facilitar o transporte manual de cargas deverão ser usados meios técnicos apropriados.</t>
+        </is>
+      </c>
+      <c r="K681" t="inlineStr">
+        <is>
+          <t>Sempre que o trabalho puder ser executado na posição sentada, o posto de trabalho deve ser planejado ou adaptado para essa posição.</t>
+        </is>
+      </c>
+      <c r="L681" t="inlineStr">
+        <is>
+          <t>Para as atividades em que os trabalhos devam ser realizados sentados, a partir da análise ergonômica do trabalho, poderá ser exigido suporte para os pés, que se adapte ao comprimento da perna do trabalhador.</t>
+        </is>
+      </c>
+      <c r="M681" t="inlineStr">
+        <is>
+          <t>Para as atividades em que os trabalhos devam ser realizados em pé, devem ser colocados assentos para descanso em locais em que possam ser utilizados por todos os trabalhadores durante as pausas.</t>
+        </is>
+      </c>
+      <c r="N681" t="inlineStr">
+        <is>
+          <t>A organização do trabalho, para efeito desta NR, deve levar em consideração, no mínimo, as normas de produção; o modo operatório e a exigência de tempo.</t>
+        </is>
+      </c>
+      <c r="O681" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P681" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q681" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>682</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>CEBRASPE</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>Prefeitura de São Luís - MA</t>
+        </is>
+      </c>
+      <c r="D682" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="E682" t="inlineStr">
+        <is>
+          <t>No que se refere ao desenvolvimento sustentável, assinale a opção correta.</t>
+        </is>
+      </c>
+      <c r="F682" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G682" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H682" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I682" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J682" t="inlineStr">
+        <is>
+          <t>A reciclagem contribui com a sustentabilidade, mas gera prejuízos aos que nela investem, pois os produtos reciclados são de má qualidade e pouco consumidos.</t>
+        </is>
+      </c>
+      <c r="K682" t="inlineStr">
+        <is>
+          <t>Mudanças nos padrões de consumo são desnecessárias para a eficácia do desenvolvimento sustentável.</t>
+        </is>
+      </c>
+      <c r="L682" t="inlineStr">
+        <is>
+          <t>A quantidade de lixo produzida atualmente pela humanidade se enquadra nos padrões de sustentabilidade.</t>
+        </is>
+      </c>
+      <c r="M682" t="inlineStr">
+        <is>
+          <t>A sustentabilidade implica em ação conjunta entre o Estado, por meio de suas políticas, e a sociedade, por meio de suas ações, em prol da preservação do meio ambiente.</t>
+        </is>
+      </c>
+      <c r="N682" t="inlineStr">
+        <is>
+          <t>A tecnologia necessária para o desenvolvimento de energias renováveis é incipiente, de maneira que o investimento nesse setor pouco contribui para o desenvolvimento sustentável.</t>
+        </is>
+      </c>
+      <c r="O682" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P682" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q682" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>683</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>IDIB</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>Câmara de Petrolina - PE</t>
+        </is>
+      </c>
+      <c r="D683" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E683" t="inlineStr">
+        <is>
+          <t>Segundo a Comissão Mundial sobre Meio Ambiente e Desenvolvimento da Organização das Nações Unidas (1972), a definição mais aceita para desenvolvimento sustentável é a que diz respeito ao desenvolvimento capaz de suprir as necessidades da geração atual sem comprometer a capacidade de atender as necessidades das futuras gerações. É o desenvolvimento que não esgota os recursos para o futuro.
+Atribua “V” se verdadeiro ou “F” se falso para o que se afirma a seguir sobre desenvolvimento sustentável:
+( ) O desenvolvimento sustentável tem como uma de suas metas reduzir o acúmulo de gases poluentes na atmosfera.
+( ) Para que haja desenvolvimento sustentável, é necessário o cumprimento dos requisitos ambientais para a continuidade, através do tempo, dos padrões de produção e do consumo desejados; por esse ângulo, contraria o crescimento econômico puro e restrito.
+( ) O desenvolvimento sustentável recomenda redução do uso de matérias-primas e produtos, o aumento da reciclagem e a reutilização.
+( ) Erradicar a pobreza em todas as suas formas e lugares, promover uma educação de qualidade, trabalho decente e crescimento econômico são alguns dos objetivos do desenvolvimento sustentável.
+A sequência correta, no sentido de cima para baixo, é:</t>
+        </is>
+      </c>
+      <c r="F683" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G683" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H683" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I683" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J683" t="inlineStr">
+        <is>
+          <t>V, F, F, V</t>
+        </is>
+      </c>
+      <c r="K683" t="inlineStr">
+        <is>
+          <t>F, F, V, F</t>
+        </is>
+      </c>
+      <c r="L683" t="inlineStr">
+        <is>
+          <t>V, V, V, V</t>
+        </is>
+      </c>
+      <c r="M683" t="inlineStr">
+        <is>
+          <t>V, V, F, F</t>
+        </is>
+      </c>
+      <c r="N683" t="inlineStr"/>
+      <c r="O683" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P683" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q683" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>684</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>PUC-PR</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>DPE-PR</t>
+        </is>
+      </c>
+      <c r="D684" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="E684" t="inlineStr">
+        <is>
+          <t>Assinale a alternativa CORRETA sobre o tema Rio +20:</t>
+        </is>
+      </c>
+      <c r="F684" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G684" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H684" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I684" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J684" t="inlineStr">
+        <is>
+          <t>Trata-se de Conferência Internacional sobre as condições de preservação para os 20 principais rios do Planeta. Foi realizada no Brasil em julho de 2012.</t>
+        </is>
+      </c>
+      <c r="K684" t="inlineStr">
+        <is>
+          <t>Trata-se de Conferência das Nações Unidas sobre desenvolvimento sustentável. Um dos seus objetivos foi discutir a agenda do desenvolvimento sustentável para as próximas décadas.</t>
+        </is>
+      </c>
+      <c r="L684" t="inlineStr">
+        <is>
+          <t>Trata-se de evento musical Rock realizado no Rio de Janeiro em julho de 2012 para levantar recursos para fundações de Economia Verde.</t>
+        </is>
+      </c>
+      <c r="M684" t="inlineStr">
+        <is>
+          <t>A Economia Verde foi o único tema tratado na Rio + 20.</t>
+        </is>
+      </c>
+      <c r="N684" t="inlineStr">
+        <is>
+          <t>A denominação Rio + 20 está relacionada aos G20, grupo dos 20 países mais ricos do mundo.</t>
+        </is>
+      </c>
+      <c r="O684" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P684" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q684" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>685</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>UFPR</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>ITAIPU BINACIONAL</t>
+        </is>
+      </c>
+      <c r="D685" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E685" t="inlineStr">
+        <is>
+          <t>Sobre os Objetivos do Desenvolvimento Sustentável (ODS), é INCORRETO afirmar:</t>
+        </is>
+      </c>
+      <c r="F685" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G685" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H685" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I685" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J685" t="inlineStr">
+        <is>
+          <t>O objetivo 1 indica a necessidade de acabar com a pobreza em todas as suas formas, em todos os lugares.</t>
+        </is>
+      </c>
+      <c r="K685" t="inlineStr">
+        <is>
+          <t>Até 2030, o Brasil deve dobrar a produtividade agrícola e a renda dos pequenos produtores de alimentos.</t>
+        </is>
+      </c>
+      <c r="L685" t="inlineStr">
+        <is>
+          <t>Reforçar a prevenção e o tratamento do abuso de substâncias, incluindo o abuso de drogas entorpecentes e o uso nocivo do álcool.</t>
+        </is>
+      </c>
+      <c r="M685" t="inlineStr">
+        <is>
+          <t>Até 2030, aumentar substancialmente o contingente de professores qualificados, inclusive por meio da cooperação internacional para a formação de professores nos países em desenvolvimento.</t>
+        </is>
+      </c>
+      <c r="N685" t="inlineStr">
+        <is>
+          <t>Até 2030, aumentar substancialmente a participação de energias não renováveis na matriz energética global.</t>
+        </is>
+      </c>
+      <c r="O685" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P685" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q685" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>686</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>CEBRASPE</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>Instituto Rio Branco</t>
+        </is>
+      </c>
+      <c r="D686" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="E686" t="inlineStr">
+        <is>
+          <t>A respeito da agenda internacional contemporânea, julgue o item que se segue.
+A agenda do desenvolvimento global esteve centrada, desde o ano 2000, nos Objetivos de Desenvolvimento do Milênio (ODMs), os quais, findo o prazo para sua consecução, darão lugar aos Objetivos de Desenvolvimento Sustentável (ODS).</t>
+        </is>
+      </c>
+      <c r="F686" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G686" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H686" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I686" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J686" t="inlineStr">
+        <is>
+          <t>O objetivo 1 indica a necessidade de acabar com a pobreza em todas as suas formas, em todos os lugares.</t>
+        </is>
+      </c>
+      <c r="K686" t="inlineStr">
+        <is>
+          <t>Até 2030, o Brasil deve dobrar a produtividade agrícola e a renda dos pequenos produtores de alimentos.</t>
+        </is>
+      </c>
+      <c r="L686" t="inlineStr">
+        <is>
+          <t>Reforçar a prevenção e o tratamento do abuso de substâncias, incluindo o abuso de drogas entorpecentes e o uso nocivo do álcool.</t>
+        </is>
+      </c>
+      <c r="M686" t="inlineStr">
+        <is>
+          <t>Até 2030, aumentar substancialmente o contingente de professores qualificados, inclusive por meio da cooperação internacional para a formação de professores nos países em desenvolvimento.</t>
+        </is>
+      </c>
+      <c r="N686" t="inlineStr">
+        <is>
+          <t>Até 2030, aumentar substancialmente a participação de energias não renováveis na matriz energética global.</t>
+        </is>
+      </c>
+      <c r="O686" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P686" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q686" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>687</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>Prefeitura de Teresina - PI</t>
+        </is>
+      </c>
+      <c r="D687" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E687" t="inlineStr">
+        <is>
+          <t>Sobre os princípios e fundamentos estabelecidos pelas políticas públicas brasileiras relacionadas à gestão ambiental,</t>
+        </is>
+      </c>
+      <c r="F687" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G687" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H687" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I687" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J687" t="inlineStr">
+        <is>
+          <t>o meio ambiente é um patrimônio público a ser, necessariamente, assegurado e protegido, tendo em vista o uso privado.</t>
+        </is>
+      </c>
+      <c r="K687" t="inlineStr">
+        <is>
+          <t>a dessedentação de animais e o consumo humano representam o uso prioritário dos recursos hídricos sob qualquer circunstância.</t>
+        </is>
+      </c>
+      <c r="L687" t="inlineStr">
+        <is>
+          <t>a ecoeficiência prioriza a redução do impacto ambiental em detrimento do fornecimento de bens e serviços qualificados.</t>
+        </is>
+      </c>
+      <c r="M687" t="inlineStr">
+        <is>
+          <t>a diversidade biológica tem valor intrínseco, independentemente de seu valor para o homem ou potencial para uso humano.</t>
+        </is>
+      </c>
+      <c r="N687" t="inlineStr">
+        <is>
+          <t>a educação ambiental é essencial, estando sob responsabilidade prioritária do processo educativo formal.</t>
+        </is>
+      </c>
+      <c r="O687" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P687" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q687" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>688</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>FUMARC</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>COPASA</t>
+        </is>
+      </c>
+      <c r="D688" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E688" t="inlineStr">
+        <is>
+          <t>Podemos afirmar que o objetivo básico da Gestão Ambiental é a busca da otimização do uso dos recursos que o homem tem à sua disposição, sejam de ordem financeira, material ou humana. Assim, considerando os princípios e aplicações da Gestão Ambiental, identifique com V as afirmativas verdadeiras e com F, as falsas:
+( ) Atuar sobre as modificações causadas no meio ambiente, pelo uso e/ou descarte dos bens e detritos gerados pelas atividades humanas, a partir de um plano de ação viável técnica e economicamente, com prioridades perfeitamente definidas, é meio para se atingir os objetivos.
+( ) Efetuar diagnóstico ambiental da área de atuação, a partir de estudos e pesquisas dirigidos à busca de soluções para os problemas que forem detectados.
+( ) São instrumentos utilizados: monitoramentos, controles, taxações, imposições, subsídios, divulgações, obras e ações mitigadoras.
+( ) Manter saudável o meio ambiente, mesmo que às custas das necessidades humanas atuais, pois não podemos comprometer o atendimento das necessidades das gerações futuras.
+A sequência CORRETA, de cima para baixo, é:</t>
+        </is>
+      </c>
+      <c r="F688" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G688" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H688" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I688" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J688" t="inlineStr">
+        <is>
+          <t>F, F, V, V</t>
+        </is>
+      </c>
+      <c r="K688" t="inlineStr">
+        <is>
+          <t>F, V, F, V.</t>
+        </is>
+      </c>
+      <c r="L688" t="inlineStr">
+        <is>
+          <t>V, F, V, F</t>
+        </is>
+      </c>
+      <c r="M688" t="inlineStr">
+        <is>
+          <t>V, V, V, F</t>
+        </is>
+      </c>
+      <c r="N688" t="inlineStr"/>
+      <c r="O688" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P688" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q688" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>689</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>IBFC</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>Prefeitura de Cabo de Santo Agostinho - PE</t>
+        </is>
+      </c>
+      <c r="D689" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E689" t="inlineStr">
+        <is>
+          <t>Um Sistema de Gestão Ambiental (SGA) está fundamentado na adoção de medidas preventivas à ocorrência de impactos adversos ao meio ambiente e baseia-se em cinco princípios. Sobre os princípios de um SGA, assinale a alternativa &lt;u&gt;incorreta&lt;/u&gt;.</t>
+        </is>
+      </c>
+      <c r="F689" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G689" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H689" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I689" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J689" t="inlineStr">
+        <is>
+          <t>É necessário realizar avaliações qualitativas e quantitativas do desempenho ambiental da empresa.</t>
+        </is>
+      </c>
+      <c r="K689" t="inlineStr">
+        <is>
+          <t>Um plano de ação deve ser elaborado para atender aos requisitos da política ambiental.</t>
+        </is>
+      </c>
+      <c r="L689" t="inlineStr">
+        <is>
+          <t>As condições para o cumprimento dos objetivos ambientais devem ser asseguradas.</t>
+        </is>
+      </c>
+      <c r="M689" t="inlineStr">
+        <is>
+          <t>A política ambiental não deve sofrer modificações, uma vez que, bem elaborada não há necessidade de aperfeiçoamento.</t>
+        </is>
+      </c>
+      <c r="N689" t="inlineStr"/>
+      <c r="O689" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P689" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q689" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>690</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>CCV</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>UFC</t>
+        </is>
+      </c>
+      <c r="D690" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="E690" t="inlineStr">
+        <is>
+          <t>A gestão ambiental tem um papel relevante para o desempenho competitivo das organizações e possui alguns conceitos importantes para sua melhor compreensão. Marque a alternativa que traz esses conceitos da forma correta.</t>
+        </is>
+      </c>
+      <c r="F690" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G690" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H690" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I690" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J690" t="inlineStr">
+        <is>
+          <t>Impactos ambientais são as alterações negativas induzidas pelas atividades humanas.</t>
+        </is>
+      </c>
+      <c r="K690" t="inlineStr">
+        <is>
+          <t>Os impactos ambientais estão vinculados somente a fluxos energéticos e de materiais.</t>
+        </is>
+      </c>
+      <c r="L690" t="inlineStr">
+        <is>
+          <t>Aspectos ambientais são definidos como o elemento de atividades, produtos ou serviços de uma organização que podem interagir com o meio ambiente.</t>
+        </is>
+      </c>
+      <c r="M690" t="inlineStr">
+        <is>
+          <t>Produção mais Limpa (PmaisL) é uma metodologia que busca identificar os resíduos gerados para promover uma adequada reutilização ou reciclagem.</t>
+        </is>
+      </c>
+      <c r="N690" t="inlineStr">
+        <is>
+          <t>A logística reversa estuda os fluxos de materiais que vão do usuário final do processo logístico original a um novo ponto de consumo ou reaproveitamento, em virtude desses produtos terem apresentado algum tipo de defeito.</t>
+        </is>
+      </c>
+      <c r="O690" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P690" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q690" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>691</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>CEBRASPE</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>FUB</t>
+        </is>
+      </c>
+      <c r="D691" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E691" t="inlineStr">
+        <is>
+          <t>A respeito de gestão ambiental, julgue o item a seguir.
+Os objetivos da gestão ambiental incluem dotar a empresa de instrumentos que permitam reduzir danos ao meio ambiente, mesmo que os benefícios advindos não excedam os custos de implantação.</t>
+        </is>
+      </c>
+      <c r="F691" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G691" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H691" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I691" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J691" t="inlineStr">
+        <is>
+          <t>Impactos ambientais são as alterações negativas induzidas pelas atividades humanas.</t>
+        </is>
+      </c>
+      <c r="K691" t="inlineStr">
+        <is>
+          <t>Os impactos ambientais estão vinculados somente a fluxos energéticos e de materiais.</t>
+        </is>
+      </c>
+      <c r="L691" t="inlineStr">
+        <is>
+          <t>Aspectos ambientais são definidos como o elemento de atividades, produtos ou serviços de uma organização que podem interagir com o meio ambiente.</t>
+        </is>
+      </c>
+      <c r="M691" t="inlineStr">
+        <is>
+          <t>Produção mais Limpa (PmaisL) é uma metodologia que busca identificar os resíduos gerados para promover uma adequada reutilização ou reciclagem.</t>
+        </is>
+      </c>
+      <c r="N691" t="inlineStr">
+        <is>
+          <t>A logística reversa estuda os fluxos de materiais que vão do usuário final do processo logístico original a um novo ponto de consumo ou reaproveitamento, em virtude desses produtos terem apresentado algum tipo de defeito.</t>
+        </is>
+      </c>
+      <c r="O691" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P691" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q691" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>692</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>Câmara Legislativa do Distrito Federal</t>
+        </is>
+      </c>
+      <c r="D692" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E692" t="inlineStr">
+        <is>
+          <t>A coluna à esquerda apresenta os diferentes destinos de resíduos sólidos no ambiente e a coluna à direita, respectivamente, um aspecto positivo e um negativo destes destinos.
+A correta correlação entre cada tipo de destino com um par de aspectos positivos e negativos é:</t>
+        </is>
+      </c>
+      <c r="F692" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G692" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H692" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I692" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J692" t="inlineStr">
+        <is>
+          <t>1-d; 2-c; 3-b; 4-a; 5-e</t>
+        </is>
+      </c>
+      <c r="K692" t="inlineStr">
+        <is>
+          <t>1-e; 2-d; 3-a; 4-b; 5-c</t>
+        </is>
+      </c>
+      <c r="L692" t="inlineStr">
+        <is>
+          <t>1-b; 2-e; 3-d; 4-c; 5-a</t>
+        </is>
+      </c>
+      <c r="M692" t="inlineStr">
+        <is>
+          <t>1-a; 2-b; 3-c; 4-e; 5-d</t>
+        </is>
+      </c>
+      <c r="N692" t="inlineStr">
+        <is>
+          <t>1-c; 2-a; 3-e; 4-d; 5-b</t>
+        </is>
+      </c>
+      <c r="O692" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P692" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q692" t="n">
+        <v>0</v>
+      </c>
+      <c r="R692" t="inlineStr">
+        <is>
+          <t>ae87eb6b-82a8-4066-979e-2833b53eab2d.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>693</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>CODEBA</t>
+        </is>
+      </c>
+      <c r="D693" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E693" t="inlineStr">
+        <is>
+          <t>A NBR nº 10004/04 da ABNT classifica os resíduos sólidos quanto aos riscos potenciais à saúde humana ou de contaminação do meio ambiente. Segundo esse instrumento legal, os resíduos são classificados como perigosos por suas características. Relacione as características listadas a seguir às respectivas propriedades.
+1. Inflamabilidade
+2. Reatividade
+3. Patogenicidade
+( ) Contém, ou apresenta a suspeita de conter, agentes etiológicos, ácido desoxiribonucleico (ADN) ou ácido ribonucleico (ARN) recombinantes, organismos geneticamente modificados, plasmídios, cloroplastos, mitocôndrias ou toxinas capazes de produzir doenças em homens, animais ou vegetais.
+( ) Gerar gases, vapores e fumos tóxicos em quantidades suficientes capazes de provocar danos à saúde pública ou ao meio ambiente, quando misturados com a água.
+( ) Não ser líquida e ser é capaz de, sob condições de temperatura e pressão de 25ºC e 0,1 MPa (1 atm), produzir fogo por fricção, absorção de umidade ou por alterações químicas espontâneas e, quando inflamada, queimar vigorosa e persistentemente, dificultando a extinção do fogo.
+Assinale a opção que mostra a relação correta, de cima para baixo.</t>
+        </is>
+      </c>
+      <c r="F693" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G693" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H693" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I693" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J693" t="inlineStr">
+        <is>
+          <t>1 – 3 – 2</t>
+        </is>
+      </c>
+      <c r="K693" t="inlineStr">
+        <is>
+          <t>1 – 2 – 3</t>
+        </is>
+      </c>
+      <c r="L693" t="inlineStr">
+        <is>
+          <t>2 – 3 – 1</t>
+        </is>
+      </c>
+      <c r="M693" t="inlineStr">
+        <is>
+          <t>3 – 2 – 1</t>
+        </is>
+      </c>
+      <c r="N693" t="inlineStr">
+        <is>
+          <t>1 – 2 – 3</t>
+        </is>
+      </c>
+      <c r="O693" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P693" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q693" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>694</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>CONSULPAM</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>Prefeitura de Viana - ES</t>
+        </is>
+      </c>
+      <c r="D694" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E694" t="inlineStr">
+        <is>
+          <t>Infelizmente, devido ao baixo grau de instrução e de conscientização da sociedade brasileira, os resíduos perigosos gerados todos os dias em nossos domicílios são descartados de forma incorreta, provocando danos ambientais graves e colocando em risco a vida de muitos seres vivos, incluindo os seres humanos. Celulares e suas baterias muitas vezes são descartados em lixo comum. De acordo com nossa legislação, as baterias e celulares:</t>
+        </is>
+      </c>
+      <c r="F694" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G694" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H694" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I694" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J694" t="inlineStr">
+        <is>
+          <t>Devem ser descartados em sacos especiais adquiridos em lojas especializadas.</t>
+        </is>
+      </c>
+      <c r="K694" t="inlineStr">
+        <is>
+          <t>Devem ser encaminhados aos fabricantes.</t>
+        </is>
+      </c>
+      <c r="L694" t="inlineStr">
+        <is>
+          <t>Devem incinerados em fornos domésticos a fim de evitar a contaminação do lençol freático.</t>
+        </is>
+      </c>
+      <c r="M694" t="inlineStr">
+        <is>
+          <t>Devem ser encaminhadas a usinas de reciclagem a fim de aproveitar os metais presentes nas baterias.</t>
+        </is>
+      </c>
+      <c r="N694" t="inlineStr"/>
+      <c r="O694" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P694" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q694" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>695</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>FUMARC</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>COPASA</t>
+        </is>
+      </c>
+      <c r="D695" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E695" t="inlineStr">
+        <is>
+          <t>Nenhum método de disposição final de lodos residuais está isento de inconvenientes. Entre os métodos mais comuns usados na disposição estão, EXCETO:</t>
+        </is>
+      </c>
+      <c r="F695" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G695" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H695" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I695" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J695" t="inlineStr">
+        <is>
+          <t>Compostagem para hortaliças folhosas.</t>
+        </is>
+      </c>
+      <c r="K695" t="inlineStr">
+        <is>
+          <t>Eliminação em aterros sanitários.</t>
+        </is>
+      </c>
+      <c r="L695" t="inlineStr">
+        <is>
+          <t>Fertilizantes para árvores de grande porte.</t>
+        </is>
+      </c>
+      <c r="M695" t="inlineStr">
+        <is>
+          <t>Incineração.</t>
+        </is>
+      </c>
+      <c r="N695" t="inlineStr"/>
+      <c r="O695" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P695" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q695" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>696</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>SABESP</t>
+        </is>
+      </c>
+      <c r="D696" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E696" t="inlineStr">
+        <is>
+          <t>As estações de tratamento de esgoto, na sua maioria, fazem o tratamento e o posterior despejo em um corpo receptor (rio, riacho, lagoa, etc.) e têm uma especial atenção com os resíduos gerados no processo de tratamento, principalmente o lodo. Apesar de ser constituído em sua maior parte por matéria orgânica, o lodo representa riscos ao meio ambiente e, se mal destinado, pode contaminar solos ou outras áreas se for arrastado por água de chuva.
+Considere as afirmativas abaixo.
+I. O lodo pode ser despejado no corpo receptor (rio, riacho, lago, etc.) para degradação da matéria orgânica pelos microrganismos presentes na água.
+II. O lodo pode ser enviado para tratamento térmico (incineração).
+III. O lodo pode ser enviado para agricultores próximos à estação para uso como adubo de hortaliças.
+IV. O lodo pode ser enviado para aterro sanitário.
+Está correto o que se afirma APENAS em:</t>
+        </is>
+      </c>
+      <c r="F696" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G696" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H696" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I696" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J696" t="inlineStr">
+        <is>
+          <t>IV.</t>
+        </is>
+      </c>
+      <c r="K696" t="inlineStr">
+        <is>
+          <t>I, II e III.</t>
+        </is>
+      </c>
+      <c r="L696" t="inlineStr">
+        <is>
+          <t>I e III.</t>
+        </is>
+      </c>
+      <c r="M696" t="inlineStr">
+        <is>
+          <t>I, II e IV.</t>
+        </is>
+      </c>
+      <c r="N696" t="inlineStr">
+        <is>
+          <t>II e IV.</t>
+        </is>
+      </c>
+      <c r="O696" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P696" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q696" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>697</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>FUMAR</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>COPASA</t>
+        </is>
+      </c>
+      <c r="D697" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E697" t="inlineStr">
+        <is>
+          <t>Uma Estação de Tratamento de Esgoto (ETE) é responsável por tratar a água poluída e devolvê-la ao meio ambiente em forma de água tratada, formando um ciclo de reaproveitamento sustentável. O esgoto captado por tanques é submetido a uma série de etapas até que a água poluída esteja apta a ser reutilizada ou devolvida sem ser uma ameaça à saúde e ao meio em que vivemos.
+Em qual das alternativas a função apresentada &lt;u&gt;NÃO &lt;/u&gt;corresponde a etapa do tratamento?</t>
+        </is>
+      </c>
+      <c r="F697" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G697" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H697" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I697" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J697" t="inlineStr">
+        <is>
+          <t>Decantador: remove líquidos em suspensão.</t>
+        </is>
+      </c>
+      <c r="K697" t="inlineStr">
+        <is>
+          <t>Desarenador: faz a retirada da areia depositada.</t>
+        </is>
+      </c>
+      <c r="L697" t="inlineStr">
+        <is>
+          <t>Digestão Anaeróbica: faz a decomposição da matéria orgânica na ausência de oxigênio.</t>
+        </is>
+      </c>
+      <c r="M697" t="inlineStr">
+        <is>
+          <t>Gradeamento: faz a retirada de sólidos grosseiros.</t>
+        </is>
+      </c>
+      <c r="N697" t="inlineStr"/>
+      <c r="O697" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P697" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q697" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>698</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>FGV</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>COMPESA</t>
+        </is>
+      </c>
+      <c r="D698" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E698" t="inlineStr">
+        <is>
+          <t>Efluentes precisam ser tratados antes de serem lançados nos cursos d´água. O tratamento ideal para cada tipo de efluente é indicado de acordo com a carga poluidora e a presença de contaminantes.
+As opções a seguir apresentam tipos de tratamento primário de efluentes, &lt;u&gt;à exceção de uma&lt;/u&gt;. Assinalea:</t>
+        </is>
+      </c>
+      <c r="F698" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G698" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H698" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I698" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J698" t="inlineStr">
+        <is>
+          <t>O processo de decantação consiste em deixar a mistura em repouso para que, em razão da diferença de densidade e da ação da gravidade, os sólidos se sedimentem.</t>
+        </is>
+      </c>
+      <c r="K698" t="inlineStr">
+        <is>
+          <t>Na flotação, as partículas em suspensão aderem às bolhas de ar adicionadas a uma suspensão coloidal, as quais são arrastadas para a superfície do líquido, formando uma espuma que pode ser removida da solução.</t>
+        </is>
+      </c>
+      <c r="L698" t="inlineStr">
+        <is>
+          <t>A função de uma bacia de equalização é dar robustez ao sistema, ao absorver variações bruscas na qualidade do efluente.</t>
+        </is>
+      </c>
+      <c r="M698" t="inlineStr">
+        <is>
+          <t>A neutralização utiliza produtos químicos para neutralizar o pH do efluente.</t>
+        </is>
+      </c>
+      <c r="N698" t="inlineStr">
+        <is>
+          <t>Nos filtros de percolação ocorre o desenvolvimento de microrganismos que se agrupam em flocos ou grânulos nos interstícios do material.</t>
+        </is>
+      </c>
+      <c r="O698" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P698" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q698" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>699</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>SABESP</t>
+        </is>
+      </c>
+      <c r="D699" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E699" t="inlineStr">
+        <is>
+          <t>No tratamento de esgotos há uma variação de sistemas de tratamento que se mostram mais adequados de acordo com o tipo de efluente a ser tratado (doméstico ou industrial). No sistema de lodos ativados, o processo é estritamente.</t>
+        </is>
+      </c>
+      <c r="F699" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G699" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H699" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I699" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J699" t="inlineStr">
+        <is>
+          <t>químico e aeróbio.</t>
+        </is>
+      </c>
+      <c r="K699" t="inlineStr">
+        <is>
+          <t>biológico e anaeróbio.</t>
+        </is>
+      </c>
+      <c r="L699" t="inlineStr">
+        <is>
+          <t>biológico e aeróbio.</t>
+        </is>
+      </c>
+      <c r="M699" t="inlineStr">
+        <is>
+          <t>químico e anaeróbio.</t>
+        </is>
+      </c>
+      <c r="N699" t="inlineStr">
+        <is>
+          <t>misto.</t>
+        </is>
+      </c>
+      <c r="O699" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P699" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q699" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>ESPP</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>BANPARÁ</t>
+        </is>
+      </c>
+      <c r="D700" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="E700" t="inlineStr">
+        <is>
+          <t>Os principais elementos a serem utilizados pelas empresas com vistas a melhorar seu grau de eco-eficiência são:
+I. redução do consumo de energia,
+II. redução do consumo de matérias-prima,
+III. redução da emissão de substâncias tóxicas,
+IV. otimização do uso sustentável de recursos renováveis e aumento da reciclabilidade, prolongamento do ciclo de vida dos produtos,
+V. aumento da intensidade de serviço (redução de desperdícios)
+VI. agregação de valor aos bens e serviços
+Das afirmações acima:</t>
+        </is>
+      </c>
+      <c r="F700" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G700" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H700" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I700" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J700" t="inlineStr">
+        <is>
+          <t>Exceto a II, as demais estão corretas.</t>
+        </is>
+      </c>
+      <c r="K700" t="inlineStr">
+        <is>
+          <t>Todas estão corretas.</t>
+        </is>
+      </c>
+      <c r="L700" t="inlineStr">
+        <is>
+          <t>Exceto a IV, as demais estão corretas.</t>
+        </is>
+      </c>
+      <c r="M700" t="inlineStr">
+        <is>
+          <t>Exceto a III, as demais estão corretas.</t>
+        </is>
+      </c>
+      <c r="N700" t="inlineStr">
+        <is>
+          <t>Exceto a V, as demais estão corretas.</t>
+        </is>
+      </c>
+      <c r="O700" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P700" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q700" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>PREFEITURA DE TERESINA - PI</t>
+        </is>
+      </c>
+      <c r="D701" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E701" t="inlineStr">
+        <is>
+          <t>A produção mais limpa requer a implementação de estratégias ambientais preventivas integradas aos processos, produtos e serviços para se alcançar a eficiência ecológica, reduzindo riscos. Assim é fundamental destacar que a minimização de resíduos no local onde são gerados (redução na fonte), envolve, diretamente, práticas como:</t>
+        </is>
+      </c>
+      <c r="F701" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G701" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H701" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I701" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J701" t="inlineStr">
+        <is>
+          <t>reuso (prática ou técnica que permite o descarte de resíduos gerados), reciclagem (tecnologia que impede a transformação dos resíduos), recuperação de materiais ou energia e reciclagem (induzir o uso dos resíduos).</t>
+        </is>
+      </c>
+      <c r="K701" t="inlineStr">
+        <is>
+          <t>reuso (qualquer prática ou técnica que permite a reutilização de resíduos gerados), reciclagem (qualquer técnica ou tecnologia que permite o reaproveitamento dos resíduos), recuperação de materiais ou energia e reciclagem (reduzir os resíduos).</t>
+        </is>
+      </c>
+      <c r="L701" t="inlineStr">
+        <is>
+          <t>reuso (prática que impede a reutilização de resíduos gerados), reciclagem (tecnologia que permite o reaproveitamento dos resíduos), recuperação de materiais ou energia e reciclagem (reduzir os resíduos).</t>
+        </is>
+      </c>
+      <c r="M701" t="inlineStr">
+        <is>
+          <t>reuso (Princípio dos 3 R’s, Reduzir, Reutilizar e Reciclar) que proporciona a condição de aumentar a poluição, reduzir de maneira significativa e destinar de forma correta o resíduo gerado.</t>
+        </is>
+      </c>
+      <c r="N701" t="inlineStr">
+        <is>
+          <t>reuso (Princípio dos 3 R’s, Reduzir, Reutilizar e Reciclar) que proporciona a condição de aumentar a poluição, reduzir de maneira insignificante e destinar de forma correta o resíduo gerado.</t>
+        </is>
+      </c>
+      <c r="O701" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P701" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q701" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>702</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>IF-RS</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>IF-RS</t>
+        </is>
+      </c>
+      <c r="D702" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="E702" t="inlineStr">
+        <is>
+          <t>O conceito de produção mais limpa, inicialmente designado como tecnologia limpa, foi desenvolvido pelo Programa das Nações Unidas para o Meio Ambiente (PNUMA) e significa aplicar, de forma contínua e integrada, uma estratégia ambiental aos processos, produtos e serviços de uma indústria, a fim de aumentar a eficiência e reduzir os riscos ao meio ambiente e ao ser humano.
+As alternativas abaixo são resultados da adoção do conceito de tecnologia limpa, EXCETO:</t>
+        </is>
+      </c>
+      <c r="F702" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G702" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H702" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I702" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J702" t="inlineStr">
+        <is>
+          <t>Eliminação de vazamentos e perdas no processo.</t>
+        </is>
+      </c>
+      <c r="K702" t="inlineStr">
+        <is>
+          <t>Otimização das reações químicas, que tem como resultado a maximização do uso de matérias-primas e, quando possível, a redução na geração de resíduos.</t>
+        </is>
+      </c>
+      <c r="L702" t="inlineStr">
+        <is>
+          <t>Eliminação do uso de matérias-primas e de insumos que contenham substâncias perigosas.</t>
+        </is>
+      </c>
+      <c r="M702" t="inlineStr">
+        <is>
+          <t>Segregação, na origem, dos resíduos perigosos e não perigosos.</t>
+        </is>
+      </c>
+      <c r="N702" t="inlineStr">
+        <is>
+          <t>Promoção e estímulo do reprocessamento e da reciclagem interna.</t>
+        </is>
+      </c>
+      <c r="O702" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P702" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q702" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>703</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>PREFEITURA DE TERESINA - PI</t>
+        </is>
+      </c>
+      <c r="D703" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E703" t="inlineStr">
+        <is>
+          <t>No que diz respeito ao gerenciamento ambiental, contrapõe-se o uso dos princípios das Técnicas de Fim-de-Tubo e Técnicas de Produção Mais Limpa.
+Analise as ações abaixo.
+I. Os resíduos, os efluentes e as emissões são controlados através de equipamentos de tratamento.
+II. Leva a custos adicionais.
+III. A proteção ambiental atua como uma parte integrante do design do produto e da engenharia de processo.
+IV. Prevenção da geração de resíduos, efluentes e emissões na fonte. Procurar evitar matérias-primas potencialmente tóxicas.
+V. Ajuda a reduzir custos.
+VI. Proteção ambiental é um assunto para especialistas competentes.
+São ações ligadas as Técnicas de Fim-de-Tubo (1) e de Produção Mais Limpa (2), respectivamente:</t>
+        </is>
+      </c>
+      <c r="F703" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G703" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H703" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I703" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J703" t="inlineStr">
+        <is>
+          <t>1: I, II, VI − 2: III, IV, V.</t>
+        </is>
+      </c>
+      <c r="K703" t="inlineStr">
+        <is>
+          <t>1: I, III, V − 2: II, IV, VI.</t>
+        </is>
+      </c>
+      <c r="L703" t="inlineStr">
+        <is>
+          <t>1: II, IV, V − 2: I, III, VI.</t>
+        </is>
+      </c>
+      <c r="M703" t="inlineStr">
+        <is>
+          <t>1: III, IV, V − 2: I, II, VI.</t>
+        </is>
+      </c>
+      <c r="N703" t="inlineStr">
+        <is>
+          <t>1: IV, V, VI − 2: I, II, III.</t>
+        </is>
+      </c>
+      <c r="O703" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P703" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q703" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>704</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>DPE-RS</t>
+        </is>
+      </c>
+      <c r="D704" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="E704" t="inlineStr">
+        <is>
+          <t>NÃO se refere a Logística Reversa:</t>
+        </is>
+      </c>
+      <c r="F704" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G704" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H704" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I704" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J704" t="inlineStr">
+        <is>
+          <t>As aplicações e implantações de medidas de logística reversa para evitar problemas ambientais, em que se olha apenas o fim de tubo (EOP − End-of-Pipe), é apenas um paliativo, sendo necessário, a médio e longo prazo, buscar soluções mais eficientes e mais eficazes.</t>
+        </is>
+      </c>
+      <c r="K704" t="inlineStr">
+        <is>
+          <t>A produção mais limpa não é estratégia voltada à prevenção de emissão de poluentes na origem do processo produtivo.</t>
+        </is>
+      </c>
+      <c r="L704" t="inlineStr">
+        <is>
+          <t>O objetivo da logística reversa tradicional é enfrentar os problemas ambientais de forma a obter soluções imediatas.</t>
+        </is>
+      </c>
+      <c r="M704" t="inlineStr">
+        <is>
+          <t>No gerenciamento de resíduos sólidos, deve ser observada a seguinte ordem de prioridade: não geração, redução, reutilização, reciclagem e tratamento dos resíduos sólidos, bem como disposição final ambientalmente adequada dos rejeitos.</t>
+        </is>
+      </c>
+      <c r="N704" t="inlineStr">
+        <is>
+          <t>Uma boa maneira de evitar o impacto ambiental dos produtos e dos processos produtivos é o da pesquisa e desenvolvimento. Nessa fase, a logística reversa da empresa pode auxiliar nos problemas ambientais antes mesmo de eles começarem.</t>
+        </is>
+      </c>
+      <c r="O704" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P704" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q704" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>705</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>PREFEITURA DE TERESINA - PI</t>
+        </is>
+      </c>
+      <c r="D705" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E705" t="inlineStr">
+        <is>
+          <t>As normas brasileiras que definem a rotulagem ambiental e análise do ciclo de vida são, respectivamente:</t>
+        </is>
+      </c>
+      <c r="F705" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G705" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H705" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I705" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J705" t="inlineStr">
+        <is>
+          <t>ABNT NBR ISO 9001; SA 8000.</t>
+        </is>
+      </c>
+      <c r="K705" t="inlineStr">
+        <is>
+          <t>OHSAS 18000; ABNT NBR ISO 14001.</t>
+        </is>
+      </c>
+      <c r="L705" t="inlineStr">
+        <is>
+          <t>ABNT NBR ISO 14024; ABNT NBR ISO 14040.</t>
+        </is>
+      </c>
+      <c r="M705" t="inlineStr">
+        <is>
+          <t>ABNT NBR ISO 14004; ABNT NBR ISO 14031.</t>
+        </is>
+      </c>
+      <c r="N705" t="inlineStr">
+        <is>
+          <t>Guia ISO 64; ABNT NBR ISO 14063.</t>
+        </is>
+      </c>
+      <c r="O705" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P705" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q705" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>706</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>FGV</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>Prefeitura de Salvador - BA</t>
+        </is>
+      </c>
+      <c r="D706" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="E706" t="inlineStr">
+        <is>
+          <t>Com relação ao ciclo de vida de projetos e de produtos, analise as afirmativas a seguir.
+I. Os ciclos de vida do projeto e do produto se superpõem, mas o do produto perdura enquanto este estiver sendo oferecido.
+II. O ciclo de vida do projeto e o ciclo de vida do seu produto são iguais, terminando quando o produto é entregue acabado.
+III. O ciclo de vida do produto e o ciclo de vida do projeto não mantém relação de causalidade e dependem dos stakeholders.
+Está correto o que se afirma em:</t>
+        </is>
+      </c>
+      <c r="F706" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G706" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H706" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I706" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J706" t="inlineStr">
+        <is>
+          <t>I, somente.</t>
+        </is>
+      </c>
+      <c r="K706" t="inlineStr">
+        <is>
+          <t>II, somente.</t>
+        </is>
+      </c>
+      <c r="L706" t="inlineStr">
+        <is>
+          <t>III, somente.</t>
+        </is>
+      </c>
+      <c r="M706" t="inlineStr">
+        <is>
+          <t>I e II, somente.</t>
+        </is>
+      </c>
+      <c r="N706" t="inlineStr">
+        <is>
+          <t>I, II e III.</t>
+        </is>
+      </c>
+      <c r="O706" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P706" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q706" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="n">
+        <v>707</v>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>GESTÃO CONCURSO</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>EMATER-MG</t>
+        </is>
+      </c>
+      <c r="D707" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E707" t="inlineStr">
+        <is>
+          <t>A Lei nº 6.938, de 31 de agosto de 1981, dispõe sobre a Política Nacional do Meio Ambiente, seus fins e mecanismos de formulação e aplicação, e dá outras providências.
+Avalie o que se afirma constar nessa Lei, em seu artigo 4º, como objetivos da Política Nacional do Meio Ambiente.
+I. Compatibilização do desenvolvimento econômico-social com a preservação da qualidade do meio ambiente e do equilíbrio ecológico.
+II. Definição de áreas prioritárias de ação governamental relativas à qualidade e ao equilíbrio ecológico, atendendo aos interesses da União, dos Estados, do Distrito Federal, dos Territórios e dos Municípios.
+III. Estabelecimento de critérios e padrões de qualidade ambiental e de normas relativas ao uso e manejo de recursos ambientais.
+IV. Estabelecimento da política de preços mínimos para os produtos agrícolas em produção orgânica e de agricultura familiar.
+Está correto apenas o que se afirma em</t>
+        </is>
+      </c>
+      <c r="F707" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G707" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H707" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I707" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J707" t="inlineStr">
+        <is>
+          <t>III.</t>
+        </is>
+      </c>
+      <c r="K707" t="inlineStr">
+        <is>
+          <t>II e IV</t>
+        </is>
+      </c>
+      <c r="L707" t="inlineStr">
+        <is>
+          <t>I e IV.</t>
+        </is>
+      </c>
+      <c r="M707" t="inlineStr">
+        <is>
+          <t>I, II e III.</t>
+        </is>
+      </c>
+      <c r="N707" t="inlineStr"/>
+      <c r="O707" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P707" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q707" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="n">
+        <v>708</v>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>BIORIO</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>IFRN</t>
+        </is>
+      </c>
+      <c r="D708" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="E708" t="inlineStr">
+        <is>
+          <t>São objetivos da auditoria do Sistema de Gestão Ambiental (SGA), EXCETO:</t>
+        </is>
+      </c>
+      <c r="F708" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G708" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H708" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I708" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J708" t="inlineStr">
+        <is>
+          <t>determinar se o SGA segue os requisitos da normatização.</t>
+        </is>
+      </c>
+      <c r="K708" t="inlineStr">
+        <is>
+          <t>fornecer informação sobre os resultados da auditoria à gerência da organização.</t>
+        </is>
+      </c>
+      <c r="L708" t="inlineStr">
+        <is>
+          <t>determinar se o SGA segue ou não o planejado para a gestão ambiental</t>
+        </is>
+      </c>
+      <c r="M708" t="inlineStr">
+        <is>
+          <t>determinar sanções aos que não tenham atingido suas respectivas metas.</t>
+        </is>
+      </c>
+      <c r="N708" t="inlineStr">
+        <is>
+          <t>determinar se o SGA tem sido ou não devidamente implementado e mantido.</t>
+        </is>
+      </c>
+      <c r="O708" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P708" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q708" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="n">
+        <v>709</v>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>TCE-PA</t>
+        </is>
+      </c>
+      <c r="D709" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E709" t="inlineStr">
+        <is>
+          <t>O aumento crescente da consciência ambiental e a escassez de recursos naturais influenciam cada vez mais as organizações a contribuírem de forma sistematizada na redução dos impactos ambientais associados aos seus processos. Com relação ao sistema de gestão ambiental (SGA) de empresas e sua normatização, julgue o próximo item.
+Somente a norma regulamentadora que trata dos requisitos com orientações para uso do SGA descreve os requisitos que podem ser objetivamente auditados para fins de certificação/registro ambiental e(ou) de autodeclaração do SGA de uma organização.</t>
+        </is>
+      </c>
+      <c r="F709" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G709" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H709" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I709" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J709" t="inlineStr"/>
+      <c r="K709" t="inlineStr"/>
+      <c r="L709" t="inlineStr"/>
+      <c r="M709" t="inlineStr"/>
+      <c r="N709" t="inlineStr"/>
+      <c r="O709" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P709" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q709" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="n">
+        <v>710</v>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>TCE-PA</t>
+        </is>
+      </c>
+      <c r="D710" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E710" t="inlineStr">
+        <is>
+          <t>O aumento crescente da consciência ambiental e a escassez de recursos naturais influenciam cada vez mais as organizações a contribuírem de forma sistematizada na redução dos impactos ambientais associados aos seus processos. Com relação ao sistema de gestão ambiental (SGA) de empresas e sua normatização, julgue o próximo item.
+A conduta ética, a apresentação justa, o devido cuidado profissional, a independência e a abordagem baseada em evidência são princípios que fazem da auditoria uma ferramenta eficaz e confiável em apoio a políticas de gestão e controle do SGA.</t>
+        </is>
+      </c>
+      <c r="F710" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G710" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H710" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I710" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J710" t="inlineStr"/>
+      <c r="K710" t="inlineStr"/>
+      <c r="L710" t="inlineStr"/>
+      <c r="M710" t="inlineStr"/>
+      <c r="N710" t="inlineStr"/>
+      <c r="O710" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P710" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q710" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="n">
+        <v>711</v>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>TCE-PA</t>
+        </is>
+      </c>
+      <c r="D711" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E711" t="inlineStr">
+        <is>
+          <t>O aumento crescente da consciência ambiental e a escassez de recursos naturais influenciam cada vez mais as organizações a contribuírem de forma sistematizada na redução dos impactos ambientais associados aos seus processos. Com relação ao sistema de gestão ambiental (SGA) de empresas e sua normatização, julgue o próximo item.
+São requisitos básicos para qualquer organização que deseje implementar um sistema de gestão ambiental, em conformidade com a NBR que trata dos requisitos com orientações para uso do SGA, estabelecer, documentar e implementar, de forma pontual e bem definida, o início, o meio e o fim desse sistema.</t>
+        </is>
+      </c>
+      <c r="F711" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G711" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H711" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I711" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J711" t="inlineStr"/>
+      <c r="K711" t="inlineStr"/>
+      <c r="L711" t="inlineStr"/>
+      <c r="M711" t="inlineStr"/>
+      <c r="N711" t="inlineStr"/>
+      <c r="O711" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P711" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q711" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="n">
+        <v>712</v>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>TCE-PA</t>
+        </is>
+      </c>
+      <c r="D712" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E712" t="inlineStr">
+        <is>
+          <t>O aumento crescente da consciência ambiental e a escassez de recursos naturais influenciam cada vez mais as organizações a contribuírem de forma sistematizada na redução dos impactos ambientais associados aos seus processos. Com relação ao sistema de gestão ambiental (SGA) de empresas e sua normatização, julgue o próximo item.
+Até três sistemas de gestão da qualidade e de gestão ambiental podem ser auditados juntos, o que consiste em uma auditoria combinada, também conhecida como auditoria conjunta.</t>
+        </is>
+      </c>
+      <c r="F712" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G712" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H712" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I712" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J712" t="inlineStr"/>
+      <c r="K712" t="inlineStr"/>
+      <c r="L712" t="inlineStr"/>
+      <c r="M712" t="inlineStr"/>
+      <c r="N712" t="inlineStr"/>
+      <c r="O712" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P712" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q712" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="n">
+        <v>713</v>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>TCE-PA</t>
+        </is>
+      </c>
+      <c r="D713" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E713" t="inlineStr">
+        <is>
+          <t>O aumento crescente da consciência ambiental e a escassez de recursos naturais influenciam cada vez mais as organizações a contribuírem de forma sistematizada na redução dos impactos ambientais associados aos seus processos. Com relação ao sistema de gestão ambiental (SGA) de empresas e sua normatização, julgue o próximo item.
+A política ambiental de uma empresa deve ser estabelecida a partir das intenções e dos princípios gerais da organização em relação ao seu desempenho ambiental, conforme formalmente expresso pela alta administração.</t>
+        </is>
+      </c>
+      <c r="F713" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G713" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H713" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I713" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J713" t="inlineStr"/>
+      <c r="K713" t="inlineStr"/>
+      <c r="L713" t="inlineStr"/>
+      <c r="M713" t="inlineStr"/>
+      <c r="N713" t="inlineStr"/>
+      <c r="O713" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P713" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q713" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="n">
+        <v>714</v>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>ESAF</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>MF</t>
+        </is>
+      </c>
+      <c r="D714" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E714" t="inlineStr">
+        <is>
+          <t>Em relação à Responsabilidade Social e à Norma Brasileira de Diretrizes sobre Responsabilidade Social– ABNTNBR ISO 26000:2010, assinale a afirmativa incorreta.</t>
+        </is>
+      </c>
+      <c r="F714" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G714" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H714" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I714" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J714" t="inlineStr">
+        <is>
+          <t>Tanto as demandas por maior responsabilidade social quanto a Norma ABNT NBR ISO 26000 : 2010 têm como destinatárias as organizações da sociedade civil, as organizações empresariais e as organizações governamentais.</t>
+        </is>
+      </c>
+      <c r="K714" t="inlineStr">
+        <is>
+          <t>Entre os fatores que contribuem para que a sociedade reivindique maior responsabilidade social do meio empresarial, estão o acesso à informação, o aumento e agravamento das questões ambientais decorrentes da atividade produtiva e o reconhecimento de que o poder econômico exerce forte influência sobre a sociedade e sobre os governos em todo o mundo.</t>
+        </is>
+      </c>
+      <c r="L714" t="inlineStr">
+        <is>
+          <t>A norma ABNT NBR ISO 26000 : 2010 é idêntica, em conteúdo técnico, à norma internacional ISO que trata de Responsabilidade Social. Ela fornece diretrizes para os usuários e, ao contrário de algumas normas ISO, não visa à certificação.</t>
+        </is>
+      </c>
+      <c r="M714" t="inlineStr">
+        <is>
+          <t>A responsabilidade social está diretamente relacionada à identificação dos impactos causados pelos diferentes tipos de organização em decorrência de suas decisões e atividades, propondo que estas sejam abordadas de forma a contribuir para o desenvolvimento sustentável.</t>
+        </is>
+      </c>
+      <c r="N714" t="inlineStr">
+        <is>
+          <t>A erradicação do trabalho infantil e do trabalho escravo não são temas relacionados à responsabilidade social, pois já existem políticas governamentais voltadas ao enfrentamento destes problemas</t>
+        </is>
+      </c>
+      <c r="O714" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P714" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q714" t="n">
+        <v>0</v>
+      </c>
+      <c r="R714" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
:lady_beetle: bug de sistema captar A de Alternativa no gabarito consertado
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R714"/>
+  <dimension ref="A1:R726"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -59855,7 +59855,968 @@
       <c r="Q714" t="n">
         <v>0</v>
       </c>
-      <c r="R714" t="inlineStr"/>
+    </row>
+    <row r="715">
+      <c r="A715" t="n">
+        <v>715</v>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>TRT 3ª Região</t>
+        </is>
+      </c>
+      <c r="D715" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="E715" t="inlineStr">
+        <is>
+          <t>A Responsabilidade Social está normatizada na ISO 26000 que versa pela incorporação de práticas socioambientais nos processos decisórios e a responsabilização pelos impactos de suas atividades na sociedade e meio ambiente. Para certificação a empresa deve integrar, implementar e promover</t>
+        </is>
+      </c>
+      <c r="F715" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G715" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H715" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I715" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J715" t="inlineStr">
+        <is>
+          <t>as práticas econômicas a um comportamento socialmente responsável.</t>
+        </is>
+      </c>
+      <c r="K715" t="inlineStr">
+        <is>
+          <t>o comportamento socialmente responsável em toda empresa.</t>
+        </is>
+      </c>
+      <c r="L715" t="inlineStr">
+        <is>
+          <t>práticas socioeducativas nas atividades fim, visando a mitigação do impacto ambiental.</t>
+        </is>
+      </c>
+      <c r="M715" t="inlineStr">
+        <is>
+          <t>um comportamento responsável no âmbito interno, visando uma melhor relação com o entorno.</t>
+        </is>
+      </c>
+      <c r="N715" t="inlineStr">
+        <is>
+          <t>ações socioambientais sem impactar nos aspectos econômicos da empresa.</t>
+        </is>
+      </c>
+      <c r="O715" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P715" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q715" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="n">
+        <v>716</v>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>INSS</t>
+        </is>
+      </c>
+      <c r="D716" t="inlineStr">
+        <is>
+          <t>2008</t>
+        </is>
+      </c>
+      <c r="E716" t="inlineStr">
+        <is>
+          <t>Em relação à responsabilidade socioambiental corporativa, julgue os itens seguintes.
+A noção de responsabilidade socioambiental relaciona-se ao propósito de maximização dos lucros da corporação, que termina por beneficiar a sociedade na forma de empregos, salários e impostos, parte dos quais pode ser empregada em conservação ambiental.</t>
+        </is>
+      </c>
+      <c r="F716" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G716" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H716" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I716" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J716" t="inlineStr"/>
+      <c r="K716" t="inlineStr"/>
+      <c r="L716" t="inlineStr"/>
+      <c r="M716" t="inlineStr"/>
+      <c r="N716" t="inlineStr"/>
+      <c r="O716" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P716" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q716" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="n">
+        <v>717</v>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D717" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="E717" t="inlineStr">
+        <is>
+          <t>A NBR ISO 14001:2004 especifica os principais requisitos de um Sistema de Gestão Ambiental (SGA), de modo que as questões ambientais sejam integradas à administração global de uma organização ou empresa.
+Qual é a denominação de um requisito do SGA e sua(s) respectiva(s) fase(s)?</t>
+        </is>
+      </c>
+      <c r="F717" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G717" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H717" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I717" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J717" t="inlineStr">
+        <is>
+          <t>Auditoria do SGA e fase de análise crítica</t>
+        </is>
+      </c>
+      <c r="K717" t="inlineStr">
+        <is>
+          <t>Documentação do SGA e fases de verificação e ação corretiva</t>
+        </is>
+      </c>
+      <c r="L717" t="inlineStr">
+        <is>
+          <t>Monitoramento e medição e fase de planejamento</t>
+        </is>
+      </c>
+      <c r="M717" t="inlineStr">
+        <is>
+          <t>Estrutura e responsabilidades e fase de política ambiental</t>
+        </is>
+      </c>
+      <c r="N717" t="inlineStr">
+        <is>
+          <t>Preparação e atendimento a emergências e fases de implementação e operação</t>
+        </is>
+      </c>
+      <c r="O717" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P717" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q717" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="n">
+        <v>718</v>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>IFPA</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>IFPA</t>
+        </is>
+      </c>
+      <c r="D718" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="E718" t="inlineStr">
+        <is>
+          <t>Um sistema de gestão ambiental (SGA) se constitui em um conjunto de procedimentos sistematizados que são desenvolvidos para que as questões ambientais sejam integradas à administração global de um empreendimento e possibilite a obtenção de melhores resultados no desempenho global da empresa. Sendo assim, com relação aos elementos de um SGA, é incorreto afirmar que:</t>
+        </is>
+      </c>
+      <c r="F718" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G718" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H718" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I718" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J718" t="inlineStr">
+        <is>
+          <t>Para que o comprometimento com a melhoria possa ser efetivo, todos os atores que constituem a organização devem de forma contínua aplicar a revisão do sistema de gestão ambiental, assegurando que este continue adequado e efetivo.</t>
+        </is>
+      </c>
+      <c r="K718" t="inlineStr">
+        <is>
+          <t>A política ambiental dá um senso global de direção, apresenta os princípios de ação para uma organização, sendo estabelecidas metas relativas de desempenho e responsabilidade ambiental, contra as quais todas as ações subsequentes serão julgadas.</t>
+        </is>
+      </c>
+      <c r="L718" t="inlineStr">
+        <is>
+          <t>Com base na política ambiental, a organização deve fazer um planejamento com o objetivo de atender aos requisitos estabelecidos.</t>
+        </is>
+      </c>
+      <c r="M718" t="inlineStr">
+        <is>
+          <t>O processo de implementação e operação do SGA deve ser conduzido de forma a serem atingidos os objetivos e as metas estabelecidas.</t>
+        </is>
+      </c>
+      <c r="N718" t="inlineStr">
+        <is>
+          <t>É necessário que sejam desenvolvidos procedimentos para monitorar e medir as principais características das operações e atividades que podem causar um impacto significativo no meio ambiente, ao mesmo tempo em que devem ser estabelecidos os procedimentos referentes às ações corretivas que devem ser tomadas para eliminar as causas reais ou potenciais, que poderiam resultar em um impacto no meio ambiente.</t>
+        </is>
+      </c>
+      <c r="O718" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P718" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q718" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="n">
+        <v>719</v>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>VUNESP</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>CEAGESP</t>
+        </is>
+      </c>
+      <c r="D719" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="E719" t="inlineStr">
+        <is>
+          <t>A necessidade de demonstrar, junto às partes interessadas, um comportamento ambiental aceitável, estimula as organizações a adotarem sistemas de gestão ambiental, como aquele prescrito na NBR ISO n.º 14001. De acordo com essa norma,</t>
+        </is>
+      </c>
+      <c r="F719" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G719" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H719" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I719" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J719" t="inlineStr">
+        <is>
+          <t>as iniciativas da organização, em relação ao treinamento, conscientização e desenvolvimento de competências, além dos aspectos ambientais, devem contemplar os aspectos da segurança e saúde no trabalho, que impactam o sistema de produção.</t>
+        </is>
+      </c>
+      <c r="K719" t="inlineStr">
+        <is>
+          <t>uma avaliação ambiental inicial deve cobrir quatro áreas: requisitos legais e regulamentares; identificação dos aspectos ambientais significativos; exame das práticas e procedimentos de gestão ambiental existentes e avaliação dos dados provenientes de investigações anteriores.</t>
+        </is>
+      </c>
+      <c r="L719" t="inlineStr">
+        <is>
+          <t>para atender a seus objetivos com todas as partes interessadas em seu desempenho ambiental, a organização deve atender a seus requisitos legais, não sendo necessário subscrever eventuais códigos de prática da indústria, acordos voluntários e outras diretrizes de caráter não regulamentar.</t>
+        </is>
+      </c>
+      <c r="M719" t="inlineStr">
+        <is>
+          <t>as auditorias não podem ser executadas por pessoal interno à organização e devem verificar de forma sistemática os documentos e as práticas para obter evidências de que a organização está em conformidade, de acordo com padrões objetivos, com o disposto na norma.</t>
+        </is>
+      </c>
+      <c r="N719" t="inlineStr">
+        <is>
+          <t>todos os impactos ambientais possíveis nos recursos naturais, flora, fauna e suas interrelações devem receber adequada valoração de acordo com as diversas abordagens, como intensidade de reação da opinião pública e custo direto de medidas de mitigação.</t>
+        </is>
+      </c>
+      <c r="O719" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P719" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q719" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="n">
+        <v>720</v>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Cespe</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>Polícia Científica</t>
+        </is>
+      </c>
+      <c r="D720" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E720" t="inlineStr">
+        <is>
+          <t>Acerca da NBR ISO n.º 14.001, que estabelece diretrizes básicas para um sistema de gestão ambiental (SGA), assinale a opção correta.</t>
+        </is>
+      </c>
+      <c r="F720" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G720" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H720" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I720" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J720" t="inlineStr">
+        <is>
+          <t>O SGA substitui as políticas de gestão ambiental anteriormente implementadas em uma organização.</t>
+        </is>
+      </c>
+      <c r="K720" t="inlineStr">
+        <is>
+          <t>A política ambiental refere-se às intenções e aos princípios gerais da organização relacionados a seu desempenho ambiental, conforme formalmente expresso pela alta administração.</t>
+        </is>
+      </c>
+      <c r="L720" t="inlineStr">
+        <is>
+          <t>Para que a implantação de um SGA em uma organização seja bem-sucedida, é necessário que as funções e responsabilidades ambientais sejam compreendidas como funções da gestão ambiental, ou seja, como atribuições dos seus gestores, de modo a não interferirem em outras áreas da organização, a fim de que conflitos internos sejam evitados.</t>
+        </is>
+      </c>
+      <c r="M720" t="inlineStr">
+        <is>
+          <t>Um SGA implementado em determinada organização deve ser aplicado simultaneamente em todas as áreas de atividade dessa empresa, com o propósito de aprimorar o desempenho ambiental geral da organização.</t>
+        </is>
+      </c>
+      <c r="N720" t="inlineStr">
+        <is>
+          <t>O aspecto ambiental de uma organização é um componente de suas atividades, seus produtos ou seus serviços que pode interagir com o meio ambiente sem causar impacto ambiental.</t>
+        </is>
+      </c>
+      <c r="O720" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P720" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q720" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="n">
+        <v>721</v>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>PREFEITURA DE TERESINA - PI</t>
+        </is>
+      </c>
+      <c r="D721" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E721" t="inlineStr">
+        <is>
+          <t>A norma ISO 14001 define política ambiental como</t>
+        </is>
+      </c>
+      <c r="F721" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G721" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H721" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I721" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J721" t="inlineStr">
+        <is>
+          <t>qualquer modificação do meio ambiente, adversa ou benéfica, que resulte, no todo ou em parte, dos aspectos ambientais da organização.</t>
+        </is>
+      </c>
+      <c r="K721" t="inlineStr">
+        <is>
+          <t>requisito de desempenho detalhado, aplicável à organização ou à parte dela, resultante dos objetivos ambientais e que necessita ser estabelecido e atendido para que tais objetivos sejam atingidos.</t>
+        </is>
+      </c>
+      <c r="L721" t="inlineStr">
+        <is>
+          <t>processo sistemático, independente e documentado para obter evidência e avaliá-la objetivamente para determinar a extensão na qual os critérios de auditoria do sistema da gestão ambiental estabelecidos pela organização são atendidos.</t>
+        </is>
+      </c>
+      <c r="M721" t="inlineStr">
+        <is>
+          <t>elemento das atividades ou produtos ou serviços de uma organização que pode interagir com o meio ambiente e que pode causar impacto ambiental significativo.</t>
+        </is>
+      </c>
+      <c r="N721" t="inlineStr">
+        <is>
+          <t>intenções e princípios gerais de uma organização em relação ao seu desempenho ambiental, conforme formalmente expresso pela alta administração.</t>
+        </is>
+      </c>
+      <c r="O721" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P721" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q721" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="n">
+        <v>722</v>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>SEGEP-MA</t>
+        </is>
+      </c>
+      <c r="D722" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E722" t="inlineStr">
+        <is>
+          <t>O Sistema de Gestão Ambiental − SGA consiste na estrutura, responsabilidades, práticas, procedimentos, programas e recursos mobilizados para o atendimento da política ambiental de uma organização. É característica de um SGA:</t>
+        </is>
+      </c>
+      <c r="F722" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G722" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H722" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I722" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J722" t="inlineStr">
+        <is>
+          <t>Garantir que o controle ambiental seja realizado pelo órgão ambiental oficial.</t>
+        </is>
+      </c>
+      <c r="K722" t="inlineStr">
+        <is>
+          <t>Conter requisitos que podem ser auditados objetivamente para fins de certificação.</t>
+        </is>
+      </c>
+      <c r="L722" t="inlineStr">
+        <is>
+          <t>A alta administração ser responsável pela implantação e manutenção de um sistema de gestão ambiental.</t>
+        </is>
+      </c>
+      <c r="M722" t="inlineStr">
+        <is>
+          <t>Substituir o cumprimento dos requisitos legais e regulatórios.</t>
+        </is>
+      </c>
+      <c r="N722" t="inlineStr">
+        <is>
+          <t>Não ser aplicável a todos os tipos e tamanhos de organizações.</t>
+        </is>
+      </c>
+      <c r="O722" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P722" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q722" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="n">
+        <v>723</v>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>IFRS</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>IFRS</t>
+        </is>
+      </c>
+      <c r="D723" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="E723" t="inlineStr">
+        <is>
+          <t>Em relação ao escopo da norma ABNT NBR ISO 14001:2015 são feitas as seguintes afirmativas.
+I. Especifica os requisitos para um sistema de gestão ambiental que uma organização pode usar para aumentar seu desempenho ambiental.
+II. Destina-se ao uso por uma organização que busca gerenciar suas responsabilidades ambientais de uma forma sistemática, que contribua para o pilar ambiental da sustentabilidade.
+III. Auxilia a organização a alcançar os resultados pretendidos de seu sistema de gestão ambiental, os quais agreguem valor para o meio ambiente, à organização em si e suas partes interessadas.
+IV. É aplicável a qualquer organização, independentemente do seu tamanho, tipo e natureza, e aplica-se aos aspectos ambientais das suas atividades, produtos e serviços que a organização determina poder controlar ou influenciar, considerando uma perspectiva de ciclo de vida.
+V. Pode ser usada na íntegra ou em parte para sistematicamente melhorar a gestão ambiental. As declarações de conformidade, no entanto, só são aceitas se todos os requisitos forem incorporados ao sistema de gestão ambiental da organização e atendidos sem exclusões.
+Assinale a alternativa em que todas as afirmativas estão CORRETAS:</t>
+        </is>
+      </c>
+      <c r="F723" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G723" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H723" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I723" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J723" t="inlineStr">
+        <is>
+          <t>I, II, III, IV e V.</t>
+        </is>
+      </c>
+      <c r="K723" t="inlineStr">
+        <is>
+          <t>Apenas I, II e V.</t>
+        </is>
+      </c>
+      <c r="L723" t="inlineStr">
+        <is>
+          <t>Apenas I, II, III e IV.</t>
+        </is>
+      </c>
+      <c r="M723" t="inlineStr">
+        <is>
+          <t>Apenas I, III, IV e V.</t>
+        </is>
+      </c>
+      <c r="N723" t="inlineStr">
+        <is>
+          <t>Apenas II, III e IV.</t>
+        </is>
+      </c>
+      <c r="O723" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P723" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q723" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="n">
+        <v>724</v>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>Petroquímica SUAPE</t>
+        </is>
+      </c>
+      <c r="D724" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="E724" t="inlineStr">
+        <is>
+          <t>A ISO 14001 é a norma internacionalmente conhecida que apresenta um Sistema de Gestão Ambiental (SGA). O processo de implementação desse sistema possui quatro fases. A última fase desse processo é a de</t>
+        </is>
+      </c>
+      <c r="F724" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G724" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H724" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I724" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J724" t="inlineStr">
+        <is>
+          <t>auditoria e certificação</t>
+        </is>
+      </c>
+      <c r="K724" t="inlineStr">
+        <is>
+          <t>implantação das medidas de controle</t>
+        </is>
+      </c>
+      <c r="L724" t="inlineStr">
+        <is>
+          <t>planejamento</t>
+        </is>
+      </c>
+      <c r="M724" t="inlineStr">
+        <is>
+          <t>indicação dos desvios do processo</t>
+        </is>
+      </c>
+      <c r="N724" t="inlineStr">
+        <is>
+          <t>monitoramento</t>
+        </is>
+      </c>
+      <c r="O724" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P724" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q724" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="n">
+        <v>725</v>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>UFSM</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>UFSM</t>
+        </is>
+      </c>
+      <c r="D725" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E725" t="inlineStr">
+        <is>
+          <t>A base para um sistema de gestão ambiental é fundamentada no conceito Plan-Do-Check-Act (PDCA), um processo interativo utilizado pelas organizações para alcançara melhoria contínua.
+Com relação ao ciclo PDCA, é INCORRETO afirmar:</t>
+        </is>
+      </c>
+      <c r="F725" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G725" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H725" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I725" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J725" t="inlineStr">
+        <is>
+          <t>na etapa Plan, são definidos os objetivos ambientais que devem ser coerentes com a política ambiental, mensuráveis (se viável), monitorados, comunicados e atualizados, como apropriado.</t>
+        </is>
+      </c>
+      <c r="K725" t="inlineStr">
+        <is>
+          <t>na etapa Act, poderão ser feitas melhorias como ação corretiva, melhoria contínua, mudança inovadora, inovação e reorganização.</t>
+        </is>
+      </c>
+      <c r="L725" t="inlineStr">
+        <is>
+          <t>na etapa Check, os resultados são medidos em relação à política ambiental da organização, aos objetivos ambientais e a outro critério, usando indicadores.</t>
+        </is>
+      </c>
+      <c r="M725" t="inlineStr">
+        <is>
+          <t>durante a etapa Check, são obtidas as evidências de auditoria, que consistem em registros, declarações de fato ou outra informação pertinente aos critérios de auditoria, sendo estas verificáveis ou não.</t>
+        </is>
+      </c>
+      <c r="N725" t="inlineStr">
+        <is>
+          <t>na etapa Plan, a organização determinará os aspectos ambientais, sendo estes elementos de atividades, produtos ou serviços que interagem ou podem interagir com o meio ambiente, podendo causar impactos ambientais.</t>
+        </is>
+      </c>
+      <c r="O725" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P725" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q725" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="n">
+        <v>726</v>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>NUCEPE</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>PC-PI</t>
+        </is>
+      </c>
+      <c r="D726" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="E726" t="inlineStr">
+        <is>
+          <t>“Com a temática da sustentabilidade em alta, nos dias de hoje, fica cada vez mais evidente que a consciência ambiental desempenha um papel definitivo na construção da cidadania. De forma crescente, as pessoas avaliam seus comportamentos em sociedade e como eles se refletem na conservação do nosso ecossistema. Neste sentido o Sistema de Gestão Ambiental (SGA) vem para balizar as ações corporativas em busca do equilíbrio do homem, da indústria e do meio ambiente. O objetivo da Gestão Ambiental é a busca permanente de melhoria da qualidade ambiental dos serviços, produtos e ambiente de trabalho de qualquer organização”., Assinale a alternativa que contém os processos indispensáveis ao SGA.</t>
+        </is>
+      </c>
+      <c r="F726" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G726" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H726" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I726" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J726" t="inlineStr">
+        <is>
+          <t>Realizar internamente uma autoavaliação e demonstração das conformidades.</t>
+        </is>
+      </c>
+      <c r="K726" t="inlineStr">
+        <is>
+          <t>Implementar, manter e aprimorar um sistema de gestão ambiental, assegurando-se de sua conformidade com sua política ambiental definida e demonstrando internacionalmente a competência da empresa no quesito produtividade.</t>
+        </is>
+      </c>
+      <c r="L726" t="inlineStr">
+        <is>
+          <t>Buscar certificação/registro do seu sistema de gestão ambiental com base na organização exclusivamente interna.</t>
+        </is>
+      </c>
+      <c r="M726" t="inlineStr">
+        <is>
+          <t>Implementar um sistema de gestão ambiental; assegurar-se de sua conformidade com a política ambiental do país, definindo metas a partir de referências a processos de gestão de outras organizações ou empresas.</t>
+        </is>
+      </c>
+      <c r="N726" t="inlineStr">
+        <is>
+          <t>Implementar, manter e aprimorar um sistema de gestão ambiental e assegurar-se de sua conformidade com a sua política ambiental definida.</t>
+        </is>
+      </c>
+      <c r="O726" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P726" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q726" t="n">
+        <v>0</v>
+      </c>
+      <c r="R726" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
:up: questões de gestão da inovação cadastradas
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R726"/>
+  <dimension ref="A1:R748"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -60816,7 +60816,1717 @@
       <c r="Q726" t="n">
         <v>0</v>
       </c>
-      <c r="R726" t="inlineStr"/>
+    </row>
+    <row r="727">
+      <c r="A727" t="n">
+        <v>727</v>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>IADES</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>BRB</t>
+        </is>
+      </c>
+      <c r="D727" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E727" t="inlineStr">
+        <is>
+          <t>O processo de inovação requer, como ponto de partida, novas ideias que representem algo novo ou uma melhoria significativa, capaz de gerar algum tipo de vantagem competitiva para a empresa. A rigor, não existe um caminho predeterminado para que uma nova ideia seja concebida. O método científico, ou seja, a experimentação tem sido um recurso adotado normalmente quando se trata da busca de soluções baseadas em pesquisa científica ou tecnológica. Com base no exposto, no que se refere ao conceito de ICT, assinale a alternativa correta.</t>
+        </is>
+      </c>
+      <c r="F727" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G727" t="inlineStr">
+        <is>
+          <t>Gestão da Inovação</t>
+        </is>
+      </c>
+      <c r="H727" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I727" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J727" t="inlineStr">
+        <is>
+          <t>As empresas, cada vez mais dependentes de recursos tecnológicos, restringem, na própria organização, a geração de novas ideias para o respectivo departamento de P&amp;D.</t>
+        </is>
+      </c>
+      <c r="K727" t="inlineStr">
+        <is>
+          <t>A geração de ideias tem sido um recurso cada vez mais valioso de uma empresa no respectivo processo de inovação.</t>
+        </is>
+      </c>
+      <c r="L727" t="inlineStr">
+        <is>
+          <t>A tecnologia embarcada em equipamentos e sistemas não requer um esforço de geração de ideias, posto que o processo de inovação decorre do bom uso de recursos tecnológicos preexistentes.</t>
+        </is>
+      </c>
+      <c r="M727" t="inlineStr">
+        <is>
+          <t>A geração de novas ideias no seio de uma empresa deve ser cuidadosamente resguardada como algo sigiloso e, portanto, da competência exclusiva de pessoas, de preferência com formação de pós-graduação, que assumam compromisso formal de confidencialidade com a empresa.</t>
+        </is>
+      </c>
+      <c r="N727" t="inlineStr">
+        <is>
+          <t>Por ser um processo criativo referente a cada pessoa, não é possível montar esquemas, dentro de uma empresa, para acelerar a geração de novas ideias com potencial de serem usadas no processo produtivo ou no sistema gerencial da empresa.</t>
+        </is>
+      </c>
+      <c r="O727" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P727" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q727" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="n">
+        <v>728</v>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>IFF</t>
+        </is>
+      </c>
+      <c r="E728" t="inlineStr">
+        <is>
+          <t>Um novo equipamento foi desenvolvido e instalado na linha de montagem de determinado componente eletrônico, o que permite a produção em escala com a consequente ampliação de sua venda em um mesmo nicho de mercado. Nessa situação, a inovação é classificada como inovação rotinizada</t>
+        </is>
+      </c>
+      <c r="F728" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G728" t="inlineStr">
+        <is>
+          <t>Gestão da Inovação</t>
+        </is>
+      </c>
+      <c r="H728" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I728" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J728" t="inlineStr">
+        <is>
+          <t>de Posição</t>
+        </is>
+      </c>
+      <c r="K728" t="inlineStr">
+        <is>
+          <t>de Processo</t>
+        </is>
+      </c>
+      <c r="L728" t="inlineStr">
+        <is>
+          <t>de Produto</t>
+        </is>
+      </c>
+      <c r="M728" t="inlineStr">
+        <is>
+          <t>Radical</t>
+        </is>
+      </c>
+      <c r="N728" t="inlineStr">
+        <is>
+          <t>de Paradigma</t>
+        </is>
+      </c>
+      <c r="O728" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P728" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q728" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="n">
+        <v>729</v>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>MCTI Tecnologista Pleno I</t>
+        </is>
+      </c>
+      <c r="D729" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E729" t="inlineStr">
+        <is>
+          <t>Com relação à gerência da inovação, julgue os itens que se seguem.
+Levando em conta a inovação aberta, a gerência da inovação demanda habilidades de negociação com diversos tipos de parceiros da organização.</t>
+        </is>
+      </c>
+      <c r="F729" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G729" t="inlineStr">
+        <is>
+          <t>Gestão da Inovação</t>
+        </is>
+      </c>
+      <c r="H729" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I729" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J729" t="inlineStr"/>
+      <c r="K729" t="inlineStr"/>
+      <c r="L729" t="inlineStr"/>
+      <c r="M729" t="inlineStr"/>
+      <c r="N729" t="inlineStr"/>
+      <c r="O729" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P729" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q729" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="n">
+        <v>730</v>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>IFF</t>
+        </is>
+      </c>
+      <c r="D730" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E730" t="inlineStr">
+        <is>
+          <t>O manual que estabelece e padroniza os métodos de coleta e análise dos indicadores de inovações tecnológicas de produtos e processos em empresas denomina-se:</t>
+        </is>
+      </c>
+      <c r="F730" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G730" t="inlineStr">
+        <is>
+          <t>Gestão da Inovação</t>
+        </is>
+      </c>
+      <c r="H730" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I730" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J730" t="inlineStr">
+        <is>
+          <t>Manual Frascati</t>
+        </is>
+      </c>
+      <c r="K730" t="inlineStr">
+        <is>
+          <t>Manual BPT</t>
+        </is>
+      </c>
+      <c r="L730" t="inlineStr">
+        <is>
+          <t>Manual Oslo</t>
+        </is>
+      </c>
+      <c r="M730" t="inlineStr">
+        <is>
+          <t>Manual de Patentes</t>
+        </is>
+      </c>
+      <c r="N730" t="inlineStr">
+        <is>
+          <t>Manual Canberra</t>
+        </is>
+      </c>
+      <c r="O730" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P730" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q730" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="n">
+        <v>731</v>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>CESGRANRIO</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>TC-DF</t>
+        </is>
+      </c>
+      <c r="D731" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E731" t="inlineStr">
+        <is>
+          <t>Acerca de mudança e inovação em organizações, julgue os itens a seguir.
+A classificação de impacto radical ou incremental é empregada para a análise de inovações, mas não para a análise de mudanças em organizações.</t>
+        </is>
+      </c>
+      <c r="F731" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G731" t="inlineStr">
+        <is>
+          <t>Gestão da Inovação</t>
+        </is>
+      </c>
+      <c r="H731" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I731" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J731" t="inlineStr"/>
+      <c r="K731" t="inlineStr"/>
+      <c r="L731" t="inlineStr"/>
+      <c r="M731" t="inlineStr"/>
+      <c r="N731" t="inlineStr"/>
+      <c r="O731" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P731" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q731" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="n">
+        <v>732</v>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>FGV</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>TJ-AM</t>
+        </is>
+      </c>
+      <c r="D732" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E732" t="inlineStr">
+        <is>
+          <t>No processo de mudança ou de inovação nas organizações, os gestores esbarram com as resistências de seus subordinados, que deveriam estar preparados para atuar e obter resultados mutuamente favoráveis. A esse respeito, analise os elementos a seguir.
+I. Procure singularizar a organização, ou seja, não receie detalhes.
+II. Mantenha-se continuamente atualizado sobre os objetivos, os métodos e as expectativas individuais.
+III. Transfira poder e iniciativa: incentive e recompense desafios ao status quo.
+Alguns dos comportamentos desejáveis para os atores organizacionais, em face do tema mudança nas organizações, estão relacionados</t>
+        </is>
+      </c>
+      <c r="F732" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G732" t="inlineStr">
+        <is>
+          <t>Gestão da Inovação</t>
+        </is>
+      </c>
+      <c r="H732" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I732" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J732" t="inlineStr">
+        <is>
+          <t>apenas no Elemento I</t>
+        </is>
+      </c>
+      <c r="K732" t="inlineStr">
+        <is>
+          <t>apenas no Elemento II</t>
+        </is>
+      </c>
+      <c r="L732" t="inlineStr">
+        <is>
+          <t>apenas nos Elementos I e II</t>
+        </is>
+      </c>
+      <c r="M732" t="inlineStr">
+        <is>
+          <t>apenas nos elementos II e III</t>
+        </is>
+      </c>
+      <c r="N732" t="inlineStr">
+        <is>
+          <t>nos elementos I, II e III</t>
+        </is>
+      </c>
+      <c r="O732" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P732" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q732" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="n">
+        <v>733</v>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>FUNPAR</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>ITAIPU</t>
+        </is>
+      </c>
+      <c r="D733" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E733" t="inlineStr">
+        <is>
+          <t>As inovações no âmbito de uma organização não são aleatórias, ocorrendo em relação às condições passadas e presentes da organização. A respeito das formas de inovação, considere as seguintes afirmativas:
+1. Inovações programadas são planejadas por meio de pesquisa e desenvolvimento do produto ou serviço.
+2. Inovações não programadas ocorrem quando existe sobrecarga de trabalho na organização, isto é, encontram-se disponíveis menos recursos do que é presentemente necessário.
+3. A inovação é problemática quando imposta à organização, como quando uma crise é percebida e novas ações são implementadas.
+Assinale a alternativa correta.</t>
+        </is>
+      </c>
+      <c r="F733" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G733" t="inlineStr">
+        <is>
+          <t>Gestão da Inovação</t>
+        </is>
+      </c>
+      <c r="H733" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I733" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J733" t="inlineStr">
+        <is>
+          <t>Somente a afirmativa 1 é verdadeira</t>
+        </is>
+      </c>
+      <c r="K733" t="inlineStr">
+        <is>
+          <t>Somente a afirmativa 2 é verdadeira</t>
+        </is>
+      </c>
+      <c r="L733" t="inlineStr">
+        <is>
+          <t>Somente a afirmativa 3 é verdadeira</t>
+        </is>
+      </c>
+      <c r="M733" t="inlineStr">
+        <is>
+          <t>Somente as afirmativas 1 e 3 são verdadeiras</t>
+        </is>
+      </c>
+      <c r="N733" t="inlineStr">
+        <is>
+          <t>Todas as afirmativas são verdadeiras</t>
+        </is>
+      </c>
+      <c r="O733" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P733" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q733" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="n">
+        <v>734</v>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>UFRJ</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>UFRJ</t>
+        </is>
+      </c>
+      <c r="D734" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E734" t="inlineStr">
+        <is>
+          <t>É inegável o papel que a inovação exerce sobre as organizações. A função tecnologia, no âmbito de qualquer organização e, em especial, no âmbito de uma Instituição de Ciência e Tecnologia, como a UFRJ, exerce um papel importante. Como desafio à busca por produção de conhecimentos novos, requer uma gestão estratégica que possa compreender e dar conta de toda a complexidade presente no processo de inovação, ou mesmo, a Cadeia de Conhecimento. Pensar a função tecnologia e realizar a sua gestão é um dos maiores desafios da função tecnologia. Assinale a opção que apresenta os tipos de inovação, segundo o Manual de Oslo.</t>
+        </is>
+      </c>
+      <c r="F734" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G734" t="inlineStr">
+        <is>
+          <t>Gestão da Inovação</t>
+        </is>
+      </c>
+      <c r="H734" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I734" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J734" t="inlineStr">
+        <is>
+          <t>Inovação de Produto, Inovação de Serviços, Inovação de Processos e Inovação Organizacional.</t>
+        </is>
+      </c>
+      <c r="K734" t="inlineStr">
+        <is>
+          <t>Inovação de Produto, Inovação de Processos, Inovação de Marketing e Inovação Organizacional</t>
+        </is>
+      </c>
+      <c r="L734" t="inlineStr">
+        <is>
+          <t>Inovação de Produto, Inovação de Processos, Inovação de Serviços e Inovação de Pessoas.</t>
+        </is>
+      </c>
+      <c r="M734" t="inlineStr">
+        <is>
+          <t>Inovação de Produto, Inovação de Pessoas, Inovação de Marketing e Inovação Organizacional.</t>
+        </is>
+      </c>
+      <c r="N734" t="inlineStr">
+        <is>
+          <t>Inovação de Processos, Inovação de Serviços, Inovação de Pessoas e Inovação Organizacional.</t>
+        </is>
+      </c>
+      <c r="O734" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P734" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q734" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="n">
+        <v>735</v>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>IADES</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>Metrô-DF</t>
+        </is>
+      </c>
+      <c r="D735" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E735" t="inlineStr">
+        <is>
+          <t>De acordo com os conceitos modernos de administração, a inovação leva as organizações e (ou) a nação a uma situação de:</t>
+        </is>
+      </c>
+      <c r="F735" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G735" t="inlineStr">
+        <is>
+          <t>Gestão da Inovação</t>
+        </is>
+      </c>
+      <c r="H735" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I735" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J735" t="inlineStr">
+        <is>
+          <t>aumento de arrecadação.</t>
+        </is>
+      </c>
+      <c r="K735" t="inlineStr">
+        <is>
+          <t>aumento de competitividade.</t>
+        </is>
+      </c>
+      <c r="L735" t="inlineStr">
+        <is>
+          <t>aumento da máquina pública.</t>
+        </is>
+      </c>
+      <c r="M735" t="inlineStr">
+        <is>
+          <t>aumento do custo de vida.</t>
+        </is>
+      </c>
+      <c r="N735" t="inlineStr">
+        <is>
+          <t>diminuição de processos.</t>
+        </is>
+      </c>
+      <c r="O735" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P735" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q735" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="n">
+        <v>736</v>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>IFF</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>RJ</t>
+        </is>
+      </c>
+      <c r="D736" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E736" t="inlineStr">
+        <is>
+          <t>Para que se confirme como inovação, é necessário que a mudança tecnológica lançada por uma organização no mercado</t>
+        </is>
+      </c>
+      <c r="F736" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G736" t="inlineStr">
+        <is>
+          <t>Gestão da Inovação</t>
+        </is>
+      </c>
+      <c r="H736" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I736" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J736" t="inlineStr">
+        <is>
+          <t>tenha valor de troca e valor de uso.</t>
+        </is>
+      </c>
+      <c r="K736" t="inlineStr">
+        <is>
+          <t>tenha valor de uso, ainda que não tenha valor de troca.</t>
+        </is>
+      </c>
+      <c r="L736" t="inlineStr">
+        <is>
+          <t>seja qualitativamente melhor que a tecnologia então vigente.</t>
+        </is>
+      </c>
+      <c r="M736" t="inlineStr">
+        <is>
+          <t>seja tecnicamente viável, ainda que seja inviável economicamente.</t>
+        </is>
+      </c>
+      <c r="N736" t="inlineStr">
+        <is>
+          <t>seja resultado de atividade de pesquisa e desenvolvimento (P&amp;</t>
+        </is>
+      </c>
+      <c r="O736" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P736" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q736" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="n">
+        <v>737</v>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>TJ-CE</t>
+        </is>
+      </c>
+      <c r="D737" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E737" t="inlineStr">
+        <is>
+          <t>Com relação à melhoria de processos, assinale a opção correta. Nesse sentido, considere que a sigla FMEA, sempre que empregada, se refere a failure mode and effect analysis.</t>
+        </is>
+      </c>
+      <c r="F737" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G737" t="inlineStr">
+        <is>
+          <t>Gestão da Manutenção e Confiabilidade</t>
+        </is>
+      </c>
+      <c r="H737" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I737" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J737" t="inlineStr">
+        <is>
+          <t>O processo cuja automação dispensa a intervenção humana apresenta índice de confiabilidade de 99,9%.</t>
+        </is>
+      </c>
+      <c r="K737" t="inlineStr">
+        <is>
+          <t>A automação permite diminuição dos custos de mão de obra direta, porém não possibilita a redução da variabilidade da operação.</t>
+        </is>
+      </c>
+      <c r="L737" t="inlineStr">
+        <is>
+          <t>FMEA consiste em uma ferramenta de gestão da produção que, a partir de uma lista de verificação, identifica possíveis falhas antes de sua ocorrência.</t>
+        </is>
+      </c>
+      <c r="M737" t="inlineStr">
+        <is>
+          <t>Downsizing constitui um mecanismo de diminuição das potenciais falhas de processo.</t>
+        </is>
+      </c>
+      <c r="N737" t="inlineStr">
+        <is>
+          <t>FMEA consiste em uma ferramenta de análise de falhas aplicável apenas a casos de produção de produtos, não sendo empregada na produção de serviços.</t>
+        </is>
+      </c>
+      <c r="O737" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P737" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q737" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="n">
+        <v>738</v>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>UFG</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>CS-UFG</t>
+        </is>
+      </c>
+      <c r="D738" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E738" t="inlineStr">
+        <is>
+          <t>O pensamento “enxuto” considera que devem ser reduzidos os desperdícios de todos os níveis do processo de produção. O gerente de produção de uma determinada empresa participa de um projeto de desenvolvimento de produto, que objetiva obter uma nova plataforma de um modelo já existente na empresa. Levando em consideração o pensamento enxuto, o gerente de produção propõe para a equipe de desenvolvimento o uso da técnica Failure Mode and Effect Analysis (FMEA), tanto no desenvolvimento de produto como no novo processo de produção.
+Considerando as suas especificidades,</t>
+        </is>
+      </c>
+      <c r="F738" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G738" t="inlineStr">
+        <is>
+          <t>Gestão da Manutenção e Confiabilidade</t>
+        </is>
+      </c>
+      <c r="H738" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I738" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J738" t="inlineStr">
+        <is>
+          <t>a elaboração do FMEA de um processo requer como fontes de informações necessárias os dados dos fornecedores.</t>
+        </is>
+      </c>
+      <c r="K738" t="inlineStr">
+        <is>
+          <t>a aplicação da técnica FMEA tem como objetivo aumentar a produtividade do processo.</t>
+        </is>
+      </c>
+      <c r="L738" t="inlineStr">
+        <is>
+          <t>o índice de risco no FMEA resulta da multiplicação entre os índices de severidade (S), ocorrência (O) e detecção (</t>
+        </is>
+      </c>
+      <c r="M738" t="inlineStr">
+        <is>
+          <t>o uso da técnica FMEA no projeto de um novo produto possibilita a redução de dois tipos de desperdícios do pensamento enxuto: defeitos e superprodução.</t>
+        </is>
+      </c>
+      <c r="N738" t="inlineStr"/>
+      <c r="O738" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P738" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q738" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="n">
+        <v>739</v>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>CCV</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>UFC</t>
+        </is>
+      </c>
+      <c r="D739" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E739" t="inlineStr">
+        <is>
+          <t>Para o planejamento e controle da qualidade podem ser usadas diversas ferramentas e técnicas. Sobre estas ferramentas e técnicas é correto dizer que:</t>
+        </is>
+      </c>
+      <c r="F739" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G739" t="inlineStr">
+        <is>
+          <t>Gestão da Manutenção e Confiabilidade</t>
+        </is>
+      </c>
+      <c r="H739" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I739" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J739" t="inlineStr">
+        <is>
+          <t>A folha de verificação é uma ferramenta para desenhar o processo.</t>
+        </is>
+      </c>
+      <c r="K739" t="inlineStr">
+        <is>
+          <t>A análise de Pareto procura identificar as causas que estão gerando determinado efeito no processo.</t>
+        </is>
+      </c>
+      <c r="L739" t="inlineStr">
+        <is>
+          <t>A técnica FMEA é utilizada para avaliação e redução de riscos e falhas em projetos e processos.</t>
+        </is>
+      </c>
+      <c r="M739" t="inlineStr">
+        <is>
+          <t>As cartas de controle do processo relacionam os principais fatores que estão provocando os maiores efeitos.</t>
+        </is>
+      </c>
+      <c r="N739" t="inlineStr">
+        <is>
+          <t>O histograma é uma ferramenta para identificar as possíveis correlações entre os problemas e o tempo ou entre problemas e suas possíveis causas.</t>
+        </is>
+      </c>
+      <c r="O739" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P739" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q739" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>740</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>RLU-DF</t>
+        </is>
+      </c>
+      <c r="D740" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E740" t="inlineStr">
+        <is>
+          <t>Com relação à análise das causas raízes de falha (RCFA) e à análise de modos de efeitos de falhas (FMEA), julgue o item a seguir.
+RCFA é o método qualitativo de análise de confiabilidade que envolve o estudo dos modos de falha, especialmente em equipamentos industriais, que podem ocorrer em cada item, o que determina os efeitos de cada modo de falha sobre outros itens e sobre a função específica do conjunto.</t>
+        </is>
+      </c>
+      <c r="F740" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G740" t="inlineStr">
+        <is>
+          <t>Gestão da Manutenção e Confiabilidade</t>
+        </is>
+      </c>
+      <c r="H740" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I740" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J740" t="inlineStr">
+        <is>
+          <t>I, somente.</t>
+        </is>
+      </c>
+      <c r="K740" t="inlineStr">
+        <is>
+          <t>II, somente.</t>
+        </is>
+      </c>
+      <c r="L740" t="inlineStr">
+        <is>
+          <t>III, somente.</t>
+        </is>
+      </c>
+      <c r="M740" t="inlineStr">
+        <is>
+          <t>I e II, somente.</t>
+        </is>
+      </c>
+      <c r="N740" t="inlineStr">
+        <is>
+          <t>I, II e III.</t>
+        </is>
+      </c>
+      <c r="O740" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P740" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q740" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="n">
+        <v>741</v>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>RLU-DF</t>
+        </is>
+      </c>
+      <c r="D741" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E741" t="inlineStr">
+        <is>
+          <t>Com relação à análise das causas raízes de falha (RCFA) e à análise de modos de efeitos de falhas (FMEA), julgue o item a seguir.
+A identificação das possíveis causas do problema é um dos passos da RCFA, análise que pode ser considerada uma simplificação da FMEA, sendo esta entendida como um método lógico quantitativo cujo objetivo é identificar as combinações das falhas nos equipamentos ou componentes de um sistema ou nos erros humanos que possam resultar em um evento ou acidente.</t>
+        </is>
+      </c>
+      <c r="F741" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G741" t="inlineStr">
+        <is>
+          <t>Gestão da Manutenção e Confiabilidade</t>
+        </is>
+      </c>
+      <c r="H741" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I741" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J741" t="inlineStr"/>
+      <c r="K741" t="inlineStr"/>
+      <c r="L741" t="inlineStr"/>
+      <c r="M741" t="inlineStr"/>
+      <c r="N741" t="inlineStr"/>
+      <c r="O741" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P741" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q741" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="n">
+        <v>742</v>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>CESPE</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>RLU-DF</t>
+        </is>
+      </c>
+      <c r="D742" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E742" t="inlineStr">
+        <is>
+          <t>Com relação à análise das causas raízes de falha (RCFA) e à análise de modos de efeitos de falhas (FMEA), julgue o item a seguir.
+Para superar deficiências do projeto, a FMEA de projeto não enfatiza o controle dos processos implantados.</t>
+        </is>
+      </c>
+      <c r="F742" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G742" t="inlineStr">
+        <is>
+          <t>Gestão da Manutenção e Confiabilidade</t>
+        </is>
+      </c>
+      <c r="H742" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I742" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="J742" t="inlineStr"/>
+      <c r="K742" t="inlineStr"/>
+      <c r="L742" t="inlineStr"/>
+      <c r="M742" t="inlineStr"/>
+      <c r="N742" t="inlineStr"/>
+      <c r="O742" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P742" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q742" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="n">
+        <v>743</v>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="E743" t="inlineStr">
+        <is>
+          <t>A principal característica da manutenção produtiva total (TPM) é a:</t>
+        </is>
+      </c>
+      <c r="F743" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G743" t="inlineStr">
+        <is>
+          <t>Gestão da Manutenção e Confiabilidade</t>
+        </is>
+      </c>
+      <c r="H743" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I743" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J743" t="inlineStr">
+        <is>
+          <t>realização de paradas em intervalos regulares.</t>
+        </is>
+      </c>
+      <c r="K743" t="inlineStr">
+        <is>
+          <t>transformação do operador do equipamento em um parceiro na sua manutenção.</t>
+        </is>
+      </c>
+      <c r="L743" t="inlineStr">
+        <is>
+          <t>detecção do início da degradação de um componente, o controle do seu avanço e a antevisão do limite aceitável dessa degradação</t>
+        </is>
+      </c>
+      <c r="M743" t="inlineStr">
+        <is>
+          <t>paralisação do equipamento sempre que ocorrer o desvio de algum parâmetro que está sendo monitorado.</t>
+        </is>
+      </c>
+      <c r="N743" t="inlineStr">
+        <is>
+          <t>realização do serviço em um equipamento sob falha, justamente para sanar essa falha.</t>
+        </is>
+      </c>
+      <c r="O743" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P743" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q743" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="n">
+        <v>744</v>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>FGV</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>TJ-AM</t>
+        </is>
+      </c>
+      <c r="D744" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E744" t="inlineStr">
+        <is>
+          <t>O Quebra Zero, na filosofia da Manutenção Produtiva Total (TPM), é o principal fator que prejudica o rendimento operacional. As máquinas devem ser projetadas para trabalhar com zero defeito e algumas medidas são fundamentais para obtenção e conquista da quebra zero.
+I. A máquina não pode parar durante o período em que foi programada para operar consiste na filosofia do Quebra Zero.
+II. Fazer previsão da vida média através de técnicas de diagnóstico consiste em sanar os pontos falhos decorrentes de projeto.
+III. Limpeza da área, asseio e ordem determina uma estruturação das condições básicas para a operação.
+Assinale:</t>
+        </is>
+      </c>
+      <c r="F744" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G744" t="inlineStr">
+        <is>
+          <t>Gestão da Manutenção e Confiabilidade</t>
+        </is>
+      </c>
+      <c r="H744" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I744" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J744" t="inlineStr">
+        <is>
+          <t>se somente a afirmativa I estiver correta.</t>
+        </is>
+      </c>
+      <c r="K744" t="inlineStr">
+        <is>
+          <t>se somente a afirmativa II estiver correta.</t>
+        </is>
+      </c>
+      <c r="L744" t="inlineStr">
+        <is>
+          <t>se somente as afirmativas I e II estiverem corretas.</t>
+        </is>
+      </c>
+      <c r="M744" t="inlineStr">
+        <is>
+          <t>se somente as afirmativas I e III estiverem corretas.</t>
+        </is>
+      </c>
+      <c r="N744" t="inlineStr">
+        <is>
+          <t>se todas as afirmativas estiverem corretas.</t>
+        </is>
+      </c>
+      <c r="O744" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P744" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q744" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="n">
+        <v>745</v>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>FGV</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>TJ-GO</t>
+        </is>
+      </c>
+      <c r="D745" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E745" t="inlineStr">
+        <is>
+          <t>O 5S é geralmente tratado dentro do pilar “Manutenção Autônoma” do TPM. Em empresas que têm sérios problemas de ordem comportamental e cultural, os quais estão espelhados nos aspectos de desperdício, desarrumação, sujeira, acidentes, doenças ocupacionais e indisciplina, o 5S deve ser tratado como uma base para mudança dos hábitos, atitudes e valores das pessoas, repercutindo numa preparação ambiental propícia à implantação do TPM. Considerandose seus principais benefícios, é correto afirmar que o 5S:</t>
+        </is>
+      </c>
+      <c r="F745" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G745" t="inlineStr">
+        <is>
+          <t>Gestão da Manutenção e Confiabilidade</t>
+        </is>
+      </c>
+      <c r="H745" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I745" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J745" t="inlineStr">
+        <is>
+          <t>combate as perdas através de estudos técnicos da produção</t>
+        </is>
+      </c>
+      <c r="K745" t="inlineStr">
+        <is>
+          <t>tem uma visão mais funcional que o TPM com relação ao zelo pelos equipamentos;</t>
+        </is>
+      </c>
+      <c r="L745" t="inlineStr">
+        <is>
+          <t>busca padronizar também as atividades de operação e manutenção;</t>
+        </is>
+      </c>
+      <c r="M745" t="inlineStr">
+        <is>
+          <t>quanto à higiene, tem uma preocupação mais voltada para o bem estar dos ambientes;</t>
+        </is>
+      </c>
+      <c r="N745" t="inlineStr">
+        <is>
+          <t>tem uma preocupação com redução de perdas de produto e contaminação do meio ambiente pelos equipamentos.</t>
+        </is>
+      </c>
+      <c r="O745" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P745" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q745" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="n">
+        <v>746</v>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>FAURGS</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>TJ-RS</t>
+        </is>
+      </c>
+      <c r="D746" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E746" t="inlineStr">
+        <is>
+          <t>Que tipo de manutenção inclui todas as ações necessárias para que um equipamento passe do estado falho para o estado operacional ou disponível</t>
+        </is>
+      </c>
+      <c r="F746" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G746" t="inlineStr">
+        <is>
+          <t>Gestão da Manutenção e Confiabilidade</t>
+        </is>
+      </c>
+      <c r="H746" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I746" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J746" t="inlineStr">
+        <is>
+          <t>Preventiva baseada na condição.</t>
+        </is>
+      </c>
+      <c r="K746" t="inlineStr">
+        <is>
+          <t>Preventiva baseada no tempo.</t>
+        </is>
+      </c>
+      <c r="L746" t="inlineStr">
+        <is>
+          <t>Preventiva.</t>
+        </is>
+      </c>
+      <c r="M746" t="inlineStr">
+        <is>
+          <t>Corretiva.</t>
+        </is>
+      </c>
+      <c r="N746" t="inlineStr">
+        <is>
+          <t>Preventiva planejada.</t>
+        </is>
+      </c>
+      <c r="O746" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P746" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q746" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="n">
+        <v>747</v>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D747" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="E747" t="inlineStr">
+        <is>
+          <t>Manutenção é o termo usado para abordar a forma pela qual as organizações tentam evitar as falhas cuidando de suas instalações físicas.
+Quando a falha é previsível, a abordagem que visa a realizar manutenção somente quando as instalações precisarem dela, antes da quebra, é denominada manutenção</t>
+        </is>
+      </c>
+      <c r="F747" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G747" t="inlineStr">
+        <is>
+          <t>Gestão da Manutenção e Confiabilidade</t>
+        </is>
+      </c>
+      <c r="H747" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I747" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J747" t="inlineStr">
+        <is>
+          <t>Automática</t>
+        </is>
+      </c>
+      <c r="K747" t="inlineStr">
+        <is>
+          <t>Conservadora</t>
+        </is>
+      </c>
+      <c r="L747" t="inlineStr">
+        <is>
+          <t>Corretiva</t>
+        </is>
+      </c>
+      <c r="M747" t="inlineStr">
+        <is>
+          <t>Preventiva</t>
+        </is>
+      </c>
+      <c r="N747" t="inlineStr">
+        <is>
+          <t>Preditiva</t>
+        </is>
+      </c>
+      <c r="O747" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P747" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q747" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="n">
+        <v>748</v>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>PETROBRAS</t>
+        </is>
+      </c>
+      <c r="D748" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E748" t="inlineStr">
+        <is>
+          <t>A gestão da manutenção como função estratégica das organizações é diretamente responsável pela disponibilidade dos ativos, tendo importância fundamental nos resultados das organizações. Esses resultados serão tanto melhores quanto mais eficaz for a gestão da manutenção.
+São métodos de manutenção os listados a seguir, EXCETO o de manutenção</t>
+        </is>
+      </c>
+      <c r="F748" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G748" t="inlineStr">
+        <is>
+          <t>Gestão da Manutenção e Confiabilidade</t>
+        </is>
+      </c>
+      <c r="H748" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I748" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J748" t="inlineStr">
+        <is>
+          <t>temporal</t>
+        </is>
+      </c>
+      <c r="K748" t="inlineStr">
+        <is>
+          <t>preventiva</t>
+        </is>
+      </c>
+      <c r="L748" t="inlineStr">
+        <is>
+          <t>corretiva</t>
+        </is>
+      </c>
+      <c r="M748" t="inlineStr">
+        <is>
+          <t>preditiva</t>
+        </is>
+      </c>
+      <c r="N748" t="inlineStr">
+        <is>
+          <t>produtiva total</t>
+        </is>
+      </c>
+      <c r="O748" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P748" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q748" t="n">
+        <v>0</v>
+      </c>
+      <c r="R748" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
:lady_beetle: correção do sistema não consegui captar os gabaritos dos pdfs extras de questos em CE, além de conseguir resolver os casos onde as letras das alternativas estão entre parênteses
</commit_message>
<xml_diff>
--- a/banco_de_dados/questoes_concurso.xlsx
+++ b/banco_de_dados/questoes_concurso.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R748"/>
+  <dimension ref="A1:R762"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -62526,7 +62526,1147 @@
       <c r="Q748" t="n">
         <v>0</v>
       </c>
-      <c r="R748" t="inlineStr"/>
+    </row>
+    <row r="749">
+      <c r="A749" t="n">
+        <v>749</v>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>FCM</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>CEFETMINAS</t>
+        </is>
+      </c>
+      <c r="D749" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="E749" t="inlineStr">
+        <is>
+          <t>É fundamental que o conhecimento tácito e o conhecimento explícito se relacionem em sinergia nas empresas e nos órgãos públicos.
+Avalie as definições sobre a construção
+( ) Socialização: o conhecimento tácito é repassado por meio de experiências.
+( ) Exteriorização: o conhecimento tácito é traduzido em conceitos explícitos, por meio da utilização de metáforas, analogias e símbolos.
+( ) Combinação: o conhecimento explícito é construído reunindo conhecimentos explícitos provenientes de várias fontes.de conhecimento.
+( ) Internalização: é o final do ciclo, o conhecimento explícito, após ser internalizado, não passa novamente a ser um conhecimento tácito.
+De acordo com as definições, a sequência correta é:</t>
+        </is>
+      </c>
+      <c r="F749" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G749" t="inlineStr">
+        <is>
+          <t>Gestão do Conhecimento e Tecnologia</t>
+        </is>
+      </c>
+      <c r="H749" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I749" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J749" t="inlineStr">
+        <is>
+          <t>V, V, V, F</t>
+        </is>
+      </c>
+      <c r="K749" t="inlineStr">
+        <is>
+          <t>V, F, F, V</t>
+        </is>
+      </c>
+      <c r="L749" t="inlineStr">
+        <is>
+          <t>F, V, F, F</t>
+        </is>
+      </c>
+      <c r="M749" t="inlineStr">
+        <is>
+          <t>F, F, V, V</t>
+        </is>
+      </c>
+      <c r="N749" t="inlineStr"/>
+      <c r="O749" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P749" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q749" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="n">
+        <v>750</v>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>Transpetro</t>
+        </is>
+      </c>
+      <c r="D750" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E750" t="inlineStr">
+        <is>
+          <t>O que é o conceito de bullwhip-effect (efeito chicote) em uma cadeia de suprimento?</t>
+        </is>
+      </c>
+      <c r="F750" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G750" t="inlineStr">
+        <is>
+          <t>Gestão da Cadeia de Suprimentos</t>
+        </is>
+      </c>
+      <c r="H750" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I750" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J750" t="inlineStr">
+        <is>
+          <t>Um tipo de equipamento de transporte utilizado para movimentar mercadorias em longas distâncias.</t>
+        </is>
+      </c>
+      <c r="K750" t="inlineStr">
+        <is>
+          <t>A variação sazonal na demanda por produtos.</t>
+        </is>
+      </c>
+      <c r="L750" t="inlineStr">
+        <is>
+          <t>A amplificação da demanda, à medida que se move da ponta do consumidor de uma cadeia de suprimento para o fornecedor.</t>
+        </is>
+      </c>
+      <c r="M750" t="inlineStr">
+        <is>
+          <t>Um método de avaliação de fornecedores com base em suas classificações.</t>
+        </is>
+      </c>
+      <c r="N750" t="inlineStr">
+        <is>
+          <t>A velocidade com que os produtos são entregues aos clientes.</t>
+        </is>
+      </c>
+      <c r="O750" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P750" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q750" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="n">
+        <v>751</v>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>Transpetro</t>
+        </is>
+      </c>
+      <c r="D751" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E751" t="inlineStr">
+        <is>
+          <t>As três dimensões da sustentabilidade, segundo o conceito de triple bottom line, são as seguintes:</t>
+        </is>
+      </c>
+      <c r="F751" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G751" t="inlineStr">
+        <is>
+          <t>Sustentabilidade</t>
+        </is>
+      </c>
+      <c r="H751" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I751" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J751" t="inlineStr">
+        <is>
+          <t>econômica, política e ambiental</t>
+        </is>
+      </c>
+      <c r="K751" t="inlineStr">
+        <is>
+          <t>social, econômica e cultural</t>
+        </is>
+      </c>
+      <c r="L751" t="inlineStr">
+        <is>
+          <t>ambiental, econômica e social</t>
+        </is>
+      </c>
+      <c r="M751" t="inlineStr">
+        <is>
+          <t>cultural, ambiental e social</t>
+        </is>
+      </c>
+      <c r="N751" t="inlineStr">
+        <is>
+          <t>política, cultural e social.</t>
+        </is>
+      </c>
+      <c r="O751" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P751" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q751" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="n">
+        <v>752</v>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>Transpetro</t>
+        </is>
+      </c>
+      <c r="D752" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E752" t="inlineStr">
+        <is>
+          <t>O seguinte critério é usado para avaliar a qualidade e a maturidade de um sistema organizacional na engenharia organizacional:</t>
+        </is>
+      </c>
+      <c r="F752" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G752" t="inlineStr">
+        <is>
+          <t>Engenharia Organizacional</t>
+        </is>
+      </c>
+      <c r="H752" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I752" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J752" t="inlineStr">
+        <is>
+          <t>Critério EFQM</t>
+        </is>
+      </c>
+      <c r="K752" t="inlineStr">
+        <is>
+          <t>Critério CMMI</t>
+        </is>
+      </c>
+      <c r="L752" t="inlineStr">
+        <is>
+          <t>Critério ISO 9001</t>
+        </is>
+      </c>
+      <c r="M752" t="inlineStr">
+        <is>
+          <t>Critério PDCA</t>
+        </is>
+      </c>
+      <c r="N752" t="inlineStr">
+        <is>
+          <t>Critério COBIT</t>
+        </is>
+      </c>
+      <c r="O752" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P752" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q752" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="n">
+        <v>753</v>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>Transpetro</t>
+        </is>
+      </c>
+      <c r="D753" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E753" t="inlineStr">
+        <is>
+          <t>Qual abordagem de engenharia organizacional se concentra na adequação entre contexto, estrutura e desempenho das empresas?</t>
+        </is>
+      </c>
+      <c r="F753" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G753" t="inlineStr">
+        <is>
+          <t>Engenharia Organizacional</t>
+        </is>
+      </c>
+      <c r="H753" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I753" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J753" t="inlineStr">
+        <is>
+          <t>Teoria das Relações Humanas</t>
+        </is>
+      </c>
+      <c r="K753" t="inlineStr">
+        <is>
+          <t>Teoria da Contingência</t>
+        </is>
+      </c>
+      <c r="L753" t="inlineStr">
+        <is>
+          <t>Teoria institucional</t>
+        </is>
+      </c>
+      <c r="M753" t="inlineStr">
+        <is>
+          <t>Gestão por Objetivos (MBO)</t>
+        </is>
+      </c>
+      <c r="N753" t="inlineStr">
+        <is>
+          <t>Benchmarking</t>
+        </is>
+      </c>
+      <c r="O753" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P753" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q753" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="n">
+        <v>754</v>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>Transpetro</t>
+        </is>
+      </c>
+      <c r="D754" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E754" t="inlineStr">
+        <is>
+          <t>O grande volume de dados gerados por sensores, máquinas e equipamentos na Indústria 4.0 é chamado, em sistemas de informação, de Big Data. Para funcionar de forma eficiente, o Big Data tem alguns atributos chamados de Vs do Big Data.
+Esses atributos são</t>
+        </is>
+      </c>
+      <c r="F754" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G754" t="inlineStr">
+        <is>
+          <t>Gestão do Conhecimento e Tecnologia</t>
+        </is>
+      </c>
+      <c r="H754" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I754" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J754" t="inlineStr">
+        <is>
+          <t>Velocidade, Volume, Variedade, Veracidade, Valor</t>
+        </is>
+      </c>
+      <c r="K754" t="inlineStr">
+        <is>
+          <t>Velocidade, Volume, Variedade, Veracidade, Vigência</t>
+        </is>
+      </c>
+      <c r="L754" t="inlineStr">
+        <is>
+          <t>Velocidade, Volume, Variedade, Veracidade, Valor, Viabilidade</t>
+        </is>
+      </c>
+      <c r="M754" t="inlineStr">
+        <is>
+          <t>Velocidade, Volume, Variedade, Veracidade, Valor, Viabilidade, Vigência</t>
+        </is>
+      </c>
+      <c r="N754" t="inlineStr">
+        <is>
+          <t>Velocidade, Variedade, Veracidade, Valor, Viabilidade, Vigência</t>
+        </is>
+      </c>
+      <c r="O754" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P754" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q754" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="n">
+        <v>755</v>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>Transpetro</t>
+        </is>
+      </c>
+      <c r="D755" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E755" t="inlineStr">
+        <is>
+          <t>O termo Indústria 4.0 foi cunhado em 2011 na feira de Hanover, na Alemanha, para designar fábricas inteligentes onde os sistemas físicos e virtuais cooperam de forma global e flexível.
+Essa colaboração é propiciada pelas seguintes tecnologias habilitadoras</t>
+        </is>
+      </c>
+      <c r="F755" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G755" t="inlineStr">
+        <is>
+          <t>Gestão do Conhecimento e Tecnologia</t>
+        </is>
+      </c>
+      <c r="H755" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I755" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J755" t="inlineStr">
+        <is>
+          <t>Internet das Coisas ou Internet Of Things (Iot), Simulação Digital, Cyber-Security ou Segurança Digital, Integração de Sistemas</t>
+        </is>
+      </c>
+      <c r="K755" t="inlineStr">
+        <is>
+          <t>Robôs Autônomos, Internet das Coisas ou Internet Of Things (Iot), Cyber-Security ou Segurança Digital, Computação na Nuvem, Manufatura Aditiva, Big Data, Realidade Aumentada (“Augmented Reality”)</t>
+        </is>
+      </c>
+      <c r="L755" t="inlineStr">
+        <is>
+          <t>Robôs Autônomos, Internet das Coisas ou Internet Of Things (Iot), Simulação Digital, Cyber-Security ou Segurança Digital, Integração de Sistemas, Computação na Nuvem, Manufatura Aditiva, Big Data.</t>
+        </is>
+      </c>
+      <c r="M755" t="inlineStr">
+        <is>
+          <t>Robôs Autônomos, Internet das Coisas ou Internet Of Things (Iot), Simulação Digital, Integração de Sistemas, Computação na Nuvem, Manufatura Aditiva, Big Data, Realidade Aumentada (“Augmented Reality”).</t>
+        </is>
+      </c>
+      <c r="N755" t="inlineStr">
+        <is>
+          <t>Robôs Autônomos, Internet das Coisas ou Internet Of Things (Iot), Simulação Digital, Cyber-Security ou Segurança Digital, Integração de Sistemas, Computação na Nuvem, Manufatura Aditiva, Big Data, Realidade Aumentada (“Augmented Reality”).</t>
+        </is>
+      </c>
+      <c r="O755" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P755" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q755" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="n">
+        <v>756</v>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>Transpetro</t>
+        </is>
+      </c>
+      <c r="D756" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E756" t="inlineStr">
+        <is>
+          <t>O bom gerenciamento da cadeia de suprimentos é fundamental para as empresas, por tratar-se da(o)</t>
+        </is>
+      </c>
+      <c r="F756" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G756" t="inlineStr">
+        <is>
+          <t>Gestão da Cadeia de Suprimentos</t>
+        </is>
+      </c>
+      <c r="H756" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I756" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J756" t="inlineStr">
+        <is>
+          <t>estrutura organizacional que define as responsabilidades, as funções e as relações entre os diferentes agentes da logística empresarial.(</t>
+        </is>
+      </c>
+      <c r="K756" t="inlineStr">
+        <is>
+          <t>rede de organizações envolvidas na produção, na transformação e na distribuição de um produto ou serviço desde os fornecedores até os clientes finais.(</t>
+        </is>
+      </c>
+      <c r="L756" t="inlineStr">
+        <is>
+          <t>sistema de informação que integra e coordena os dados e os fluxos de informação entre os diversos elos da logística empresarial.(</t>
+        </is>
+      </c>
+      <c r="M756" t="inlineStr">
+        <is>
+          <t>conjunto de processos que ligam as atividades de planejamento, de execução e de controle da logística empresarial em uma organização.(</t>
+        </is>
+      </c>
+      <c r="N756" t="inlineStr">
+        <is>
+          <t>modelo de gestão que busca otimizar o desempenho da logística empresarial por meio da melhoria contínua dos processos e da qualidade</t>
+        </is>
+      </c>
+      <c r="O756" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P756" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q756" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="n">
+        <v>757</v>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>Transpetro</t>
+        </is>
+      </c>
+      <c r="D757" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E757" t="inlineStr">
+        <is>
+          <t>Sobre a diferença entre logística inbound e outbound, tem-se que a logística inbound é a que se refere ao fluxo de bens e serviços</t>
+        </is>
+      </c>
+      <c r="F757" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G757" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="H757" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I757" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J757" t="inlineStr">
+        <is>
+          <t>que entram na organização, enquanto a logística outbound é a que se refere ao fluxo de bens e serviços que saem da organização.</t>
+        </is>
+      </c>
+      <c r="K757" t="inlineStr">
+        <is>
+          <t>que saem da organização, enquanto a logística outbound é a que se refere ao fluxo de bens e serviços que entram na organização.</t>
+        </is>
+      </c>
+      <c r="L757" t="inlineStr">
+        <is>
+          <t>entre a organização e seus fornecedores, enquanto a logística outbound é a que se refere ao fluxo de bens e serviços entre a organização e seus clientes.</t>
+        </is>
+      </c>
+      <c r="M757" t="inlineStr">
+        <is>
+          <t>entre a organização e seus clientes, enquanto a logística outbound é a que se refere ao fluxo de bens e serviços entre a organização e seus fornecedores.</t>
+        </is>
+      </c>
+      <c r="N757" t="inlineStr">
+        <is>
+          <t>dentro da organização, enquanto a logística outbound é a que se refere ao fluxo de bens e serviços fora da organização.</t>
+        </is>
+      </c>
+      <c r="O757" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P757" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q757" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="n">
+        <v>758</v>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>Transpetro</t>
+        </is>
+      </c>
+      <c r="D758" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E758" t="inlineStr">
+        <is>
+          <t>Um Centro de Distribuição (CD) é uma</t>
+        </is>
+      </c>
+      <c r="F758" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G758" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="H758" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I758" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J758" t="inlineStr">
+        <is>
+          <t>rede de canais de distribuição que conecta os produtores aos consumidores finais.</t>
+        </is>
+      </c>
+      <c r="K758" t="inlineStr">
+        <is>
+          <t>área geográfica onde se concentram os clientes potenciais ou efetivos de um determinado produto ou serviço.</t>
+        </is>
+      </c>
+      <c r="L758" t="inlineStr">
+        <is>
+          <t>instalação física onde são armazenados temporariamente os produtos acabados antes de serem enviados aos clientes finais.</t>
+        </is>
+      </c>
+      <c r="M758" t="inlineStr">
+        <is>
+          <t>estratégia de marketing que visa aumentar a disponibilidade, a acessibilidade e a visibilidade dos produtos no mercado.</t>
+        </is>
+      </c>
+      <c r="N758" t="inlineStr">
+        <is>
+          <t>unidade operacional onde são realizadas as atividades de recebimento, de armazenagem, de separação, de embalagem e de expedição dos produtos ao longo da cadeia de suprimentos.</t>
+        </is>
+      </c>
+      <c r="O758" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="P758" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q758" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="n">
+        <v>759</v>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>Transpetro</t>
+        </is>
+      </c>
+      <c r="D759" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E759" t="inlineStr">
+        <is>
+          <t>O sistema dutoviário de transportes no Brasil é aquele que utiliza tubulações para transportar produtos. Esse modal surgiu no país na década de 50 e tem algumas vantagens, como baixo custo operacional, alta capacidade de carga, menor emissão de poluentes, maior segurança e funcionamento contínuo. Por outro lado, também tem algumas desvantagens, como baixa velocidade, pouca flexibilidade de destinos e de produtos e infraestrutura precária.
+Considerando-se o exposto, quais são os principais produtos transportados pelo modal dutoviário no Brasil?</t>
+        </is>
+      </c>
+      <c r="F759" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G759" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="H759" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I759" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J759" t="inlineStr">
+        <is>
+          <t>Óleo, carvão, cimento e água</t>
+        </is>
+      </c>
+      <c r="K759" t="inlineStr">
+        <is>
+          <t>Óleo, gás, minério e sal-gema</t>
+        </is>
+      </c>
+      <c r="L759" t="inlineStr">
+        <is>
+          <t>Óleo, minério, sal-gema e carvão</t>
+        </is>
+      </c>
+      <c r="M759" t="inlineStr">
+        <is>
+          <t>Gás, sal-gema, cimento e água</t>
+        </is>
+      </c>
+      <c r="N759" t="inlineStr">
+        <is>
+          <t>Minério, carvão, cimento e água.</t>
+        </is>
+      </c>
+      <c r="O759" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P759" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q759" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="n">
+        <v>760</v>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>Transpetro</t>
+        </is>
+      </c>
+      <c r="D760" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E760" t="inlineStr">
+        <is>
+          <t>Buscando atender à demanda de clientes, a manufatura utiliza três principais estratégias: antecipação da demanda, aumentando a capacidade produtiva antes que a demanda ocorra; seguimento da demanda, aguardando que a demanda ultrapasse a capacidade produtiva para aumentar a capacidade; e uma estratégia mista, combinando antecipação e seguimento da demanda.
+Em indústrias de fluxo contínuo de produção, como siderúrgicas ou fábricas de celulose, a estratégia mais utilizada é a de seguir a demanda, pois nesse tipo de indústria</t>
+        </is>
+      </c>
+      <c r="F760" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G760" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="H760" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I760" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J760" t="inlineStr">
+        <is>
+          <t>a complexidade do processo produtivo em fluxo contínuo exige maior tempo de planejamento para expandir.</t>
+        </is>
+      </c>
+      <c r="K760" t="inlineStr">
+        <is>
+          <t>a demanda tem uma grande elasticidade, e os cliente aguardam as expansões.</t>
+        </is>
+      </c>
+      <c r="L760" t="inlineStr">
+        <is>
+          <t>os tempos de realização da expansão são demasiadamente longos.</t>
+        </is>
+      </c>
+      <c r="M760" t="inlineStr">
+        <is>
+          <t>os valores financeiros necessários para a expansão são muito altos, tornando a antecipação inviável.</t>
+        </is>
+      </c>
+      <c r="N760" t="inlineStr">
+        <is>
+          <t>os fornecedores de máquinas e equipamentos para a indústria de fluxo contínuo demandam maior tempo de entrega.</t>
+        </is>
+      </c>
+      <c r="O760" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P760" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q760" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="n">
+        <v>761</v>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>Transpetro</t>
+        </is>
+      </c>
+      <c r="D761" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E761" t="inlineStr">
+        <is>
+          <t>Qual é a diferença entre missão e visão no planejamento estratégico?</t>
+        </is>
+      </c>
+      <c r="F761" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G761" t="inlineStr">
+        <is>
+          <t>Engenharia Organizacional</t>
+        </is>
+      </c>
+      <c r="H761" t="inlineStr">
+        <is>
+          <t>Fácil</t>
+        </is>
+      </c>
+      <c r="I761" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J761" t="inlineStr">
+        <is>
+          <t>Missão é a razão de ser da empresa, e visão é a situação desejada para o futuro.(</t>
+        </is>
+      </c>
+      <c r="K761" t="inlineStr">
+        <is>
+          <t>Missão é a situação desejada para o futuro, e visão é a razão de ser da empresa.(</t>
+        </is>
+      </c>
+      <c r="L761" t="inlineStr">
+        <is>
+          <t>Missão é o conjunto de valores que guiam as decisões da empresa, e visão é o diferencial competitivo que ela oferece.(</t>
+        </is>
+      </c>
+      <c r="M761" t="inlineStr">
+        <is>
+          <t>Missão é o diferencial competitivo que a empresa oferece, e visão é o conjunto de valores que guiam as decisões da empresa.(</t>
+        </is>
+      </c>
+      <c r="N761" t="inlineStr">
+        <is>
+          <t>Missão e visão são sinônimos no planejamento estratégico.</t>
+        </is>
+      </c>
+      <c r="O761" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P761" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q761" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="n">
+        <v>762</v>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Cesgranrio</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>Transpetro</t>
+        </is>
+      </c>
+      <c r="D762" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E762" t="inlineStr">
+        <is>
+          <t>No planejamento estratégico, quais são as características das metas SMART?</t>
+        </is>
+      </c>
+      <c r="F762" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="G762" t="inlineStr">
+        <is>
+          <t>Engenharia Organizacional</t>
+        </is>
+      </c>
+      <c r="H762" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="I762" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="J762" t="inlineStr">
+        <is>
+          <t>Simples, Mensuráveis, Alcançáveis, Relevantes e Temporais</t>
+        </is>
+      </c>
+      <c r="K762" t="inlineStr">
+        <is>
+          <t>Específicas, Mensuráveis, Atribuíveis, Realistas e Temporais</t>
+        </is>
+      </c>
+      <c r="L762" t="inlineStr">
+        <is>
+          <t>Específicas, Mensuráveis, Alcançáveis, Relevantes e Temporais</t>
+        </is>
+      </c>
+      <c r="M762" t="inlineStr">
+        <is>
+          <t>Estratégicas, Mensuráveis, Ajustáveis, Realistas e Temporais</t>
+        </is>
+      </c>
+      <c r="N762" t="inlineStr">
+        <is>
+          <t>Estratégicas, Mensuráveis, Alcançáveis, Responsáveis e Temporais</t>
+        </is>
+      </c>
+      <c r="O762" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P762" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q762" t="n">
+        <v>0</v>
+      </c>
+      <c r="R762" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>